<commit_message>
refactor: chart color change
</commit_message>
<xml_diff>
--- a/DBLP-OpenAlex-testing/zeroshot-entity-aligned-DBLP-OpenAlex/zero_shot_mistral_dblp_openalex_results_comparison.xlsx
+++ b/DBLP-OpenAlex-testing/zeroshot-entity-aligned-DBLP-OpenAlex/zero_shot_mistral_dblp_openalex_results_comparison.xlsx
@@ -160,22 +160,22 @@
     <t>What is the average number of co-authors for research papers published by Gustaf S\u00F6derlind?</t>
   </si>
   <si>
-    <t>['https://semopenalex.org/work/W2805460435', 'https://semopenalex.org/work/W2788968669', 'https://semopenalex.org/work/W3134422373', 'https://semopenalex.org/work/W4390737683', 'https://semopenalex.org/work/W3202715770', 'https://semopenalex.org/work/W2957110867', 'https://semopenalex.org/work/W2100407406', 'https://semopenalex.org/work/W3048792033', 'https://semopenalex.org/work/W4406267825', 'https://semopenalex.org/work/W2844810377', 'https://semopenalex.org/work/W3205075200', 'https://semopenalex.org/work/W2974444355', 'https://semopenalex.org/work/W2897762537', 'https://semopenalex.org/work/W2996342798', 'https://semopenalex.org/work/W3158463786', 'https://semopenalex.org/work/W4396568545', 'https://semopenalex.org/work/W2397277866', 'https://semopenalex.org/work/W2772966323', 'https://semopenalex.org/work/W2792290921', 'https://semopenalex.org/work/W2979701877', 'https://semopenalex.org/work/W2948196949', 'https://semopenalex.org/work/W4206136166', 'https://semopenalex.org/work/W2780277126', 'https://semopenalex.org/work/W4238294234', 'https://semopenalex.org/work/W4293863370', 'https://semopenalex.org/work/W2226359063', 'https://semopenalex.org/work/W2996971450', 'https://semopenalex.org/work/W4367671449', 'https://semopenalex.org/work/W1999760195', 'https://semopenalex.org/work/W2903944530']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4386065896', 'https://semopenalex.org/work/W4403094633', 'https://semopenalex.org/work/W4312804251', 'https://semopenalex.org/work/W4390604119']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/source/S81770430', 'https://semopenalex.org/source/S191726168', 'https://semopenalex.org/source/S2764455111', 'https://semopenalex.org/source/S78082969', 'https://semopenalex.org/source/S144771191', 'https://semopenalex.org/source/S4306400806', 'https://semopenalex.org/source/S4306515065', 'https://semopenalex.org/source/S161516442', 'https://semopenalex.org/source/S4363608094', 'https://semopenalex.org/source/S4306531565', 'https://semopenalex.org/source/S4210168194', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S4363608845', 'https://semopenalex.org/source/S4306402492', 'https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S2492086750', 'https://semopenalex.org/source/S4363608762', 'https://semopenalex.org/source/S2485537415', 'https://semopenalex.org/source/S4306463937', 'https://semopenalex.org/source/S4210202905', 'https://semopenalex.org/source/S106296714', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4363608109', 'https://semopenalex.org/source/S4363607726', 'https://semopenalex.org/source/S4306401809', 'https://semopenalex.org/source/S110206669', 'https://semopenalex.org/source/S4210170305', 'https://semopenalex.org/source/S47192491', 'https://semopenalex.org/source/S4363608767', 'https://semopenalex.org/source/S36033921', 'https://semopenalex.org/source/S71857517', 'https://semopenalex.org/source/S2764900261', 'https://semopenalex.org/source/S4210177381', 'https://semopenalex.org/source/S4210226185', 'https://semopenalex.org/source/S11065456', 'https://semopenalex.org/source/S4306402579', 'https://semopenalex.org/source/S4306402523', 'https://semopenalex.org/source/S4306533040', 'https://semopenalex.org/source/S106685023', 'https://semopenalex.org/source/S4210172589', 'https://semopenalex.org/source/S4306402607', 'https://semopenalex.org/source/S11479521', 'https://semopenalex.org/source/S35927321', 'https://semopenalex.org/source/S4306500161', 'https://semopenalex.org/source/S30698027', 'https://semopenalex.org/source/S45693802', 'https://semopenalex.org/source/S4363607707', 'https://semopenalex.org/source/S186357190', 'https://semopenalex.org/source/S4210231404', 'https://semopenalex.org/source/S2486411021', 'https://semopenalex.org/source/S58832373', 'https://semopenalex.org/source/S207319443', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S2595131146', 'https://semopenalex.org/source/S4121844', 'https://semopenalex.org/source/S4306401843', 'https://semopenalex.org/source/S33781645', 'https://semopenalex.org/source/S127900037', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S27924493', 'https://semopenalex.org/source/S414566', 'https://semopenalex.org/source/S2764461748', 'https://semopenalex.org/source/S129236917', 'https://semopenalex.org/source/S4306401596', 'https://semopenalex.org/source/S4363607857', 'https://semopenalex.org/source/S4306536006', 'https://semopenalex.org/source/S4306402105', 'https://semopenalex.org/source/S150382113', 'https://semopenalex.org/source/S10169007', 'https://semopenalex.org/source/S60779006', 'https://semopenalex.org/source/S4363607873', 'https://semopenalex.org/source/S4363607862', 'https://semopenalex.org/source/S4363608755', 'https://semopenalex.org/source/S4210191458']</t>
-  </si>
-  <si>
-    <t>['Learning to Mine Chinese Coordinate Terms Using the Web', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering Task-Specific Styles', 'BiCWS: Mining Cognitive Differences from Bilingual Web Search Results', 'Learning to Recommend Quotes for Writing', 'Evaluating Self-Generated Documents for Enhancing Retrieval-Augmented  Generation with Large Language Models', 'A New Benchmark and Reverse Validation Method for Passage-level Hallucination Detection', 'https://semopenalex.org/source/S4363607764', 'Evaluating Factuality in Cross-lingual Summarization', 'Emotion Classification in Microblog Texts Using Class Sequential Rules', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S4306525036', 'Semantic Dependency Parsing via Book Embedding', 'Joint Decoding of Tree Transduction Models for Sentence Compression', 'History Matters: Temporal Knowledge Editing in Large Language Model', 'Diversifying Neural Text Generation with Part-of-Speech Guided Softmax and Sampling', 'Language Generation via DAG Transduction', 'https://semopenalex.org/source/S4363608767', 'Evaluating and Mitigating Number Hallucinations in Large Vision-Language  Models: A Consistency Perspective', 'IGSQL: Database Schema Interaction Graph Based Neural Model for Context-Dependent Text-to-SQL Generation', 'Cross-Lingual Sentiment Classification with Bilingual Document Representation Learning', 'Using only cross-document relationships for both generic and topic-focused multi-document summarizations', 'Single document keyphrase extraction using neighborhood knowledge', 'Towards a Neural Network Approach to Abstractive Multi-Document Summarization', 'On the Helpfulness of Document Context to Sentence Simplification', 'Combining Content and Context Similarities for Image Retrieval', 'https://semopenalex.org/source/S4306420508', 'A Comprehensive Evaluation of Constrained Text Generation for Large Language Models', 'Benchmarking Knowledge Boundary for Large Language Model: A Different  Perspective on Model Evaluation', 'TransModality: An End2End Fusion Method with Transformer for Multimodal Sentiment Analysis', 'https://semopenalex.org/source/S4363608852', 'Peking: Profiling Syntactic Tree Parsing Techniques for Semantic Graph Parsing', 'A Measure Based on Optimal Matching in Graph Theory for Document Similarity', 'Document Similarity Search Based on Generic Summaries', 'Towards a unified approach to document similarity search using manifold-ranking of blocks', 'https://semopenalex.org/source/S4306420577', 'Learning to Identify Ambiguous and Misleading News Headlines', 'https://semopenalex.org/source/S2501765825', 'https://semopenalex.org/source/S29980478', 'Towards Document-Level Paraphrase Generation with Sentence Rewriting and Reordering', 'A Simple Information-Based Approach to Unsupervised Domain-Adaptive Aspect-Based Sentiment Analysis', 'https://semopenalex.org/source/S4363608652', 'A New Retrieval Model Based on TextTiling for Document Similarity Search', 'MC-MKE: A Fine-Grained Multimodal Knowledge Editing Benchmark  Emphasizing Modality Consistency', 'A Semi-Supervised Approach for Low-Resourced Text Generation', 'A Neural Approach to Pun Generation', 'A Data-Driven, Factorization Parser for CCG Dependency Structures', 'Findings of the Association for Computational Linguistics: ACL 2023', 'Automatic Text Simplification&lt;i&gt;Horacio Saggion&lt;/i&gt; (Universitat Pompeu Fabra) Morgan &amp;amp; Claypool (Synthesis Lectures on Human Language Technologies, edited by Graeme Hirst, volume 37), 2017, xvi+121 pp; paperback, ISBN 978-1-62705-868-1; ebook, ISBN 978-1-62705-869-8; doi:10.2200/S00700ED1V01Y201602HLT032', 'PKUTM participation at TAC 2011 Summarization Track.', 'Creative Destruction: Can Language Models Interpret Oxymorons?', 'Missing Information, Unresponsive Authors, Experimental Flaws: The Impossibility of Assessing the Reproducibility of Previous Human Evaluations in NLP', 'Exploiting syntactic and semantic relationships between terms for opinion retrieval', 'Towards Automatic Construction of News Overview Articles by News Synthesis', 'Controllable Unsupervised Text Attribute Transfer via Editing Entangled Latent Representation', 'https://semopenalex.org/source/S4306420006', 'Cross-language document summarization via extraction and ranking of multiple summaries', 'BAB-QA: A New Neural Model for Emotion Detection in Multi-party Dialogue', 'Learning Bilingual Embedding Model for Cross-Language Sentiment Classification', 'A Comparative Analysis of Knowledge-Intensive and Data-Intensive Semantic Parsers', 'PaCoST: Paired Confidence Significance Testing for Benchmark  Contamination Detection in Large Language Models', 'Timeline Generation through Evolutionary Trans-Temporal Summarization', 'How Do Seq2Seq Models Perform on End-to-End Data-to-Text Generation?', 'Improving Grammatical Error Correction with Data Augmentation by Editing Latent Representation', 'https://semopenalex.org/source/S81770430', 'https://semopenalex.org/source/S4363605144', 'Exploiting neighborhood knowledge for single document summarization and keyphrase extraction', 'Modeling and prediction of modulus of elasticity of laminated veneer lumber based on laminated plate theory', 'AMRec: An Intelligent System for Academic Method Recommendation', 'Cross Modal Training for ASR Error Correction with Contrastive Learning', 'Overview of the NLPCC 2023 Shared Task: Chinese Spelling Check', 'Making Better Use of Bilingual Information for Cross-Lingual AMR Parsing', 'https://semopenalex.org/source/S155526855', 'PosterBot: A System for Generating Posters of Scientific Papers with Neural Models', 'Beyond topical similarity: a structural similarity measure for retrieving highly similar documents', 'Overview of the NLPCC 2018 Shared Task: Grammatical Error Correction', 'Comparative News Summarization Using Linear Programming', 'Re-evaluating Automatic LLM System Ranking for Alignment with Human  Preference', 'Reducing Approximation and Estimation Errors for Chinese Lexical Processing with Heterogeneous Annotations', 'https://semopenalex.org/source/S104780363', 'ParaSCI: A Large Scientific Paraphrase Dataset for Longer Paraphrase Generation', 'BrailleSUM: A News Summarization System for the Blind and Visually Impaired People', 'Collective Opinion Target Extraction in Chinese Microblogs', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S106296714', 'A New Re-ranking Method for Generic Chinese Text Summarization and Its Evaluation', 'Neural Content Extraction for Poster Generation of Scientific Papers', 'SMART-RAG: Selection using Determinantal Matrices for Augmented  Retrieval', 'Data-driven, PCFG-based and Pseudo-PCFG-based Models for Chinese Dependency Parsing', 'Automatic Slides Generation for Scholarly Papers: A Fine-Grained Dataset and Baselines (Student Abstract)', 'WaterPool: A Watermark Mitigating Trade-offs among Imperceptibility,  Efficacy and Robustness', 'COSSUM: Towards Conversation-Oriented Structured Summarization for Automatic Medical Insurance Assessment', 'QuoteRec', 'Update Summarization Based on Co-Ranking with Constraints', 'Defining and Detecting Vulnerability in Human Evaluation Guidelines: A  Preliminary Study Towards Reliable NLG Evaluation', 'CMiner: Opinion Extraction and Summarization for Chinese Microblogs', 'https://semopenalex.org/source/S62018274', 'Compressive document summarization via sparse optimization', 'Is Summary Useful or Not? An Extrinsic Human Evaluation of Text Summaries on Downstream Tasks', 'DPP-Based Adversarial Prompt Searching for Lanugage Models', 'A Syntax-Guided Grammatical Error Correction Model with Dependency Tree Correction', 'CUGE: A Chinese Language Understanding and Generation Evaluation Benchmark', 'Semantic Role Labeling for Learner Chinese: the Importance of Syntactic Parsing and L2-L1 Parallel Data', 'https://semopenalex.org/source/S79460864', 'ATSUM: Extracting Attractive Summaries for News Propagation on Microblogs', 'Towards a Universal Sentiment Classifier in Multiple languages', 'PPSGen: Learning-Based Presentation Slides Generation for Academic Papers', 'https://semopenalex.org/source/S192650101', "x-index: a fantastic new indicator for quantifying a scientist's scientific impact", 'Evolutionary timeline summarization', 'https://semopenalex.org/source/S30698027', 'AMRec: an intelligent system for academic method recommendation', 'OpinSummEval: Revisiting Automated Evaluation for Opinion Summarization', 'Chinese Spelling Check with Nearest Neighbors', 'https://semopenalex.org/source/S2729999759', 'Bilingual Co-Training for Sentiment Classification of Chinese Product Reviews', 'Themis: A Reference-free NLG Evaluation Language Model with Flexibility and Interpretability', 'https://semopenalex.org/source/S205754296', 'Stabilization/solidification of lead- and cadmium-containing tailings for cemented paste backfill by using clinker-free binders', 'Abstractive Document Summarization with a Graph-Based Attentional Neural Model', 'A Comprehensive Evaluation and Analysis Study for Chinese Spelling Check', 'Comparing Knowledge-Intensive and Data-Intensive Models for English Resource Semantic Parsing', 'PPSGen: learning to generate presentation slides for academic papers', 'Single document summarization with document expansion', 'PKUTM at TREC 2010 Blog Track', 'Continual Learning for Neural Machine Translation', 'Are LLM-based Evaluators Confusing NLG Quality Criteria?', 'A New Dataset and Empirical Study for Sentence Simplification in Chinese', 'Neural Sentence Simplification with Semantic Dependency Information', 'https://semopenalex.org/source/S56561474', 'CrossDial: An Entertaining Dialogue Dataset of Chinese Crosstalk', 'Teaching the Pre-trained Model to Generate Simple Texts for Text Simplification', 'https://semopenalex.org/source/S4210191458', 'Adrenergic α1A receptor modulates cultured urothelium structure', 'Are all literature citations equally important? Automatic citation strength estimation and its applications', 'Cross-Language Document Summarization Based on Machine Translation Quality Prediction', 'https://semopenalex.org/source/S4306421043', 'CodeQA: A Question Answering Dataset for Source Code Comprehension', 'Revisiting Pivot-Based Paraphrase Generation: Language Is Not the Only Optional Pivot', 'https://semopenalex.org/source/S4363608774', 'Hierarchical Attention Networks for Sentence Ordering', 'MOVER: Mask, Over-generate and Rank for Hyperbole Generation', 'AKMiner: Domain-Specific Knowledge Graph Mining from Academic Literatures', 'Manifold-ranking based topic-focused multi-document summarization', 'Representation Learning for Aspect Category Detection in Online Reviews', 'Phrase-Based Presentation Slides Generation for Academic Papers', 'Recent advances of neural text generation: Core tasks, datasets, models and challenges', 'Automated Similarity Metric Generation for Recommendation', 'An Empirical Study of Automatic Post-Editing', 'https://semopenalex.org/source/S4363606692', 'BiRdQA: A Bilingual Dataset for Question Answering on Tricky Riddles', 'https://semopenalex.org/source/S4363607979', 'How to Describe Images in a More Funny Way? Towards a Modular Approach to Cross-Modal Sarcasm Generation', 'Themis: Towards Flexible and Interpretable NLG Evaluation', 'WikiTableEdit: A Benchmark for Table Editing by Natural Language  Instruction', 'Social Biases in Automatic Evaluation Metrics for NLG', 'Comparative news summarization using concept-based optimization', 'Analyzing and Evaluating Correlation Measures in NLG Meta-Evaluation', 'Peking: Building Semantic Dependency Graphs with a Hybrid Parser', 'ContraSolver: Self-Alignment of Language Models by Resolving Internal  Preference Contradictions', 'ALCUNA: Large Language Models Meet New Knowledge', 'GraDual: Graph-based Dual-modal Representation for Image-Text Matching', 'DSGram: Dynamic Weighting Sub-Metrics for Grammatical Error Correction  in the Era of Large Language Models', 'Learning a Product Relevance Model from Click-Through Data in E-Commerce', 'Clinical challenges and management of primary renal epithelioid angiomyolipoma of duplex kidney with paraneoplastic syndrome', 'Extract Salient Words with WordRank for Effective Similarity Search in Text Data', 'https://semopenalex.org/source/S4363606669', 'Deep Dependency Substructure-Based Learning for Multidocument Summarization', 'Neural Text Generation with Part-of-Speech Guided Softmax.', 'Towards a Unified Approach Based on Affinity Graph to Various Multi-document Summarizations', 'Leveraging Diverse Lexical Chains to Construct Essays for Chinese College Entrance Examination', 'Greedy Flipping for Constrained Word Deletion', 'Describe Images in a Boring Way: Towards Cross-Modal Sarcasm Generation', 'https://semopenalex.org/source/S4306419999', 'https://semopenalex.org/source/S4363607702', 'INS: An Interactive Chinese News Synthesis System', 'Enhancing Large Language Models in Coding Through Multi-Perspective Self-Consistency', 'Block-Based Similarity Search on the Web Using Manifold-Ranking', 'Recent advances in document summarization', 'https://semopenalex.org/source/S4363608773', 'https://semopenalex.org/source/S162583102', 'Human-like Summarization Evaluation with ChatGPT', 'Nearest Neighbor Knowledge Distillation for Neural Machine Translation', 'https://semopenalex.org/source/S74113319', 'A Comparative Study of Cross-Lingual Sentiment Classification', 'The Impact of Family Care on the Subjective Well-Being of the Elderly: The Mediation Role of General Self-Efficacy and Psychological Resilience', 'Tweet Timeline Generation with Determinantal Point Processes', 'Attention-based LSTM Network for Cross-Lingual Sentiment Classification', 'MicroScholar: Mining Scholarly Information from Chinese Microblogs', 'Exploiting Summarization Data to Help Text Simplification', 'Reference Matters: Benchmarking Factual Error Correction for Dialogue Summarization with Fine-grained Evaluation Framework', 'Learning to Identify Comparative Sentences in Chinese Text', 'Better than Random: Reliable NLG Human Evaluation with Constrained Active Sampling', 'https://semopenalex.org/source/S4306401280', 'SRRank: Leveraging Semantic Roles for Extractive Multi-Document Summarization', 'RST Discourse Parsing as Text-to-Text Generation', 'Improving Word Embeddings for Antonym Detection Using Thesauri and SentiWordNet', 'https://semopenalex.org/source/S4306418267', 'Towards Constructing Sports News from Live Text Commentary', 'Microscale and macroscale strength behaviors of blast furnace slag- cement based materials: Modeling and analysis', 'https://semopenalex.org/source/S4210183871', 'https://semopenalex.org/source/S87067389', 'Generating Diverse and Descriptive Image Captions Using Visual Paraphrases', 'A Feedback-learning Mechanism Based on the Semantic Topological Network', 'CLOpinionMiner: Opinion Target Extraction in a Cross-Language Scenario', 'Overview of the NLPCC 2018 Shared Task: Single Document Summarization', 'https://semopenalex.org/source/S4306419219', 'https://semopenalex.org/source/S2764825856', 'CC-Riddle: A Question Answering Dataset of Chinese Character Riddles', 'Adverse Drug Events Detection, Extraction and Normalization from Online Comments of Chinese Patent Medicines', 'Mining and Analyzing the Future Works in Scientific Articles', 'Models See Hallucinations: Evaluating the Factuality in Video Captioning', 'Document-Level Text Simplification: Dataset, Criteria and Baseline', 'Visual Question Generation Under Multi-granularity Cross-Modal Interaction', 'Massive Styles Transfer with Limited Labeled Data', 'Transition-Based Parsing for Deep Dependency Structures', 'Summarizing the differences in multilingual news', 'AMR-To-Text Generation with Graph Transformer', 'Multi-Document Summarization via Discriminative Summary Reranking', 'SimpleBERT: A Pre-trained Model That Learns to Generate Simple Words', 'https://semopenalex.org/source/S4210197613', 'https://semopenalex.org/source/S2764455111', 'Parsing Chinese Sentences with Grammatical Relations', 'https://semopenalex.org/source/S161516442', "&lt;scp&gt;WL&lt;/scp&gt;‐index: Leveraging citation mention number to quantify an individual's scientific impact", 'https://semopenalex.org/source/S174847851', 'Automatic Labeling of Topic Models Using Text Summaries', 'Dependency-based Mixture Language Models', 'Constructing a Family Tree of Ten Indo-European Languages with Delexicalized Cross-linguistic Transfer Patterns', 'WikiIns: A High-Quality Dataset for Controlled Text Editing by Natural Language Instruction', 'Exploring the Impact of Vision Features in News Image Captioning', 'https://semopenalex.org/source/S4306419142', 'https://semopenalex.org/source/S4210169297', 'EAMA : Entity-Aware Multimodal Alignment Based Approach for News Image  Captioning', 'https://semopenalex.org/source/S4387280317', 'DeepDial: Passage Completion on Dialogs', 'https://semopenalex.org/source/S4363608670', 'Graph-based multi-modality learning for topic-focused multi-document summarization', 'Hierarchical Graph Summarization: Leveraging Hybrid Information through Visible and Invisible Linkage', 'Visual Information Guided Zero-Shot Paraphrase Generation', 'Overview of the NLPCC 2017 Shared Task: Single Document Summarization', 'SemSUM: Semantic Dependency Guided Neural Abstractive Summarization', 'Phrase-based Compressive Cross-Language Summarization', 'Parsing to 1-Endpoint-Crossing, Pagenumber-2 Graphs', 'Automated Chess Commentator Powered by Neural Chess Engine', 'Using Bilingual Information for Cross-Language Document Summarization', 'Automatic Text Simplification', 'MultiSumm: Towards a Unified Model for Multi-Lingual Abstractive Summarization', 'Summarization is (Almost) Dead', 'Learning Diachronic Word Embeddings with Iterative Stable Information Alignment', 'Selecting Large Language Model to Fine-tune via Rectified Scaling Law', 'Counterfactual Representation Augmentation for Cross-Domain Sentiment Analysis', 'Named Entity Recognition in Chinese News Comments on the Web', 'Using Proportional Transportation Distances for Measuring Document Similarity', 'Defining and Detecting Vulnerability in Human Evaluation Guidelines: A Preliminary Study Towards Reliable NLG Evaluation', 'Bridging the Domain Gap: Improve Informal Language Translation via Counterfactual Domain Adaptation', 'Exploring Discourse Structure in Document-level Machine Translation', 'A novel document similarity measure based on earth mover’s distance', 'Quasi-Second-Order Parsing for 1-Endpoint-Crossing, Pagenumber-2 Graphs', 'Pushing Paraphrase Away from Original Sentence: A Multi-Round Paraphrase Generation Approach', 'Joint Matrix Factorization and Manifold-Ranking for Topic-Focused Multi-Document Summarization', 'Image Matters: A New Dataset and Empirical Study for Multimodal Hyperbole Detection', 'Document Similarity Search Based on Manifold-Ranking of TextTiles', 'Images2Poem', 'Towards Automatic Generation of Entertaining Dialogues in Chinese Crosstalks', 'The Great Importance of Cross-Document Relationships for Multi-document Summarization', 'Overview of the NLPCC-ICCPOL 2016 Shared Task: Sports News Generation from Live Webcast Scripts', 'Pre- and In-Parsing Models for Neural Empty Category Detection', 'SUBTOPIC‐BASED MULTIMODALITY RANKING FOR TOPIC‐FOCUSED MULTIDOCUMENT SUMMARIZATION', 'Effects of additional ring-fusion site on dual reactivity based dynamic covalent chemistry', 'Incorporating Cross-Document Relationships Between Sentences for Single Document Summarizations', 'Collaborative Data Cleaning for Sentiment Classification with Noisy Training Corpus', 'Towards Accurate and Efficient Chinese Part-of-Speech Tagging', 'Document-Based HITS Model for Multi-document Summarization', 'An Improved k-means Algorithm for Documents Clustering', 'PKU Paraphrase Bank: A Sentence-Level Paraphrase Corpus for Chinese', 'Point Precisely: Towards Ensuring the Precision of Data in Generated Texts Using Delayed Copy Mechanism', 'https://semopenalex.org/source/S80113298', 'https://semopenalex.org/source/S4306400349', 'Accurate SHRG-Based Semantic Parsing', 'https://semopenalex.org/source/S4363608991', 'A Neural Approach to Irony Generation', 'Better than Random: Reliable NLG Human Evaluation with Constrained  Active Sampling', 'DialSummEval: Revisiting Summarization Evaluation for Dialogues', 'PKUSUMSUM : A Java Platform for Multilingual Document Summarization', '$B^4$: A Black-Box Scrubbing Attack on LLM Watermarks', 'Towards a Novel Association Measure via Web Search Results Mining', 'Overview of Baidu Cup 2016: Challenge on Entity Search', 'Learning to Find Comparable Entities on the Web', 'https://semopenalex.org/source/S4363608757', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering  Task-Specific Styles', 'Overview of the NLPCC 2015 Shared Task: Weibo-Oriented Chinese News Summarization', 'SituatedGen: Incorporating Geographical and Temporal Contexts into Generative Commonsense Reasoning', 'WordRank-Based Lexical Signatures for Finding Lost or Related Web Pages']</t>
-  </si>
-  <si>
-    <t>['Glacier Monitoring Using Frequency Domain Offset Tracking Applied to Sentinel-1 Images: A Product Performance Comparison', 'A Novel Tool for Unsupervised Flood Mapping Using Sentinel-1 Images', 'https://semopenalex.org/source/S4306400993', 'Urban Area Mapping Using Multitemporal SAR Images in Combination with Self-Organizing Map Clustering and Object-Based Image Analysis', 'https://semopenalex.org/source/S2764455111', 'Analytical Evaluation of the Baseline Decorrelation in Bistatic Interferometric SAR Systems', "Deciphering Earth's Movements: Unveiling Subsidence and Displacement in Capo Colonna Through SAR and CGPS", 'https://semopenalex.org/source/S2496917176', 'Cardinal Effect in Bistatic SAR Imagery: Analysis and Physical Interpretation', 'An Analytical Formulation of the Correlation of GNSS-R Signals', 'Integration of SAR and GEOBIA for the Analysis of Time-Series Data', 'Feature Extraction From Multitemporal SAR Images Using Selforganizing Map Clustering and Object-Based Image Analysis', 'Efficient Simulation of Extended-Scene SAR Raw Signals with Any Acquisition Mode', 'Closed-Form Anisotropic Polarimetric Two-Scale Model for Fast Evaluation of Sea Surface Backscattering', 'Small Reservoirs Extraction in Semiarid Regions Using Multitemporal Synthetic Aperture Radar Images', 'Despeckling of Multifrequency SAR Data Using Electromagnetic Scattering Models', 'Scattering Along the Specular Direction from the Sea Modeled as a Fractal Surface', 'Using GEOBIA for feature extraction from multitemporal SAR images: Preliminary results', 'Maritime Surveillance Using Spaceborne GNSS-Reflectometry: The Role of the Scattering Configuration and Receiving Polarization Channel', 'https://semopenalex.org/source/S4363605409', 'https://semopenalex.org/source/S2485537415', 'https://semopenalex.org/source/S4306498310', 'Bistatic Scattering From Anisotropic Rough Surfaces via a Closed-Form Two-Scale Model', 'Efficient Processing for Far-From-Transmitter Formation-Flying SAR Receivers', 'https://semopenalex.org/source/S126920919', 'Analytical Formulation of Scattering From Anisotropic Power-Law Spectrum Surfaces: Getting Rid of the Cutoff Wavenumber', 'https://semopenalex.org/source/S4306498155', 'A Unified Formulation of SAR Raw Signals From Extended Scenes for All Acquisition Modes With Application to Simulation', 'Coprime synthetic aperture radars', 'Assessing Performance of Multitemporal SAR Image Despeckling Filters via a Benchmarking Tool', 'Sensitivity analysis of a scattering-based nonlocal means Despeckling Algorithm', 'https://semopenalex.org/source/S4306508950', 'https://semopenalex.org/source/S4306402478', 'https://semopenalex.org/source/S4210227020', 'https://semopenalex.org/source/S4363608188', 'A Novel Analytical Formulation of the Correlation of GNSS-R Signals Scattered by a Natural Fractal Surface', 'Baseline Decorrelation in Bistatic Interferometric SAR Systems Over Bare Soil Surfaces', 'https://semopenalex.org/source/S111326731', 'Acquisition modes', 'https://semopenalex.org/source/S4306402651', 'SAR Radiometric Calibration Based on Differential Geometry: From Theory to Experimentation on SAOCOM Imagery', 'Two-Scale Model for the Evaluation of Sea-Surface Scattering in GNSS-R Ship-Detection Applications', 'https://semopenalex.org/source/S4377196294', 'Scattering-based Despeckling of Multi-frequency SAR Data', 'Polarimetric Two-Scale Model for Soil Moisture Estimation from Hybrid Compact Polarimetry SAR Data', 'https://semopenalex.org/source/S4210178770', 'Time-Domain and Monostatic-like Frequency-Domain Methods for Bistatic SAR Simulation', 'Electromagnetic Scattering from Fractional Brownian Motion Surfaces via the Small Slope Approximation', 'Link Budget Analysis for GNSS-R Sea Surface Return in Arbitrary Acquisition Geometries Using BA-PTSM', 'Retrieval of high-resolution topography of the Titan’ surface by using Cassini SAR data', 'https://semopenalex.org/source/S4363604196', 'Fractal-Based Local Range Slope Estimation from Single SAR Image with Applications to SAR Despeckling and Topographic Mapping', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S4306463440', 'Spaceborne GNSS-Reflectometry for Ship-Detection Applications: Impact of Acquisition Geometry and Polarization', 'Pol-SARAS: A Fully Polarimetric SAR Raw Signal Simulator for Extended Soil Surfaces', 'Integrated Infrastructure Monitoring Procedure for Road Network Management', 'A New Tool for Road Network Deformations Monitoring Through Space-Born SAR Data and In-Situ Instruments', 'Unsupervised Rapid Flood Mapping Using Sentinel-1 GRD SAR Images', 'Sea state and wind speed', 'Polarimetric Two-Scale Model for the Evaluation of Bistatic Scattering from Anisotropic Sea Surfaces', 'Planning 5G Networks Under EMF Constraints: State of the Art and Vision', 'Ambiguity problems and their mitigation', 'https://semopenalex.org/source/S101949793', 'https://semopenalex.org/source/S43295729', 'X-Band SAR Antenna Design for a CubeSat Formation-Flying Remote Sensing Mission', 'https://semopenalex.org/source/S4363608006', 'Closed-form Polarimetric Two-Scale Model for sea scattering evaluation', 'Introduction', 'https://semopenalex.org/source/S117727964', 'Flood Detection with SAR: A Review of Techniques and Datasets', 'Addressing ices in the solar system via their fractal dimension measurement', 'An Analytical Formulation for the Correlation of Surface-Scattered Fields at Two Bistatic Radar Receivers', 'Bistatic scattering from a canonical building', 'Earth Environmental Monitoring Using Multi-Temporal Synthetic Aperture Radar: A Critical Review of Selected Applications', 'The Role of Resolution in the Estimation of Fractal Dimension Maps From SAR Data', 'Long-Term Satellite Monitoring of the Slumgullion Landslide Using Space-Borne Synthetic Aperture Radar Sub-Pixel Offset Tracking', 'Benchmarking Framework for Multitemporal SAR Despeckling', 'Railway Bridge Monitoring with Sar: A Case Study']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/source/S4210218191', 'Graph Compression', 'A multi-objective genetic algorithm for compression of weighted graphs to simplify epidemic analysis', '2022 IEEE conference on computational intelligence in bioinformatics and computational biology (IEEE CIBCB, 2022)', 'All lockdowns are not equal: Reducing epidemic impact through evolutionary computation', 'Evolutionary Computation', 'Network Induction', 'Promoting Diversity in the Evolution of Biological Sequence Data', 'https://semopenalex.org/source/S104797584', 'https://semopenalex.org/source/S4210216571', 'Freezing of gait in Parkinson’s disease: Classification using computational intelligence', 'Introduction', 'Network Induction Issues', 'What Drives Evolution of Self-Driving Automata?', 'Conference Report on 2022 IEEE Conference on Computational Intelligence in Bioinformatics and Computational Biology (IEEE CIBCB 2022) [Conference Report]', 'AI Versus Epidemics', 'https://semopenalex.org/source/S4363604921', 'https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S4363605353', 'https://semopenalex.org/source/S99347777', 'Dungeons, Dragons, and Data Breaches: Analyzing AI Attacks on Various Network Configurations', 'https://semopenalex.org/source/S140556538', 'Vaccine Distribution']</t>
+    <t>['https://semopenalex.org/work/W2788968669', 'https://semopenalex.org/work/W1999760195', 'https://semopenalex.org/work/W2226359063', 'https://semopenalex.org/work/W2780277126', 'https://semopenalex.org/work/W2957110867', 'https://semopenalex.org/work/W2844810377', 'https://semopenalex.org/work/W2772966323', 'https://semopenalex.org/work/W2903944530', 'https://semopenalex.org/work/W3205075200', 'https://semopenalex.org/work/W2974444355', 'https://semopenalex.org/work/W4367671449', 'https://semopenalex.org/work/W2397277866', 'https://semopenalex.org/work/W4206136166', 'https://semopenalex.org/work/W4238294234', 'https://semopenalex.org/work/W3048792033', 'https://semopenalex.org/work/W2996971450', 'https://semopenalex.org/work/W4396568545', 'https://semopenalex.org/work/W2979701877', 'https://semopenalex.org/work/W2792290921', 'https://semopenalex.org/work/W3134422373', 'https://semopenalex.org/work/W3202715770', 'https://semopenalex.org/work/W3158463786', 'https://semopenalex.org/work/W2100407406', 'https://semopenalex.org/work/W2897762537', 'https://semopenalex.org/work/W4293863370', 'https://semopenalex.org/work/W2996342798', 'https://semopenalex.org/work/W2948196949', 'https://semopenalex.org/work/W4390737683', 'https://semopenalex.org/work/W2805460435', 'https://semopenalex.org/work/W4406267825']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4390604119', 'https://semopenalex.org/work/W4403094633', 'https://semopenalex.org/work/W4312804251', 'https://semopenalex.org/work/W4386065896']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S33781645', 'https://semopenalex.org/source/S4363608094', 'https://semopenalex.org/source/S30698027', 'https://semopenalex.org/source/S4363608767', 'https://semopenalex.org/source/S4306536006', 'https://semopenalex.org/source/S2492086750', 'https://semopenalex.org/source/S4210226185', 'https://semopenalex.org/source/S150382113', 'https://semopenalex.org/source/S4306402492', 'https://semopenalex.org/source/S207319443', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S11065456', 'https://semopenalex.org/source/S4210202905', 'https://semopenalex.org/source/S81770430', 'https://semopenalex.org/source/S106685023', 'https://semopenalex.org/source/S35927321', 'https://semopenalex.org/source/S127900037', 'https://semopenalex.org/source/S4363607873', 'https://semopenalex.org/source/S4210231404', 'https://semopenalex.org/source/S10169007', 'https://semopenalex.org/source/S191726168', 'https://semopenalex.org/source/S2764455111', 'https://semopenalex.org/source/S4210191458', 'https://semopenalex.org/source/S4363607857', 'https://semopenalex.org/source/S4306402579', 'https://semopenalex.org/source/S4306515065', 'https://semopenalex.org/source/S4363607862', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S4306402105', 'https://semopenalex.org/source/S4306500161', 'https://semopenalex.org/source/S4306402607', 'https://semopenalex.org/source/S4363608762', 'https://semopenalex.org/source/S4210168194', 'https://semopenalex.org/source/S27924493', 'https://semopenalex.org/source/S4306533040', 'https://semopenalex.org/source/S4121844', 'https://semopenalex.org/source/S414566', 'https://semopenalex.org/source/S4363607707', 'https://semopenalex.org/source/S11479521', 'https://semopenalex.org/source/S60779006', 'https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S106296714', 'https://semopenalex.org/source/S4306401843', 'https://semopenalex.org/source/S4363608845', 'https://semopenalex.org/source/S110206669', 'https://semopenalex.org/source/S2485537415', 'https://semopenalex.org/source/S2764461748', 'https://semopenalex.org/source/S58832373', 'https://semopenalex.org/source/S4306463937', 'https://semopenalex.org/source/S4306402523', 'https://semopenalex.org/source/S2764900261', 'https://semopenalex.org/source/S4363607726', 'https://semopenalex.org/source/S2595131146', 'https://semopenalex.org/source/S4210177381', 'https://semopenalex.org/source/S129236917', 'https://semopenalex.org/source/S4210170305', 'https://semopenalex.org/source/S4210172589', 'https://semopenalex.org/source/S144771191', 'https://semopenalex.org/source/S4306401809', 'https://semopenalex.org/source/S4363608109', 'https://semopenalex.org/source/S4306531565', 'https://semopenalex.org/source/S45693802', 'https://semopenalex.org/source/S36033921', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S4306400806', 'https://semopenalex.org/source/S47192491', 'https://semopenalex.org/source/S2486411021', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S186357190', 'https://semopenalex.org/source/S4363608755', 'https://semopenalex.org/source/S161516442', 'https://semopenalex.org/source/S71857517', 'https://semopenalex.org/source/S78082969', 'https://semopenalex.org/source/S4306401596']</t>
+  </si>
+  <si>
+    <t>['The Great Importance of Cross-Document Relationships for Multi-document Summarization', 'Quasi-Second-Order Parsing for 1-Endpoint-Crossing, Pagenumber-2 Graphs', 'https://semopenalex.org/source/S4306420577', 'https://semopenalex.org/source/S30698027', 'QuoteRec', 'https://semopenalex.org/source/S192650101', 'Greedy Flipping for Constrained Word Deletion', 'Towards Constructing Sports News from Live Text Commentary', 'Evaluating Factuality in Cross-lingual Summarization', 'Massive Styles Transfer with Limited Labeled Data', 'https://semopenalex.org/source/S162583102', 'Are all literature citations equally important? Automatic citation strength estimation and its applications', 'Neural Sentence Simplification with Semantic Dependency Information', 'Exploring the Impact of Vision Features in News Image Captioning', 'Themis: A Reference-free NLG Evaluation Language Model with Flexibility and Interpretability', 'A Data-Driven, Factorization Parser for CCG Dependency Structures', "&lt;scp&gt;WL&lt;/scp&gt;‐index: Leveraging citation mention number to quantify an individual's scientific impact", 'Document-Based HITS Model for Multi-document Summarization', 'Point Precisely: Towards Ensuring the Precision of Data in Generated Texts Using Delayed Copy Mechanism', 'Learning a Product Relevance Model from Click-Through Data in E-Commerce', 'CC-Riddle: A Question Answering Dataset of Chinese Character Riddles', 'https://semopenalex.org/source/S4363607979', 'Document Similarity Search Based on Manifold-Ranking of TextTiles', 'Using only cross-document relationships for both generic and topic-focused multi-document summarizations', 'Hierarchical Graph Summarization: Leveraging Hybrid Information through Visible and Invisible Linkage', 'MC-MKE: A Fine-Grained Multimodal Knowledge Editing Benchmark  Emphasizing Modality Consistency', 'Representation Learning for Aspect Category Detection in Online Reviews', 'https://semopenalex.org/source/S174847851', 'Pre- and In-Parsing Models for Neural Empty Category Detection', 'Towards a Novel Association Measure via Web Search Results Mining', 'Recent advances in document summarization', 'PKUTM participation at TAC 2011 Summarization Track.', 'https://semopenalex.org/source/S4210197613', 'SemSUM: Semantic Dependency Guided Neural Abstractive Summarization', 'Phrase-based Compressive Cross-Language Summarization', 'Learning to Mine Chinese Coordinate Terms Using the Web', 'AKMiner: Domain-Specific Knowledge Graph Mining from Academic Literatures', 'A Comprehensive Evaluation of Constrained Text Generation for Large Language Models', 'Semantic Dependency Parsing via Book Embedding', 'Tweet Timeline Generation with Determinantal Point Processes', 'Summarization is (Almost) Dead', 'Extract Salient Words with WordRank for Effective Similarity Search in Text Data', 'Exploiting syntactic and semantic relationships between terms for opinion retrieval', 'A New Re-ranking Method for Generic Chinese Text Summarization and Its Evaluation', 'https://semopenalex.org/source/S4363608774', 'Peking: Profiling Syntactic Tree Parsing Techniques for Semantic Graph Parsing', 'Social Biases in Automatic Evaluation Metrics for NLG', 'AMRec: an intelligent system for academic method recommendation', 'Exploiting neighborhood knowledge for single document summarization and keyphrase extraction', 'Cross-language document summarization via extraction and ranking of multiple summaries', 'Is Summary Useful or Not? An Extrinsic Human Evaluation of Text Summaries on Downstream Tasks', 'CodeQA: A Question Answering Dataset for Source Code Comprehension', 'Diversifying Neural Text Generation with Part-of-Speech Guided Softmax and Sampling', 'Automatic Text Simplification', 'https://semopenalex.org/source/S4363605144', 'Emotion Classification in Microblog Texts Using Class Sequential Rules', 'Automated Similarity Metric Generation for Recommendation', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering Task-Specific Styles', 'Single document keyphrase extraction using neighborhood knowledge', 'https://semopenalex.org/source/S4363607702', 'Comparing Knowledge-Intensive and Data-Intensive Models for English Resource Semantic Parsing', 'MultiSumm: Towards a Unified Model for Multi-Lingual Abstractive Summarization', 'Leveraging Diverse Lexical Chains to Construct Essays for Chinese College Entrance Examination', 'https://semopenalex.org/source/S4387280317', 'https://semopenalex.org/source/S4363606692', 'The Impact of Family Care on the Subjective Well-Being of the Elderly: The Mediation Role of General Self-Efficacy and Psychological Resilience', 'https://semopenalex.org/source/S74113319', 'Overview of Baidu Cup 2016: Challenge on Entity Search', 'https://semopenalex.org/source/S4306421043', 'Hierarchical Attention Networks for Sentence Ordering', 'Towards a unified approach to document similarity search using manifold-ranking of blocks', 'Beyond topical similarity: a structural similarity measure for retrieving highly similar documents', 'An Improved k-means Algorithm for Documents Clustering', 'A Syntax-Guided Grammatical Error Correction Model with Dependency Tree Correction', 'https://semopenalex.org/source/S4363608652', 'Parsing to 1-Endpoint-Crossing, Pagenumber-2 Graphs', 'Accurate SHRG-Based Semantic Parsing', 'Human-like Summarization Evaluation with ChatGPT', 'https://semopenalex.org/source/S4363606669', 'SRRank: Leveraging Semantic Roles for Extractive Multi-Document Summarization', 'Revisiting Pivot-Based Paraphrase Generation: Language Is Not the Only Optional Pivot', 'Automatic Text Simplification&lt;i&gt;Horacio Saggion&lt;/i&gt; (Universitat Pompeu Fabra) Morgan &amp;amp; Claypool (Synthesis Lectures on Human Language Technologies, edited by Graeme Hirst, volume 37), 2017, xvi+121 pp; paperback, ISBN 978-1-62705-868-1; ebook, ISBN 978-1-62705-869-8; doi:10.2200/S00700ED1V01Y201602HLT032', 'https://semopenalex.org/source/S4363608852', 'Semantic Role Labeling for Learner Chinese: the Importance of Syntactic Parsing and L2-L1 Parallel Data', 'Manifold-ranking based topic-focused multi-document summarization', 'https://semopenalex.org/source/S2501765825', 'SUBTOPIC‐BASED MULTIMODALITY RANKING FOR TOPIC‐FOCUSED MULTIDOCUMENT SUMMARIZATION', 'Improving Word Embeddings for Antonym Detection Using Thesauri and SentiWordNet', 'Stabilization/solidification of lead- and cadmium-containing tailings for cemented paste backfill by using clinker-free binders', 'https://semopenalex.org/source/S2764455111', 'Parsing Chinese Sentences with Grammatical Relations', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S4306420508', 'Towards a Universal Sentiment Classifier in Multiple languages', 'Generating Diverse and Descriptive Image Captions Using Visual Paraphrases', 'INS: An Interactive Chinese News Synthesis System', 'https://semopenalex.org/source/S4363608757', 'Compressive document summarization via sparse optimization', 'A Simple Information-Based Approach to Unsupervised Domain-Adaptive Aspect-Based Sentiment Analysis', 'PPSGen: learning to generate presentation slides for academic papers', 'Findings of the Association for Computational Linguistics: ACL 2023', 'Towards Automatic Generation of Entertaining Dialogues in Chinese Crosstalks', 'Overview of the NLPCC-ICCPOL 2016 Shared Task: Sports News Generation from Live Webcast Scripts', 'An Empirical Study of Automatic Post-Editing', 'Describe Images in a Boring Way: Towards Cross-Modal Sarcasm Generation', 'https://semopenalex.org/source/S4210169297', 'Combining Content and Context Similarities for Image Retrieval', 'https://semopenalex.org/source/S4306420006', 'History Matters: Temporal Knowledge Editing in Large Language Model', 'Towards Automatic Construction of News Overview Articles by News Synthesis', 'TransModality: An End2End Fusion Method with Transformer for Multimodal Sentiment Analysis', 'AMRec: An Intelligent System for Academic Method Recommendation', 'Reducing Approximation and Estimation Errors for Chinese Lexical Processing with Heterogeneous Annotations', 'Modeling and prediction of modulus of elasticity of laminated veneer lumber based on laminated plate theory', 'Update Summarization Based on Co-Ranking with Constraints', 'Towards a Neural Network Approach to Abstractive Multi-Document Summarization', 'ATSUM: Extracting Attractive Summaries for News Propagation on Microblogs', 'CLOpinionMiner: Opinion Target Extraction in a Cross-Language Scenario', 'DPP-Based Adversarial Prompt Searching for Lanugage Models', 'Learning to Identify Comparative Sentences in Chinese Text', 'Dependency-based Mixture Language Models', 'CUGE: A Chinese Language Understanding and Generation Evaluation Benchmark', 'Evaluating Self-Generated Documents for Enhancing Retrieval-Augmented  Generation with Large Language Models', 'https://semopenalex.org/source/S4306419142', 'Exploiting Summarization Data to Help Text Simplification', 'Making Better Use of Bilingual Information for Cross-Lingual AMR Parsing', 'Joint Matrix Factorization and Manifold-Ranking for Topic-Focused Multi-Document Summarization', 'GraDual: Graph-based Dual-modal Representation for Image-Text Matching', 'https://semopenalex.org/source/S4363608670', 'Overview of the NLPCC 2018 Shared Task: Grammatical Error Correction', 'How to Describe Images in a More Funny Way? Towards a Modular Approach to Cross-Modal Sarcasm Generation', 'WikiTableEdit: A Benchmark for Table Editing by Natural Language  Instruction', 'Learning to Identify Ambiguous and Misleading News Headlines', 'PosterBot: A System for Generating Posters of Scientific Papers with Neural Models', 'Learning to Recommend Quotes for Writing', 'https://semopenalex.org/source/S4306401280', 'On the Helpfulness of Document Context to Sentence Simplification', 'Evolutionary timeline summarization', 'Collective Opinion Target Extraction in Chinese Microblogs', 'Evaluating and Mitigating Number Hallucinations in Large Vision-Language  Models: A Consistency Perspective', 'PaCoST: Paired Confidence Significance Testing for Benchmark  Contamination Detection in Large Language Models', 'Phrase-Based Presentation Slides Generation for Academic Papers', 'https://semopenalex.org/source/S2729999759', 'PKUSUMSUM : A Java Platform for Multilingual Document Summarization', 'RST Discourse Parsing as Text-to-Text Generation', 'A Neural Approach to Irony Generation', 'Peking: Building Semantic Dependency Graphs with a Hybrid Parser', 'Incorporating Cross-Document Relationships Between Sentences for Single Document Summarizations', 'https://semopenalex.org/source/S4363607764', 'Block-Based Similarity Search on the Web Using Manifold-Ranking', 'https://semopenalex.org/source/S4363608991', 'https://semopenalex.org/source/S205754296', 'https://semopenalex.org/source/S2764825856', 'A Semi-Supervised Approach for Low-Resourced Text Generation', 'Single document summarization with document expansion', 'WaterPool: A Watermark Mitigating Trade-offs among Imperceptibility,  Efficacy and Robustness', 'Cross Modal Training for ASR Error Correction with Contrastive Learning', 'Overview of the NLPCC 2023 Shared Task: Chinese Spelling Check', 'Automatic Slides Generation for Scholarly Papers: A Fine-Grained Dataset and Baselines (Student Abstract)', 'Recent advances of neural text generation: Core tasks, datasets, models and challenges', 'https://semopenalex.org/source/S104780363', 'Using Bilingual Information for Cross-Language Document Summarization', 'Comparative news summarization using concept-based optimization', 'Counterfactual Representation Augmentation for Cross-Domain Sentiment Analysis', 'COSSUM: Towards Conversation-Oriented Structured Summarization for Automatic Medical Insurance Assessment', 'Images2Poem', 'https://semopenalex.org/source/S4210183871', 'Timeline Generation through Evolutionary Trans-Temporal Summarization', 'Defining and Detecting Vulnerability in Human Evaluation Guidelines: A Preliminary Study Towards Reliable NLG Evaluation', 'DeepDial: Passage Completion on Dialogs', 'Automated Chess Commentator Powered by Neural Chess Engine', 'BrailleSUM: A News Summarization System for the Blind and Visually Impaired People', 'DialSummEval: Revisiting Summarization Evaluation for Dialogues', 'Language Generation via DAG Transduction', 'BiCWS: Mining Cognitive Differences from Bilingual Web Search Results', 'Selecting Large Language Model to Fine-tune via Rectified Scaling Law', 'A Measure Based on Optimal Matching in Graph Theory for Document Similarity', 'https://semopenalex.org/source/S4306525036', 'Image Matters: A New Dataset and Empirical Study for Multimodal Hyperbole Detection', 'https://semopenalex.org/source/S155526855', 'Missing Information, Unresponsive Authors, Experimental Flaws: The Impossibility of Assessing the Reproducibility of Previous Human Evaluations in NLP', 'Visual Question Generation Under Multi-granularity Cross-Modal Interaction', 'CMiner: Opinion Extraction and Summarization for Chinese Microblogs', 'How Do Seq2Seq Models Perform on End-to-End Data-to-Text Generation?', 'https://semopenalex.org/source/S4306419219', 'DSGram: Dynamic Weighting Sub-Metrics for Grammatical Error Correction  in the Era of Large Language Models', 'Neural Text Generation with Part-of-Speech Guided Softmax.', 'PKUTM at TREC 2010 Blog Track', 'Cross-Language Document Summarization Based on Machine Translation Quality Prediction', 'https://semopenalex.org/source/S80113298', 'Nearest Neighbor Knowledge Distillation for Neural Machine Translation', 'SimpleBERT: A Pre-trained Model That Learns to Generate Simple Words', 'A Comparative Study of Cross-Lingual Sentiment Classification', 'Using Proportional Transportation Distances for Measuring Document Similarity', 'WikiIns: A High-Quality Dataset for Controlled Text Editing by Natural Language Instruction', 'https://semopenalex.org/source/S62018274', 'SMART-RAG: Selection using Determinantal Matrices for Augmented  Retrieval', 'Data-driven, PCFG-based and Pseudo-PCFG-based Models for Chinese Dependency Parsing', 'Re-evaluating Automatic LLM System Ranking for Alignment with Human  Preference', 'Continual Learning for Neural Machine Translation', 'https://semopenalex.org/source/S29980478', 'A Neural Approach to Pun Generation', 'WordRank-Based Lexical Signatures for Finding Lost or Related Web Pages', "x-index: a fantastic new indicator for quantifying a scientist's scientific impact", 'Benchmarking Knowledge Boundary for Large Language Model: A Different  Perspective on Model Evaluation', 'MOVER: Mask, Over-generate and Rank for Hyperbole Generation', 'Clinical challenges and management of primary renal epithelioid angiomyolipoma of duplex kidney with paraneoplastic syndrome', 'Better than Random: Reliable NLG Human Evaluation with Constrained Active Sampling', 'Defining and Detecting Vulnerability in Human Evaluation Guidelines: A  Preliminary Study Towards Reliable NLG Evaluation', 'https://semopenalex.org/source/S56561474', 'Overview of the NLPCC 2018 Shared Task: Single Document Summarization', 'A Feedback-learning Mechanism Based on the Semantic Topological Network', 'Adrenergic α1A receptor modulates cultured urothelium structure', 'Mining and Analyzing the Future Works in Scientific Articles', 'Automatic Labeling of Topic Models Using Text Summaries', 'CrossDial: An Entertaining Dialogue Dataset of Chinese Crosstalk', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering  Task-Specific Styles', 'Summarizing the differences in multilingual news', 'Overview of the NLPCC 2017 Shared Task: Single Document Summarization', 'https://semopenalex.org/source/S4363608767', 'Multi-Document Summarization via Discriminative Summary Reranking', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4363608773', 'A Comparative Analysis of Knowledge-Intensive and Data-Intensive Semantic Parsers', 'https://semopenalex.org/source/S87067389', 'A Comprehensive Evaluation and Analysis Study for Chinese Spelling Check', 'Bilingual Co-Training for Sentiment Classification of Chinese Product Reviews', 'https://semopenalex.org/source/S81770430', 'Named Entity Recognition in Chinese News Comments on the Web', 'Controllable Unsupervised Text Attribute Transfer via Editing Entangled Latent Representation', 'ALCUNA: Large Language Models Meet New Knowledge', 'Reference Matters: Benchmarking Factual Error Correction for Dialogue Summarization with Fine-grained Evaluation Framework', 'Collaborative Data Cleaning for Sentiment Classification with Noisy Training Corpus', 'MicroScholar: Mining Scholarly Information from Chinese Microblogs', '$B^4$: A Black-Box Scrubbing Attack on LLM Watermarks', 'Document-Level Text Simplification: Dataset, Criteria and Baseline', 'https://semopenalex.org/source/S4210191458', 'Overview of the NLPCC 2015 Shared Task: Weibo-Oriented Chinese News Summarization', 'ParaSCI: A Large Scientific Paraphrase Dataset for Longer Paraphrase Generation', 'Enhancing Large Language Models in Coding Through Multi-Perspective Self-Consistency', 'Attention-based LSTM Network for Cross-Lingual Sentiment Classification', 'Neural Content Extraction for Poster Generation of Scientific Papers', 'Creative Destruction: Can Language Models Interpret Oxymorons?', 'A novel document similarity measure based on earth mover’s distance', 'Themis: Towards Flexible and Interpretable NLG Evaluation', 'Bridging the Domain Gap: Improve Informal Language Translation via Counterfactual Domain Adaptation', 'Cross-Lingual Sentiment Classification with Bilingual Document Representation Learning', 'Chinese Spelling Check with Nearest Neighbors', 'BiRdQA: A Bilingual Dataset for Question Answering on Tricky Riddles', 'Microscale and macroscale strength behaviors of blast furnace slag- cement based materials: Modeling and analysis', 'https://semopenalex.org/source/S106296714', 'IGSQL: Database Schema Interaction Graph Based Neural Model for Context-Dependent Text-to-SQL Generation', 'Joint Decoding of Tree Transduction Models for Sentence Compression', 'https://semopenalex.org/source/S79460864', 'Learning Bilingual Embedding Model for Cross-Language Sentiment Classification', 'A New Dataset and Empirical Study for Sentence Simplification in Chinese', 'Pushing Paraphrase Away from Original Sentence: A Multi-Round Paraphrase Generation Approach', 'Adverse Drug Events Detection, Extraction and Normalization from Online Comments of Chinese Patent Medicines', 'Towards Accurate and Efficient Chinese Part-of-Speech Tagging', 'AMR-To-Text Generation with Graph Transformer', 'Graph-based multi-modality learning for topic-focused multi-document summarization', 'https://semopenalex.org/source/S4306418267', 'EAMA : Entity-Aware Multimodal Alignment Based Approach for News Image  Captioning', 'SituatedGen: Incorporating Geographical and Temporal Contexts into Generative Commonsense Reasoning', 'Are LLM-based Evaluators Confusing NLG Quality Criteria?', 'PPSGen: Learning-Based Presentation Slides Generation for Academic Papers', 'Abstractive Document Summarization with a Graph-Based Attentional Neural Model', 'Teaching the Pre-trained Model to Generate Simple Texts for Text Simplification', 'Learning to Find Comparable Entities on the Web', 'ContraSolver: Self-Alignment of Language Models by Resolving Internal  Preference Contradictions', 'PKU Paraphrase Bank: A Sentence-Level Paraphrase Corpus for Chinese', 'Analyzing and Evaluating Correlation Measures in NLG Meta-Evaluation', 'Document Similarity Search Based on Generic Summaries', 'Learning Diachronic Word Embeddings with Iterative Stable Information Alignment', 'BAB-QA: A New Neural Model for Emotion Detection in Multi-party Dialogue', 'https://semopenalex.org/source/S4306419999', 'Exploring Discourse Structure in Document-level Machine Translation', 'Comparative News Summarization Using Linear Programming', 'A New Benchmark and Reverse Validation Method for Passage-level Hallucination Detection', 'Visual Information Guided Zero-Shot Paraphrase Generation', 'https://semopenalex.org/source/S4306400194', 'Models See Hallucinations: Evaluating the Factuality in Video Captioning', 'https://semopenalex.org/source/S161516442', 'Towards a Unified Approach Based on Affinity Graph to Various Multi-document Summarizations', 'Better than Random: Reliable NLG Human Evaluation with Constrained  Active Sampling', 'Improving Grammatical Error Correction with Data Augmentation by Editing Latent Representation', 'Deep Dependency Substructure-Based Learning for Multidocument Summarization', 'A New Retrieval Model Based on TextTiling for Document Similarity Search', 'Transition-Based Parsing for Deep Dependency Structures', 'Constructing a Family Tree of Ten Indo-European Languages with Delexicalized Cross-linguistic Transfer Patterns', 'OpinSummEval: Revisiting Automated Evaluation for Opinion Summarization', 'Effects of additional ring-fusion site on dual reactivity based dynamic covalent chemistry', 'Towards Document-Level Paraphrase Generation with Sentence Rewriting and Reordering']</t>
+  </si>
+  <si>
+    <t>['SAR Radiometric Calibration Based on Differential Geometry: From Theory to Experimentation on SAOCOM Imagery', 'https://semopenalex.org/source/S111326731', 'Unsupervised Rapid Flood Mapping Using Sentinel-1 GRD SAR Images', 'Analytical Evaluation of the Baseline Decorrelation in Bistatic Interferometric SAR Systems', 'Integrated Infrastructure Monitoring Procedure for Road Network Management', 'Small Reservoirs Extraction in Semiarid Regions Using Multitemporal Synthetic Aperture Radar Images', 'Sea state and wind speed', 'A New Tool for Road Network Deformations Monitoring Through Space-Born SAR Data and In-Situ Instruments', 'Closed-Form Anisotropic Polarimetric Two-Scale Model for Fast Evaluation of Sea Surface Backscattering', 'A Novel Analytical Formulation of the Correlation of GNSS-R Signals Scattered by a Natural Fractal Surface', 'https://semopenalex.org/source/S4363604196', 'An Analytical Formulation for the Correlation of Surface-Scattered Fields at Two Bistatic Radar Receivers', 'Urban Area Mapping Using Multitemporal SAR Images in Combination with Self-Organizing Map Clustering and Object-Based Image Analysis', 'Planning 5G Networks Under EMF Constraints: State of the Art and Vision', 'Glacier Monitoring Using Frequency Domain Offset Tracking Applied to Sentinel-1 Images: A Product Performance Comparison', 'Maritime Surveillance Using Spaceborne GNSS-Reflectometry: The Role of the Scattering Configuration and Receiving Polarization Channel', 'https://semopenalex.org/source/S43295729', 'https://semopenalex.org/source/S4306498310', 'https://semopenalex.org/source/S117727964', 'https://semopenalex.org/source/S2764455111', 'Despeckling of Multifrequency SAR Data Using Electromagnetic Scattering Models', 'https://semopenalex.org/source/S4210227020', 'Integration of SAR and GEOBIA for the Analysis of Time-Series Data', 'https://semopenalex.org/source/S4306400993', 'Sensitivity analysis of a scattering-based nonlocal means Despeckling Algorithm', 'Assessing Performance of Multitemporal SAR Image Despeckling Filters via a Benchmarking Tool', 'Introduction', 'Scattering Along the Specular Direction from the Sea Modeled as a Fractal Surface', 'Baseline Decorrelation in Bistatic Interferometric SAR Systems Over Bare Soil Surfaces', 'Using GEOBIA for feature extraction from multitemporal SAR images: Preliminary results', 'https://semopenalex.org/source/S2496917176', 'Feature Extraction From Multitemporal SAR Images Using Selforganizing Map Clustering and Object-Based Image Analysis', 'Bistatic scattering from a canonical building', 'Ambiguity problems and their mitigation', 'Time-Domain and Monostatic-like Frequency-Domain Methods for Bistatic SAR Simulation', 'Analytical Formulation of Scattering From Anisotropic Power-Law Spectrum Surfaces: Getting Rid of the Cutoff Wavenumber', 'Flood Detection with SAR: A Review of Techniques and Datasets', 'Two-Scale Model for the Evaluation of Sea-Surface Scattering in GNSS-R Ship-Detection Applications', 'Retrieval of high-resolution topography of the Titan’ surface by using Cassini SAR data', 'An Analytical Formulation of the Correlation of GNSS-R Signals', 'Link Budget Analysis for GNSS-R Sea Surface Return in Arbitrary Acquisition Geometries Using BA-PTSM', 'Fractal-Based Local Range Slope Estimation from Single SAR Image with Applications to SAR Despeckling and Topographic Mapping', 'https://semopenalex.org/source/S4306402651', 'https://semopenalex.org/source/S4363608188', 'https://semopenalex.org/source/S2485537415', 'https://semopenalex.org/source/S4306402478', 'Closed-form Polarimetric Two-Scale Model for sea scattering evaluation', 'Cardinal Effect in Bistatic SAR Imagery: Analysis and Physical Interpretation', 'Coprime synthetic aperture radars', 'Electromagnetic Scattering from Fractional Brownian Motion Surfaces via the Small Slope Approximation', 'Benchmarking Framework for Multitemporal SAR Despeckling', 'Efficient Simulation of Extended-Scene SAR Raw Signals with Any Acquisition Mode', 'Addressing ices in the solar system via their fractal dimension measurement', 'https://semopenalex.org/source/S4306463440', 'A Novel Tool for Unsupervised Flood Mapping Using Sentinel-1 Images', 'Pol-SARAS: A Fully Polarimetric SAR Raw Signal Simulator for Extended Soil Surfaces', 'Long-Term Satellite Monitoring of the Slumgullion Landslide Using Space-Borne Synthetic Aperture Radar Sub-Pixel Offset Tracking', 'https://semopenalex.org/source/S4377196294', 'https://semopenalex.org/source/S101949793', 'Spaceborne GNSS-Reflectometry for Ship-Detection Applications: Impact of Acquisition Geometry and Polarization', 'Acquisition modes', 'Efficient Processing for Far-From-Transmitter Formation-Flying SAR Receivers', 'https://semopenalex.org/source/S4306498155', 'A Unified Formulation of SAR Raw Signals From Extended Scenes for All Acquisition Modes With Application to Simulation', 'Railway Bridge Monitoring with Sar: A Case Study', 'https://semopenalex.org/source/S4306508950', 'https://semopenalex.org/source/S4210178770', 'https://semopenalex.org/source/S4306401280', "Deciphering Earth's Movements: Unveiling Subsidence and Displacement in Capo Colonna Through SAR and CGPS", 'Scattering-based Despeckling of Multi-frequency SAR Data', 'https://semopenalex.org/source/S4363605409', 'X-Band SAR Antenna Design for a CubeSat Formation-Flying Remote Sensing Mission', 'Bistatic Scattering From Anisotropic Rough Surfaces via a Closed-Form Two-Scale Model', 'Earth Environmental Monitoring Using Multi-Temporal Synthetic Aperture Radar: A Critical Review of Selected Applications', 'Polarimetric Two-Scale Model for the Evaluation of Bistatic Scattering from Anisotropic Sea Surfaces', 'Polarimetric Two-Scale Model for Soil Moisture Estimation from Hybrid Compact Polarimetry SAR Data', 'The Role of Resolution in the Estimation of Fractal Dimension Maps From SAR Data', 'https://semopenalex.org/source/S126920919', 'https://semopenalex.org/source/S4363608006']</t>
+  </si>
+  <si>
+    <t>['Vaccine Distribution', 'Introduction', 'https://semopenalex.org/source/S4363605353', 'Graph Compression', 'Promoting Diversity in the Evolution of Biological Sequence Data', 'AI Versus Epidemics', 'Conference Report on 2022 IEEE Conference on Computational Intelligence in Bioinformatics and Computational Biology (IEEE CIBCB 2022) [Conference Report]', 'https://semopenalex.org/source/S4210218191', 'A multi-objective genetic algorithm for compression of weighted graphs to simplify epidemic analysis', 'https://semopenalex.org/source/S99347777', 'https://semopenalex.org/source/S4306525036', '2022 IEEE conference on computational intelligence in bioinformatics and computational biology (IEEE CIBCB, 2022)', 'Network Induction', 'Network Induction Issues', 'Evolutionary Computation', 'https://semopenalex.org/source/S4363604921', 'Dungeons, Dragons, and Data Breaches: Analyzing AI Attacks on Various Network Configurations', 'What Drives Evolution of Self-Driving Automata?', 'https://semopenalex.org/source/S104797584', 'https://semopenalex.org/source/S4210216571', 'https://semopenalex.org/source/S140556538', 'All lockdowns are not equal: Reducing epidemic impact through evolutionary computation', 'Freezing of gait in Parkinson’s disease: Classification using computational intelligence']</t>
   </si>
   <si>
     <t>['true']</t>
@@ -184,13 +184,13 @@
     <t>['false']</t>
   </si>
   <si>
-    <t>['https://semopenalex.org/work/W2805259552', 'https://semopenalex.org/work/W2116751005', 'https://semopenalex.org/work/W2950767750', 'https://semopenalex.org/work/W1864513555', 'https://semopenalex.org/work/W2241753404', 'https://semopenalex.org/work/W2891828336', 'https://semopenalex.org/work/W1828916228', 'https://semopenalex.org/work/W1989790075', 'https://semopenalex.org/work/W4232393324', 'https://semopenalex.org/work/W2106697542', 'https://semopenalex.org/work/W2103637183', 'https://semopenalex.org/work/W4294643449', 'https://semopenalex.org/work/W2163547689', 'https://semopenalex.org/work/W4309830289', 'https://semopenalex.org/work/W2025458350', 'https://semopenalex.org/work/W2164697291', 'https://semopenalex.org/work/W3097663184', 'https://semopenalex.org/work/W2934437784', 'https://semopenalex.org/work/W1993524608', 'https://semopenalex.org/work/W2591258888', 'https://semopenalex.org/work/W2984425774', 'https://semopenalex.org/work/W2108057985', 'https://semopenalex.org/work/W2005858158', 'https://semopenalex.org/work/W2040835538', 'https://semopenalex.org/work/W2117368578', 'https://semopenalex.org/work/W2902616013', 'https://semopenalex.org/work/W2130721121', 'https://semopenalex.org/work/W2594176303', 'https://semopenalex.org/work/W2161770118', 'https://semopenalex.org/work/W4402699738', 'https://semopenalex.org/work/W1881771041', 'https://semopenalex.org/work/W2048025952', 'https://semopenalex.org/work/W2912726147', 'https://semopenalex.org/work/W2500472126', 'https://semopenalex.org/work/W2141052825', 'https://semopenalex.org/work/W1984186332', 'https://semopenalex.org/work/W4397026396', 'https://semopenalex.org/work/W1814798360', 'https://semopenalex.org/work/W2150042449', 'https://semopenalex.org/work/W1984866494', 'https://semopenalex.org/work/W2129361591', 'https://semopenalex.org/work/W2063331068', 'https://semopenalex.org/work/W2165331646', 'https://semopenalex.org/work/W2143820350', 'https://semopenalex.org/work/W125371902', 'https://semopenalex.org/work/W4403704152', 'https://semopenalex.org/work/W2883797206', 'https://semopenalex.org/work/W2169931542', 'https://semopenalex.org/work/W2139649788', 'https://semopenalex.org/work/W2059944861', 'https://semopenalex.org/work/W4385938192', 'https://semopenalex.org/work/W2151073381', 'https://semopenalex.org/work/W2170329684', 'https://semopenalex.org/work/W4387430828', 'https://semopenalex.org/work/W2136510471', 'https://semopenalex.org/work/W2026114584', 'https://semopenalex.org/work/W2949908757', 'https://semopenalex.org/work/W2106738903', 'https://semopenalex.org/work/W3103773508', 'https://semopenalex.org/work/W4383472744', 'https://semopenalex.org/work/W2547849178', 'https://semopenalex.org/work/W2120952077', 'https://semopenalex.org/work/W4362508498', 'https://semopenalex.org/work/W2160846724', 'https://semopenalex.org/work/W2133887756', 'https://semopenalex.org/work/W3196466252', 'https://semopenalex.org/work/W169488611', 'https://semopenalex.org/work/W2075739489', 'https://semopenalex.org/work/W2111182668', 'https://semopenalex.org/work/W2182254337', 'https://semopenalex.org/work/W2110043300', 'https://semopenalex.org/work/W2143075489', 'https://semopenalex.org/work/W2143053621', 'https://semopenalex.org/work/W4288374763', 'https://semopenalex.org/work/W2018354435', 'https://semopenalex.org/work/W2112866668', 'https://semopenalex.org/work/W3180681495', 'https://semopenalex.org/work/W1685599524', 'https://semopenalex.org/work/W2096939401', 'https://semopenalex.org/work/W3162654685', 'https://semopenalex.org/work/W1993842801', 'https://semopenalex.org/work/W3165143095', 'https://semopenalex.org/work/W1988328721', 'https://semopenalex.org/work/W2013218112', 'https://semopenalex.org/work/W2035239234', 'https://semopenalex.org/work/W2970159846', 'https://semopenalex.org/work/W2958049034', 'https://semopenalex.org/work/W2162031088', 'https://semopenalex.org/work/W2279111001', 'https://semopenalex.org/work/W2805042680', 'https://semopenalex.org/work/W2140684562', 'https://semopenalex.org/work/W4389138629', 'https://semopenalex.org/work/W2788351666', 'https://semopenalex.org/work/W4394744533', 'https://semopenalex.org/work/W2160431219', 'https://semopenalex.org/work/W2140807309', 'https://semopenalex.org/work/W2636221734', 'https://semopenalex.org/work/W4302382703', 'https://semopenalex.org/work/W3010742537', 'https://semopenalex.org/work/W2117161818', 'https://semopenalex.org/work/W2126230854', 'https://semopenalex.org/work/W2137477396', 'https://semopenalex.org/work/W4400572667', 'https://semopenalex.org/work/W2007203285', 'https://semopenalex.org/work/W2939804650', 'https://semopenalex.org/work/W4386728307', 'https://semopenalex.org/work/W2017812570', 'https://semopenalex.org/work/W4315606555', 'https://semopenalex.org/work/W2144185926', 'https://semopenalex.org/work/W1971056102', 'https://semopenalex.org/work/W2939947188', 'https://semopenalex.org/work/W4231953543', 'https://semopenalex.org/work/W4401753946', 'https://semopenalex.org/work/W2035899572', 'https://semopenalex.org/work/W2963504418', 'https://semopenalex.org/work/W1976082632', 'https://semopenalex.org/work/W2955178723', 'https://semopenalex.org/work/W2116180989', 'https://semopenalex.org/work/W4386728269', 'https://semopenalex.org/work/W4290556151', 'https://semopenalex.org/work/W2109820484', 'https://semopenalex.org/work/W2112250360', 'https://semopenalex.org/work/W2013030361', 'https://semopenalex.org/work/W2127735446', 'https://semopenalex.org/work/W2117083020', 'https://semopenalex.org/work/W3000267050', 'https://semopenalex.org/work/W2107462260', 'https://semopenalex.org/work/W3002449320', 'https://semopenalex.org/work/W2055834582', 'https://semopenalex.org/work/W2003410902', 'https://semopenalex.org/work/W2084633773', 'https://semopenalex.org/work/W2168925869', 'https://semopenalex.org/work/W2158368814', 'https://semopenalex.org/work/W2898646732', 'https://semopenalex.org/work/W4287198234', 'https://semopenalex.org/work/W2094507611', 'https://semopenalex.org/work/W4249394463', 'https://semopenalex.org/work/W4298016756', 'https://semopenalex.org/work/W4400905987', 'https://semopenalex.org/work/W4404179957', 'https://semopenalex.org/work/W2114658777', 'https://semopenalex.org/work/W2150258751', 'https://semopenalex.org/work/W2129001064', 'https://semopenalex.org/work/W2102935592', 'https://semopenalex.org/work/W2166805843', 'https://semopenalex.org/work/W1764485696', 'https://semopenalex.org/work/W855221475', 'https://semopenalex.org/work/W2801854492', 'https://semopenalex.org/work/W4387322833', 'https://semopenalex.org/work/W1975302208', 'https://semopenalex.org/work/W1963919043', 'https://semopenalex.org/work/W2970497931', 'https://semopenalex.org/work/W2078098401', 'https://semopenalex.org/work/W2125836087', 'https://semopenalex.org/work/W2129859788', 'https://semopenalex.org/work/W2537624010', 'https://semopenalex.org/work/W2949567914', 'https://semopenalex.org/work/W4248583122', 'https://semopenalex.org/work/W3092177264', 'https://semopenalex.org/work/W3144738859', 'https://semopenalex.org/work/W2745032981', 'https://semopenalex.org/work/W2037489965', 'https://semopenalex.org/work/W2120280503', 'https://semopenalex.org/work/W2018384246', 'https://semopenalex.org/work/W2155153848', 'https://semopenalex.org/work/W2988626048', 'https://semopenalex.org/work/W2190195640', 'https://semopenalex.org/work/W4388829566', 'https://semopenalex.org/work/W2128722362', 'https://semopenalex.org/work/W2145332056', 'https://semopenalex.org/work/W3010349365', 'https://semopenalex.org/work/W1747115033', 'https://semopenalex.org/work/W2169956538', 'https://semopenalex.org/work/W2026055324', 'https://semopenalex.org/work/W1969428279', 'https://semopenalex.org/work/W1882111414', 'https://semopenalex.org/work/W2949402315', 'https://semopenalex.org/work/W1983410565', 'https://semopenalex.org/work/W2210029275', 'https://semopenalex.org/work/W4403926088', 'https://semopenalex.org/work/W2007101240', 'https://semopenalex.org/work/W2223218801', 'https://semopenalex.org/work/W2097669227', 'https://semopenalex.org/work/W1984896113', 'https://semopenalex.org/work/W1492310094', 'https://semopenalex.org/work/W2099441560', 'https://semopenalex.org/work/W2115355054', 'https://semopenalex.org/work/W2044764741', 'https://semopenalex.org/work/W2128821548', 'https://semopenalex.org/work/W2126535187', 'https://semopenalex.org/work/W3179268546', 'https://semopenalex.org/work/W3200113339', 'https://semopenalex.org/work/W2119239701', 'https://semopenalex.org/work/W2018680103', 'https://semopenalex.org/work/W2095121969', 'https://semopenalex.org/work/W2293728320', 'https://semopenalex.org/work/W2090955007', 'https://semopenalex.org/work/W4393531447', 'https://semopenalex.org/work/W2970012313', 'https://semopenalex.org/work/W2158642611', 'https://semopenalex.org/work/W4386728227', 'https://semopenalex.org/work/W2165018097', 'https://semopenalex.org/work/W2160014433', 'https://semopenalex.org/work/W2950247931', 'https://semopenalex.org/work/W2114885066', 'https://semopenalex.org/work/W4304207591', 'https://semopenalex.org/work/W2001708147', 'https://semopenalex.org/work/W3104967842', 'https://semopenalex.org/work/W2108491840', 'https://semopenalex.org/work/W2114391062', 'https://semopenalex.org/work/W2072116332', 'https://semopenalex.org/work/W4322706631', 'https://semopenalex.org/work/W2080412418', 'https://semopenalex.org/work/W2701634507', 'https://semopenalex.org/work/W2124480047', 'https://semopenalex.org/work/W2002799652', 'https://semopenalex.org/work/W2124543240', 'https://semopenalex.org/work/W2140749977', 'https://semopenalex.org/work/W3163954017', 'https://semopenalex.org/work/W4289306231', 'https://semopenalex.org/work/W2098408658', 'https://semopenalex.org/work/W2044542062', 'https://semopenalex.org/work/W2128254445', 'https://semopenalex.org/work/W2140316862', 'https://semopenalex.org/work/W3009810166', 'https://semopenalex.org/work/W1565749342', 'https://semopenalex.org/work/W2150474553', 'https://semopenalex.org/work/W1507181737', 'https://semopenalex.org/work/W3129332190', 'https://semopenalex.org/work/W4256384691', 'https://semopenalex.org/work/W2746198904', 'https://semopenalex.org/work/W2138646635', 'https://semopenalex.org/work/W3176828173', 'https://semopenalex.org/work/W4401498566', 'https://semopenalex.org/work/W2108797761', 'https://semopenalex.org/work/W2521295940', 'https://semopenalex.org/work/W2770676961', 'https://semopenalex.org/work/W1564509605', 'https://semopenalex.org/work/W1945014867', 'https://semopenalex.org/work/W2147993784', 'https://semopenalex.org/work/W2041032353', 'https://semopenalex.org/work/W2053928191', 'https://semopenalex.org/work/W1970184235', 'https://semopenalex.org/work/W4394868342', 'https://semopenalex.org/work/W2988564852', 'https://semopenalex.org/work/W2963927825', 'https://semopenalex.org/work/W1989282861', 'https://semopenalex.org/work/W2134671262', 'https://semopenalex.org/work/W1778342465', 'https://semopenalex.org/work/W4226253448', 'https://semopenalex.org/work/W2544362511', 'https://semopenalex.org/work/W2094757833', 'https://semopenalex.org/work/W3043975171', 'https://semopenalex.org/work/W2441173492', 'https://semopenalex.org/work/W2107105182', 'https://semopenalex.org/work/W2100527158', 'https://semopenalex.org/work/W3161900557', 'https://semopenalex.org/work/W2945382159', 'https://semopenalex.org/work/W2963612078', 'https://semopenalex.org/work/W2924551290', 'https://semopenalex.org/work/W1867833735', 'https://semopenalex.org/work/W2755327666', 'https://semopenalex.org/work/W2075650606', 'https://semopenalex.org/work/W2019064108', 'https://semopenalex.org/work/W2791061193', 'https://semopenalex.org/work/W4299390071', 'https://semopenalex.org/work/W2938524150', 'https://semopenalex.org/work/W2294916470', 'https://semopenalex.org/work/W4283028880', 'https://semopenalex.org/work/W2113885710', 'https://semopenalex.org/work/W2108634960', 'https://semopenalex.org/work/W4298078907', 'https://semopenalex.org/work/W2149742409', 'https://semopenalex.org/work/W2172643935', 'https://semopenalex.org/work/W1813016789', 'https://semopenalex.org/work/W2784488119', 'https://semopenalex.org/work/W835410257', 'https://semopenalex.org/work/W2949122408', 'https://semopenalex.org/work/W1831978873', 'https://semopenalex.org/work/W2951231774', 'https://semopenalex.org/work/W2086613112', 'https://semopenalex.org/work/W2111934195', 'https://semopenalex.org/work/W2032435948', 'https://semopenalex.org/work/W4205889589', 'https://semopenalex.org/work/W3084462124', 'https://semopenalex.org/work/W1774599862', 'https://semopenalex.org/work/W4387698499', 'https://semopenalex.org/work/W2697509747', 'https://semopenalex.org/work/W1600396855', 'https://semopenalex.org/work/W3107843792', 'https://semopenalex.org/work/W4405444483', 'https://semopenalex.org/work/W2124085076', 'https://semopenalex.org/work/W2791467061', 'https://semopenalex.org/work/W2171858716', 'https://semopenalex.org/work/W2167460076', 'https://semopenalex.org/work/W2127722806', 'https://semopenalex.org/work/W3111054769', 'https://semopenalex.org/work/W2158537680', 'https://semopenalex.org/work/W4284707241', 'https://semopenalex.org/work/W2111557101', 'https://semopenalex.org/work/W2102152654', 'https://semopenalex.org/work/W2145568341', 'https://semopenalex.org/work/W2084295409', 'https://semopenalex.org/work/W2109495528', 'https://semopenalex.org/work/W2130561641', 'https://semopenalex.org/work/W2027160844', 'https://semopenalex.org/work/W4388118224', 'https://semopenalex.org/work/W2605257447', 'https://semopenalex.org/work/W1797286681', 'https://semopenalex.org/work/W2188482746', 'https://semopenalex.org/work/W2798274156', 'https://semopenalex.org/work/W2133913871', 'https://semopenalex.org/work/W2114059901', 'https://semopenalex.org/work/W2296243746', 'https://semopenalex.org/work/W2020196086', 'https://semopenalex.org/work/W1028196162', 'https://semopenalex.org/work/W1684154970', 'https://semopenalex.org/work/W2245018327', 'https://semopenalex.org/work/W4283760386', 'https://semopenalex.org/work/W2277416294', 'https://semopenalex.org/work/W2138395721', 'https://semopenalex.org/work/W2486186027', 'https://semopenalex.org/work/W2337354189', 'https://semopenalex.org/work/W3015206436', 'https://semopenalex.org/work/W2130794128', 'https://semopenalex.org/work/W2088188946', 'https://semopenalex.org/work/W2806687546', 'https://semopenalex.org/work/W2138556535', 'https://semopenalex.org/work/W3098360176', 'https://semopenalex.org/work/W2027156706', 'https://semopenalex.org/work/W2118343132', 'https://semopenalex.org/work/W2618462601', 'https://semopenalex.org/work/W8218751', 'https://semopenalex.org/work/W1995977330', 'https://semopenalex.org/work/W2131938193', 'https://semopenalex.org/work/W2786494993', 'https://semopenalex.org/work/W2136849809', 'https://semopenalex.org/work/W3015454417', 'https://semopenalex.org/work/W2336180720', 'https://semopenalex.org/work/W2021159593', 'https://semopenalex.org/work/W2133682680', 'https://semopenalex.org/work/W1868782008', 'https://semopenalex.org/work/W2108862142', 'https://semopenalex.org/work/W2052527654', 'https://semopenalex.org/work/W2109383404', 'https://semopenalex.org/work/W2171286517', 'https://semopenalex.org/work/W4225966372', 'https://semopenalex.org/work/W2972140606', 'https://semopenalex.org/work/W2785643816', 'https://semopenalex.org/work/W2150180245', 'https://semopenalex.org/work/W2137966369', 'https://semopenalex.org/work/W1990472383', 'https://semopenalex.org/work/W2055673378', 'https://semopenalex.org/work/W2114028749', 'https://semopenalex.org/work/W2098410722', 'https://semopenalex.org/work/W2115596980', 'https://semopenalex.org/work/W4299311104', 'https://semopenalex.org/work/W1784288318', 'https://semopenalex.org/work/W1530322092', 'https://semopenalex.org/work/W2141480726', 'https://semopenalex.org/work/W842176471', 'https://semopenalex.org/work/W2663325069', 'https://semopenalex.org/work/W2118103599', 'https://semopenalex.org/work/W1968153028', 'https://semopenalex.org/work/W2898681335', 'https://semopenalex.org/work/W2120889368', 'https://semopenalex.org/work/W2003260793', 'https://semopenalex.org/work/W2892075135', 'https://semopenalex.org/work/W1989616605', 'https://semopenalex.org/work/W2949657987', 'https://semopenalex.org/work/W1969115782', 'https://semopenalex.org/work/W1976296868', 'https://semopenalex.org/work/W2126043778', 'https://semopenalex.org/work/W4223588778', 'https://semopenalex.org/work/W2003603103', 'https://semopenalex.org/work/W2763660685', 'https://semopenalex.org/work/W1940162557', 'https://semopenalex.org/work/W2162696202', 'https://semopenalex.org/work/W2159524123', 'https://semopenalex.org/work/W205233311', 'https://semopenalex.org/work/W2811277086', 'https://semopenalex.org/work/W1602846904', 'https://semopenalex.org/work/W2065892151', 'https://semopenalex.org/work/W3103915668', 'https://semopenalex.org/work/W3097189301', 'https://semopenalex.org/work/W1965141814', 'https://semopenalex.org/work/W610096311', 'https://semopenalex.org/work/W4224949960', 'https://semopenalex.org/work/W4297748597', 'https://semopenalex.org/work/W2129898633', 'https://semopenalex.org/work/W2121752514', 'https://semopenalex.org/work/W2164044612', 'https://semopenalex.org/work/W4225288565', 'https://semopenalex.org/work/W1809937706', 'https://semopenalex.org/work/W1783191689', 'https://semopenalex.org/work/W2033157981', 'https://semopenalex.org/work/W2043499328', 'https://semopenalex.org/work/W2114379490', 'https://semopenalex.org/work/W3163624263', 'https://semopenalex.org/work/W1895161527', 'https://semopenalex.org/work/W2102302018', 'https://semopenalex.org/work/W2097084589', 'https://semopenalex.org/work/W2122776646', 'https://semopenalex.org/work/W4386362571', 'https://semopenalex.org/work/W2992547694', 'https://semopenalex.org/work/W1992781262', 'https://semopenalex.org/work/W2108934479', 'https://semopenalex.org/work/W2304264384', 'https://semopenalex.org/work/W4402559984', 'https://semopenalex.org/work/W2102592853', 'https://semopenalex.org/work/W2003520411', 'https://semopenalex.org/work/W2920551025', 'https://semopenalex.org/work/W2334675349', 'https://semopenalex.org/work/W2487376240', 'https://semopenalex.org/work/W2185477524', 'https://semopenalex.org/work/W2979998822', 'https://semopenalex.org/work/W2806925689', 'https://semopenalex.org/work/W2135428614', 'https://semopenalex.org/work/W2006713327', 'https://semopenalex.org/work/W2168665985', 'https://semopenalex.org/work/W4299652167', 'https://semopenalex.org/work/W2249000025', 'https://semopenalex.org/work/W2958959679', 'https://semopenalex.org/work/W2064969586', 'https://semopenalex.org/work/W2120659763', 'https://semopenalex.org/work/W2127324110', 'https://semopenalex.org/work/W2152537098', 'https://semopenalex.org/work/W2918802163', 'https://semopenalex.org/work/W4313525046', 'https://semopenalex.org/work/W2160616608', 'https://semopenalex.org/work/W2160492008', 'https://semopenalex.org/work/W2108017142', 'https://semopenalex.org/work/W4308236214', 'https://semopenalex.org/work/W2163889321', 'https://semopenalex.org/work/W4379033886', 'https://semopenalex.org/work/W2166197815', 'https://semopenalex.org/work/W2141798281', 'https://semopenalex.org/work/W2054059427', 'https://semopenalex.org/work/W2280892290', 'https://semopenalex.org/work/W2728552870', 'https://semopenalex.org/work/W4244875117', 'https://semopenalex.org/work/W4200630260', 'https://semopenalex.org/work/W2014068777', 'https://semopenalex.org/work/W4233630823', 'https://semopenalex.org/work/W2618786793', 'https://semopenalex.org/work/W2078616504', 'https://semopenalex.org/work/W3158448776', 'https://semopenalex.org/work/W2059916190', 'https://semopenalex.org/work/W1967770515', 'https://semopenalex.org/work/W2134429331', 'https://semopenalex.org/work/W4376141221', 'https://semopenalex.org/work/W2501553433', 'https://semopenalex.org/work/W4288482042', 'https://semopenalex.org/work/W1624008340', 'https://semopenalex.org/work/W1785723168', 'https://semopenalex.org/work/W1967447459', 'https://semopenalex.org/work/W3127203349', 'https://semopenalex.org/work/W2024240534', 'https://semopenalex.org/work/W2791120428', 'https://semopenalex.org/work/W3098900881', 'https://semopenalex.org/work/W2165066371', 'https://semopenalex.org/work/W3047457796', 'https://semopenalex.org/work/W2123482670', 'https://semopenalex.org/work/W4393439986', 'https://semopenalex.org/work/W2077616584', 'https://semopenalex.org/work/W4282004224', 'https://semopenalex.org/work/W2103254499', 'https://semopenalex.org/work/W2152477879', 'https://semopenalex.org/work/W4301512502', 'https://semopenalex.org/work/W1667912148', 'https://semopenalex.org/work/W2568027424', 'https://semopenalex.org/work/W1818779082', 'https://semopenalex.org/work/W2119454020', 'https://semopenalex.org/work/W2230831981', 'https://semopenalex.org/work/W2903667675', 'https://semopenalex.org/work/W86912345', 'https://semopenalex.org/work/W2130502393', 'https://semopenalex.org/work/W2182267970', 'https://semopenalex.org/work/W2144570150', 'https://semopenalex.org/work/W2949618677', 'https://semopenalex.org/work/W2806144920', 'https://semopenalex.org/work/W1861730306', 'https://semopenalex.org/work/W2491625832', 'https://semopenalex.org/work/W2101094458', 'https://semopenalex.org/work/W2266109773', 'https://semopenalex.org/work/W605016662', 'https://semopenalex.org/work/W1808004798', 'https://semopenalex.org/work/W609082053', 'https://semopenalex.org/work/W2162281264', 'https://semopenalex.org/work/W1817934356', 'https://semopenalex.org/work/W4388483721', 'https://semopenalex.org/work/W1867432869', 'https://semopenalex.org/work/W1696074034', 'https://semopenalex.org/work/W2167187798', 'https://semopenalex.org/work/W2035561336', 'https://semopenalex.org/work/W1984118997', 'https://semopenalex.org/work/W1996041609', 'https://semopenalex.org/work/W2165131653', 'https://semopenalex.org/work/W2981712458', 'https://semopenalex.org/work/W2168793726', 'https://semopenalex.org/work/W2740763524', 'https://semopenalex.org/work/W4297422548', 'https://semopenalex.org/work/W2149513726', 'https://semopenalex.org/work/W2242734504', 'https://semopenalex.org/work/W4388235556', 'https://semopenalex.org/work/W2950434959', 'https://semopenalex.org/work/W2109453625', 'https://semopenalex.org/work/W2053078240', 'https://semopenalex.org/work/W3036861309', 'https://semopenalex.org/work/W2119248338', 'https://semopenalex.org/work/W2602238908', 'https://semopenalex.org/work/W2792903117', 'https://semopenalex.org/work/W4301439726', 'https://semopenalex.org/work/W2952168395', 'https://semopenalex.org/work/W2956308890', 'https://semopenalex.org/work/W1532372374', 'https://semopenalex.org/work/W2400256934', 'https://semopenalex.org/work/W2537630632', 'https://semopenalex.org/work/W949508384', 'https://semopenalex.org/work/W1988343658', 'https://semopenalex.org/work/W2953215316', 'https://semopenalex.org/work/W2144099933', 'https://semopenalex.org/work/W2032099309', 'https://semopenalex.org/work/W2991868466', 'https://semopenalex.org/work/W1812926078', 'https://semopenalex.org/work/W2123832893', 'https://semopenalex.org/work/W2142005762', 'https://semopenalex.org/work/W1971037148', 'https://semopenalex.org/work/W2765225938', 'https://semopenalex.org/work/W2056448690', 'https://semopenalex.org/work/W2143708007', 'https://semopenalex.org/work/W2100279715', 'https://semopenalex.org/work/W1975277950', 'https://semopenalex.org/work/W2785502402', 'https://semopenalex.org/work/W2128912491', 'https://semopenalex.org/work/W2950185045', 'https://semopenalex.org/work/W1857284394', 'https://semopenalex.org/work/W2764441237', 'https://semopenalex.org/work/W2982533818', 'https://semopenalex.org/work/W2970592033', 'https://semopenalex.org/work/W2035640322', 'https://semopenalex.org/work/W4390050192', 'https://semopenalex.org/work/W2115943920', 'https://semopenalex.org/work/W4281762710', 'https://semopenalex.org/work/W2145173682', 'https://semopenalex.org/work/W3194819591', 'https://semopenalex.org/work/W2160284518', 'https://semopenalex.org/work/W4381304944', 'https://semopenalex.org/work/W3183518399', 'https://semopenalex.org/work/W2195712461', 'https://semopenalex.org/work/W2104091137', 'https://semopenalex.org/work/W1855265535', 'https://semopenalex.org/work/W3199731519', 'https://semopenalex.org/work/W2042583427', 'https://semopenalex.org/work/W2015282877', 'https://semopenalex.org/work/W2103969908', 'https://semopenalex.org/work/W1891629850', 'https://semopenalex.org/work/W2020493940', 'https://semopenalex.org/work/W2611380909', 'https://semopenalex.org/work/W2106039030', 'https://semopenalex.org/work/W2106233876', 'https://semopenalex.org/work/W234261451', 'https://semopenalex.org/work/W2162965487', 'https://semopenalex.org/work/W2169536566', 'https://semopenalex.org/work/W2148267424', 'https://semopenalex.org/work/W3094576801', 'https://semopenalex.org/work/W2155624091', 'https://semopenalex.org/work/W2159718141', 'https://semopenalex.org/work/W2118420236', 'https://semopenalex.org/work/W2158693223', 'https://semopenalex.org/work/W2117127275', 'https://semopenalex.org/work/W656907390', 'https://semopenalex.org/work/W3098873033', 'https://semopenalex.org/work/W3106431100', 'https://semopenalex.org/work/W4386352568', 'https://semopenalex.org/work/W2085980614', 'https://semopenalex.org/work/W2026970166', 'https://semopenalex.org/work/W4377043292', 'https://semopenalex.org/work/W1971235196', 'https://semopenalex.org/work/W2125239611', 'https://semopenalex.org/work/W2138621265', 'https://semopenalex.org/work/W1884565435', 'https://semopenalex.org/work/W2158228464', 'https://semopenalex.org/work/W2017148819', 'https://semopenalex.org/work/W2100814254', 'https://semopenalex.org/work/W2119876849', 'https://semopenalex.org/work/W2162485250', 'https://semopenalex.org/work/W2145983295', 'https://semopenalex.org/work/W2294282334', 'https://semopenalex.org/work/W1828712802', 'https://semopenalex.org/work/W4401750498', 'https://semopenalex.org/work/W2141801703', 'https://semopenalex.org/work/W1964567495', 'https://semopenalex.org/work/W2395280900', 'https://semopenalex.org/work/W2077024675', 'https://semopenalex.org/work/W3106213621', 'https://semopenalex.org/work/W2046546110', 'https://semopenalex.org/work/W2189600142', 'https://semopenalex.org/work/W2408555870', 'https://semopenalex.org/work/W2113359099', 'https://semopenalex.org/work/W2124699087', 'https://semopenalex.org/work/W2166862038', 'https://semopenalex.org/work/W2099998345', 'https://semopenalex.org/work/W4300434862', 'https://semopenalex.org/work/W2166153231', 'https://semopenalex.org/work/W1995899361', 'https://semopenalex.org/work/W2143286465', 'https://semopenalex.org/work/W1985231173', 'https://semopenalex.org/work/W2308119766', 'https://semopenalex.org/work/W4304701022', 'https://semopenalex.org/work/W2119330876', 'https://semopenalex.org/work/W2142780243', 'https://semopenalex.org/work/W2106903616', 'https://semopenalex.org/work/W2481609999', 'https://semopenalex.org/work/W4309877015', 'https://semopenalex.org/work/W4311488571', 'https://semopenalex.org/work/W4298025544', 'https://semopenalex.org/work/W3093907665', 'https://semopenalex.org/work/W2155252144', 'https://semopenalex.org/work/W2048467330', 'https://semopenalex.org/work/W2327976118', 'https://semopenalex.org/work/W2035930173', 'https://semopenalex.org/work/W2383111726', 'https://semopenalex.org/work/W2092230235', 'https://semopenalex.org/work/W3088481514', 'https://semopenalex.org/work/W4386728284', 'https://semopenalex.org/work/W2135421180', 'https://semopenalex.org/work/W2055070400', 'https://semopenalex.org/work/W3164197023', 'https://semopenalex.org/work/W2039091249', 'https://semopenalex.org/work/W2733144798', 'https://semopenalex.org/work/W2439315773', 'https://semopenalex.org/work/W2977723824', 'https://semopenalex.org/work/W2998913556', 'https://semopenalex.org/work/W4388567240', 'https://semopenalex.org/work/W2399804733', 'https://semopenalex.org/work/W3166787465', 'https://semopenalex.org/work/W2106900553', 'https://semopenalex.org/work/W1825244231', 'https://semopenalex.org/work/W2940821791', 'https://semopenalex.org/work/W4243743111', 'https://semopenalex.org/work/W3106512002', 'https://semopenalex.org/work/W6747142', 'https://semopenalex.org/work/W4283215612', 'https://semopenalex.org/work/W1502655780', 'https://semopenalex.org/work/W2096933831', 'https://semopenalex.org/work/W2920910927', 'https://semopenalex.org/work/W4402350832', 'https://semopenalex.org/work/W2054656164', 'https://semopenalex.org/work/W2974617835', 'https://semopenalex.org/work/W3003820456', 'https://semopenalex.org/work/W3137611772', 'https://semopenalex.org/work/W4288088101', 'https://semopenalex.org/work/W2170015373', 'https://semopenalex.org/work/W2122128429', 'https://semopenalex.org/work/W2178506535', 'https://semopenalex.org/work/W4297897521', 'https://semopenalex.org/work/W4298181338', 'https://semopenalex.org/work/W2107882641', 'https://semopenalex.org/work/W2287663230', 'https://semopenalex.org/work/W4283396505', 'https://semopenalex.org/work/W1694434332', 'https://semopenalex.org/work/W2189224346', 'https://semopenalex.org/work/W1946393290', 'https://semopenalex.org/work/W2063650998', 'https://semopenalex.org/work/W4298174976', 'https://semopenalex.org/work/W2151679725', 'https://semopenalex.org/work/W2892539592', 'https://semopenalex.org/work/W989118312', 'https://semopenalex.org/work/W2132288860', 'https://semopenalex.org/work/W2143623375', 'https://semopenalex.org/work/W4402502594', 'https://semopenalex.org/work/W1587379027', 'https://semopenalex.org/work/W1965551074', 'https://semopenalex.org/work/W2075899871', 'https://semopenalex.org/work/W4386728368', 'https://semopenalex.org/work/W2120967246', 'https://semopenalex.org/work/W2168204206', 'https://semopenalex.org/work/W4297229624', 'https://semopenalex.org/work/W2963345994', 'https://semopenalex.org/work/W4298871721', 'https://semopenalex.org/work/W2160172952', 'https://semopenalex.org/work/W2039909063', 'https://semopenalex.org/work/W1820714040', 'https://semopenalex.org/work/W2017830666', 'https://semopenalex.org/work/W1987895141', 'https://semopenalex.org/work/W4287256164', 'https://semopenalex.org/work/W2112567022', 'https://semopenalex.org/work/W1972847653', 'https://semopenalex.org/work/W2012992134', 'https://semopenalex.org/work/W2129518598', 'https://semopenalex.org/work/W4226379915', 'https://semopenalex.org/work/W2131459843', 'https://semopenalex.org/work/W2135604443', 'https://semopenalex.org/work/W3088822975', 'https://semopenalex.org/work/W2127631196', 'https://semopenalex.org/work/W2182338449', 'https://semopenalex.org/work/W1958624633', 'https://semopenalex.org/work/W2166315125', 'https://semopenalex.org/work/W218303851', 'https://semopenalex.org/work/W2131745743', 'https://semopenalex.org/work/W2545039763', 'https://semopenalex.org/work/W2148407475', 'https://semopenalex.org/work/W2102549524', 'https://semopenalex.org/work/W2112502349', 'https://semopenalex.org/work/W2122768752', 'https://semopenalex.org/work/W4312819449', 'https://semopenalex.org/work/W2185641310', 'https://semopenalex.org/work/W3214000901', 'https://semopenalex.org/work/W4403900474', 'https://semopenalex.org/work/W4223992723', 'https://semopenalex.org/work/W2963455631', 'https://semopenalex.org/work/W4307786837', 'https://semopenalex.org/work/W3036970724', 'https://semopenalex.org/work/W2030896881', 'https://semopenalex.org/work/W2025968816', 'https://semopenalex.org/work/W615388181', 'https://semopenalex.org/work/W2133118701', 'https://semopenalex.org/work/W4386081510', 'https://semopenalex.org/work/W3206047407', 'https://semopenalex.org/work/W2151961258', 'https://semopenalex.org/work/W4221163077', 'https://semopenalex.org/work/W2086931264', 'https://semopenalex.org/work/W1794193518', 'https://semopenalex.org/work/W1883544968', 'https://semopenalex.org/work/W2136390628', 'https://semopenalex.org/work/W1976452778', 'https://semopenalex.org/work/W1993109981', 'https://semopenalex.org/work/W1951572853', 'https://semopenalex.org/work/W2902929870', 'https://semopenalex.org/work/W2283163132', 'https://semopenalex.org/work/W2769244027', 'https://semopenalex.org/work/W2125505095', 'https://semopenalex.org/work/W4384811612', 'https://semopenalex.org/work/W2140436532', 'https://semopenalex.org/work/W2125427453', 'https://semopenalex.org/work/W2097867503', 'https://semopenalex.org/work/W2040652823', 'https://semopenalex.org/work/W2101633987', 'https://semopenalex.org/work/W2171540325', 'https://semopenalex.org/work/W2477294189', 'https://semopenalex.org/work/W2185221298', 'https://semopenalex.org/work/W1975448877', 'https://semopenalex.org/work/W2171258724', 'https://semopenalex.org/work/W3134221682', 'https://</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W1975028026', 'https://semopenalex.org/work/W3036463368', 'https://semopenalex.org/work/W2346980133', 'https://semopenalex.org/work/W4379033872', 'https://semopenalex.org/work/W1834136374', 'https://semopenalex.org/work/W2551155618', 'https://semopenalex.org/work/W1993514406', 'https://semopenalex.org/work/W2075286904', 'https://semopenalex.org/work/W4387085789', 'https://semopenalex.org/work/W4406805368', 'https://semopenalex.org/work/W4366598255', 'https://semopenalex.org/work/W4310446060', 'https://semopenalex.org/work/W2008208122', 'https://semopenalex.org/work/W2114418543', 'https://semopenalex.org/work/W4211259494', 'https://semopenalex.org/work/W4251839844', 'https://semopenalex.org/work/W4309619903', 'https://semopenalex.org/work/W2897414246', 'https://semopenalex.org/work/W4256454723', 'https://semopenalex.org/work/W1976594634', 'https://semopenalex.org/work/W2899305210', 'https://semopenalex.org/work/W3204110051', 'https://semopenalex.org/work/W3201213010', 'https://semopenalex.org/work/W3035628382', 'https://semopenalex.org/work/W3204393727', 'https://semopenalex.org/work/W2972889118', 'https://semopenalex.org/work/W2611685970', 'https://semopenalex.org/work/W2966384546', 'https://semopenalex.org/work/W2520661109', 'https://semopenalex.org/work/W2752031858', 'https://semopenalex.org/work/W2899389394', 'https://semopenalex.org/work/W2519914856', 'https://semopenalex.org/work/W4214504130', 'https://semopenalex.org/work/W4312841490', 'https://semopenalex.org/work/W2940716241', 'https://semopenalex.org/work/W2102667737', 'https://semopenalex.org/work/W2061583538', 'https://semopenalex.org/work/W4238249729', 'https://semopenalex.org/work/W2131570437', 'https://semopenalex.org/work/W2598459295', 'https://semopenalex.org/work/W3096658838', 'https://semopenalex.org/work/W4324151651', 'https://semopenalex.org/work/W2793897377', 'https://semopenalex.org/work/W2602397751', 'https://semopenalex.org/work/W862033376', 'https://semopenalex.org/work/W2139733095', 'https://semopenalex.org/work/W2973140914', 'https://semopenalex.org/work/W2789478762', 'https://semopenalex.org/work/W4232727837', 'https://semopenalex.org/work/W4224255688', 'https://semopenalex.org/work/W3024164567', 'https://semopenalex.org/work/W2888386951', 'https://semopenalex.org/work/W3035727063', 'https://semopenalex.org/work/W3028614762', 'https://semopenalex.org/work/W2102905932', 'https://semopenalex.org/work/W3161889270', 'https://semopenalex.org/work/W4294891921', 'https://semopenalex.org/work/W4404026276', 'https://semopenalex.org/work/W3197280612', 'https://semopenalex.org/work/W3030735111', 'https://semopenalex.org/work/W3007521088', 'https://semopenalex.org/work/W4383220643', 'https://semopenalex.org/work/W4396832885', 'https://semopenalex.org/work/W2110284634', 'https://semopenalex.org/work/W2602429360', 'https://semopenalex.org/work/W2613908791', 'https://semopenalex.org/work/W3011317564', 'https://semopenalex.org/work/W4386929049', 'https://semopenalex.org/work/W2790187313', 'https://semopenalex.org/work/W4391210282', 'https://semopenalex.org/work/W4214684069', 'https://semopenalex.org/work/W3126826400', 'https://semopenalex.org/work/W2973016298', 'https://semopenalex.org/work/W4233748389', 'https://semopenalex.org/work/W3178374478', 'https://semopenalex.org/work/W4389256452', 'https://semopenalex.org/work/W2465877051', 'https://semopenalex.org/work/W2591593006', 'https://semopenalex.org/work/W2625122753', 'https://semopenalex.org/work/W3043824623', 'https://semopenalex.org/work/W2007978709', 'https://semopenalex.org/work/W2072697691', 'https://semopenalex.org/work/W3030577208', 'https://semopenalex.org/work/W3047192924', 'https://semopenalex.org/work/W4366967286', 'https://semopenalex.org/work/W4393067517', 'https://semopenalex.org/work/W4308467568', 'https://semopenalex.org/work/W2012358521', 'https://semopenalex.org/work/W2057014910', 'https://semopenalex.org/work/W3196785132', 'https://semopenalex.org/work/W1877041815', 'https://semopenalex.org/work/W2973132733', 'https://semopenalex.org/work/W4377250056', 'https://semopenalex.org/work/W4324150147', 'https://semopenalex.org/work/W2121082751', 'https://semopenalex.org/work/W4393102879', 'https://semopenalex.org/work/W2133951180', 'https://semopenalex.org/work/W3032857618', 'https://semopenalex.org/work/W4324152586', 'https://semopenalex.org/work/W2774467220', 'https://semopenalex.org/work/W2798335699', 'https://semopenalex.org/work/W2159491375', 'https://semopenalex.org/work/W2898627444', 'https://semopenalex.org/work/W3015284588', 'https://semopenalex.org/work/W4287071181', 'https://semopenalex.org/work/W2078369692', 'https://semopenalex.org/work/W2033680836', 'https://semopenalex.org/work/W3028180736', 'https://semopenalex.org/work/W4210450354', 'https://semopenalex.org/work/W4224305168', 'https://semopenalex.org/work/W2753363725', 'https://semopenalex.org/work/W4404915142', 'https://semopenalex.org/work/W3163521409', 'https://semopenalex.org/work/W2737450254', 'https://semopenalex.org/work/W3094759305', 'https://semopenalex.org/work/W4324154015', 'https://semopenalex.org/work/W4210768549', 'https://semopenalex.org/work/W2752493326', 'https://semopenalex.org/work/W4312605566', 'https://semopenalex.org/work/W2754101670', 'https://semopenalex.org/work/W2913475584', 'https://semopenalex.org/work/W2944843734', 'https://semopenalex.org/work/W3033704563', 'https://semopenalex.org/work/W2755164339', 'https://semopenalex.org/work/W2055070571', 'https://semopenalex.org/work/W3162177365', 'https://semopenalex.org/work/W2752042616', 'https://semopenalex.org/work/W3201451193', 'https://semopenalex.org/work/W4366588423', 'https://semopenalex.org/work/W2978280554', 'https://semopenalex.org/work/W3009160614', 'https://semopenalex.org/work/W3135072684', 'https://semopenalex.org/work/W3190617503', 'https://semopenalex.org/work/W4224242333', 'https://semopenalex.org/work/W3215451397', 'https://semopenalex.org/work/W2263778529', 'https://semopenalex.org/work/W2346600598', 'https://semopenalex.org/work/W4234952088', 'https://semopenalex.org/work/W4312646439', 'https://semopenalex.org/work/W3141512745', 'https://semopenalex.org/work/W4366549587', 'https://semopenalex.org/work/W2750727230', 'https://semopenalex.org/work/W2091382943', 'https://semopenalex.org/work/W2152557601', 'https://semopenalex.org/work/W4393877125', 'https://semopenalex.org/work/W2561633795', 'https://semopenalex.org/work/W2762577600', 'https://semopenalex.org/work/W3091007149', 'https://semopenalex.org/work/W2548042282', 'https://semopenalex.org/work/W3186694431', 'https://semopenalex.org/work/W2611151946', 'https://semopenalex.org/work/W3171875220', 'https://semopenalex.org/work/W3000816869', 'https://semopenalex.org/work/W4387606708', 'https://semopenalex.org/work/W2154752229', 'https://semopenalex.org/work/W2942324097', 'https://semopenalex.org/work/W4399126764', 'https://semopenalex.org/work/W2885122621', 'https://semopenalex.org/work/W2896178739', 'https://semopenalex.org/work/W3003204379', 'https://semopenalex.org/work/W2752658305', 'https://semopenalex.org/work/W3095367321', 'https://semopenalex.org/work/W4402722131', 'https://semopenalex.org/work/W3193717464', 'https://semopenalex.org/work/W3022986551', 'https://semopenalex.org/work/W2946308339', 'https://semopenalex.org/work/W2810881717', 'https://semopenalex.org/work/W3084729599', 'https://semopenalex.org/work/W2537880674', 'https://semopenalex.org/work/W2904910662', 'https://semopenalex.org/work/W3160199101', 'https://semopenalex.org/work/W2401872729', 'https://semopenalex.org/work/W3119309106', 'https://semopenalex.org/work/W4221065578', 'https://semopenalex.org/work/W2898667062', 'https://semopenalex.org/work/W2977979696', 'https://semopenalex.org/work/W1985504739', 'https://semopenalex.org/work/W2136876773', 'https://semopenalex.org/work/W2461856634', 'https://semopenalex.org/work/W1510660243', 'https://semopenalex.org/work/W2902941289', 'https://semopenalex.org/work/W4391423303', 'https://semopenalex.org/work/W2052607251', 'https://semopenalex.org/work/W2775793881', 'https://semopenalex.org/work/W2108512685', 'https://semopenalex.org/work/W3181801907', 'https://semopenalex.org/work/W4387421144', 'https://semopenalex.org/work/W2087800309', 'https://semopenalex.org/work/W1704771702', 'https://semopenalex.org/work/W2751622533', 'https://semopenalex.org/work/W3032662532', 'https://semopenalex.org/work/W2610780371', 'https://semopenalex.org/work/W2519250278', 'https://semopenalex.org/work/W2901616108', 'https://semopenalex.org/work/W2090841027', 'https://semopenalex.org/work/W2903849727', 'https://semopenalex.org/work/W2972600126', 'https://semopenalex.org/work/W2968293343', 'https://semopenalex.org/work/W4213455276', 'https://semopenalex.org/work/W4366583934', 'https://semopenalex.org/work/W2088270376', 'https://semopenalex.org/work/W2137846113', 'https://semopenalex.org/work/W2977617583', 'https://semopenalex.org/work/W4404569483', 'https://semopenalex.org/work/W791468510', 'https://semopenalex.org/work/W4229043996', 'https://semopenalex.org/work/W3193396842', 'https://semopenalex.org/work/W4393908582', 'https://semopenalex.org/work/W3163085734', 'https://semopenalex.org/work/W2088502162', 'https://semopenalex.org/work/W4211095911', 'https://semopenalex.org/work/W3121062173', 'https://semopenalex.org/work/W2962975962', 'https://semopenalex.org/work/W3062298123', 'https://semopenalex.org/work/W2752490344', 'https://semopenalex.org/work/W3202016550', 'https://semopenalex.org/work/W2811468211', 'https://semopenalex.org/work/W3033866035', 'https://semopenalex.org/work/W3183940262', 'https://semopenalex.org/work/W2610676428', 'https://semopenalex.org/work/W2920869031', 'https://semopenalex.org/work/W3034123328', 'https://semopenalex.org/work/W4402722090', 'https://semopenalex.org/work/W2605978692', 'https://semopenalex.org/work/W1524596993', 'https://semopenalex.org/work/W4385856456', 'https://semopenalex.org/work/W1998431265', 'https://semopenalex.org/work/W3117330688', 'https://semopenalex.org/work/W4200018492', 'https://semopenalex.org/work/W2899333601', 'https://semopenalex.org/work/W4394883037', 'https://semopenalex.org/work/W2738622408', 'https://semopenalex.org/work/W2165066165', 'https://semopenalex.org/work/W4400189062', 'https://semopenalex.org/work/W2610274107', 'https://semopenalex.org/work/W2089266363', 'https://semopenalex.org/work/W3161959528', 'https://semopenalex.org/work/W4230967253', 'https://semopenalex.org/work/W2519458229', 'https://semopenalex.org/work/W2913594206', 'https://semopenalex.org/work/W3206712787', 'https://semopenalex.org/work/W4400430993', 'https://semopenalex.org/work/W2753801751', 'https://semopenalex.org/work/W2528963299', 'https://semopenalex.org/work/W2108911539', 'https://semopenalex.org/work/W4394825420', 'https://semopenalex.org/work/W3110075456', 'https://semopenalex.org/work/W2942738233', 'https://semopenalex.org/work/W3003369003', 'https://semopenalex.org/work/W4307475355', 'https://semopenalex.org/work/W4225133274', 'https://semopenalex.org/work/W2898822823', 'https://semopenalex.org/work/W1553133540', 'https://semopenalex.org/work/W3188766356', 'https://semopenalex.org/work/W2986358413', 'https://semopenalex.org/work/W4324150573', 'https://semopenalex.org/work/W4389897704', 'https://semopenalex.org/work/W4379879736', 'https://semopenalex.org/work/W2921058600', 'https://semopenalex.org/work/W2898145840', 'https://semopenalex.org/work/W2753671526', 'https://semopenalex.org/work/W4404977899', 'https://semopenalex.org/work/W2515389026', 'https://semopenalex.org/work/W4225473762', 'https://semopenalex.org/work/W1981715407', 'https://semopenalex.org/work/W4239396382', 'https://semopenalex.org/work/W4399763801', 'https://semopenalex.org/work/W2409578015', 'https://semopenalex.org/work/W1860259465', 'https://semopenalex.org/work/W4200616097', 'https://semopenalex.org/work/W4307204790', 'https://semopenalex.org/work/W2092202628', 'https://semopenalex.org/work/W3112090964', 'https://semopenalex.org/work/W3110591323', 'https://semopenalex.org/work/W2518694405', 'https://semopenalex.org/work/W2972759039', 'https://semopenalex.org/work/W2054886944', 'https://semopenalex.org/work/W3028790862', 'https://semopenalex.org/work/W1985142918', 'https://semopenalex.org/work/W2903417746', 'https://semopenalex.org/work/W2929751249', 'https://semopenalex.org/work/W2177601947', 'https://semopenalex.org/work/W3165155612', 'https://semopenalex.org/work/W4315777028', 'https://semopenalex.org/work/W2037697732', 'https://semopenalex.org/work/W2294561329', 'https://semopenalex.org/work/W1568803211', 'https://semopenalex.org/work/W2977597077', 'https://semopenalex.org/work/W2725971658', 'https://semopenalex.org/work/W2921194733', 'https://semopenalex.org/work/W4361189030', 'https://semopenalex.org/work/W2293208404', 'https://semopenalex.org/work/W2576215493', 'https://semopenalex.org/work/W1751138515', 'https://semopenalex.org/work/W3203088685', 'https://semopenalex.org/work/W2068367136', 'https://semopenalex.org/work/W2978422619', 'https://semopenalex.org/work/W2975736083', 'https://semopenalex.org/work/W4214593503', 'https://semopenalex.org/work/W2895512277', 'https://semopenalex.org/work/W2968884122', 'https://semopenalex.org/work/W1771936601', 'https://semopenalex.org/work/W2017727997', 'https://semopenalex.org/work/W4319452484', 'https://semopenalex.org/work/W4404373433', 'https://semopenalex.org/work/W3143959337', 'https://semopenalex.org/work/W2909558410', 'https://semopenalex.org/work/W4292261957', 'https://semopenalex.org/work/W3161202338', 'https://semopenalex.org/work/W3163078982', 'https://semopenalex.org/work/W2977911811', 'https://semopenalex.org/work/W1965526182', 'https://semopenalex.org/work/W3130372017', 'https://semopenalex.org/work/W3182364466', 'https://semopenalex.org/work/W2567779880', 'https://semopenalex.org/work/W2072490274', 'https://semopenalex.org/work/W2557881781', 'https://semopenalex.org/work/W2981708234', 'https://semopenalex.org/work/W2129488573', 'https://semopenalex.org/work/W4200525013', 'https://semopenalex.org/work/W3198359754', 'https://semopenalex.org/work/W2736312195', 'https://semopenalex.org/work/W2024357873', 'https://semopenalex.org/work/W2149683870', 'https://semopenalex.org/work/W4287729941', 'https://semopenalex.org/work/W3142764819', 'https://semopenalex.org/work/W2751429127', 'https://semopenalex.org/work/W2755506150', 'https://semopenalex.org/work/W2791540051', 'https://semopenalex.org/work/W2519558346', 'https://semopenalex.org/work/W3184531492', 'https://semopenalex.org/work/W2067004171', 'https://semopenalex.org/work/W2768260654', 'https://semopenalex.org/work/W2795503716', 'https://semopenalex.org/work/W2156243282', 'https://semopenalex.org/work/W2976524236', 'https://semopenalex.org/work/W4401406766', 'https://semopenalex.org/work/W3096988350', 'https://semopenalex.org/work/W4283397308', 'https://semopenalex.org/work/W2973046614', 'https://semopenalex.org/work/W2344158693', 'https://semopenalex.org/work/W3162832522', 'https://semopenalex.org/work/W1993984611', 'https://semopenalex.org/work/W2520077052', 'https://semopenalex.org/work/W2520352456', 'https://semopenalex.org/work/W3029899401', 'https://semopenalex.org/work/W3033480106', 'https://semopenalex.org/work/W4245844025', 'https://semopenalex.org/work/W1484203263', 'https://semopenalex.org/work/W2899470128', 'https://semopenalex.org/work/W2019487042', 'https://semopenalex.org/work/W3033839905', 'https://semopenalex.org/work/W1710215999', 'https://semopenalex.org/work/W4386163788', 'https://semopenalex.org/work/W1246643588', 'https://semopenalex.org/work/W2519730427', 'https://semopenalex.org/work/W2273076933', 'https://semopenalex.org/work/W3095740806', 'https://semopenalex.org/work/W2346027641', 'https://semopenalex.org/work/W2902563098', 'https://semopenalex.org/work/W2288812598', 'https://semopenalex.org/work/W2256119246', 'https://semopenalex.org/work/W2513683703', 'https://semopenalex.org/work/W3163921267', 'https://semopenalex.org/work/W2169202944', 'https://semopenalex.org/work/W3177151358', 'https://semopenalex.org/work/W3037695612', 'https://semopenalex.org/work/W4366583171', 'https://semopenalex.org/work/W2318574332', 'https://semopenalex.org/work/W2972702127', 'https://semopenalex.org/work/W2033617925', 'https://semopenalex.org/work/W3121775658', 'https://semopenalex.org/work/W2082538501', 'https://semopenalex.org/work/W4225088745', 'https://semopenalex.org/work/W2119929248', 'https://semopenalex.org/work/W1982984133', 'https://semopenalex.org/work/W3188420011', 'https://semopenalex.org/work/W4241289669', 'https://semopenalex.org/work/W4366597679', 'https://semopenalex.org/work/W2921533080', 'https://semopenalex.org/work/W3160545975', 'https://semopenalex.org/work/W4404873047', 'https://semopenalex.org/work/W4393067390', 'https://semopenalex.org/work/W3112877194', 'https://semopenalex.org/work/W3161974712', 'https://semopenalex.org/work/W3206366132', 'https://semopenalex.org/work/W4241528240', 'https://semopenalex.org/work/W2898820983', 'https://semopenalex.org/work/W3030149602', 'https://semopenalex.org/work/W3196772354', 'https://semopenalex.org/work/W2410138785', 'https://semopenalex.org/work/W4392429145', 'https://semopenalex.org/work/W3194688439', 'https://semopenalex.org/work/W2795581336', 'https://semopenalex.org/work/W3005470382', 'https://semopenalex.org/work/W2187647369', 'https://semopenalex.org/work/W4389891943', 'https://semopenalex.org/work/W4230032809', 'https://semopenalex.org/work/W3200245219', 'https://semopenalex.org/work/W4366547357', 'https://semopenalex.org/work/W2079488626', 'https://semopenalex.org/work/W2294361658', 'https://semopenalex.org/work/W4312572845', 'https://semopenalex.org/work/W2060118520', 'https://semopenalex.org/work/W3090583924', 'https://semopenalex.org/work/W4393752214', 'https://semopenalex.org/work/W2063007215', 'https://semopenalex.org/work/W2978827769', 'https://semopenalex.org/work/W2972419497', 'https://semopenalex.org/work/W1522158218', 'https://semopenalex.org/work/W2080327955', 'https://semopenalex.org/work/W4220905243', 'https://semopenalex.org/work/W4312282153', 'https://semopenalex.org/work/W4242142265', 'https://semopenalex.org/work/W3031395001', 'https://semopenalex.org/work/W3163327897', 'https://semopenalex.org/work/W3095347735', 'https://semopenalex.org/work/W2752561456', 'https://semopenalex.org/work/W4224279084']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2109186457', 'https://semopenalex.org/work/W2290200834', 'https://semopenalex.org/work/W2024336304', 'https://semopenalex.org/work/W1908879184', 'https://semopenalex.org/work/W2146002591', 'https://semopenalex.org/work/W2074193071', 'https://semopenalex.org/work/W325059703', 'https://semopenalex.org/work/W2407231546', 'https://semopenalex.org/work/W3157283285', 'https://semopenalex.org/work/W2140805995', 'https://semopenalex.org/work/W2953533689', 'https://semopenalex.org/work/W4401808601', 'https://semopenalex.org/work/W328613600', 'https://semopenalex.org/work/W2809782991', 'https://semopenalex.org/work/W2883856658', 'https://semopenalex.org/work/W2170741870', 'https://semopenalex.org/work/W2730743430', 'https://semopenalex.org/work/W2615205062', 'https://semopenalex.org/work/W3042004637', 'https://semopenalex.org/work/W2103224970', 'https://semopenalex.org/work/W3187351556', 'https://semopenalex.org/work/W2139436497', 'https://semopenalex.org/work/W2064672353', 'https://semopenalex.org/work/W2571158126', 'https://semopenalex.org/work/W2473052796', 'https://semopenalex.org/work/W4387005904', 'https://semopenalex.org/work/W2157519619', 'https://semopenalex.org/work/W49790452', 'https://semopenalex.org/work/W4390187585', 'https://semopenalex.org/work/W1526915766', 'https://semopenalex.org/work/W2146520711', 'https://semopenalex.org/work/W2070269076', 'https://semopenalex.org/work/W1587236616', 'https://semopenalex.org/work/W979651393', 'https://semopenalex.org/work/W4391156256', 'https://semopenalex.org/work/W3206895939', 'https://semopenalex.org/work/W4392713273', 'https://semopenalex.org/work/W2941373095', 'https://semopenalex.org/work/W2405266982', 'https://semopenalex.org/work/W4401578804', 'https://semopenalex.org/work/W2804376295', 'https://semopenalex.org/work/W2110574373', 'https://semopenalex.org/work/W857122145', 'https://semopenalex.org/work/W2886396839', 'https://semopenalex.org/work/W1979988378', 'https://semopenalex.org/work/W149383384', 'https://semopenalex.org/work/W2542642724', 'https://semopenalex.org/work/W4205619442', 'https://semopenalex.org/work/W2138291705', 'https://semopenalex.org/work/W4400946621', 'https://semopenalex.org/work/W4405935629', 'https://semopenalex.org/work/W12268595', 'https://semopenalex.org/work/W2608491785', 'https://semopenalex.org/work/W4392942581', 'https://semopenalex.org/work/W2884188352', 'https://semopenalex.org/work/W2023972619', 'https://semopenalex.org/work/W2072209700', 'https://semopenalex.org/work/W2204033782', 'https://semopenalex.org/work/W2484374542', 'https://semopenalex.org/work/W2042756792', 'https://semopenalex.org/work/W2768649200', 'https://semopenalex.org/work/W2074068839', 'https://semopenalex.org/work/W1992495634', 'https://semopenalex.org/work/W2530140145', 'https://semopenalex.org/work/W2098016930', 'https://semopenalex.org/work/W2089241417', 'https://semopenalex.org/work/W1518248903', 'https://semopenalex.org/work/W1999508547', 'https://semopenalex.org/work/W2170201418', 'https://semopenalex.org/work/W2064476539', 'https://semopenalex.org/work/W3089291192', 'https://semopenalex.org/work/W1991853935', 'https://semopenalex.org/work/W2340283416', 'https://semopenalex.org/work/W2062957328', 'https://semopenalex.org/work/W4401943800', 'https://semopenalex.org/work/W4390188024', 'https://semopenalex.org/work/W4206807237', 'https://semopenalex.org/work/W4389921335', 'https://semopenalex.org/work/W2967954143', 'https://semopenalex.org/work/W2088723639', 'https://semopenalex.org/work/W52623672', 'https://semopenalex.org/work/W2341007259', 'https://semopenalex.org/work/W2106211998', 'https://semopenalex.org/work/W2163881253', 'https://semopenalex.org/work/W2536107053', 'https://semopenalex.org/work/W1993325111', 'https://semopenalex.org/work/W2166211129', 'https://semopenalex.org/work/W3027319226', 'https://semopenalex.org/work/W2293459815', 'https://semopenalex.org/work/W2412127048', 'https://semopenalex.org/work/W1910867531', 'https://semopenalex.org/work/W2062904953', 'https://semopenalex.org/work/W2139255754', 'https://semopenalex.org/work/W2903177638', 'https://semopenalex.org/work/W2579158977', 'https://semopenalex.org/work/W4401579183', 'https://semopenalex.org/work/W1973125618', 'https://semopenalex.org/work/W2188362632', 'https://semopenalex.org/work/W2144918660', 'https://semopenalex.org/work/W2895854254', 'https://semopenalex.org/work/W1508821613', 'https://semopenalex.org/work/W2034050419', 'https://semopenalex.org/work/W2560712448', 'https://semopenalex.org/work/W2516286998', 'https://semopenalex.org/work/W2401333290', 'https://semopenalex.org/work/W214032606', 'https://semopenalex.org/work/W2981465620', 'https://semopenalex.org/work/W2240362173', 'https://semopenalex.org/work/W2122571865', 'https://semopenalex.org/work/W2072553352', 'https://semopenalex.org/work/W2171606781', 'https://semopenalex.org/work/W2043269074', 'https://semopenalex.org/work/W2748533023', 'https://semopenalex.org/work/W2166520679', 'https://semopenalex.org/work/W2162338867', 'https://semopenalex.org/work/W2068524892', 'https://semopenalex.org/work/W2761828172', 'https://semopenalex.org/work/W2907364096', 'https://semopenalex.org/work/W1531223514', 'https://semopenalex.org/work/W2001905011', 'https://semopenalex.org/work/W4296365397', 'https://semopenalex.org/work/W2032099346', 'https://semopenalex.org/work/W2148646851', 'https://semopenalex.org/work/W2768928198', 'https://semopenalex.org/work/W2163180953', 'https://semopenalex.org/work/W1999134690', 'https://semopenalex.org/work/W4206307909', 'https://semopenalex.org/work/W1922706319', 'https://semopenalex.org/work/W1995950498', 'https://semopenalex.org/work/W4231226382', 'https://semopenalex.org/work/W2401381263', 'https://semopenalex.org/work/W1982314073', 'https://semopenalex.org/work/W2945691872', 'https://semopenalex.org/work/W2967876484', 'https://semopenalex.org/work/W2954164432', 'https://semopenalex.org/work/W1967568969', 'https://semopenalex.org/work/W2044900380', 'https://semopenalex.org/work/W3136727059', 'https://semopenalex.org/work/W2188799909', 'https://semopenalex.org/work/W2945300184', 'https://semopenalex.org/work/W2612282432', 'https://semopenalex.org/work/W102421301', 'https://semopenalex.org/work/W2747040169', 'https://semopenalex.org/work/W2742916377', 'https://semopenalex.org/work/W2155718231', 'https://semopenalex.org/work/W2805153701', 'https://semopenalex.org/work/W4327767801', 'https://semopenalex.org/work/W2159139699', 'https://semopenalex.org/work/W4285815179', 'https://semopenalex.org/work/W2124870235', 'https://semopenalex.org/work/W2019708772', 'https://semopenalex.org/work/W2073709132', 'https://semopenalex.org/work/W4321614042', 'https://semopenalex.org/work/W4367360032', 'https://semopenalex.org/work/W4404030068', 'https://semopenalex.org/work/W2884636426', 'https://semopenalex.org/work/W1584206897', 'https://semopenalex.org/work/W2901316497', 'https://semopenalex.org/work/W2052982204', 'https://semopenalex.org/work/W2289584941', 'https://semopenalex.org/work/W2786601708', 'https://semopenalex.org/work/W2515896452', 'https://semopenalex.org/work/W4255531846', 'https://semopenalex.org/work/W2275014257', 'https://semopenalex.org/work/W4365802790', 'https://semopenalex.org/work/W4285172618', 'https://semopenalex.org/work/W2203509984', 'https://semopenalex.org/work/W1544524730', 'https://semopenalex.org/work/W3162144158', 'https://semopenalex.org/work/W4253850266', 'https://semopenalex.org/work/W2293958373', 'https://semopenalex.org/work/W139668830', 'https://semopenalex.org/work/W2998201073', 'https://semopenalex.org/work/W2120216356', 'https://semopenalex.org/work/W1422159917', 'https://semopenalex.org/work/W4405094102', 'https://semopenalex.org/work/W2139454561', 'https://semopenalex.org/work/W2091944075', 'https://semopenalex.org/work/W2142484380', 'https://semopenalex.org/work/W2130803541', 'https://semopenalex.org/work/W2056096508', 'https://semopenalex.org/work/W4240672112', 'https://semopenalex.org/work/W3096110661', 'https://semopenalex.org/work/W1823956242', 'https://semopenalex.org/work/W2964982644', 'https://semopenalex.org/work/W2165818457', 'https://semopenalex.org/work/W4210325270', 'https://semopenalex.org/work/W2063650982', 'https://semopenalex.org/work/W2162066092', 'https://semopenalex.org/work/W2112107898', 'https://semopenalex.org/work/W4387450689', 'https://semopenalex.org/work/W2145747218', 'https://semopenalex.org/work/W2024612964', 'https://semopenalex.org/work/W4390512166', 'https://semopenalex.org/work/W1990193612', 'https://semopenalex.org/work/W2896727063', 'https://semopenalex.org/work/W2413863213', 'https://semopenalex.org/work/W2210223524', 'https://semopenalex.org/work/W2754948093', 'https://semopenalex.org/work/W2756387886', 'https://semopenalex.org/work/W4206683427', 'https://semopenalex.org/work/W2024786226', 'https://semopenalex.org/work/W2138320177', 'https://semopenalex.org/work/W1870822388', 'https://semopenalex.org/work/W2104408001', 'https://semopenalex.org/work/W2055278155', 'https://semopenalex.org/work/W1497865469', 'https://semopenalex.org/work/W4250489070', 'https://semopenalex.org/work/W2111759980', 'https://semopenalex.org/work/W4285216643', 'https://semopenalex.org/work/W4404030648', 'https://semopenalex.org/work/W2288534976', 'https://semopenalex.org/work/W2077737077', 'https://semopenalex.org/work/W2625986270', 'https://semopenalex.org/work/W2004738891', 'https://semopenalex.org/work/W4237620799', 'https://semopenalex.org/work/W3211349420', 'https://semopenalex.org/work/W2069369796', 'https://semopenalex.org/work/W2935942569', 'https://semopenalex.org/work/W4366964206', 'https://semopenalex.org/work/W2398987072', 'https://semopenalex.org/work/W158943908', 'https://semopenalex.org/work/W3132353162', 'https://semopenalex.org/work/W2135598717', 'https://semopenalex.org/work/W4285503152', 'https://semopenalex.org/work/W1633573314', 'https://semopenalex.org/work/W2031625065', 'https://semopenalex.org/work/W2134444560', 'https://semopenalex.org/work/W4205613083', 'https://semopenalex.org/work/W2482354811', 'https://semopenalex.org/work/W2146033518', 'https://semopenalex.org/work/W1544888628', 'https://semopenalex.org/work/W2130832779', 'https://semopenalex.org/work/W1501172792', 'https://semopenalex.org/work/W1986827696', 'https://semopenalex.org/work/W2028566173', 'https://semopenalex.org/work/W4253131601', 'https://semopenalex.org/work/W2039163755', 'https://semopenalex.org/work/W2096075530', 'https://semopenalex.org/work/W2557110996', 'https://semopenalex.org/work/W2586727473', 'https://semopenalex.org/work/W4238734812', 'https://semopenalex.org/work/W2888177496', 'https://semopenalex.org/work/W2112535726', 'https://semopenalex.org/work/W2356144191', 'https://semopenalex.org/work/W2029818237', 'https://semopenalex.org/work/W2903545243', 'https://semopenalex.org/work/W2079895649', 'https://semopenalex.org/work/W2024012113', 'https://semopenalex.org/work/W2786772278', 'https://semopenalex.org/work/W3085760006', 'https://semopenalex.org/work/W51211239', 'https://semopenalex.org/work/W2295164153', 'https://semopenalex.org/work/W2041334917', 'https://semopenalex.org/work/W143942840', 'https://semopenalex.org/work/W2803258972', 'https://semopenalex.org/work/W1965382252', 'https://semopenalex.org/work/W2160391119', 'https://semopenalex.org/work/W4392577068', 'https://semopenalex.org/work/W2992245431', 'https://semopenalex.org/work/W2538630038', 'https://semopenalex.org/work/W4249963731', 'https://semopenalex.org/work/W1969657871', 'https://semopenalex.org/work/W2923039095', 'https://semopenalex.org/work/W1661735121', 'https://semopenalex.org/work/W2165377954', 'https://semopenalex.org/work/W2111277352', 'https://semopenalex.org/work/W2109705305', 'https://semopenalex.org/work/W196228518', 'https://semopenalex.org/work/W2600068329', 'https://semopenalex.org/work/W4252981000', 'https://semopenalex.org/work/W2062243122', 'https://semopenalex.org/work/W2092005371', 'https://semopenalex.org/work/W1574380960', 'https://semopenalex.org/work/W3211844447', 'https://semopenalex.org/work/W2161966477', 'https://semopenalex.org/work/W2532152395', 'https://semopenalex.org/work/W25440647', 'https://semopenalex.org/work/W2743920271', 'https://semopenalex.org/work/W2145701421', 'https://semopenalex.org/work/W2108304242', 'https://semopenalex.org/work/W4230332361', 'https://semopenalex.org/work/W41465441', 'https://semopenalex.org/work/W2961776981', 'https://semopenalex.org/work/W4312778763', 'https://semopenalex.org/work/W1990091852', 'https://semopenalex.org/work/W2625256202', 'https://semopenalex.org/work/W2794572176', 'https://semopenalex.org/work/W2550667658', 'https://semopenalex.org/work/W2611767226', 'https://semopenalex.org/work/W4237745095', 'https://semopenalex.org/work/W2113043545', 'https://semopenalex.org/work/W2271801361', 'https://semopenalex.org/work/W4385626270', 'https://semopenalex.org/work/W4229053674', 'https://semopenalex.org/work/W2480965638', 'https://semopenalex.org/work/W2528842892', 'https://semopenalex.org/work/W4289655844', 'https://semopenalex.org/work/W3097508557', 'https://semopenalex.org/work/W2495352272', 'https://semopenalex.org/work/W3096330417', 'https://semopenalex.org/work/W4205212276', 'https://semopenalex.org/work/W2917706508', 'https://semopenalex.org/work/W2138922641', 'https://semopenalex.org/work/W2154510046', 'https://semopenalex.org/work/W2078326945', 'https://semopenalex.org/work/W2769445687', 'https://semopenalex.org/work/W2138433001', 'https://semopenalex.org/work/W2184299809', 'https://semopenalex.org/work/W4389321773', 'https://semopenalex.org/work/W2496554705', 'https://semopenalex.org/work/W2115899637', 'https://semopenalex.org/work/W2550712691', 'https://semopenalex.org/work/W1520936229', 'https://semopenalex.org/work/W1497099843', 'https://semopenalex.org/work/W3130320973', 'https://semopenalex.org/work/W2596027452', 'https://semopenalex.org/work/W2124560301', 'https://semopenalex.org/work/W4247476769', 'https://semopenalex.org/work/W2749110496', 'https://semopenalex.org/work/W3041653159', 'https://semopenalex.org/work/W4253265224', 'https://semopenalex.org/work/W2165300716', 'https://semopenalex.org/work/W2149899452', 'https://semopenalex.org/work/W1494063694', 'https://semopenalex.org/work/W1967157693', 'https://semopenalex.org/work/W3157167113', 'https://semopenalex.org/work/W2033725854', 'https://semopenalex.org/work/W2230115501', 'https://semopenalex.org/work/W2475285031', 'https://semopenalex.org/work/W2108876125', 'https://semopenalex.org/work/W2095834672', 'https://semopenalex.org/work/W4253855517', 'https://semopenalex.org/work/W2150998397', 'https://semopenalex.org/work/W3107887875', 'https://semopenalex.org/work/W2011410844', 'https://semopenalex.org/work/W4210708907', 'https://semopenalex.org/work/W2061231005', 'https://semopenalex.org/work/W2144253537', 'https://semopenalex.org/work/W2068973986', 'https://semopenalex.org/work/W2128563460', 'https://semopenalex.org/work/W67894965', 'https://semopenalex.org/work/W2080996134', 'https://semopenalex.org/work/W2116314971', 'https://semopenalex.org/work/W2028754220', 'https://semopenalex.org/work/W2903213374', 'https://semopenalex.org/work/W2125308824', 'https://semopenalex.org/work/W1608886591', 'https://semopenalex.org/work/W2527344267', 'https://semopenalex.org/work/W2002312562', 'https://semopenalex.org/work/W2751662694', 'https://semopenalex.org/work/W2666172191', 'https://semopenalex.org/work/W2929921254', 'https://semopenalex.org/work/W2293958210', 'https://semopenalex.org/work/W2413288731', 'https://semopenalex.org/work/W4252093019', 'https://semopenalex.org/work/W2785105341', 'https://semopenalex.org/work/W3095279071', 'https://semopenalex.org/work/W2947626283', 'https://semopenalex.org/work/W2132364404', 'https://semopenalex.org/work/W2072776346', 'https://semopenalex.org/work/W2124054384', 'https://semopenalex.org/work/W2945412056', 'https://semopenalex.org/work/W4316659889', 'https://semopenalex.org/work/W2496567738', 'https://semopenalex.org/work/W2624802634', 'https://semopenalex.org/work/W2171510346', 'https://semopenalex.org/work/W2965366155', 'https://semopenalex.org/work/W2134768851', 'https://semopenalex.org/work/W1538415416', 'https://semopenalex.org/work/W2411894725', 'https://semopenalex.org/work/W2490092534', 'https://semopenalex.org/work/W1973148750', 'https://semopenalex.org/work/W2288294525', 'https://semopenalex.org/work/W2092477317', 'https://semopenalex.org/work/W4285408205', 'https://semopenalex.org/work/W2015849174', 'https://semopenalex.org/work/W2036165062', 'https://semopenalex.org/work/W2494421230', 'https://semopenalex.org/work/W3023797106', 'https://semopenalex.org/work/W1489534528', 'https://semopenalex.org/work/W652412083', 'https://semopenalex.org/work/W1494162500', 'https://semopenalex.org/work/W1569686365', 'https://semopenalex.org/work/W3206640136', 'https://semopenalex.org/work/W565256208', 'https://semopenalex.org/work/W2512795596', 'https://semopenalex.org/work/W4394742902', 'https://semopenalex.org/work/W2125143433', 'https://semopenalex.org/work/W2012912450', 'https://semopenalex.org/work/W1974886156', 'https://semopenalex.org/work/W2044431283', 'https://semopenalex.org/work/W1979289740', 'https://semopenalex.org/work/W2569889271', 'https://semopenalex.org/work/W1999149743', 'https://semopenalex.org/work/W4286571613', 'https://semopenalex.org/work/W4396894716', 'https://semopenalex.org/work/W2202036745', 'https://semopenalex.org/work/W1985701940', 'https://semopenalex.org/work/W1978851795', 'https://semopenalex.org/work/W1995308547', 'https://semopenalex.org/work/W2111424373', 'https://semopenalex.org/work/W2120355631', 'https://semopenalex.org/work/W2291113318', 'https://semopenalex.org/work/W4233681091', 'https://semopenalex.org/work/W2098948701', 'https://semopenalex.org/work/W3017143302', 'https://semopenalex.org/work/W1791684062', 'https://semopenalex.org/work/W2124703480', 'https://semopenalex.org/work/W160837981', 'https://semopenalex.org/work/W2397834607', 'https://semopenalex.org/work/W3206850855', 'https://semopenalex.org/work/W2150298155', 'https://semopenalex.org/work/W3092453362', 'https://semopenalex.org/work/W4376630019', 'https://semopenalex.org/work/W2111964097', 'https://semopenalex.org/work/W2108162045', 'https://semopenalex.org/work/W2219017076', 'https://semopenalex.org/work/W2084854878', 'https://semopenalex.org/work/W3016161880', 'https://semopenalex.org/work/W2102190590', 'https://semopenalex.org/work/W4400946519', 'https://semopenalex.org/work/W2478910470', 'https://semopenalex.org/work/W2485878525', 'https://semopenalex.org/work/W2606501011', 'https://semopenalex.org/work/W2554047600', 'https://semopenalex.org/work/W1517253300', 'https://semopenalex.org/work/W3200674364', 'https://semopenalex.org/work/W3129067525', 'https://semopenalex.org/work/W2132053703', 'https://semopenalex.org/work/W2497743975', 'https://semopenalex.org/work/W1992253076', 'https://semopenalex.org/work/W2501830935', 'https://semopenalex.org/work/W2289149676', 'https://semopenalex.org/work/W2246286794', 'https://semopenalex.org/work/W2166217821', 'https://semopenalex.org/work/W2077200079', 'https://semopenalex.org/work/W2144750318', 'https://semopenalex.org/work/W2129869483', 'https://semopenalex.org/work/W2034507787', 'https://semopenalex.org/work/W126878419', 'https://semopenalex.org/work/W4396665589', 'https://semopenalex.org/work/W1840794446', 'https://semopenalex.org/work/W4401021691', 'https://semopenalex.org/work/W2159662334', 'https://semopenalex.org/work/W1990019789', 'https://semopenalex.org/work/W3021203574', 'https://semopenalex.org/work/W3095131015', 'https://semopenalex.org/work/W146617261', 'https://semopenalex.org/work/W159035867', 'https://semopenalex.org/work/W2157188908', 'https://semopenalex.org/work/W2147895050', 'https://semopenalex.org/work/W2077174735', 'https://semopenalex.org/work/W4252463735', 'https://semopenalex.org/work/W6907768', 'https://semopenalex.org/work/W858120236', 'https://semopenalex.org/work/W1577463177', 'https://semopenalex.org/work/W2108240852', 'https://semopenalex.org/work/W4244005678', 'https://semopenalex.org/work/W4294672395', 'https://semopenalex.org/work/W2094708864', 'https://semopenalex.org/work/W2079466034', 'https://semopenalex.org/work/W2170913025', 'https://semopenalex.org/work/W2166826477', 'https://semopenalex.org/work/W2484645626', 'https://semopenalex.org/work/W2789144447', 'https://semopenalex.org/work/W4306173842', 'https://semopenalex.org/work/W2127414738', 'https://semopenalex.org/work/W1874259713', 'https://semopenalex.org/work/W2401583884', 'https://semopenalex.org/work/W2150650760', 'https://semopenalex.org/work/W1419972110', 'https://semopenalex.org/work/W2025546942', 'https://semopenalex.org/work/W402024038', 'https://semopenalex.org/work/W4402830551', 'https://semopenalex.org/work/W2085435476', 'https://semopenalex.org/work/W2800308132', 'https://semopenalex.org/work/W2075578427', 'https://semopenalex.org/work/W2112979372', 'https://semopenalex.org/work/W2095968352', 'https://semopenalex.org/work/W2136654140', 'https://semopenalex.org/work/W2212338561', 'https://semopenalex.org/work/W2612784784', 'https://semopenalex.org/work/W1506027738', 'https://semopenalex.org/work/W2804891820', 'https://semopenalex.org/work/W2076330335', 'https://semopenalex.org/work/W1448329507', 'https://semopenalex.org/work/W1857000584', 'https://semopenalex.org/work/W2950468099', 'https://semopenalex.org/work/W1999631843', 'https://semopenalex.org/work/W49611838', 'https://semopenalex.org/work/W3175708501', 'https://semopenalex.org/work/W2181791275', 'https://semopenalex.org/work/W1967677932', 'https://semopenalex.org/work/W2161454411', 'https://semopenalex.org/work/W2123532445', 'https://semopenalex.org/work/W2627083872', 'https://semopenalex.org/work/W2060283246', 'https://semopenalex.org/work/W3013997466', 'https://semopenalex.org/work/W1971283588', 'https://semopenalex.org/work/W2163138922', 'https://semopenalex.org/work/W1481133633', 'https://semopenalex.org/work/W2070215238', 'https://semopenalex.org/work/W2133522196', 'https://semopenalex.org/work/W2167521347', 'https://semopenalex.org/work/W2029131637', 'https://semopenalex.org/work/W2902487276', 'https://semopenalex.org/work/W3160200186', 'https://semopenalex.org/work/W2080817506', 'https://semopenalex.org/work/W1860740456', 'https://semopenalex.org/work/W1998201483', 'https://semopenalex.org/work/W2883395494', 'https://semopenalex.org/work/W2147456231', 'https://semopenalex.org/work/W2576879514', 'https://semopenalex.org/work/W2786657846', 'https://semopenalex.org/work/W2895967513', 'https://semopenalex.org/work/W4386814402', 'https://semopenalex.org/work/W3004301528', 'https://semopenalex.org/work/W2755469263', 'https://semopenalex.org/work/W1560982985', 'https://semopenalex.org/work/W4392188385', 'https://semopenalex.org/work/W2906163189', 'https://semopenalex.org/work/W2101787599', 'https://semopenalex.org/work/W48804293', 'https://semopenalex.org/work/W33403252', 'https://semopenalex.org/work/W2983014989', 'https://semopenalex.org/work/W4240245530', 'https://semopenalex.org/work/W2789263069', 'https://semopenalex.org/work/W1488510230', 'https://semopenalex.org/work/W2982452767', 'https://semopenalex.org/work/W4294672356', 'https://semopenalex.org/work/W2147139299', 'https://semopenalex.org/work/W2754307650', 'https://semopenalex.org/work/W2293095660', 'https://semopenalex.org/work/W4393146711', 'https://semopenalex.org/work/W2145502705', 'https://semopenalex.org/work/W2066111880', 'https://semopenalex.org/work/W2910014621', 'https://semopenalex.org/work/W2995911827', 'https://semopenalex.org/work/W2172143183', 'https://semopenalex.org/work/W1923826352', 'https://semopenalex.org/work/W3118215277', 'https://semopenalex.org/work/W72692433', 'https://semopenalex.org/work/W4400238477', 'https://semopenalex.org/work/W3179020455', 'https://semopenalex.org/work/W2014241426', 'https://semopenalex.org/work/W4367360059', 'https://semopenalex.org/work/W1943042767', 'https://semopenalex.org/work/W4249594017', 'https://semopenalex.org/work/W2890543403', 'https://semopenalex.org/work/W2137861763', 'https://semopenalex.org/work/W2058904901', 'https://semopenalex.org/work/W1994278842', 'https://semopenalex.org/work/W2610600517', 'https://semopenalex.org/work/W2085207404', 'https://semopenalex.org/work/W1969462495', 'https://semopenalex.org/work/W1969516436', 'https://semopenalex.org/work/W4405120549', 'https://semopenalex.org/work/W2885100636', 'https://semopenalex.org/work/W2079664409', 'https://semopenalex.org/work/W2161545800', 'https://semopenalex.org/work/W2290447772', 'https://semopenalex.org/work/W1933806665', 'https://semopenalex.org/work/W2513883066', 'https://semopenalex.org/work/W2903194584', 'https://semopenalex.org/work/W2496039851', 'https://semopenalex.org/work/W1608276691', 'https://semopenalex.org/work/W2027452379', 'https://semopenalex.org/work/W2968852933', 'https://semopenalex.org/work/W2119033694', 'https://semopenalex.org/work/W2510781223', 'https://semopenalex.org/work/W2532447822', 'https://semopenalex.org/work/W1549886897', 'https://semopenalex.org/work/W2895817859', 'https://semopenalex.org/work/W4376526615', 'https://semopenalex.org/work/W1514325539', 'https://semopenalex.org/work/W2058293659', 'https://semopenalex.org/work/W2755359845', 'https://semopenalex.org/work/W2044237546', 'https://semopenalex.org/work/W2016989291', 'https://semopenalex.org/work/W2130007135', 'https://semopenalex.org/work/W2620890574', 'https://semopenalex.org/work/W2158569759', 'https://semopenalex.org/work/W2966031361', 'https://semopenalex.org/work/W1492737188', 'https://semopenalex.org/work/W1991026653', 'https://semopenalex.org/work/W2156138095', 'https://semopenalex.org/work/W2786606238', 'https://semopenalex.org/work/W2559559327', 'https://semopenalex.org/work/W1573590416', 'https://semopenalex.org/work/W1654176175', 'https://semopenalex.org/work/W2024468903', 'https://semopenalex.org/work/W2968293641', 'https://semopenalex.org/work/W2055684776', 'https://semopenalex.org/work/W2744837872', 'https://semopenalex.org/work/W2035518282', 'https://semopenalex.org/work/W2142079724', 'https://semopenalex.org/work/W2065803961', 'https://semopenalex.org/work/W2034179412', 'https://semopenalex.org/work/W2475545374', 'https://semopenalex.org/work/W2107191431', 'https://semopenalex.org/work/W3196495759', 'https://semopenalex.org/work/W2153457047', 'https://semopenalex.org/work/W1516689139', 'https://semopenalex.org/work/W2081189334', 'https://semopenalex.org/work/W1986540981', 'https://semopenalex.org/work/W2948995623', 'https://semopenalex.org/work/W2106421914', 'https://semopenalex.org/work/W1516117757', 'https://semopenalex.org/work/W2041108261', 'https://semopenalex.org/work/W1177607589', 'https://semopenalex.org/work/W2564132746', 'https://semopenalex.org/work/W3017031701', 'https://semopenalex.org/work/W2401687993', 'https://semopenalex.org/work/W2131405606', 'https://semopenalex.org/work/W2161850606', 'https://semopenalex.org/work/W2334327213']</t>
+    <t>['https://semopenalex.org/work/W1769279530', 'https://semopenalex.org/work/W2059916190', 'https://semopenalex.org/work/W2397071937', 'https://semopenalex.org/work/W4315606555', 'https://semopenalex.org/work/W2491625832', 'https://semopenalex.org/work/W4287666146', 'https://semopenalex.org/work/W2230831981', 'https://semopenalex.org/work/W2950185045', 'https://semopenalex.org/work/W2162281264', 'https://semopenalex.org/work/W1995977330', 'https://semopenalex.org/work/W2151042992', 'https://semopenalex.org/work/W2039574235', 'https://semopenalex.org/work/W2572400646', 'https://semopenalex.org/work/W2784488119', 'https://semopenalex.org/work/W3180681495', 'https://semopenalex.org/work/W2158642611', 'https://semopenalex.org/work/W2111182668', 'https://semopenalex.org/work/W2162965487', 'https://semopenalex.org/work/W2605257447', 'https://semopenalex.org/work/W2013218112', 'https://semopenalex.org/work/W2169536566', 'https://semopenalex.org/work/W4287551966', 'https://semopenalex.org/work/W2169931542', 'https://semopenalex.org/work/W4390050192', 'https://semopenalex.org/work/W4301439726', 'https://semopenalex.org/work/W2241683853', 'https://semopenalex.org/work/W2902929870', 'https://semopenalex.org/work/W2017148819', 'https://semopenalex.org/work/W2077616584', 'https://semopenalex.org/work/W2134671262', 'https://semopenalex.org/work/W1602846904', 'https://semopenalex.org/work/W2072128484', 'https://semopenalex.org/work/W2138395721', 'https://semopenalex.org/work/W1773125178', 'https://semopenalex.org/work/W2119876849', 'https://semopenalex.org/work/W2085980614', 'https://semopenalex.org/work/W1694434332', 'https://semopenalex.org/work/W2112866668', 'https://semopenalex.org/work/W1987580879', 'https://semopenalex.org/work/W2020493940', 'https://semopenalex.org/work/W2114059901', 'https://semopenalex.org/work/W6747142', 'https://semopenalex.org/work/W2898704942', 'https://semopenalex.org/work/W2126535187', 'https://semopenalex.org/work/W266384355', 'https://semopenalex.org/work/W4386728307', 'https://semopenalex.org/work/W2003603103', 'https://semopenalex.org/work/W3127203349', 'https://semopenalex.org/work/W4386728259', 'https://semopenalex.org/work/W4281762710', 'https://semopenalex.org/work/W4310002000', 'https://semopenalex.org/work/W3112939012', 'https://semopenalex.org/work/W2188482746', 'https://semopenalex.org/work/W2164826027', 'https://semopenalex.org/work/W4301499895', 'https://semopenalex.org/work/W2806925689', 'https://semopenalex.org/work/W2115596980', 'https://semopenalex.org/work/W2151795643', 'https://semopenalex.org/work/W234261451', 'https://semopenalex.org/work/W2102152654', 'https://semopenalex.org/work/W2733144798', 'https://semopenalex.org/work/W2035640322', 'https://semopenalex.org/work/W4406195226', 'https://semopenalex.org/work/W1990472383', 'https://semopenalex.org/work/W1968153028', 'https://semopenalex.org/work/W1987772002', 'https://semopenalex.org/work/W2096933831', 'https://semopenalex.org/work/W3012587348', 'https://semopenalex.org/work/W3106512002', 'https://semopenalex.org/work/W4298871721', 'https://semopenalex.org/work/W2148131061', 'https://semopenalex.org/work/W2065628492', 'https://semopenalex.org/work/W2106233876', 'https://semopenalex.org/work/W2115811215', 'https://semopenalex.org/work/W2135180572', 'https://semopenalex.org/work/W2952571072', 'https://semopenalex.org/work/W1748985154', 'https://semopenalex.org/work/W2171286517', 'https://semopenalex.org/work/W2786494993', 'https://semopenalex.org/work/W2166862038', 'https://semopenalex.org/work/W2168665985', 'https://semopenalex.org/work/W2145983295', 'https://semopenalex.org/work/W2098408658', 'https://semopenalex.org/work/W1857284394', 'https://semopenalex.org/work/W4386728290', 'https://semopenalex.org/work/W2178506535', 'https://semopenalex.org/work/W4389078369', 'https://semopenalex.org/work/W2006798507', 'https://semopenalex.org/work/W2167193873', 'https://semopenalex.org/work/W2159784132', 'https://semopenalex.org/work/W2133585139', 'https://semopenalex.org/work/W2924551290', 'https://semopenalex.org/work/W2113689008', 'https://semopenalex.org/work/W2123717445', 'https://semopenalex.org/work/W1507181737', 'https://semopenalex.org/work/W2949908757', 'https://semopenalex.org/work/W4388638199', 'https://semopenalex.org/work/W2805042680', 'https://semopenalex.org/work/W3030025515', 'https://semopenalex.org/work/W4244875117', 'https://semopenalex.org/work/W1990902012', 'https://semopenalex.org/work/W2153006233', 'https://semopenalex.org/work/W2026055324', 'https://semopenalex.org/work/W2143779229', 'https://semopenalex.org/work/W2790500092', 'https://semopenalex.org/work/W2136849809', 'https://semopenalex.org/work/W2144570150', 'https://semopenalex.org/work/W2103254499', 'https://semopenalex.org/work/W2981712458', 'https://semopenalex.org/work/W4224933374', 'https://semopenalex.org/work/W2168111317', 'https://semopenalex.org/work/W1532372374', 'https://semopenalex.org/work/W2048467330', 'https://semopenalex.org/work/W1814798360', 'https://semopenalex.org/work/W2129361591', 'https://semopenalex.org/work/W1976452778', 'https://semopenalex.org/work/W2296243746', 'https://semopenalex.org/work/W4288095457', 'https://semopenalex.org/work/W2084295409', 'https://semopenalex.org/work/W4301512502', 'https://semopenalex.org/work/W2100814254', 'https://semopenalex.org/work/W3092177264', 'https://semopenalex.org/work/W2125427453', 'https://semopenalex.org/work/W3010742537', 'https://semopenalex.org/work/W1696074034', 'https://semopenalex.org/work/W4307786837', 'https://semopenalex.org/work/W1999197804', 'https://semopenalex.org/work/W4225288565', 'https://semopenalex.org/work/W2185221298', 'https://semopenalex.org/work/W2166500461', 'https://semopenalex.org/work/W3123138559', 'https://semopenalex.org/work/W1565749342', 'https://semopenalex.org/work/W2101310031', 'https://semopenalex.org/work/W2164044612', 'https://semopenalex.org/work/W2587913063', 'https://semopenalex.org/work/W2127735446', 'https://semopenalex.org/work/W1667912148', 'https://semopenalex.org/work/W4309830289', 'https://semopenalex.org/work/W1820714040', 'https://semopenalex.org/work/W2763756011', 'https://semopenalex.org/work/W2140267446', 'https://semopenalex.org/work/W2801854492', 'https://semopenalex.org/work/W2167460076', 'https://semopenalex.org/work/W2143780518', 'https://semopenalex.org/work/W1783191689', 'https://semopenalex.org/work/W2161268655', 'https://semopenalex.org/work/W4298016756', 'https://semopenalex.org/work/W4389138629', 'https://semopenalex.org/work/W2164511982', 'https://semopenalex.org/work/W2054656164', 'https://semopenalex.org/work/W2547849178', 'https://semopenalex.org/work/W2104091137', 'https://semopenalex.org/work/W2568027424', 'https://semopenalex.org/work/W2111934195', 'https://semopenalex.org/work/W3214000901', 'https://semopenalex.org/work/W2117083020', 'https://semopenalex.org/work/W1808004798', 'https://semopenalex.org/work/W1990606258', 'https://semopenalex.org/work/W4299390071', 'https://semopenalex.org/work/W1951572853', 'https://semopenalex.org/work/W3016021663', 'https://semopenalex.org/work/W2970497931', 'https://semopenalex.org/work/W3088481514', 'https://semopenalex.org/work/W4307934118', 'https://semopenalex.org/work/W1975448877', 'https://semopenalex.org/work/W2109988731', 'https://semopenalex.org/work/W2017830666', 'https://semopenalex.org/work/W4225966372', 'https://semopenalex.org/work/W2963927825', 'https://semopenalex.org/work/W2892075135', 'https://semopenalex.org/work/W2508911234', 'https://semopenalex.org/work/W2246111347', 'https://semopenalex.org/work/W4406807628', 'https://semopenalex.org/work/W4288374763', 'https://semopenalex.org/work/W2125523397', 'https://semopenalex.org/work/W2949618677', 'https://semopenalex.org/work/W989952323', 'https://semopenalex.org/work/W2124543240', 'https://semopenalex.org/work/W619554517', 'https://semopenalex.org/work/W3009810166', 'https://semopenalex.org/work/W1868782008', 'https://semopenalex.org/work/W2108057985', 'https://semopenalex.org/work/W2970592033', 'https://semopenalex.org/work/W4388829566', 'https://semopenalex.org/work/W949508384', 'https://semopenalex.org/work/W2003410902', 'https://semopenalex.org/work/W2032979218', 'https://semopenalex.org/work/W2151073381', 'https://semopenalex.org/work/W1946393290', 'https://semopenalex.org/work/W1967447459', 'https://semopenalex.org/work/W4297966944', 'https://semopenalex.org/work/W4298078907', 'https://semopenalex.org/work/W2030004233', 'https://semopenalex.org/work/W2557336675', 'https://semopenalex.org/work/W4299311104', 'https://semopenalex.org/work/W2477294189', 'https://semopenalex.org/work/W2137313509', 'https://semopenalex.org/work/W3199731519', 'https://semopenalex.org/work/W2982533818', 'https://semopenalex.org/work/W4402350832', 'https://semopenalex.org/work/W1989616605', 'https://semopenalex.org/work/W2118103599', 'https://semopenalex.org/work/W2591258888', 'https://semopenalex.org/work/W2131459843', 'https://semopenalex.org/work/W2396828855', 'https://semopenalex.org/work/W2316293614', 'https://semopenalex.org/work/W2101522113', 'https://semopenalex.org/work/W4248583122', 'https://semopenalex.org/work/W2974617835', 'https://semopenalex.org/work/W4390977353', 'https://semopenalex.org/work/W4300587259', 'https://semopenalex.org/work/W3196466252', 'https://semopenalex.org/work/W2101608590', 'https://semopenalex.org/work/W2481609999', 'https://semopenalex.org/work/W2150388917', 'https://semopenalex.org/work/W2117368578', 'https://semopenalex.org/work/W2891725356', 'https://semopenalex.org/work/W2213498014', 'https://semopenalex.org/work/W2027743940', 'https://semopenalex.org/work/W2089183963', 'https://semopenalex.org/work/W2146692894', 'https://semopenalex.org/work/W4287230780', 'https://semopenalex.org/work/W855221475', 'https://semopenalex.org/work/W3046488911', 'https://semopenalex.org/work/W4388118224', 'https://semopenalex.org/work/W2463302795', 'https://semopenalex.org/work/W4311488571', 'https://semopenalex.org/work/W2500472126', 'https://semopenalex.org/work/W2999073519', 'https://semopenalex.org/work/W2150258751', 'https://semopenalex.org/work/W2086931264', 'https://semopenalex.org/work/W2151961258', 'https://semopenalex.org/work/W2104561024', 'https://semopenalex.org/work/W3158448776', 'https://semopenalex.org/work/W4379653995', 'https://semopenalex.org/work/W4313525046', 'https://semopenalex.org/work/W2055834582', 'https://semopenalex.org/work/W2122883310', 'https://semopenalex.org/work/W2150591965', 'https://semopenalex.org/work/W2159063898', 'https://semopenalex.org/work/W2190195640', 'https://semopenalex.org/work/W1984186332', 'https://semopenalex.org/work/W1989282861', 'https://semopenalex.org/work/W2117070909', 'https://semopenalex.org/work/W2186730704', 'https://semopenalex.org/work/W3165143095', 'https://semopenalex.org/work/W2040835538', 'https://semopenalex.org/work/W2136275432', 'https://semopenalex.org/work/W1993524608', 'https://semopenalex.org/work/W3094576801', 'https://semopenalex.org/work/W4403900474', 'https://semopenalex.org/work/W2141798281', 'https://semopenalex.org/work/W2150180245', 'https://semopenalex.org/work/W218303851', 'https://semopenalex.org/work/W2063331068', 'https://semopenalex.org/work/W2162031088', 'https://semopenalex.org/work/W2119330876', 'https://semopenalex.org/work/W4381304944', 'https://semopenalex.org/work/W2060717066', 'https://semopenalex.org/work/W2143286465', 'https://semopenalex.org/work/W2903667675', 'https://semopenalex.org/work/W615388181', 'https://semopenalex.org/work/W4288088101', 'https://semopenalex.org/work/W3084462124', 'https://semopenalex.org/work/W3183518399', 'https://semopenalex.org/work/W1501647712', 'https://semopenalex.org/work/W4298025544', 'https://semopenalex.org/work/W2041032353', 'https://semopenalex.org/work/W4394868342', 'https://semopenalex.org/work/W2970012313', 'https://semopenalex.org/work/W2958049034', 'https://semopenalex.org/work/W3103773508', 'https://semopenalex.org/work/W2140684562', 'https://semopenalex.org/work/W2002799652', 'https://semopenalex.org/work/W2950348067', 'https://semopenalex.org/work/W2210029275', 'https://semopenalex.org/work/W3206047407', 'https://semopenalex.org/work/W1571761681', 'https://semopenalex.org/work/W2160014433', 'https://semopenalex.org/work/W1684154970', 'https://semopenalex.org/work/W4285201772', 'https://semopenalex.org/work/W1999564901', 'https://semopenalex.org/work/W4247814650', 'https://semopenalex.org/work/W2155686486', 'https://semopenalex.org/work/W1794193518', 'https://semopenalex.org/work/W2050921210', 'https://semopenalex.org/work/W2162575857', 'https://semopenalex.org/work/W2033157981', 'https://semopenalex.org/work/W3183317559', 'https://semopenalex.org/work/W2761162478', 'https://semopenalex.org/work/W2160492008', 'https://semopenalex.org/work/W3115993754', 'https://semopenalex.org/work/W2019064108', 'https://semopenalex.org/work/W4302382703', 'https://semopenalex.org/work/W2242734504', 'https://semopenalex.org/work/W2764441237', 'https://semopenalex.org/work/W609082053', 'https://semopenalex.org/work/W2147993784', 'https://semopenalex.org/work/W2099441560', 'https://semopenalex.org/work/W3085042870', 'https://semopenalex.org/work/W1965141814', 'https://semopenalex.org/work/W3190979825', 'https://semopenalex.org/work/W1825244231', 'https://semopenalex.org/work/W2130502393', 'https://semopenalex.org/work/W2158228464', 'https://semopenalex.org/work/W2023804683', 'https://semopenalex.org/work/W2001708147', 'https://semopenalex.org/work/W2131745743', 'https://semopenalex.org/work/W4405444483', 'https://semopenalex.org/work/W2701634507', 'https://semopenalex.org/work/W1747115033', 'https://semopenalex.org/work/W2975505367', 'https://semopenalex.org/work/W2249000025', 'https://semopenalex.org/work/W4243966075', 'https://semopenalex.org/work/W4253923565', 'https://semopenalex.org/work/W3200113339', 'https://semopenalex.org/work/W3134221682', 'https://semopenalex.org/work/W2152477879', 'https://semopenalex.org/work/W2117687155', 'https://semopenalex.org/work/W1971037148', 'https://semopenalex.org/work/W2972140606', 'https://semopenalex.org/work/W2007670367', 'https://semopenalex.org/work/W4386728181', 'https://semopenalex.org/work/W2934437784', 'https://semopenalex.org/work/W2541647902', 'https://semopenalex.org/work/W4289306231', 'https://semopenalex.org/work/W2033769372', 'https://semopenalex.org/work/W2441173492', 'https://semopenalex.org/work/W2156984667', 'https://semopenalex.org/work/W2136497745', 'https://semopenalex.org/work/W2039712435', 'https://semopenalex.org/work/W2145876651', 'https://semopenalex.org/work/W4304207591', 'https://semopenalex.org/work/W2126607152', 'https://semopenalex.org/work/W2096086749', 'https://semopenalex.org/work/W2785502402', 'https://semopenalex.org/work/W2064969586', 'https://semopenalex.org/work/W1965551074', 'https://semopenalex.org/work/W2287663230', 'https://semopenalex.org/work/W2100556278', 'https://semopenalex.org/work/W2097084589', 'https://semopenalex.org/work/W1624008340', 'https://semopenalex.org/work/W1764485696', 'https://semopenalex.org/work/W1982662510', 'https://semopenalex.org/work/W3026367662', 'https://semopenalex.org/work/W2114658777', 'https://semopenalex.org/work/W2170432288', 'https://semopenalex.org/work/W4298181338', 'https://semopenalex.org/work/W4226379915', 'https://semopenalex.org/work/W2130767560', 'https://semopenalex.org/work/W1976082632', 'https://semopenalex.org/work/W2166315125', 'https://semopenalex.org/work/W1984866494', 'https://semopenalex.org/work/W4388235556', 'https://semopenalex.org/work/W1764115161', 'https://semopenalex.org/work/W2150869369', 'https://semopenalex.org/work/W2945382159', 'https://semopenalex.org/work/W2891828336', 'https://semopenalex.org/work/W2050578629', 'https://semopenalex.org/work/W2950247931', 'https://semopenalex.org/work/W2028525469', 'https://semopenalex.org/work/W3161900557', 'https://semopenalex.org/work/W2003520411', 'https://semopenalex.org/work/W2908750658', 'https://semopenalex.org/work/W4226267095', 'https://semopenalex.org/work/W4401750498', 'https://semopenalex.org/work/W2152537098', 'https://semopenalex.org/work/W2327976118', 'https://semopenalex.org/work/W2170076025', 'https://semopenalex.org/work/W4206389288', 'https://semopenalex.org/work/W1985231173', 'https://semopenalex.org/work/W2223218801', 'https://semopenalex.org/work/W2115355054', 'https://semopenalex.org/work/W2035239234', 'https://semopenalex.org/work/W2185064755', 'https://semopenalex.org/work/W2057477395', 'https://semopenalex.org/work/W2119239701', 'https://semopenalex.org/work/W2953215316', 'https://semopenalex.org/work/W2162969215', 'https://semopenalex.org/work/W252315070', 'https://semopenalex.org/work/W2102168079', 'https://semopenalex.org/work/W1566503145', 'https://semopenalex.org/work/W2100527158', 'https://semopenalex.org/work/W4397026396', 'https://semopenalex.org/work/W3106431100', 'https://semopenalex.org/work/W3118410217', 'https://semopenalex.org/work/W4402699738', 'https://semopenalex.org/work/W2113674028', 'https://semopenalex.org/work/W4387430828', 'https://semopenalex.org/work/W2055673378', 'https://semopenalex.org/work/W4283028880', 'https://semopenalex.org/work/W2103637183', 'https://semopenalex.org/work/W4231953543', 'https://semopenalex.org/work/W2140316862', 'https://semopenalex.org/work/W2145332056', 'https://semopenalex.org/work/W4385652243', 'https://semopenalex.org/work/W1940162557', 'https://semopenalex.org/work/W2110745932', 'https://semopenalex.org/work/W2938524150', 'https://semopenalex.org/work/W4298174976', 'https://semopenalex.org/work/W2142195632', 'https://semopenalex.org/work/W4405562746', 'https://semopenalex.org/work/W2140333889', 'https://semopenalex.org/work/W1824121449', 'https://semopenalex.org/work/W4313478262', 'https://semopenalex.org/work/W1530322092', 'https://semopenalex.org/work/W4255556357', 'https://semopenalex.org/work/W2977723824', 'https://semopenalex.org/work/W2117626227', 'https://semopenalex.org/work/W2141592093', 'https://semopenalex.org/work/W2149962365', 'https://semopenalex.org/work/W2120952077', 'https://semopenalex.org/work/W3107843792', 'https://semopenalex.org/work/W1958624633', 'https://semopenalex.org/work/W1784288318', 'https://semopenalex.org/work/W2940395492', 'https://semopenalex.org/work/W605016662', 'https://semopenalex.org/work/W2111128642', 'https://semopenalex.org/work/W3106213621', 'https://semopenalex.org/work/W4404179957', 'https://semopenalex.org/work/W2121529688', 'https://semopenalex.org/work/W2992547694', 'https://semopenalex.org/work/W2021159593', 'https://semopenalex.org/work/W4312628239', 'https://semopenalex.org/work/W2027156706', 'https://semopenalex.org/work/W2014068777', 'https://semopenalex.org/work/W2152035989', 'https://semopenalex.org/work/W4294643449', 'https://semopenalex.org/work/W2065892151', 'https://semopenalex.org/work/W2129001064', 'https://semopenalex.org/work/W2955178723', 'https://semopenalex.org/work/W1970184235', 'https://semopenalex.org/work/W2998913556', 'https://semopenalex.org/work/W2042583427', 'https://semopenalex.org/work/W2045551387', 'https://semopenalex.org/work/W2075769341', 'https://semopenalex.org/work/W2147023251', 'https://semopenalex.org/work/W2066062210', 'https://semopenalex.org/work/W1976296868', 'https://semopenalex.org/work/W2963345994', 'https://semopenalex.org/work/W4386728284', 'https://semopenalex.org/work/W2130721121', 'https://semopenalex.org/work/W2127722806', 'https://semopenalex.org/work/W4401498566', 'https://semopenalex.org/work/W2148907823', 'https://semopenalex.org/work/W2106039030', 'https://semopenalex.org/work/W4386728368', 'https://semopenalex.org/work/W2109453625', 'https://semopenalex.org/work/W4388483721', 'https://semopenalex.org/work/W2106903616', 'https://semopenalex.org/work/W2133075431', 'https://semopenalex.org/work/W4322832362', 'https://semopenalex.org/work/W2133682680', 'https://semopenalex.org/work/W2124085076', 'https://semopenalex.org/work/W2963612078', 'https://semopenalex.org/work/W2131668274', 'https://semopenalex.org/work/W2119454020', 'https://semopenalex.org/work/W2103969908', 'https://semopenalex.org/work/W1864513555', 'https://semopenalex.org/work/W2106738903', 'https://semopenalex.org/work/W2165131653', 'https://semopenalex.org/work/W4393951149', 'https://semopenalex.org/work/W2143708007', 'https://semopenalex.org/work/W1971235196', 'https://semopenalex.org/work/W2159524123', 'https://semopenalex.org/work/W4304194230', 'https://semopenalex.org/work/W4322706631', 'https://semopenalex.org/work/W1996956434', 'https://semopenalex.org/work/W4292214108', 'https://semopenalex.org/work/W2148407475', 'https://semopenalex.org/work/W3098873033', 'https://semopenalex.org/work/W2123482670', 'https://semopenalex.org/work/W4377043292', 'https://semopenalex.org/work/W2088188946', 'https://semopenalex.org/work/W2101094458', 'https://semopenalex.org/work/W4386728227', 'https://semopenalex.org/work/W2399804733', 'https://semopenalex.org/work/W125371902', 'https://semopenalex.org/work/W2944254439', 'https://semopenalex.org/work/W3036970724', 'https://semopenalex.org/work/W2142780243', 'https://semopenalex.org/work/W2155485257', 'https://semopenalex.org/work/W2119248338', 'https://semopenalex.org/work/W2746485297', 'https://semopenalex.org/work/W4387322833', 'https://semopenalex.org/work/W1828712802', 'https://semopenalex.org/work/W2018680103', 'https://semopenalex.org/work/W2018206842', 'https://semopenalex.org/work/W4403926088', 'https://semopenalex.org/work/W2439315773', 'https://semopenalex.org/work/W3048660463', 'https://semopenalex.org/work/W2101981713', 'https://semopenalex.org/work/W2098410722', 'https://semopenalex.org/work/W2133913871', 'https://semopenalex.org/work/W2166197815', 'https://semopenalex.org/work/W1552869711', 'https://semopenalex.org/work/W4287256164', 'https://semopenalex.org/work/W4379033886', 'https://semopenalex.org/work/W2153901619', 'https://semopenalex.org/work/W4396898129', 'https://semopenalex.org/work/W4403704152', 'https://semopenalex.org/work/W1867432869', 'https://semopenalex.org/work/W2170329684', 'https://semopenalex.org/work/W2127324110', 'https://semopenalex.org/work/W3000267050', 'https://semopenalex.org/work/W2188413581', 'https://semopenalex.org/work/W4224861303', 'https://semopenalex.org/work/W3093907665', 'https://semopenalex.org/work/W2544362511', 'https://semopenalex.org/work/W2963504418', 'https://semopenalex.org/work/W2189224346', 'https://semopenalex.org/work/W2063650998', 'https://semopenalex.org/work/W4247141155', 'https://semopenalex.org/work/W4299652167', 'https://semopenalex.org/work/W3194819591', 'https://semopenalex.org/work/W2949657987', 'https://semopenalex.org/work/W3002449320', 'https://semopenalex.org/work/W2039091249', 'https://semopenalex.org/work/W4256384691', 'https://semopenalex.org/work/W4288482042', 'https://semopenalex.org/work/W2383111726', 'https://semopenalex.org/work/W2334675349', 'https://semopenalex.org/work/W1809937706', 'https://semopenalex.org/work/W2155252144', 'https://semopenalex.org/work/W2160846724', 'https://semopenalex.org/work/W2035136970', 'https://semopenalex.org/work/W2107462260', 'https://semopenalex.org/work/W2073431334', 'https://semopenalex.org/work/W2129859788', 'https://semopenalex.org/work/W2051137523', 'https://semopenalex.org/work/W2144185926', 'https://semopenalex.org/work/W3162654685', 'https://semopenalex.org/work/W2106616524', 'https://semopenalex.org/work/W2616097381', 'https://semopenalex.org/work/W2003260793', 'https://semopenalex.org/work/W2107882641', 'https://semopenalex.org/work/W1996041609', 'https://semopenalex.org/work/W1685599524', 'https://semopenalex.org/work/W2068189057', 'https://semopenalex.org/work/W2018627313', 'https://semopenalex.org/work/W2949567914', 'https://semopenalex.org/work/W2899417085', 'https://semopenalex.org/work/W1881094281', 'https://semopenalex.org/work/W2035899572', 'https://semopenalex.org/work/W3129332190', 'https://semopenalex.org/work/W4397028652', 'https://semopenalex.org/work/W2137117880', 'https://semopenalex.org/work/W4386728269', 'https://semopenalex.org/work/W2890986802', 'https://semopenalex.org/work/W2020196086', 'https://semopenalex.org/work/W2158693223', 'https://semopenalex.org/work/W2245018327', 'https://semopenalex.org/work/W2558578462', 'https://semopenalex.org/work/W2102302018', 'https://semopenalex.org/work/W2185435830', 'https://semopenalex.org/work/W1774599862', 'https://semopenalex.org/work/W1980527047', 'https://semopenalex.org/work/W2129518598', 'https://semopenalex.org/work/W2476492488', 'https://semopenalex.org/work/W1814362492', 'https://semopenalex.org/work/W2032099309', 'https://semopenalex.org/work/W1587379027', 'https://semopenalex.org/work/W3137611772', 'https://semopenalex.org/work/W3015796941', 'https://semopenalex.org/work/W2086613112', 'https://semopenalex.org/work/W2991868466', 'https://semopenalex.org/work/W1943126751', 'https://semopenalex.org/work/W1778342465', 'https://semopenalex.org/work/W2162696202', 'https://semopenalex.org/work/W2171858716', 'https://semopenalex.org/work/W2123832893', 'https://semopenalex.org/work/W4237667777', 'https://semopenalex.org/work/W2151951544', 'https://semopenalex.org/work/W2160172952', 'https://semopenalex.org/work/W2806687546', 'https://semopenalex.org/work/W2168793726', 'https://semopenalex.org/work/W2126043778', 'https://semopenalex.org/work/W2111557101', 'https://semopenalex.org/work/W2113359099', 'https://semopenalex.org/work/W2147674767', 'https://semopenalex.org/work/W2108933378', 'https://semopenalex.org/work/W2166805843', 'https://semopenalex.org/work/W3003820456', 'https://semopenalex.org/work/W2094757833', 'https://semopenalex.org/work/W2122768752', 'https://semopenalex.org/work/W3203864625', 'https://semopenalex.org/work/W1957871232', 'https://semopenalex.org/work/W2034066646', 'https://semopenalex.org/work/W1577360515', 'https://semopenalex.org/work/W2021144192', 'https://semopenalex.org/work/W2140807309', 'https://semopenalex.org/work/W2636221734', 'https://semopenalex.org/work/W2164090505', 'https://semopenalex.org/work/W2124699087', 'https://semopenalex.org/work/W2166153231', 'https://semopenalex.org/work/W2155153848', 'https://semopenalex.org/work/W2143075489', 'https://semopenalex.org/work/W1979849178', 'https://semopenalex.org/work/W4283396505', 'https://semopenalex.org/work/W2171540325', 'https://semopenalex.org/work/W4400686367', 'https://semopenalex.org/work/W2760778129', 'https://semopenalex.org/work/W2988626048', 'https://semopenalex.org/work/W2120659763', 'https://semopenalex.org/work/W2109820484', 'https://semopenalex.org/work/W2148267424', 'https://semopenalex.org/work/W2114885066', 'https://semopenalex.org/work/W2266109773', 'https://semopenalex.org/work/W2397760318', 'https://semopenalex.org/work/W1812926078', 'https://semopenalex.org/work/W3097189301', 'https://semopenalex.org/work/W2574952845', 'https://semopenalex.org/work/W1882111414', 'https://semopenalex.org/work/W2122128429', 'https://semopenalex.org/work/W1995899361', 'https://semopenalex.org/work/W4225343232', 'https://semopenalex.org/work/W2673901561', 'https://semopenalex.org/work/W4309129028', 'https://semopenalex.org/work/W2521295940', 'https://semopenalex.org/work/W2160616608', 'https://semopenalex.org/work/W2065530904', 'https://semopenalex.org/work/W2035561336', 'https://semopenalex.org/work/W2128722362', 'https://semopenalex.org/work/W2109153110', 'https://semopenalex.org/work/W2127631196', 'https://semopenalex.org/work/W2755327666', 'https://semopenalex.org/work/W2077128747', 'https://semopenalex.org/work/W2163889321', 'https://semopenalex.org/work/W2889512408', 'https://semopenalex.org/work/W2112250360', 'https://semopenalex.org/work/W1975302208', 'https://semopenalex.org/work/W2756070092', 'https://semopenalex.org/work/W2611380909', 'https://semopenalex.org/work/W2984425774', 'https://semopenalex.org/work/W2243109900', 'https://semopenalex.org/work/W4362508498', 'https://semopenalex.org/work/W2012992134', 'https://semopenalex.org/work/W2048025952', 'https://semopenalex.org/work/W4392903531', 'https://semopenalex.org/work/W2294916470', 'https://semopenalex.org/work/W2040652823', 'https://semopenalex.org/work/W4287824497', 'https://semopenalex.org/work/W1988343658', 'https://semopenalex.org/work/W2138621265', 'https://semopenalex.org/work/W2153608957', 'https://semopenalex.org/work/W2102592853', 'https://semopenalex.org/work/W1909031490', 'https://semopenalex.org/work/W2044542062', 'https://semopenalex.org/work/W2125505095', 'https://semopenalex.org/work/W1867833735', 'https://semopenalex.org/work/W2078616504', 'https://semopenalex.org/work/W2128254445', 'https://semopenalex.org/work/W2110043300', 'https://semopenalex.org/work/W3005631622', 'https://semopenalex.org/work/W2940821791', 'https://semopenalex.org/work/W2912726147', 'https://semopenalex.org/work/W2030896881', 'https://semopenalex.org/work/W2134429331', 'https://semopenalex.org/work/W2949402315', 'https://semopenalex.org/work/W3176828173', 'https://semopenalex.org/work/W4400052969', 'https://semopenalex.org/work/W2094507611', 'https://semopenalex.org/work/W2126409288', 'https://semopenalex.org/work/W2146987051', 'https://semopenalex.org/work/W2117127275', 'https://semopenalex.org/work/W2092230235', 'https://semopenalex.org/work/W1812922818', 'https://semopenalex.org/work/W1964567495', 'https://semopenalex.org/work/W2545039763', 'https://semopenalex.org/work/W2164697291', 'https://semopenalex.org/work/W2082792607', 'https://semopenalex.org/work/W2135428614', 'https://semopenalex.org/work/W4224949960', 'https://semopenalex.org/work/W2143728623', 'https://semopenalex.org/work/W2978037608', 'https://semopenalex.org/work/W2026970166', 'https://semopenalex.org/work/W4288596410', 'https://semopenalex.org/work/W2137477396', 'https://semopenalex.org/work/W2939947188', 'https://semopenalex.org/work/W3162627549', 'https://semopenalex.org/work/W2112902331', 'https://semopenalex.org/work/W4402502594', 'https://semopenalex.org/work/W2963455631', 'https://semopenalex.org/work/W1881771041', 'https://semopenalex.org/work/W2663325069', 'https://semopenalex.org/work/W3106343576', 'https://semopenalex.org/work/W2337742825', 'https://semopenalex.org/work/W4386081510', 'https://semopenalex.org/work/W2144871920', 'https://semopenalex.org/work/W2034340815', 'https://semopenalex.org/work/W2566922557', 'https://semopenalex.org/work/W2072116332', 'https://semopenalex.org/work/W2041220458', 'https://semopenalex.org/work/W2138646635', 'https://semopenalex.org/work/W3022662194', 'https://semopenalex.org/work/W2798274156', 'https://semopenalex.org/work/W4221012413', 'https://semopenalex.org/work/W2101633987', 'https://semopenalex.org/work/W2395280900', 'https://semopenalex.org/work/W2141480726', 'https://semopenalex.org/work/W2039909063', 'https://semopenalex.org/work/W2145568341', 'https://semopenalex.org/work/W2052527654', 'https://semopenalex.org/work/W4309877015', 'https://semopenalex.org/work/W2182254337', 'https://semopenalex.org/work/W1994628498', 'https://semopenalex.org/work/W2147406818', 'https://semopenalex.org/work/W2408555870', 'https://semopenalex.org/work/W2018354435', 'https://semopenalex.org/work/W3043975171', 'https://semopenalex.org/work/W2114391062', 'https://semopenalex.org/work/W3155241911', 'https://semopenalex.org/work/W2138556535', 'https://semopenalex.org/work/W2297506387', 'https://semopenalex.org/work/W2115943920', 'https://semopenalex.org/work/W2150042449', 'https://semopenalex.org/work/W2486186027', 'https://semopenalex.org/work/W1785723168', 'https://semopenalex.org/work/W4376141221', 'https://semopenalex.org/work/W2113606224', 'https://semopenalex.org/work/W2053928191', 'https://semopenalex.org/work/W2112567022', 'https://semopenalex.org/work/W1984769758', 'https://semopenalex.org/work/W2066478156', 'https://semopenalex.org/work/W2155484207', 'https://semopenalex.org/work/W2007203285', 'https://semopenalex.org/work/W4315606073', 'https://semopenalex.org/work/W2168925869', 'https://semopenalex.org/work/W2143623375', 'https://semopenalex.org/work/W2122776646', 'https://semopenalex.org/work/W1891629850', 'https://semopenalex.org/work/W2142005762', 'https://semopenalex.org/work/W2594176303', 'https://semopenalex.org/work/W4386362810', 'https://semopenalex.org/work/W2241753404', 'https://semopenalex.org/work/W2128821548', 'https://semopenalex.org/work/W2021426840', 'https://semopenalex.org/work/W2512503502', 'https://semopenalex.org/work/W1775735896', 'https://semopenalex.org/work/W2136510471', 'https://semopenalex.org/work/W2013030361', 'https://semopenalex.org/work/W2152599017', 'https://semopenalex.org/work/W1989790075', 'https://semopenalex.org/work/W2100860054', 'https://semopenalex.org/work/W1997581342', '</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W3193717464', 'https://semopenalex.org/work/W2791540051', 'https://semopenalex.org/work/W4404915142', 'https://semopenalex.org/work/W3032857618', 'https://semopenalex.org/work/W2736312195', 'https://semopenalex.org/work/W2789478762', 'https://semopenalex.org/work/W4366547357', 'https://semopenalex.org/work/W4402722090', 'https://semopenalex.org/work/W2977597077', 'https://semopenalex.org/work/W3161959528', 'https://semopenalex.org/work/W2972702127', 'https://semopenalex.org/work/W4361189030', 'https://semopenalex.org/work/W2091382943', 'https://semopenalex.org/work/W2519558346', 'https://semopenalex.org/work/W4239396382', 'https://semopenalex.org/work/W4287729941', 'https://semopenalex.org/work/W4287071181', 'https://semopenalex.org/work/W2024357873', 'https://semopenalex.org/work/W1877041815', 'https://semopenalex.org/work/W2921058600', 'https://semopenalex.org/work/W4324152586', 'https://semopenalex.org/work/W1976594634', 'https://semopenalex.org/work/W2288812598', 'https://semopenalex.org/work/W4294891921', 'https://semopenalex.org/work/W3047192924', 'https://semopenalex.org/work/W4312572845', 'https://semopenalex.org/work/W3117330688', 'https://semopenalex.org/work/W3033839905', 'https://semopenalex.org/work/W1998431265', 'https://semopenalex.org/work/W2087800309', 'https://semopenalex.org/work/W2885122621', 'https://semopenalex.org/work/W2273076933', 'https://semopenalex.org/work/W2557881781', 'https://semopenalex.org/work/W2978827769', 'https://semopenalex.org/work/W4221065578', 'https://semopenalex.org/work/W2977979696', 'https://semopenalex.org/work/W3161974712', 'https://semopenalex.org/work/W3009160614', 'https://semopenalex.org/work/W2591593006', 'https://semopenalex.org/work/W4396832885', 'https://semopenalex.org/work/W3204393727', 'https://semopenalex.org/work/W4366967286', 'https://semopenalex.org/work/W4211259494', 'https://semopenalex.org/work/W4200616097', 'https://semopenalex.org/work/W1860259465', 'https://semopenalex.org/work/W2078369692', 'https://semopenalex.org/work/W3110075456', 'https://semopenalex.org/work/W3096658838', 'https://semopenalex.org/work/W4309619903', 'https://semopenalex.org/work/W4283397308', 'https://semopenalex.org/work/W4404977899', 'https://semopenalex.org/work/W2944843734', 'https://semopenalex.org/work/W2610676428', 'https://semopenalex.org/work/W4404026276', 'https://semopenalex.org/work/W2513683703', 'https://semopenalex.org/work/W3011317564', 'https://semopenalex.org/work/W3202016550', 'https://semopenalex.org/work/W2737450254', 'https://semopenalex.org/work/W2033617925', 'https://semopenalex.org/work/W2602429360', 'https://semopenalex.org/work/W2551155618', 'https://semopenalex.org/work/W4319452484', 'https://semopenalex.org/work/W1993514406', 'https://semopenalex.org/work/W3163327897', 'https://semopenalex.org/work/W2080327955', 'https://semopenalex.org/work/W2137846113', 'https://semopenalex.org/work/W3095740806', 'https://semopenalex.org/work/W2102905932', 'https://semopenalex.org/work/W4220905243', 'https://semopenalex.org/work/W1981715407', 'https://semopenalex.org/work/W2981708234', 'https://semopenalex.org/work/W1965526182', 'https://semopenalex.org/work/W2750727230', 'https://semopenalex.org/work/W3215451397', 'https://semopenalex.org/work/W2519914856', 'https://semopenalex.org/work/W2169202944', 'https://semopenalex.org/work/W1510660243', 'https://semopenalex.org/work/W2007978709', 'https://semopenalex.org/work/W2159491375', 'https://semopenalex.org/work/W2972600126', 'https://semopenalex.org/work/W4211095911', 'https://semopenalex.org/work/W1524596993', 'https://semopenalex.org/work/W1834136374', 'https://semopenalex.org/work/W2567779880', 'https://semopenalex.org/work/W1993984611', 'https://semopenalex.org/work/W3029899401', 'https://semopenalex.org/work/W3033704563', 'https://semopenalex.org/work/W2898145840', 'https://semopenalex.org/work/W3183940262', 'https://semopenalex.org/work/W3015284588', 'https://semopenalex.org/work/W2561633795', 'https://semopenalex.org/work/W2139733095', 'https://semopenalex.org/work/W791468510', 'https://semopenalex.org/work/W2461856634', 'https://semopenalex.org/work/W4232727837', 'https://semopenalex.org/work/W4393067517', 'https://semopenalex.org/work/W3171875220', 'https://semopenalex.org/work/W3206366132', 'https://semopenalex.org/work/W4366583934', 'https://semopenalex.org/work/W2008208122', 'https://semopenalex.org/work/W2033680836', 'https://semopenalex.org/work/W2613908791', 'https://semopenalex.org/work/W2795503716', 'https://semopenalex.org/work/W3177151358', 'https://semopenalex.org/work/W2528963299', 'https://semopenalex.org/work/W2768260654', 'https://semopenalex.org/work/W2774467220', 'https://semopenalex.org/work/W2177601947', 'https://semopenalex.org/work/W2752493326', 'https://semopenalex.org/work/W2520661109', 'https://semopenalex.org/work/W2187647369', 'https://semopenalex.org/work/W3165155612', 'https://semopenalex.org/work/W3096988350', 'https://semopenalex.org/work/W2520352456', 'https://semopenalex.org/work/W2913594206', 'https://semopenalex.org/work/W2092202628', 'https://semopenalex.org/work/W3110591323', 'https://semopenalex.org/work/W2973016298', 'https://semopenalex.org/work/W2921533080', 'https://semopenalex.org/work/W4393067390', 'https://semopenalex.org/work/W3031395001', 'https://semopenalex.org/work/W4308467568', 'https://semopenalex.org/work/W3143959337', 'https://semopenalex.org/work/W4404569483', 'https://semopenalex.org/work/W2625122753', 'https://semopenalex.org/work/W2754101670', 'https://semopenalex.org/work/W3181801907', 'https://semopenalex.org/work/W2972889118', 'https://semopenalex.org/work/W3194688439', 'https://semopenalex.org/work/W2072490274', 'https://semopenalex.org/work/W3034123328', 'https://semopenalex.org/work/W4389891943', 'https://semopenalex.org/work/W3035628382', 'https://semopenalex.org/work/W2133951180', 'https://semopenalex.org/work/W2318574332', 'https://semopenalex.org/work/W4310446060', 'https://semopenalex.org/work/W2293208404', 'https://semopenalex.org/work/W4391423303', 'https://semopenalex.org/work/W2082538501', 'https://semopenalex.org/work/W3091007149', 'https://semopenalex.org/work/W3033480106', 'https://semopenalex.org/work/W2899305210', 'https://semopenalex.org/work/W3030577208', 'https://semopenalex.org/work/W4312841490', 'https://semopenalex.org/work/W2977911811', 'https://semopenalex.org/work/W2598459295', 'https://semopenalex.org/work/W2904910662', 'https://semopenalex.org/work/W2753671526', 'https://semopenalex.org/work/W4224242333', 'https://semopenalex.org/work/W2057014910', 'https://semopenalex.org/work/W2605978692', 'https://semopenalex.org/work/W4391210282', 'https://semopenalex.org/work/W4399763801', 'https://semopenalex.org/work/W3186694431', 'https://semopenalex.org/work/W2294361658', 'https://semopenalex.org/work/W2401872729', 'https://semopenalex.org/work/W2975736083', 'https://semopenalex.org/work/W1771936601', 'https://semopenalex.org/work/W3005470382', 'https://semopenalex.org/work/W2899389394', 'https://semopenalex.org/work/W2752658305', 'https://semopenalex.org/work/W1522158218', 'https://semopenalex.org/work/W4387085789', 'https://semopenalex.org/work/W3003369003', 'https://semopenalex.org/work/W3184531492', 'https://semopenalex.org/work/W3030149602', 'https://semopenalex.org/work/W4394825420', 'https://semopenalex.org/work/W2898820983', 'https://semopenalex.org/work/W3037695612', 'https://semopenalex.org/work/W2898627444', 'https://semopenalex.org/work/W4225088745', 'https://semopenalex.org/work/W2929751249', 'https://semopenalex.org/work/W4366549587', 'https://semopenalex.org/work/W3035727063', 'https://semopenalex.org/work/W2088270376', 'https://semopenalex.org/work/W2898667062', 'https://semopenalex.org/work/W2263778529', 'https://semopenalex.org/work/W2346027641', 'https://semopenalex.org/work/W4324151651', 'https://semopenalex.org/work/W4200018492', 'https://semopenalex.org/work/W2751622533', 'https://semopenalex.org/work/W2519458229', 'https://semopenalex.org/work/W2909558410', 'https://semopenalex.org/work/W2061583538', 'https://semopenalex.org/work/W4400430993', 'https://semopenalex.org/work/W1985142918', 'https://semopenalex.org/work/W3084729599', 'https://semopenalex.org/work/W2119929248', 'https://semopenalex.org/work/W3163521409', 'https://semopenalex.org/work/W2610274107', 'https://semopenalex.org/work/W4229043996', 'https://semopenalex.org/work/W3024164567', 'https://semopenalex.org/work/W2921194733', 'https://semopenalex.org/work/W4387606708', 'https://semopenalex.org/work/W2752490344', 'https://semopenalex.org/work/W3163085734', 'https://semopenalex.org/work/W2725971658', 'https://semopenalex.org/work/W4241289669', 'https://semopenalex.org/work/W3095367321', 'https://semopenalex.org/work/W3160199101', 'https://semopenalex.org/work/W4230032809', 'https://semopenalex.org/work/W2753801751', 'https://semopenalex.org/work/W3142764819', 'https://semopenalex.org/work/W4225473762', 'https://semopenalex.org/work/W4392429145', 'https://semopenalex.org/work/W4387421144', 'https://semopenalex.org/work/W3161202338', 'https://semopenalex.org/work/W2978280554', 'https://semopenalex.org/work/W2946308339', 'https://semopenalex.org/work/W2152557601', 'https://semopenalex.org/work/W4312605566', 'https://semopenalex.org/work/W2054886944', 'https://semopenalex.org/work/W2811468211', 'https://semopenalex.org/work/W3188766356', 'https://semopenalex.org/work/W1975028026', 'https://semopenalex.org/work/W2067004171', 'https://semopenalex.org/work/W4400189062', 'https://semopenalex.org/work/W2755164339', 'https://semopenalex.org/work/W2899470128', 'https://semopenalex.org/work/W2751429127', 'https://semopenalex.org/work/W3030735111', 'https://semopenalex.org/work/W2973046614', 'https://semopenalex.org/work/W4214684069', 'https://semopenalex.org/work/W4213455276', 'https://semopenalex.org/work/W2611685970', 'https://semopenalex.org/work/W2888386951', 'https://semopenalex.org/work/W2775793881', 'https://semopenalex.org/work/W4401406766', 'https://semopenalex.org/work/W1710215999', 'https://semopenalex.org/work/W4224305168', 'https://semopenalex.org/work/W4366583171', 'https://semopenalex.org/work/W2793897377', 'https://semopenalex.org/work/W2165066165', 'https://semopenalex.org/work/W2962975962', 'https://semopenalex.org/work/W3003204379', 'https://semopenalex.org/work/W2899333601', 'https://semopenalex.org/work/W4292261957', 'https://semopenalex.org/work/W3112090964', 'https://semopenalex.org/work/W2611151946', 'https://semopenalex.org/work/W1751138515', 'https://semopenalex.org/work/W4389256452', 'https://semopenalex.org/work/W4225133274', 'https://semopenalex.org/work/W4324150573', 'https://semopenalex.org/work/W2055070571', 'https://semopenalex.org/work/W4241528240', 'https://semopenalex.org/work/W2610780371', 'https://semopenalex.org/work/W2901616108', 'https://semopenalex.org/work/W2537880674', 'https://semopenalex.org/work/W2072697691', 'https://semopenalex.org/work/W3206712787', 'https://semopenalex.org/work/W4379879736', 'https://semopenalex.org/work/W2903417746', 'https://semopenalex.org/work/W3043824623', 'https://semopenalex.org/work/W2977617583', 'https://semopenalex.org/work/W2090841027', 'https://semopenalex.org/work/W3182364466', 'https://semopenalex.org/work/W3160545975', 'https://semopenalex.org/work/W3028614762', 'https://semopenalex.org/work/W4251839844', 'https://semopenalex.org/work/W3200245219', 'https://semopenalex.org/work/W3141512745', 'https://semopenalex.org/work/W1704771702', 'https://semopenalex.org/work/W2519730427', 'https://semopenalex.org/work/W2409578015', 'https://semopenalex.org/work/W2149683870', 'https://semopenalex.org/work/W2738622408', 'https://semopenalex.org/work/W2256119246', 'https://semopenalex.org/work/W2108512685', 'https://semopenalex.org/work/W2942324097', 'https://semopenalex.org/work/W2972419497', 'https://semopenalex.org/work/W2895512277', 'https://semopenalex.org/work/W4389897704', 'https://semopenalex.org/work/W3198359754', 'https://semopenalex.org/work/W4324154015', 'https://semopenalex.org/work/W1982984133', 'https://semopenalex.org/work/W4366597679', 'https://semopenalex.org/work/W3126826400', 'https://semopenalex.org/work/W2129488573', 'https://semopenalex.org/work/W1985504739', 'https://semopenalex.org/work/W2088502162', 'https://semopenalex.org/work/W4402722131', 'https://semopenalex.org/work/W4379033872', 'https://semopenalex.org/work/W4234952088', 'https://semopenalex.org/work/W1553133540', 'https://semopenalex.org/work/W3196772354', 'https://semopenalex.org/work/W2810881717', 'https://semopenalex.org/work/W3036463368', 'https://semopenalex.org/work/W2520077052', 'https://semopenalex.org/work/W2942738233', 'https://semopenalex.org/work/W2913475584', 'https://semopenalex.org/work/W2089266363', 'https://semopenalex.org/work/W2102667737', 'https://semopenalex.org/work/W2518694405', 'https://semopenalex.org/work/W3032662532', 'https://semopenalex.org/work/W2897414246', 'https://semopenalex.org/work/W2079488626', 'https://semopenalex.org/work/W2795581336', 'https://semopenalex.org/work/W4386163788', 'https://semopenalex.org/work/W3163078982', 'https://semopenalex.org/work/W2576215493', 'https://semopenalex.org/work/W3121062173', 'https://semopenalex.org/work/W2762577600', 'https://semopenalex.org/work/W4307204790', 'https://semopenalex.org/work/W4242142265', 'https://semopenalex.org/work/W3203088685', 'https://semopenalex.org/work/W3094759305', 'https://semopenalex.org/work/W2346600598', 'https://semopenalex.org/work/W4230967253', 'https://semopenalex.org/work/W2108911539', 'https://semopenalex.org/work/W4238249729', 'https://semopenalex.org/work/W2753363725', 'https://semopenalex.org/work/W3162832522', 'https://semopenalex.org/work/W2968884122', 'https://semopenalex.org/work/W2898822823', 'https://semopenalex.org/work/W4224279084', 'https://semopenalex.org/work/W2973140914', 'https://semopenalex.org/work/W3121775658', 'https://semopenalex.org/work/W1246643588', 'https://semopenalex.org/work/W4393877125', 'https://semopenalex.org/work/W4312282153', 'https://semopenalex.org/work/W3161889270', 'https://semopenalex.org/work/W2920869031', 'https://semopenalex.org/work/W2903849727', 'https://semopenalex.org/work/W2790187313', 'https://semopenalex.org/work/W3178374478', 'https://semopenalex.org/work/W2121082751', 'https://semopenalex.org/work/W2019487042', 'https://semopenalex.org/work/W4214504130', 'https://semopenalex.org/work/W4315777028', 'https://semopenalex.org/work/W2136876773', 'https://semopenalex.org/work/W4210768549', 'https://semopenalex.org/work/W2978422619', 'https://semopenalex.org/work/W2548042282', 'https://semopenalex.org/work/W862033376', 'https://semopenalex.org/work/W4393908582', 'https://semopenalex.org/work/W3000816869', 'https://semopenalex.org/work/W3135072684', 'https://semopenalex.org/work/W2755506150', 'https://semopenalex.org/work/W4377250056', 'https://semopenalex.org/work/W2976524236', 'https://semopenalex.org/work/W4404873047', 'https://semopenalex.org/work/W2294561329', 'https://semopenalex.org/work/W4386929049', 'https://semopenalex.org/work/W2752031858', 'https://semopenalex.org/work/W3204110051', 'https://semopenalex.org/work/W3007521088', 'https://semopenalex.org/work/W2968293343', 'https://semopenalex.org/work/W2752042616', 'https://semopenalex.org/work/W2465877051', 'https://semopenalex.org/work/W3197280612', 'https://semopenalex.org/work/W2110284634', 'https://semopenalex.org/work/W4214593503', 'https://semopenalex.org/work/W2075286904', 'https://semopenalex.org/work/W2602397751', 'https://semopenalex.org/work/W4366588423', 'https://semopenalex.org/work/W2940716241', 'https://semopenalex.org/work/W2154752229', 'https://semopenalex.org/work/W3028790862', 'https://semopenalex.org/work/W3112877194', 'https://semopenalex.org/work/W2896178739', 'https://semopenalex.org/work/W3090583924', 'https://semopenalex.org/work/W2798335699', 'https://semopenalex.org/work/W2344158693', 'https://semopenalex.org/work/W3033866035', 'https://semopenalex.org/work/W2752561456', 'https://semopenalex.org/work/W4210450354', 'https://semopenalex.org/work/W4393102879', 'https://semopenalex.org/work/W2052607251', 'https://semopenalex.org/work/W3162177365', 'https://semopenalex.org/work/W4312646439', 'https://semopenalex.org/work/W2973132733', 'https://semopenalex.org/work/W2986358413', 'https://semopenalex.org/work/W4200525013', 'https://semopenalex.org/work/W4324150147', 'https://semopenalex.org/work/W4245844025', 'https://semopenalex.org/work/W4307475355', 'https://semopenalex.org/work/W4366598255', 'https://semopenalex.org/work/W2114418543', 'https://semopenalex.org/work/W3130372017', 'https://semopenalex.org/work/W3201213010', 'https://semopenalex.org/work/W2060118520', 'https://semopenalex.org/work/W3196785132', 'https://semopenalex.org/work/W2156243282', 'https://semopenalex.org/work/W2017727997', 'https://semopenalex.org/work/W3028180736', 'https://semopenalex.org/work/W3062298123', 'https://semopenalex.org/work/W4394883037', 'https://semopenalex.org/work/W2346980133', 'https://semopenalex.org/work/W4256454723', 'https://semopenalex.org/work/W2966384546', 'https://semopenalex.org/work/W2519250278', 'https://semopenalex.org/work/W4224255688', 'https://semopenalex.org/work/W3190617503', 'https://semopenalex.org/work/W1484203263', 'https://semopenalex.org/work/W3188420011', 'https://semopenalex.org/work/W2037697732', 'https://semopenalex.org/work/W3193396842', 'https://semopenalex.org/work/W4385856456', 'https://semopenalex.org/work/W4383220643', 'https://semopenalex.org/work/W2131570437', 'https://semopenalex.org/work/W1568803211', 'https://semopenalex.org/work/W4404373433', 'https://semopenalex.org/work/W2068367136', 'https://semopenalex.org/work/W2902941289', 'https://semopenalex.org/work/W3119309106', 'https://semopenalex.org/work/W4399126764', 'https://semopenalex.org/work/W2063007215', 'https://semopenalex.org/work/W2902563098', 'https://semopenalex.org/work/W4393752214', 'https://semopenalex.org/work/W2012358521', 'https://semopenalex.org/work/W3163921267', 'https://semopenalex.org/work/W2972759039', 'https://semopenalex.org/work/W3201451193', 'https://semopenalex.org/work/W2515389026', 'https://semopenalex.org/work/W4406805368', 'https://semopenalex.org/work/W3095347735', 'https://semopenalex.org/work/W4233748389', 'https://semopenalex.org/work/W3022986551', 'https://semopenalex.org/work/W2410138785']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2012912450', 'https://semopenalex.org/work/W2495352272', 'https://semopenalex.org/work/W2139255754', 'https://semopenalex.org/work/W4285815179', 'https://semopenalex.org/work/W2615205062', 'https://semopenalex.org/work/W2966031361', 'https://semopenalex.org/work/W4404030068', 'https://semopenalex.org/work/W2134768851', 'https://semopenalex.org/work/W2061231005', 'https://semopenalex.org/work/W2147895050', 'https://semopenalex.org/work/W2085435476', 'https://semopenalex.org/work/W4393146711', 'https://semopenalex.org/work/W2571158126', 'https://semopenalex.org/work/W2293958210', 'https://semopenalex.org/work/W2052982204', 'https://semopenalex.org/work/W2554047600', 'https://semopenalex.org/work/W2166520679', 'https://semopenalex.org/work/W2019708772', 'https://semopenalex.org/work/W4306173842', 'https://semopenalex.org/work/W2070215238', 'https://semopenalex.org/work/W2334327213', 'https://semopenalex.org/work/W2246286794', 'https://semopenalex.org/work/W4249594017', 'https://semopenalex.org/work/W2065803961', 'https://semopenalex.org/work/W139668830', 'https://semopenalex.org/work/W2124870235', 'https://semopenalex.org/work/W2064476539', 'https://semopenalex.org/work/W2072209700', 'https://semopenalex.org/work/W2557110996', 'https://semopenalex.org/work/W214032606', 'https://semopenalex.org/work/W2077200079', 'https://semopenalex.org/work/W2092005371', 'https://semopenalex.org/work/W2484645626', 'https://semopenalex.org/work/W4253855517', 'https://semopenalex.org/work/W4402830551', 'https://semopenalex.org/work/W2119033694', 'https://semopenalex.org/work/W2950468099', 'https://semopenalex.org/work/W2109186457', 'https://semopenalex.org/work/W3175708501', 'https://semopenalex.org/work/W3021203574', 'https://semopenalex.org/work/W1526915766', 'https://semopenalex.org/work/W2982452767', 'https://semopenalex.org/work/W2108162045', 'https://semopenalex.org/work/W2768928198', 'https://semopenalex.org/work/W4285216643', 'https://semopenalex.org/work/W2559559327', 'https://semopenalex.org/work/W2401333290', 'https://semopenalex.org/work/W2998201073', 'https://semopenalex.org/work/W2401381263', 'https://semopenalex.org/work/W2945300184', 'https://semopenalex.org/work/W2992245431', 'https://semopenalex.org/work/W3130320973', 'https://semopenalex.org/work/W2478910470', 'https://semopenalex.org/work/W2041108261', 'https://semopenalex.org/work/W2088723639', 'https://semopenalex.org/work/W2123532445', 'https://semopenalex.org/work/W2034507787', 'https://semopenalex.org/work/W4401808601', 'https://semopenalex.org/work/W2550667658', 'https://semopenalex.org/work/W2907364096', 'https://semopenalex.org/work/W2413288731', 'https://semopenalex.org/work/W3157283285', 'https://semopenalex.org/work/W2295164153', 'https://semopenalex.org/work/W1969657871', 'https://semopenalex.org/work/W2095834672', 'https://semopenalex.org/work/W2953533689', 'https://semopenalex.org/work/W3041653159', 'https://semopenalex.org/work/W1999134690', 'https://semopenalex.org/work/W2903194584', 'https://semopenalex.org/work/W3085760006', 'https://semopenalex.org/work/W2586727473', 'https://semopenalex.org/work/W1538415416', 'https://semopenalex.org/work/W2042756792', 'https://semopenalex.org/work/W2542642724', 'https://semopenalex.org/work/W2138291705', 'https://semopenalex.org/work/W4405935629', 'https://semopenalex.org/work/W2149899452', 'https://semopenalex.org/work/W4389921335', 'https://semopenalex.org/work/W2600068329', 'https://semopenalex.org/work/W4392713273', 'https://semopenalex.org/work/W4294672395', 'https://semopenalex.org/work/W2929921254', 'https://semopenalex.org/work/W2135598717', 'https://semopenalex.org/work/W2165818457', 'https://semopenalex.org/work/W2473052796', 'https://semopenalex.org/work/W1518248903', 'https://semopenalex.org/work/W2145747218', 'https://semopenalex.org/work/W2730743430', 'https://semopenalex.org/work/W2895854254', 'https://semopenalex.org/work/W1608276691', 'https://semopenalex.org/work/W3118215277', 'https://semopenalex.org/work/W2203509984', 'https://semopenalex.org/work/W3097508557', 'https://semopenalex.org/work/W652412083', 'https://semopenalex.org/work/W2496567738', 'https://semopenalex.org/work/W2124054384', 'https://semopenalex.org/work/W3092453362', 'https://semopenalex.org/work/W2515896452', 'https://semopenalex.org/work/W1860740456', 'https://semopenalex.org/work/W2150650760', 'https://semopenalex.org/work/W1633573314', 'https://semopenalex.org/work/W2610600517', 'https://semopenalex.org/work/W2116314971', 'https://semopenalex.org/work/W2077737077', 'https://semopenalex.org/work/W1967157693', 'https://semopenalex.org/work/W3096110661', 'https://semopenalex.org/work/W1992253076', 'https://semopenalex.org/work/W565256208', 'https://semopenalex.org/work/W3107887875', 'https://semopenalex.org/work/W2063650982', 'https://semopenalex.org/work/W2532447822', 'https://semopenalex.org/work/W1531223514', 'https://semopenalex.org/work/W2084854878', 'https://semopenalex.org/work/W2142079724', 'https://semopenalex.org/work/W2145701421', 'https://semopenalex.org/work/W126878419', 'https://semopenalex.org/work/W2501830935', 'https://semopenalex.org/work/W2138433001', 'https://semopenalex.org/work/W2154510046', 'https://semopenalex.org/work/W2948995623', 'https://semopenalex.org/work/W33403252', 'https://semopenalex.org/work/W2170741870', 'https://semopenalex.org/work/W4392188385', 'https://semopenalex.org/work/W1874259713', 'https://semopenalex.org/work/W1990091852', 'https://semopenalex.org/work/W4252463735', 'https://semopenalex.org/work/W2910014621', 'https://semopenalex.org/work/W2146520711', 'https://semopenalex.org/work/W2058293659', 'https://semopenalex.org/work/W4396665589', 'https://semopenalex.org/work/W2496554705', 'https://semopenalex.org/work/W2356144191', 'https://semopenalex.org/work/W2906163189', 'https://semopenalex.org/work/W12268595', 'https://semopenalex.org/work/W2092477317', 'https://semopenalex.org/work/W2397834607', 'https://semopenalex.org/work/W2072776346', 'https://semopenalex.org/work/W2039163755', 'https://semopenalex.org/work/W4285172618', 'https://semopenalex.org/work/W2033725854', 'https://semopenalex.org/work/W2068524892', 'https://semopenalex.org/work/W2146033518', 'https://semopenalex.org/work/W2137861763', 'https://semopenalex.org/work/W2803258972', 'https://semopenalex.org/work/W2625986270', 'https://semopenalex.org/work/W4285408205', 'https://semopenalex.org/work/W4237745095', 'https://semopenalex.org/work/W1501172792', 'https://semopenalex.org/work/W3160200186', 'https://semopenalex.org/work/W2883395494', 'https://semopenalex.org/work/W2945691872', 'https://semopenalex.org/work/W2070269076', 'https://semopenalex.org/work/W2901316497', 'https://semopenalex.org/work/W2064672353', 'https://semopenalex.org/work/W4390187585', 'https://semopenalex.org/work/W2538630038', 'https://semopenalex.org/work/W2789144447', 'https://semopenalex.org/work/W2066111880', 'https://semopenalex.org/work/W4400238477', 'https://semopenalex.org/work/W2923039095', 'https://semopenalex.org/work/W2098016930', 'https://semopenalex.org/work/W2786772278', 'https://semopenalex.org/work/W2536107053', 'https://semopenalex.org/work/W4376526615', 'https://semopenalex.org/work/W4387450689', 'https://semopenalex.org/work/W2089241417', 'https://semopenalex.org/work/W2550712691', 'https://semopenalex.org/work/W2130803541', 'https://semopenalex.org/work/W4405120549', 'https://semopenalex.org/work/W2761828172', 'https://semopenalex.org/work/W1974886156', 'https://semopenalex.org/work/W1654176175', 'https://semopenalex.org/work/W1969462495', 'https://semopenalex.org/work/W2131405606', 'https://semopenalex.org/work/W4327767801', 'https://semopenalex.org/work/W3157167113', 'https://semopenalex.org/work/W2016989291', 'https://semopenalex.org/work/W4296365397', 'https://semopenalex.org/work/W2666172191', 'https://semopenalex.org/work/W4206683427', 'https://semopenalex.org/work/W2044431283', 'https://semopenalex.org/work/W2885100636', 'https://semopenalex.org/work/W2130007135', 'https://semopenalex.org/work/W1910867531', 'https://semopenalex.org/work/W2103224970', 'https://semopenalex.org/work/W2144750318', 'https://semopenalex.org/work/W3162144158', 'https://semopenalex.org/work/W2107191431', 'https://semopenalex.org/work/W1978851795', 'https://semopenalex.org/work/W2411894725', 'https://semopenalex.org/work/W2756387886', 'https://semopenalex.org/work/W1971283588', 'https://semopenalex.org/work/W2101787599', 'https://semopenalex.org/work/W2230115501', 'https://semopenalex.org/work/W1994278842', 'https://semopenalex.org/work/W1986827696', 'https://semopenalex.org/work/W2079466034', 'https://semopenalex.org/work/W4253131601', 'https://semopenalex.org/work/W2485878525', 'https://semopenalex.org/work/W2606501011', 'https://semopenalex.org/work/W1979289740', 'https://semopenalex.org/work/W2044237546', 'https://semopenalex.org/work/W1965382252', 'https://semopenalex.org/work/W2596027452', 'https://semopenalex.org/work/W4386814402', 'https://semopenalex.org/work/W2073709132', 'https://semopenalex.org/work/W2115899637', 'https://semopenalex.org/work/W1791684062', 'https://semopenalex.org/work/W1577463177', 'https://semopenalex.org/work/W1922706319', 'https://semopenalex.org/work/W4400946621', 'https://semopenalex.org/work/W2755469263', 'https://semopenalex.org/work/W2060283246', 'https://semopenalex.org/work/W2161545800', 'https://semopenalex.org/work/W4289655844', 'https://semopenalex.org/work/W2085207404', 'https://semopenalex.org/work/W4394742902', 'https://semopenalex.org/work/W4385626270', 'https://semopenalex.org/work/W2129869483', 'https://semopenalex.org/work/W2076330335', 'https://semopenalex.org/work/W2288294525', 'https://semopenalex.org/work/W4237620799', 'https://semopenalex.org/work/W1492737188', 'https://semopenalex.org/work/W1520936229', 'https://semopenalex.org/work/W4389321773', 'https://semopenalex.org/work/W4367360032', 'https://semopenalex.org/work/W2034179412', 'https://semopenalex.org/work/W2785105341', 'https://semopenalex.org/work/W2967954143', 'https://semopenalex.org/work/W1549886897', 'https://semopenalex.org/work/W2150298155', 'https://semopenalex.org/work/W857122145', 'https://semopenalex.org/work/W2805153701', 'https://semopenalex.org/work/W2080817506', 'https://semopenalex.org/work/W2401687993', 'https://semopenalex.org/work/W4401579183', 'https://semopenalex.org/work/W2968293641', 'https://semopenalex.org/work/W2340283416', 'https://semopenalex.org/work/W2754948093', 'https://semopenalex.org/work/W149383384', 'https://semopenalex.org/work/W2159662334', 'https://semopenalex.org/work/W2124560301', 'https://semopenalex.org/work/W1979988378', 'https://semopenalex.org/work/W2142484380', 'https://semopenalex.org/work/W1908879184', 'https://semopenalex.org/work/W2144918660', 'https://semopenalex.org/work/W1569686365', 'https://semopenalex.org/work/W159035867', 'https://semopenalex.org/work/W1608886591', 'https://semopenalex.org/work/W2289149676', 'https://semopenalex.org/work/W2290447772', 'https://semopenalex.org/work/W2564132746', 'https://semopenalex.org/work/W1488510230', 'https://semopenalex.org/work/W328613600', 'https://semopenalex.org/work/W2095968352', 'https://semopenalex.org/work/W2024336304', 'https://semopenalex.org/work/W2496039851', 'https://semopenalex.org/work/W2612784784', 'https://semopenalex.org/work/W2161454411', 'https://semopenalex.org/work/W4233681091', 'https://semopenalex.org/work/W2484374542', 'https://semopenalex.org/work/W2111424373', 'https://semopenalex.org/work/W2405266982', 'https://semopenalex.org/work/W2903213374', 'https://semopenalex.org/work/W196228518', 'https://semopenalex.org/work/W1177607589', 'https://semopenalex.org/work/W4240245530', 'https://semopenalex.org/work/W4367360059', 'https://semopenalex.org/work/W3042004637', 'https://semopenalex.org/work/W2884188352', 'https://semopenalex.org/work/W2111277352', 'https://semopenalex.org/work/W2147139299', 'https://semopenalex.org/work/W1973148750', 'https://semopenalex.org/work/W143942840', 'https://semopenalex.org/work/W2132053703', 'https://semopenalex.org/work/W2130832779', 'https://semopenalex.org/work/W1857000584', 'https://semopenalex.org/work/W1973125618', 'https://semopenalex.org/work/W2290200834', 'https://semopenalex.org/work/W2886396839', 'https://semopenalex.org/work/W2075578427', 'https://semopenalex.org/work/W1517253300', 'https://semopenalex.org/work/W2028566173', 'https://semopenalex.org/work/W4404030648', 'https://semopenalex.org/work/W4252981000', 'https://semopenalex.org/work/W2475545374', 'https://semopenalex.org/work/W4250489070', 'https://semopenalex.org/work/W2106421914', 'https://semopenalex.org/work/W2156138095', 'https://semopenalex.org/work/W4244005678', 'https://semopenalex.org/work/W2062904953', 'https://semopenalex.org/work/W2888177496', 'https://semopenalex.org/work/W2204033782', 'https://semopenalex.org/work/W2188799909', 'https://semopenalex.org/work/W2883856658', 'https://semopenalex.org/work/W2165377954', 'https://semopenalex.org/work/W2528842892', 'https://semopenalex.org/work/W3017143302', 'https://semopenalex.org/work/W2188362632', 'https://semopenalex.org/work/W2527344267', 'https://semopenalex.org/work/W2530140145', 'https://semopenalex.org/work/W1999149743', 'https://semopenalex.org/work/W2081189334', 'https://semopenalex.org/work/W2023972619', 'https://semopenalex.org/work/W2804891820', 'https://semopenalex.org/work/W4366964206', 'https://semopenalex.org/work/W2133522196', 'https://semopenalex.org/work/W2068973986', 'https://semopenalex.org/work/W2015849174', 'https://semopenalex.org/work/W6907768', 'https://semopenalex.org/work/W2024786226', 'https://semopenalex.org/work/W52623672', 'https://semopenalex.org/work/W1544524730', 'https://semopenalex.org/work/W3004301528', 'https://semopenalex.org/work/W4249963731', 'https://semopenalex.org/work/W2903177638', 'https://semopenalex.org/work/W2412127048', 'https://semopenalex.org/work/W2172143183', 'https://semopenalex.org/work/W2786601708', 'https://semopenalex.org/work/W1933806665', 'https://semopenalex.org/work/W2044900380', 'https://semopenalex.org/work/W2494421230', 'https://semopenalex.org/work/W2139454561', 'https://semopenalex.org/work/W1489534528', 'https://semopenalex.org/work/W2754307650', 'https://semopenalex.org/work/W4391156256', 'https://semopenalex.org/work/W2171510346', 'https://semopenalex.org/work/W67894965', 'https://semopenalex.org/work/W2024468903', 'https://semopenalex.org/work/W2108240852', 'https://semopenalex.org/work/W2077174735', 'https://semopenalex.org/work/W1516117757', 'https://semopenalex.org/work/W2004738891', 'https://semopenalex.org/work/W1982314073', 'https://semopenalex.org/work/W4205619442', 'https://semopenalex.org/work/W2062243122', 'https://semopenalex.org/work/W4205212276', 'https://semopenalex.org/work/W2112979372', 'https://semopenalex.org/work/W2965366155', 'https://semopenalex.org/work/W2110574373', 'https://semopenalex.org/work/W4401021691', 'https://semopenalex.org/work/W3200674364', 'https://semopenalex.org/work/W1999631843', 'https://semopenalex.org/work/W4240672112', 'https://semopenalex.org/work/W2159139699', 'https://semopenalex.org/work/W2108876125', 'https://semopenalex.org/work/W1516689139', 'https://semopenalex.org/work/W2125308824', 'https://semopenalex.org/work/W2995911827', 'https://semopenalex.org/work/W1823956242', 'https://semopenalex.org/work/W4286571613', 'https://semopenalex.org/work/W2144253537', 'https://semopenalex.org/work/W3206895939', 'https://semopenalex.org/work/W2138922641', 'https://semopenalex.org/work/W2120216356', 'https://semopenalex.org/work/W2111759980', 'https://semopenalex.org/work/W2002312562', 'https://semopenalex.org/work/W2751662694', 'https://semopenalex.org/work/W2611767226', 'https://semopenalex.org/work/W3211349420', 'https://semopenalex.org/work/W2157188908', 'https://semopenalex.org/work/W2884636426', 'https://semopenalex.org/work/W2983014989', 'https://semopenalex.org/work/W2749110496', 'https://semopenalex.org/work/W2293095660', 'https://semopenalex.org/work/W2748533023', 'https://semopenalex.org/work/W2055684776', 'https://semopenalex.org/work/W2072553352', 'https://semopenalex.org/work/W1995308547', 'https://semopenalex.org/work/W3132353162', 'https://semopenalex.org/work/W4210325270', 'https://semopenalex.org/work/W4206307909', 'https://semopenalex.org/work/W2809782991', 'https://semopenalex.org/work/W1508821613', 'https://semopenalex.org/work/W2132364404', 'https://semopenalex.org/work/W1990019789', 'https://semopenalex.org/work/W2125143433', 'https://semopenalex.org/work/W2569889271', 'https://semopenalex.org/work/W1993325111', 'https://semopenalex.org/work/W2158569759', 'https://semopenalex.org/work/W2964982644', 'https://semopenalex.org/work/W1506027738', 'https://semopenalex.org/work/W3023797106', 'https://semopenalex.org/work/W4312778763', 'https://semopenalex.org/work/W2289584941', 'https://semopenalex.org/work/W3027319226', 'https://semopenalex.org/work/W4390188024', 'https://semopenalex.org/work/W2138320177', 'https://semopenalex.org/work/W3095131015', 'https://semopenalex.org/work/W2034050419', 'https://semopenalex.org/work/W2163180953', 'https://semopenalex.org/work/W2032099346', 'https://semopenalex.org/work/W2794572176', 'https://semopenalex.org/work/W2293958373', 'https://semopenalex.org/work/W1991026653', 'https://semopenalex.org/work/W4294672356', 'https://semopenalex.org/work/W2968852933', 'https://semopenalex.org/work/W2789263069', 'https://semopenalex.org/work/W2069369796', 'https://semopenalex.org/work/W1514325539', 'https://semopenalex.org/work/W2134444560', 'https://semopenalex.org/work/W3089291192', 'https://semopenalex.org/work/W1497099843', 'https://semopenalex.org/work/W1923826352', 'https://semopenalex.org/work/W2768649200', 'https://semopenalex.org/work/W4401943800', 'https://semopenalex.org/work/W1661735121', 'https://semopenalex.org/work/W1497865469', 'https://semopenalex.org/work/W1870822388', 'https://semopenalex.org/work/W41465441', 'https://semopenalex.org/work/W325059703', 'https://semopenalex.org/work/W2155718231', 'https://semopenalex.org/work/W2080996134', 'https://semopenalex.org/work/W2398987072', 'https://semopenalex.org/work/W3196495759', 'https://semopenalex.org/work/W2166826477', 'https://semopenalex.org/work/W2162066092', 'https://semopenalex.org/work/W1494063694', 'https://semopenalex.org/work/W2106211998', 'https://semopenalex.org/work/W2896727063', 'https://semopenalex.org/work/W49611838', 'https://semopenalex.org/work/W2291113318', 'https://semopenalex.org/work/W1985701940', 'https://semopenalex.org/work/W4231226382', 'https://semopenalex.org/work/W4321614042', 'https://semopenalex.org/work/W2120355631', 'https://semopenalex.org/work/W1967568969', 'https://semopenalex.org/work/W2219017076', 'https://semopenalex.org/work/W2074068839', 'https://semopenalex.org/work/W48804293', 'https://semopenalex.org/work/W2475285031', 'https://semopenalex.org/work/W2941373095', 'https://semopenalex.org/work/W2413863213', 'https://semopenalex.org/work/W2744837872', 'https://semopenalex.org/work/W4205613083', 'https://semopenalex.org/work/W2055278155', 'https://semopenalex.org/work/W2947626283', 'https://semopenalex.org/work/W3179020455', 'https://semopenalex.org/work/W2210223524', 'https://semopenalex.org/work/W49790452', 'https://semopenalex.org/work/W2136654140', 'https://semopenalex.org/work/W2127414738', 'https://semopenalex.org/work/W25440647', 'https://semopenalex.org/work/W1560982985', 'https://semopenalex.org/work/W2145502705', 'https://semopenalex.org/work/W2111964097', 'https://semopenalex.org/work/W2786606238', 'https://semopenalex.org/work/W2512795596', 'https://semopenalex.org/work/W2293459815', 'https://semopenalex.org/work/W2935942569', 'https://semopenalex.org/work/W2516286998', 'https://semopenalex.org/work/W2275014257', 'https://semopenalex.org/work/W2041334917', 'https://semopenalex.org/work/W4390512166', 'https://semopenalex.org/work/W4206807237', 'https://semopenalex.org/work/W2139436497', 'https://semopenalex.org/work/W1422159917', 'https://semopenalex.org/work/W2576879514', 'https://semopenalex.org/work/W2165300716', 'https://semopenalex.org/work/W4247476769', 'https://semopenalex.org/work/W2079895649', 'https://semopenalex.org/work/W4376630019', 'https://semopenalex.org/work/W2981465620', 'https://semopenalex.org/work/W2903545243', 'https://semopenalex.org/work/W146617261', 'https://semopenalex.org/work/W2170201418', 'https://semopenalex.org/work/W2212338561', 'https://semopenalex.org/work/W2024012113', 'https://semopenalex.org/work/W2036165062', 'https://semopenalex.org/work/W4387005904', 'https://semopenalex.org/work/W2497743975', 'https://semopenalex.org/work/W2608491785', 'https://semopenalex.org/work/W3013997466', 'https://semopenalex.org/work/W2150998397', 'https://semopenalex.org/work/W2035518282', 'https://semopenalex.org/work/W1998201483', 'https://semopenalex.org/work/W2954164432', 'https://semopenalex.org/work/W2490092534', 'https://semopenalex.org/work/W2288534976', 'https://semopenalex.org/work/W2184299809', 'https://semopenalex.org/work/W2074193071', 'https://semopenalex.org/work/W2161966477', 'https://semopenalex.org/work/W2755359845', 'https://semopenalex.org/work/W2024612964', 'https://semopenalex.org/work/W1587236616', 'https://semopenalex.org/work/W2804376295', 'https://semopenalex.org/work/W2482354811', 'https://semopenalex.org/work/W2113043545', 'https://semopenalex.org/work/W1990193612', 'https://semopenalex.org/work/W2961776981', 'https://semopenalex.org/work/W2001905011', 'https://semopenalex.org/work/W2161850606', 'https://semopenalex.org/work/W2162338867', 'https://semopenalex.org/work/W2786657846', 'https://semopenalex.org/work/W2917706508', 'https://semopenalex.org/work/W1999508547', 'https://semopenalex.org/work/W2240362173', 'https://semopenalex.org/work/W4392942581', 'https://semopenalex.org/work/W2098948701', 'https://semopenalex.org/work/W1995950498', 'https://semopenalex.org/work/W2148646851', 'https://semopenalex.org/work/W1573590416', 'https://semopenalex.org/work/W2091944075', 'https://semopenalex.org/work/W2078326945', 'https://semopenalex.org/work/W2109705305', 'https://semopenalex.org/work/W2146002591', 'https://semopenalex.org/work/W2800308132', 'https://semopenalex.org/work/W3096330417', 'https://semopenalex.org/work/W2902487276', 'https://semopenalex.org/work/W2147456231', 'https://semopenalex.org/work/W1584206897', 'https://semopenalex.org/work/W4396894716', 'https://semopenalex.org/work/W1986540981', 'https://semopenalex.org/work/W4229053674', 'https://semopenalex.org/work/W1574380960', 'https://semopenalex.org/work/W2624802634', 'https://semopenalex.org/work/W1494162500', 'https://semopenalex.org/work/W2166217821', 'https://semopenalex.org/work/W2157519619', 'https://semopenalex.org/work/W1969516436', 'https://semopenalex.org/work/W2043269074', 'https://semopenalex.org/work/W2153457047', 'https://semopenalex.org/work/W4238734812', 'https://semopenalex.org/work/W2170913025', 'https://semopenalex.org/work/W2079664409', 'https://semopenalex.org/work/W1992495634', 'https://semopenalex.org/work/W51211239', 'https://semopenalex.org/work/W2742916377', 'https://semopenalex.org/work/W4252093019', 'https://semopenalex.org/work/W4400946519', 'https://semopenalex.org/work/W2171606781', 'https://semopenalex.org/work/W102421301', 'https://semopenalex.org/work/W3017031701', 'https://semopenalex.org/work/W4255531846', 'https://semopenalex.org/work/W2202036745', 'https://semopenalex.org/work/W3211844447', 'https://semopenalex.org/work/W2407231546', 'https://semopenalex.org/work/W2028754220', 'https://semopenalex.org/work/W2029131637', 'https://semopenalex.org/work/W2029818237', 'https://semopenalex.org/work/W2027452379', 'https://semopenalex.org/work/W2945412056', 'https://semopenalex.org/work/W2104408001', 'https://semopenalex.org/work/W2513883066', 'https://semopenalex.org/work/W1448329507', 'https://semopenalex.org/work/W4253850266', 'https://semopenalex.org/work/W2560712448', 'https://semopenalex.org/work/W2096075530', 'https://semopenalex.org/work/W2181791275', 'https://semopenalex.org/work/W2480965638', 'https://semopenalex.org/work/W3016161880', 'https://semopenalex.org/work/W2401583884', 'https://semopenalex.org/work/W1943042767', 'https://semopenalex.org/work/W2122571865', 'https://semopenalex.org/work/W2166211129', 'https://semopenalex.org/work/W2510781223', 'https://semopenalex.org/work/W4401578804', 'https://semopenalex.org/work/W3187351556', 'https://semopenalex.org/work/W4285503152', 'https://semopenalex.org/work/W979651393', 'https://semopenalex.org/work/W4316659889', 'https://semopenalex.org/work/W2102190590', 'https://semopenalex.org/work/W4365802790', 'https://semopenalex.org/work/W1967677932', 'https://semopenalex.org/work/W2163881253', 'https://semopenalex.org/work/W2062957328', 'https://semopenalex.org/work/W2620890574', 'https://semopenalex.org/work/W2128563460', 'https://semopenalex.org/work/W2769445687', 'https://semopenalex.org/work/W2094708864', 'https://semopenalex.org/work/W4210708907', 'https://semopenalex.org/work/W3129067525', 'https://semopenalex.org/work/W1840794446', 'https://semopenalex.org/work/W1991853935', 'https://semopenalex.org/work/W1481133633', 'https://semopenalex.org/work/W858120236', 'https://semopenalex.org/work/W2025546942', 'https://semopenalex.org/work/W2612282432', 'https://semopenalex.org/work/W2579158977', 'https://semopenalex.org/work/W2895817859', 'https://semopenalex.org/work/W1419972110', 'https://semopenalex.org/work/W2627083872', 'https://semopenalex.org/work/W72692433', 'https://semopenalex.org/work/W2112535726', 'https://semopenalex.org/work/W3206850855', 'https://semopenalex.org/work/W2167521347', 'https://semopenalex.org/work/W2163138922', 'https://semopenalex.org/work/W2895967513', 'https://semopenalex.org/work/W4392577068', 'https://semopenalex.org/work/W2160391119', 'https://semopenalex.org/work/W3136727059', 'https://semopenalex.org/work/W4230332361', 'https://semopenalex.org/work/W2625256202', 'https://semopenalex.org/work/W2967876484', 'https://semopenalex.org/work/W4253265224', 'https://semopenalex.org/work/W2747040169', 'https://semopenalex.org/work/W158943908', 'https://semopenalex.org/work/W2124703480', 'https://semopenalex.org/work/W2271801361', 'https://semopenalex.org/work/W2743920271', 'https://semopenalex.org/work/W2341007259', 'https://semopenalex.org/work/W1544888628', 'https://semopenalex.org/work/W2112107898', 'https://semopenalex.org/work/W3095279071', 'https://semopenalex.org/work/W2532152395', 'https://semopenalex.org/work/W2011410844', 'https://semopenalex.org/work/W2890543403', 'https://semopenalex.org/work/W2108304242', 'https://semopenalex.org/work/W4405094102', 'https://semopenalex.org/work/W160837981', 'https://semopenalex.org/work/W2056096508', 'https://semopenalex.org/work/W2014241426', 'https://semopenalex.org/work/W3206640136', 'https://semopenalex.org/work/W2058904901', 'https://semopenalex.org/work/W2031625065', 'https://semopenalex.org/work/W2140805995', 'https://semopenalex.org/work/W402024038']</t>
   </si>
   <si>
     <t>['23.574468085106382978723404']</t>
@@ -274,28 +274,28 @@
     <t>['2.288888888888888888888889']</t>
   </si>
   <si>
-    <t>['https://semopenalex.org/authorship/W4367671449A5086727894', 'https://semopenalex.org/authorship/W2844810377A5086727894', 'https://semopenalex.org/authorship/W3205075200A5086727894', 'https://semopenalex.org/authorship/W2772966323A5086727894', 'https://semopenalex.org/authorship/W2957110867A5086727894', 'https://semopenalex.org/authorship/W2996971450A5086727894', 'https://semopenalex.org/authorship/W2979701877A5086727894', 'https://semopenalex.org/authorship/W2948196949A5086727894', 'https://semopenalex.org/authorship/W2903944530A5086727894', 'https://semopenalex.org/authorship/W3134422373A5086727894', 'https://semopenalex.org/authorship/W2974444355A5086727894', 'https://semopenalex.org/authorship/W4396568545A5086727894', 'https://semopenalex.org/authorship/W4238294234A5086727894', 'https://semopenalex.org/authorship/W3048792033A5086727894', 'https://semopenalex.org/authorship/W4390737683A5086727894', 'https://semopenalex.org/authorship/W3158463786A5086727894', 'https://semopenalex.org/authorship/W2792290921A5086727894', 'https://semopenalex.org/authorship/W2996342798A5086727894', 'https://semopenalex.org/authorship/W2100407406A5086727894', 'https://semopenalex.org/authorship/W2897762537A5086727894', 'https://semopenalex.org/authorship/W1999760195A5086727894', 'https://semopenalex.org/authorship/W2805460435A5086727894', 'https://semopenalex.org/authorship/W4293863370A5086727894', 'https://semopenalex.org/authorship/W4206136166A5086727894', 'https://semopenalex.org/authorship/W2226359063A5086727894', 'https://semopenalex.org/authorship/W3202715770A5086727894', 'https://semopenalex.org/authorship/W4406267825A5086727894', 'https://semopenalex.org/authorship/W2780277126A5086727894', 'https://semopenalex.org/authorship/W2788968669A5086727894', 'https://semopenalex.org/authorship/W2397277866A5086727894']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/location/W31662312682', 'https://semopenalex.org/location/W30032445501', 'https://semopenalex.org/location/W43666671821', 'https://semopenalex.org/location/W30948193223', 'https://semopenalex.org/location/W43887990103', 'https://semopenalex.org/location/W43887990101', 'https://semopenalex.org/location/W32072432982', 'https://semopenalex.org/location/W28080081831', 'https://semopenalex.org/location/W31662312681', 'https://semopenalex.org/location/W22774936731', 'https://semopenalex.org/location/W29566225571', 'https://semopenalex.org/location/W43869518061', 'https://semopenalex.org/location/W27676589071', 'https://semopenalex.org/location/W29837826201', 'https://semopenalex.org/location/W30482369121', 'https://semopenalex.org/location/W25122530981', 'https://semopenalex.org/location/W28080081832', 'https://semopenalex.org/location/W43998794571', 'https://semopenalex.org/location/W29581194931', 'https://semopenalex.org/location/W43129933041', 'https://semopenalex.org/location/W30052490041', 'https://semopenalex.org/location/W30849226791', 'https://semopenalex.org/location/W29784152661', 'https://semopenalex.org/location/W26018933081', 'https://semopenalex.org/location/W43868591711', 'https://semopenalex.org/location/W21285198912', 'https://semopenalex.org/location/W18955604291', 'https://semopenalex.org/location/W28087319251', 'https://semopenalex.org/location/W43924539111', 'https://semopenalex.org/location/W24778492681', 'https://semopenalex.org/location/W28844284181', 'https://semopenalex.org/location/W29664832071', 'https://semopenalex.org/location/W29454079491', 'https://semopenalex.org/location/W27630405051', 'https://semopenalex.org/location/W44051774161', 'https://semopenalex.org/location/W30458346031', 'https://semopenalex.org/location/W30426697022', 'https://semopenalex.org/location/W22966118231', 'https://semopenalex.org/location/W30882384051', 'https://semopenalex.org/location/W30886117901', 'https://semopenalex.org/location/W25391549851', 'https://semopenalex.org/location/W43061604712', 'https://semopenalex.org/location/W30376855032', 'https://semopenalex.org/location/W29054320151', 'https://semopenalex.org/location/W43124462061', 'https://semopenalex.org/location/W43233386271', 'https://semopenalex.org/location/W32019820662', 'https://semopenalex.org/location/W32083490971', 'https://semopenalex.org/location/W43882799971', 'https://semopenalex.org/location/W19231700931', 'https://semopenalex.org/location/W29951453521', 'https://semopenalex.org/location/W30426697023', 'https://semopenalex.org/location/W30955984631', 'https://semopenalex.org/location/W30948193222', 'https://semopenalex.org/location/W30497024891', 'https://semopenalex.org/location/W43791159661', 'https://semopenalex.org/location/W43068956173', 'https://semopenalex.org/location/W18774675621', 'https://semopenalex.org/location/W43870462191', 'https://semopenalex.org/location/W22261468281', 'https://semopenalex.org/location/W30915935821', 'https://semopenalex.org/location/W43046919621', 'https://semopenalex.org/location/W30885348461', 'https://semopenalex.org/location/W43870462192', 'https://semopenalex.org/location/W27396165181', 'https://semopenalex.org/location/W28970790371', 'https://semopenalex.org/location/W29649262091', 'https://semopenalex.org/location/W31900260261', 'https://semopenalex.org/location/W21311253521', 'https://semopenalex.org/location/W43068956177', 'https://semopenalex.org/location/W31656678471', 'https://semopenalex.org/location/W22190572501', 'https://semopenalex.org/location/W30127488011', 'https://semopenalex.org/location/W43068956171', 'https://semopenalex.org/location/W6149025581', 'https://semopenalex.org/location/W32174702571', 'https://semopenalex.org/location/W43061604711', 'https://semopenalex.org/location/W30345383281', 'https://semopenalex.org/location/W28832165761', 'https://semopenalex.org/location/W15068103471', 'https://semopenalex.org/location/W30948193225', 'https://semopenalex.org/location/W21285198913', 'https://semopenalex.org/location/W42000397651', 'https://semopenalex.org/location/W28060387991', 'https://semopenalex.org/location/W32072432981', 'https://semopenalex.org/location/W31871691351', 'https://semopenalex.org/location/W1079679441', 'https://semopenalex.org/location/W24669668731', 'https://semopenalex.org/location/W29781601891', 'https://semopenalex.org/location/W29566225572', 'https://semopenalex.org/location/W18770595181', 'https://semopenalex.org/location/W25077834181', 'https://semopenalex.org/location/W43068956172', 'https://semopenalex.org/location/W42383839001', 'https://semopenalex.org/location/W42210492031', 'https://semopenalex.org/location/W31006266141', 'https://semopenalex.org/location/W14838732894', 'https://semopenalex.org/location/W42209538491', 'https://semopenalex.org/location/W2926427961', 'https://semopenalex.org/location/W25842933981', 'https://semopenalex.org/location/W42932502961', 'https://semopenalex.org/location/W31628635341', 'https://semopenalex.org/location/W43833402031', 'https://semopenalex.org/location/W23977394001', 'https://semopenalex.org/location/W21660939901', 'https://semopenalex.org/location/W19698391981', 'https://semopenalex.org/location/W43829818881', 'https://semopenalex.org/location/W27920797361', 'https://semopenalex.org/location/W42262443241', 'https://semopenalex.org/location/W30032445502', 'https://semopenalex.org/location/W30801908571', 'https://semopenalex.org/location/W21285198914', 'https://semopenalex.org/location/W27703789261', 'https://semopenalex.org/location/W32147435071', 'https://semopenalex.org/location/W30950014991', 'https://semopenalex.org/location/W42051370691', 'https://semopenalex.org/location/W30455098671', 'https://semopenalex.org/location/W26115059681', 'https://semopenalex.org/location/W44050344991', 'https://semopenalex.org/location/W43063173041', 'https://semopenalex.org/location/W30376855031', 'https://semopenalex.org/location/W25193597391', 'https://semopenalex.org/location/W29946198511', 'https://semopenalex.org/location/W22938731501', 'https://semopenalex.org/location/W29414042091', 'https://semopenalex.org/location/W29888192761', 'https://semopenalex.org/location/W32107593731', 'https://semopenalex.org/location/W30888177051', 'https://semopenalex.org/location/W43061604713', 'https://semopenalex.org/location/W21034674991', 'https://semopenalex.org/location/W30052490043', 'https://semopenalex.org/location/W28837227301', 'https://semopenalex.org/location/W28884399821', 'https://semopenalex.org/location/W27654696761', 'https://semopenalex.org/location/W31656415441', 'https://semopenalex.org/location/W27956841612', 'https://semopenalex.org/location/W31471774571', 'https://semopenalex.org/location/W42474583511', 'https://semopenalex.org/location/W25862769561', 'https://semopenalex.org/location/W14838732892', 'https://semopenalex.org/location/W29859817821', 'https://semopenalex.org/location/W43823653861', 'https://semopenalex.org/location/W43061604714', 'https://semopenalex.org/location/W44068802951', 'https://semopenalex.org/location/W30948193224', 'https://semopenalex.org/location/W15375095501', 'https://semopenalex.org/location/W27487378811', 'https://semopenalex.org/location/W30401575511', 'https://semopenalex.org/location/W20243484451', 'https://semopenalex.org/location/W21285198911', 'https://semopenalex.org/location/W22966755681', 'https://semopenalex.org/location/W21902780251', 'https://semopenalex.org/location/W31749439391', 'https://semopenalex.org/location/W27555683841', 'https://semopenalex.org/location/W31803441821', 'https://semopenalex.org/location/W42833253261', 'https://semopenalex.org/location/W43063169091', 'https://semopenalex.org/location/W30919516801', 'https://semopenalex.org/location/W30365122661', 'https://semopenalex.org/location/W29640826022', 'https://semopenalex.org/location/W44068680961', 'https://semopenalex.org/location/W28000505381', 'https://semopenalex.org/location/W14838732893', 'https://semopenalex.org/location/W29131890991', 'https://semopenalex.org/location/W42261851681', 'https://semopenalex.org/location/W43829818882', 'https://semopenalex.org/location/W25986997551', 'https://semopenalex.org/location/W43887990102', 'https://semopenalex.org/location/W28959508741', 'https://semopenalex.org/location/W28967664061', 'https://semopenalex.org/location/W43068956174', 'https://semopenalex.org/location/W29315761321', 'https://semopenalex.org/location/W32147435072', 'https://semopenalex.org/location/W29421075031', 'https://semopenalex.org/location/W22786769011', 'https://semopenalex.org/location/W43861592451', 'https://semopenalex.org/location/W43068956175', 'https://semopenalex.org/location/W27530325001', 'https://semopenalex.org/location/W43902058871', 'https://semopenalex.org/location/W29916244791', 'https://semopenalex.org/location/W21429592102', 'https://semopenalex.org/location/W30426697021', 'https://semopenalex.org/location/W43926169801', 'https://semopenalex.org/location/W21429592103', 'https://semopenalex.org/location/W30827033561', 'https://semopenalex.org/location/W23912393001', 'https://semopenalex.org/location/W42856043091', 'https://semopenalex.org/location/W27940330211', 'https://semopenalex.org/location/W43105296071', 'https://semopenalex.org/location/W27862507821', 'https://semopenalex.org/location/W29640826021', 'https://semopenalex.org/location/W18172888851', 'https://semopenalex.org/location/W27956841611', 'https://semopenalex.org/location/W25305687641', 'https://semopenalex.org/location/W31515741391', 'https://semopenalex.org/location/W32088965581', 'https://semopenalex.org/location/W30044603271', 'https://semopenalex.org/location/W42930562941', 'https://semopenalex.org/location/W7665864621', 'https://semopenalex.org/location/W15969306701', 'https://semopenalex.org/location/W31452592371', 'https://semopenalex.org/location/W14838732891', 'https://semopenalex.org/location/W42909435511', 'https://semopenalex.org/location/W29511010961', 'https://semopenalex.org/location/W20222792351', 'https://semopenalex.org/location/W32135727241', 'https://semopenalex.org/location/W29843174051', 'https://semopenalex.org/location/W12015545801', 'https://semopenalex.org/location/W44052325641', 'https://semopenalex.org/location/W42265388351', 'https://semopenalex.org/location/W25627600741', 'https://semopenalex.org/location/W32163023621', 'https://semopenalex.org/location/W30948193221', 'https://semopenalex.org/location/W30956804081', 'https://semopenalex.org/location/W43211235011', 'https://semopenalex.org/location/W43811573001', 'https://semopenalex.org/location/W29468737141', 'https://semopenalex.org/location/W42312112621', 'https://semopenalex.org/location/W23999023701', 'https://semopenalex.org/location/W31656415442', 'https://semopenalex.org/location/W29000605871', 'https://semopenalex.org/location/W26115059682', 'https://semopenalex.org/location/W24710522091', 'https://semopenalex.org/location/W42309685121', 'https://semopenalex.org/location/W30891714731', 'https://semopenalex.org/location/W43068956176', 'https://semopenalex.org/location/W29655391521', 'https://semopenalex.org/location/W30455856361', 'https://semopenalex.org/location/W44035980142', 'https://semopenalex.org/location/W22435911181', 'https://semopenalex.org/location/W30052490042', 'https://semopenalex.org/location/W31033840591', 'https://semopenalex.org/location/W29421282431', 'https://semopenalex.org/location/W44027636231', 'https://semopenalex.org/location/W44009098861', 'https://semopenalex.org/location/W43854027001', 'https://semopenalex.org/location/W28078943081', 'https://semopenalex.org/location/W43931850291', 'https://semopenalex.org/location/W29946198512', 'https://semopenalex.org/location/W25305687642', 'https://semopenalex.org/location/W32019820661', 'https://semopenalex.org/location/W42059472451', 'https://semopenalex.org/location/W21263891551', 'https://semopenalex.org/location/W43855562551', 'https://semopenalex.org/location/W22465567601', 'https://semopenalex.org/location/W43856175291', 'https://semopenalex.org/location/W21429592101', 'https://semopenalex.org/location/W44035165841', 'https://semopenalex.org/location/W30897530231', 'https://semopenalex.org/location/W44035980141', 'https://semopenalex.org/location/W26266951001', 'https://semopenalex.org/location/W31656415443']</t>
-  </si>
-  <si>
-    <t>['Learning to Mine Chinese Coordinate Terms Using the Web', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering Task-Specific Styles', 'https://semopenalex.org/location/W27403899911', 'https://semopenalex.org/location/W15005290131', 'Adapting Neural Single-Document Summarization Model for Abstractive Multi-Document Summarization: A Pilot Study', 'https://semopenalex.org/location/W18552684821', 'https://semopenalex.org/location/W22518347582', 'Automatic Text Simplification Horacio Saggion (Universitat Pompeu Fabra) Morgan &amp; Claypool (Synthesis Lectures on Human Language Technologies, edited by Graeme Hirst, volume 37), 2017, xvi+121 pp; paperback, ISBN 978-1-62705-868-1; hardcover, ISBN 978-1-68173-214-5, $69.95; ebook, ISBN 978-1-62705-869-8, $39.96; doi: 10.2200/S00700ED1V01Y201602HLT032.', 'https://semopenalex.org/location/W43066765701', 'CTSUM', 'https://semopenalex.org/location/W29519376671', 'https://semopenalex.org/location/W43799335313', 'https://semopenalex.org/location/W43880320292', 'https://semopenalex.org/location/W22583498241', 'https://semopenalex.org/location/W31035855991', 'https://semopenalex.org/location/W43135339181', 'SentiGAN: Generating Sentimental Texts via Mixture Adversarial Networks', 'Emotion Classification in Microblog Texts Using Class Sequential Rules', 'Guiding Abstractive Dialogue Summarization with Content Planning', 'https://semopenalex.org/location/W42257837861', 'https://semopenalex.org/location/W19812568681', 'https://semopenalex.org/location/W29787076431', 'Exploring Context-Aware Evaluation Metrics for Machine Translation', 'https://semopenalex.org/location/W27841870711', 'https://semopenalex.org/location/W29630087173', 'Structure-Aware Pre-Training for Table-to-Text Generation', 'https://semopenalex.org/location/W22514277781', 'How to Avoid Sentences Spelling Boring? Towards a Neural Approach to Unsupervised Metaphor Generation', 'https://semopenalex.org/location/W31678084401', 'Neural Comment Generation for Source Code with Auxiliary Code Classification Task', 'https://semopenalex.org/location/W43996953271', 'Language Generation via DAG Transduction', 'https://semopenalex.org/location/W30342096831', 'https://semopenalex.org/location/W21139822041', 'https://semopenalex.org/location/W43098001052', 'https://semopenalex.org/location/W31006826081', 'Semantic Parsing for English as a Second Language', 'https://semopenalex.org/location/W44001047881', 'https://semopenalex.org/location/W32137654603', 'https://semopenalex.org/location/W29467259331', 'https://semopenalex.org/location/W42261619782', 'https://semopenalex.org/location/W31339193871', 'https://semopenalex.org/location/W44010431252', 'Using only cross-document relationships for both generic and topic-focused multi-document summarizations', 'https://semopenalex.org/location/W15387621891', 'https://semopenalex.org/location/W43931470201', 'On the Helpfulness of Document Context to Sentence Simplification', 'https://semopenalex.org/location/W43948670321', 'Combining Content and Context Similarities for Image Retrieval', 'https://semopenalex.org/location/W19216503161', 'A Comprehensive Evaluation of Constrained Text Generation for Large Language Models', 'Benchmarking Knowledge Boundary for Large Language Model: A Different  Perspective on Model Evaluation', 'TransModality: An End2End Fusion Method with Transformer for Multimodal Sentiment Analysis', 'https://semopenalex.org/location/W20482038031', 'https://semopenalex.org/location/W30431573301', 'https://semopenalex.org/location/W43068023851', 'Peking: Profiling Syntactic Tree Parsing Techniques for Semantic Graph Parsing', 'https://semopenalex.org/location/W15429908791', 'https://semopenalex.org/location/W30879979901', 'https://semopenalex.org/location/W43879295152', 'Towards a unified approach to document similarity search using manifold-ranking of blocks', 'https://semopenalex.org/location/W20360909521', 'Learning to Identify Ambiguous and Misleading News Headlines', 'Towards Document-Level Paraphrase Generation with Sentence Rewriting and Reordering', 'https://semopenalex.org/location/W42964147592', 'https://semopenalex.org/location/W22506227611', "The earth mover's distance as a semantic measure for document similarity", 'https://semopenalex.org/location/W43879637561', 'Multi-Granularity Interaction Network for Extractive and Abstractive Multi-Document Summarization', 'A New Retrieval Model Based on TextTiling for Document Similarity Search', 'MC-MKE: A Fine-Grained Multimodal Knowledge Editing Benchmark  Emphasizing Modality Consistency', 'A Semi-Supervised Approach for Low-Resourced Text Generation', 'https://semopenalex.org/location/W43924876941', 'https://semopenalex.org/location/W43879295153', 'Co-training for cross-lingual sentiment classification', 'https://semopenalex.org/location/W42883367673', 'https://semopenalex.org/location/W31531285151', 'Using bilingual knowledge and ensemble techniques for unsupervised Chinese sentiment analysis', 'https://semopenalex.org/location/W42869677632', 'https://semopenalex.org/location/W43068023853', 'Creative Destruction: Can Language Models Interpret Oxymorons?', 'https://semopenalex.org/location/W43626796312', 'Exploiting syntactic and semantic relationships between terms for opinion retrieval', 'https://semopenalex.org/location/W25115328441', 'Towards Automatic Construction of News Overview Articles by News Synthesis', 'https://semopenalex.org/location/W44042613631', 'https://semopenalex.org/location/W42261619781', 'Cross-language document summarization via extraction and ranking of multiple summaries', 'https://semopenalex.org/location/W21326438521', 'https://semopenalex.org/location/W28991688921', 'https://semopenalex.org/location/W19680356881', 'https://semopenalex.org/location/W29551932721', 'https://semopenalex.org/location/W28783543041', 'A Comparative Analysis of Knowledge-Intensive and Data-Intensive Semantic Parsers', 'https://semopenalex.org/location/W15491340771', 'https://semopenalex.org/location/W19947926601', 'https://semopenalex.org/location/W24036730301', 'Timeline Generation through Evolutionary Trans-Temporal Summarization', 'https://semopenalex.org/location/W42878546701', 'https://semopenalex.org/location/W29630087171', 'CollabRank', 'How Do Seq2Seq Models Perform on End-to-End Data-to-Text Generation?', 'https://semopenalex.org/location/W27951557541', 'Visualizing timelines', 'https://semopenalex.org/location/W43068023852', 'https://semopenalex.org/location/W43855708742', 'Exploiting neighborhood knowledge for single document summarization and keyphrase extraction', 'https://semopenalex.org/location/W43931470202', 'https://semopenalex.org/location/W43098001053', 'Modeling and prediction of modulus of elasticity of laminated veneer lumber based on laminated plate theory', 'https://semopenalex.org/location/W43092020843', 'AMRec: An Intelligent System for Academic Method Recommendation', 'Cross Modal Training for ASR Error Correction with Contrastive Learning', 'Overview of the NLPCC 2023 Shared Task: Chinese Spelling Check', 'Making Better Use of Bilingual Information for Cross-Lingual AMR Parsing', 'https://semopenalex.org/location/W32004422982', 'https://semopenalex.org/location/W29188060631', 'Beyond topical similarity: a structural similarity measure for retrieving highly similar documents', 'Routing Enforced Generative Model for Recipe Generation', 'Comparative News Summarization Using Linear Programming', 'https://semopenalex.org/location/W30127214842', 'Re-evaluating Automatic LLM System Ranking for Alignment with Human  Preference', 'Reducing Approximation and Estimation Errors for Chinese Lexical Processing with Heterogeneous Annotations', 'Collective Opinion Target Extraction in Chinese Microblogs', 'Abstractive Multi-Document Summarization via Joint Learning with Single-Document Summarization', 'https://semopenalex.org/location/W29473148431', 'https://semopenalex.org/location/W31678084402', 'Data-driven, PCFG-based and Pseudo-PCFG-based Models for Chinese Dependency Parsing', 'Automatic Slides Generation for Scholarly Papers: A Fine-Grained Dataset and Baselines (Student Abstract)', 'https://semopenalex.org/location/W20713320641', 'Learning information diffusion process on the web', 'Defining and Detecting Vulnerability in Human Evaluation Guidelines: A  Preliminary Study Towards Reliable NLG Evaluation', 'CMiner: Opinion Extraction and Summarization for Chinese Microblogs', 'https://semopenalex.org/location/W42211412062', 'Compressive document summarization via sparse optimization', 'https://semopenalex.org/location/W31065300841', 'https://semopenalex.org/location/W42261972351', 'https://semopenalex.org/location/W29174748341', 'Is Summary Useful or Not? An Extrinsic Human Evaluation of Text Summaries on Downstream Tasks', 'CUGE: A Chinese Language Understanding and Generation Evaluation Benchmark', 'https://semopenalex.org/location/W43801365211', 'https://semopenalex.org/location/W44060317991', 'https://semopenalex.org/location/W31227944381', 'https://semopenalex.org/location/W29740710332', 'https://semopenalex.org/location/W31607062801', 'https://semopenalex.org/location/W42837839231', 'https://semopenalex.org/location/W42260991373', 'ATSUM: Extracting Attractive Summaries for News Propagation on Microblogs', 'https://semopenalex.org/location/W31678084403', 'https://semopenalex.org/location/W43875611321', 'Proceedings of the 16th Conference of the European Chapter of the Association for Computational Linguistics: Main Volume', 'https://semopenalex.org/location/W42964147593', 'Towards a Universal Sentiment Classifier in Multiple languages', 'PPSGen: Learning-Based Presentation Slides Generation for Academic Papers', 'https://semopenalex.org/location/W28991688922', 'https://semopenalex.org/location/W31636541681', 'https://semopenalex.org/location/W21484376701', 'https://semopenalex.org/location/W32138258993', "x-index: a fantastic new indicator for quantifying a scientist's scientific impact", 'https://semopenalex.org/location/W21047664061', 'Evolutionary timeline summarization', 'https://semopenalex.org/location/W29308733261', 'https://semopenalex.org/location/W42882874651', 'https://semopenalex.org/location/W20088401231', 'https://semopenalex.org/location/W19738942781', 'https://semopenalex.org/location/W20527844861', 'https://semopenalex.org/location/W15483875481', 'Chinese Spelling Check with Nearest Neighbors', 'Homophonic Pun Generation with Lexically Constrained Rewriting', 'Multi-Modal Sarcasm Detection in Twitter with Hierarchical Fusion Model', 'Bilingual Co-Training for Sentiment Classification of Chinese Product Reviews', 'Automatic Generation of Citation Texts in Scholarly Papers: A Pilot Study', 'https://semopenalex.org/location/W27665803442', 'Abstractive Document Summarization with a Graph-Based Attentional Neural Model', 'CollabSum', 'https://semopenalex.org/location/W21415147001', 'Comparing Knowledge-Intensive and Data-Intensive Models for English Resource Semantic Parsing', 'Neural Review Summarization Leveraging User and Product Information', 'https://semopenalex.org/location/W31770344581', 'https://semopenalex.org/location/W27591811581', 'Single document summarization with document expansion', 'https://semopenalex.org/location/W43818268362', 'https://semopenalex.org/location/W31764380051', 'Cross-language context-aware citation recommendation in scientific articles', 'https://semopenalex.org/location/W42883367672', 'https://semopenalex.org/location/W27983034381', 'https://semopenalex.org/location/W4026736721', 'A New Dataset and Empirical Study for Sentence Simplification in Chinese', 'https://semopenalex.org/location/W43233667202', 'https://semopenalex.org/location/W32002855302', 'https://semopenalex.org/location/W31848521943', 'Adversarial Text Generation via Sequence Contrast Discrimination', 'https://semopenalex.org/location/W44001048571', 'Proceedings of the 61st Annual Meeting of the Association for Computational Linguistics (Volume 1: Long Papers)', 'https://semopenalex.org/location/W27414383491', 'https://semopenalex.org/location/W43778643421', 'https://semopenalex.org/location/W43895194311', 'Proceedings of the 61st Annual Meeting of the Association for Computational Linguistics (Volume 2: Short Papers)', 'Improved affinity graph based multi-document summarization', 'Parsing for Grammatical Relations via Graph Merging', 'https://semopenalex.org/location/W42261972353', 'https://semopenalex.org/location/W29740710331', 'TimedTextRank', 'Are all literature citations equally important? Automatic citation strength estimation and its applications', 'Cross-Language Document Summarization Based on Machine Translation Quality Prediction', 'https://semopenalex.org/location/W29709013301', 'Towards Automatic Generation of Product Reviews from Aspect-Sentiment Scores', 'https://semopenalex.org/location/W30347733621', 'Revisiting Pivot-Based Paraphrase Generation: Language Is Not the Only Optional Pivot', 'https://semopenalex.org/location/W42455043961', 'https://semopenalex.org/location/W43865668651', 'Hierarchical Attention Networks for Sentence Ordering', 'AKMiner: Domain-Specific Knowledge Graph Mining from Academic Literatures', 'https://semopenalex.org/location/W31747592142', 'https://semopenalex.org/location/W29640107141', 'Phrase-Based Presentation Slides Generation for Academic Papers', 'https://semopenalex.org/location/W42264767653', 'Recent advances of neural text generation: Core tasks, datasets, models and challenges', 'Automated Similarity Metric Generation for Recommendation', 'https://semopenalex.org/location/W42883741952', 'https://semopenalex.org/location/W42242380072', 'https://semopenalex.org/location/W32114636873', 'https://semopenalex.org/location/W43799335311', 'An Empirical Study of Automatic Post-Editing', 'https://semopenalex.org/location/W43855720261', 'Content Selection for Real-time Sports News Construction from Commentary Texts', 'https://semopenalex.org/location/W29063600401', 'How to Describe Images in a More Funny Way? Towards a Modular Approach to Cross-Modal Sarcasm Generation', 'https://semopenalex.org/location/W22699315982', 'https://semopenalex.org/location/W43874269331', 'https://semopenalex.org/location/W22755689011', 'https://semopenalex.org/location/W25352648551', 'ContraSolver: Self-Alignment of Language Models by Resolving Internal  Preference Contradictions', 'ALCUNA: Large Language Models Meet New Knowledge', 'https://semopenalex.org/location/W44047828401', 'https://semopenalex.org/location/W32085278861', 'Clinical challenges and management of primary renal epithelioid angiomyolipoma of duplex kidney with paraneoplastic syndrome', 'Extract Salient Words with WordRank for Effective Similarity Search in Text Data', 'Deep Dependency Substructure-Based Learning for Multidocument Summarization', 'https://semopenalex.org/location/W31032919082', 'https://semopenalex.org/location/W31022446661', 'https://semopenalex.org/location/W43855706662', 'https://semopenalex.org/location/W30345604441', 'https://semopenalex.org/location/W21155302631', 'Neural Text Generation with Part-of-Speech Guided Softmax.', 'https://semopenalex.org/location/W29894899231', 'Towards a Unified Approach Based on Affinity Graph to Various Multi-document Summarizations', 'MIL-Decoding: Detoxifying Language Models at Token-Level via Multiple Instance Learning', 'https://semopenalex.org/location/W20456506511', 'PaCoST: Paired Confidence Significance Testing for Benchmark Contamination Detection in Large Language Models', 'https://semopenalex.org/location/W43919879821', 'INS: An Interactive Chinese News Synthesis System', 'Block-Based Similarity Search on the Web Using Manifold-Ranking', 'Recent advances in document summarization', 'Jointly Learning to Align and Summarize for Neural Cross-Lingual Summarization', 'https://semopenalex.org/location/W43683042411', 'https://semopenalex.org/location/W32130735992', 'Human-like Summarization Evaluation with ChatGPT', 'A Comparative Study of Cross-Lingual Sentiment Classification', 'The Impact of Family Care on the Subjective Well-Being of the Elderly: The Mediation Role of General Self-Efficacy and Psychological Resilience', 'https://semopenalex.org/location/W42883367671', 'https://semopenalex.org/location/W43066765703', 'Reference Matters: Benchmarking Factual Error Correction for Dialogue Summarization with Fine-grained Evaluation Framework', 'https://semopenalex.org/location/W32125749961', 'https://semopenalex.org/location/W42264767651', 'https://semopenalex.org/location/W43855713641', 'Cross-Language Opinion Target Extraction in Review Texts', 'https://semopenalex.org/location/W26044438831', 'https://semopenalex.org/location/W43859761071', 'https://semopenalex.org/location/W43855713642', 'SRRank: Leveraging Semantic Roles for Extractive Multi-Document Summarization', 'RST Discourse Parsing as Text-to-Text Generation', 'https://semopenalex.org/location/W31032919081', 'New Datasets and Controllable Iterative Data Augmentation Method for Code-switching ASR Error Correction', 'Towards Constructing Sports News from Live Text Commentary', 'Microscale and macroscale strength behaviors of blast furnace slag- cement based materials: Modeling and analysis', 'Graph-Based Multi-Modality Learning for Clinical Decision Support', 'https://semopenalex.org/location/W43063531621', 'https://semopenalex.org/location/W29521434101', 'https://semopenalex.org/location/W29517811212', 'Generating Diverse and Descriptive Image Captions Using Visual Paraphrases', 'https://semopenalex.org/location/W43683042412', 'https://semopenalex.org/location/W21288155201', 'DelibGAN: Coarse-to-Fine Text Generation via Adversarial Network', 'https://semopenalex.org/location/W21399281001', 'https://semopenalex.org/location/W31333763863', 'https://semopenalex.org/location/W31037018011', 'Mining and Analyzing the Future Works in Scientific Articles', 'https://semopenalex.org/location/W42882874653', 'https://semopenalex.org/location/W25128623461', 'Models See Hallucinations: Evaluating the Factuality in Video Captioning', 'Document-Level Text Simplification: Dataset, Criteria and Baseline', 'https://semopenalex.org/location/W44026719651', 'Visual Question Generation Under Multi-granularity Cross-Modal Interaction', 'https://semopenalex.org/location/W21129248451', 'https://semopenalex.org/location/W30984117501', 'https://semopenalex.org/location/W42976309841', 'Summarizing the differences in multilingual news', 'Multi-Document Summarization via Discriminative Summary Reranking', 'https://semopenalex.org/location/W42837164641', 'Sense-Aware Neural Models for Pun Location in Texts', 'https://semopenalex.org/location/W29079361231', 'https://semopenalex.org/location/W42883368241', 'https://semopenalex.org/location/W30984117503', 'https://semopenalex.org/location/W30342392641', 'https://semopenalex.org/location/W42837164643', 'https://semopenalex.org/location/W43931526571', 'https://semopenalex.org/location/W22512373051', "&lt;scp&gt;WL&lt;/scp&gt;‐index: Leveraging citation mention number to quantify an individual's scientific impact", 'https://semopenalex.org/location/W29521434102', 'https://semopenalex.org/location/W21475099121', 'https://semopenalex.org/location/W31761057411', 'https://semopenalex.org/location/W8277644473', 'https://semopenalex.org/location/W43852928982', 'https://semopenalex.org/location/W19838737911', 'https://semopenalex.org/location/W42869677631', 'https://semopenalex.org/location/W20122885071', 'https://semopenalex.org/location/W43895188331', 'https://semopenalex.org/location/W25090054321', 'DeepDial: Passage Completion on Dialogs', 'Graph-based multi-modality learning for topic-focused multi-document summarization', 'https://semopenalex.org/location/W43066765702', 'User Embedding for Scholarly Microblog Recommendation', 'https://semopenalex.org/location/W27992224531', 'https://semopenalex.org/location/W30833650752', 'https://semopenalex.org/location/W16901060301', 'https://semopenalex.org/location/W43895240061', 'Hierarchical Graph Summarization: Leveraging Hybrid Information through Visible and Invisible Linkage', 'Visual Information Guided Zero-Shot Paraphrase Generation', 'Phrase-based Compressive Cross-Language Summarization', 'https://semopenalex.org/location/W19765077451', 'Automated Chess Commentator Powered by Neural Chess Engine', 'https://semopenalex.org/location/W25362389121', 'Automatic Text Simplification', 'Learning Diachronic Word Embeddings with Iterative Stable Information Alignment', 'https://semopenalex.org/location/W30034461822', 'https://semopenalex.org/location/W31990421561', 'Counterfactual Representation Augmentation for Cross-Domain Sentiment Analysis', 'Named Entity Recognition in Chinese News Comments on the Web', 'https://semopenalex.org/location/W24699317431', 'https://semopenalex.org/location/W42242380071', 'https://semopenalex.org/location/W20806564951', 'https://semopenalex.org/location/W31746799441', 'https://semopenalex.org/location/W43920119821', 'https://semopenalex.org/location/W15454762401', 'https://semopenalex.org/location/W43875596752', 'https://semopenalex.org/location/W15907088031', 'https://semopenalex.org/location/W29473148432', 'https://semopenalex.org/location/W31531285152', 'https://semopenalex.org/location/W43879637562', 'https://semopenalex.org/location/W1785624211', 'https://semopenalex.org/location/W42882874652', 'Bridging the Domain Gap: Improve Informal Language Translation via Counterfactual Domain Adaptation', 'Exploring Discourse Structure in Document-level Machine Translation', 'https://semopenalex.org/location/W43855702241', 'https://semopenalex.org/location/W25576652171', 'Multi-document Summarization Using Minimum Distortion', 'https://semopenalex.org/location/W20720502281', 'Pushing Paraphrase Away from Original Sentence: A Multi-Round Paraphrase Generation Approach', 'https://semopenalex.org/location/W27721872051', 'Joint Matrix Factorization and Manifold-Ranking for Topic-Focused Multi-Document Summarization', 'Image Matters: A New Dataset and Empirical Study for Multimodal Hyperbole Detection', 'Document Similarity Search Based on Manifold-Ranking of TextTiles', 'https://semopenalex.org/location/W21327791921', 'Harvesting Drug Effectiveness from Social Media', 'Sentiment Analysis of Peer Review Texts for Scholarly Papers', 'Multi-Domain Sentiment Classification Based on Domain-Aware Embedding and Attention', 'https://semopenalex.org/location/W27413755281', 'https://semopenalex.org/location/W43236516122', 'Towards a Unified End-to-End Approach for Fully Unsupervised Cross-Lingual Sentiment Analysis', 'https://semopenalex.org/location/W43879295151', 'The Great Importance of Cross-Document Relationships for Multi-document Summarization', 'https://semopenalex.org/location/W30127214841', 'Incorporating Cross-Document Relationships Between Sentences for Single Document Summarizations', 'https://semopenalex.org/location/W31227944383', 'https://semopenalex.org/location/W27710802441', 'https://semopenalex.org/location/W29835618061', 'https://semopenalex.org/location/W42260991371', 'https://semopenalex.org/location/W20949637751', 'https://semopenalex.org/location/W43210141361', 'https://semopenalex.org/location/W24236365061', 'Effects of Additional Ring-Fusion Site on Dual Reactivity Based Dynamic Covalent Chemistry', 'https://semopenalex.org/location/W22510249081', 'https://semopenalex.org/location/W43865668652', 'https://semopenalex.org/location/W25600575401', 'Document-Based HITS Model for Multi-document Summarization', 'T-CVAE: Transformer-Based Conditioned Variational Autoencoder for Story Completion', 'https://semopenalex.org/location/W16557712491', 'An Improved k-means Algorithm for Documents Clustering', 'https://semopenalex.org/location/W44047823791', 'https://semopenalex.org/location/W43880320291', 'Using Cross-Document Random Walks for Topic-Focused Multi-Document', 'https://semopenalex.org/location/W29631289871', 'https://semopenalex.org/location/W42133481041', 'Point Precisely: Towards Ensuring the Precision of Data in Generated Texts Using Delayed Copy Mechanism', 'A Neural Approach to Irony Generation', 'DialSummEval: Revisiting Summarization Evaluation for Dialogues', 'https://semopenalex.org/location/W23351636761', 'PKUSUMSUM : A Java Platform for Multilingual Document Summarization', 'https://semopenalex.org/location/W29872059511', 'A Neural Network Approach to Quote Recommendation in Writings', 'https://semopenalex.org/location/W22505462021', 'Named Entity Resolution in Chinese News Comments on the Web', 'https://semopenalex.org/location/W29723392302', 'Learning to Find Comparable Entities on the Web', 'https://semopenalex.org/location/W27402804981', 'https://semopenalex.org/location/W15980810811', 'https://semopenalex.org/location/W14905123281', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering  Task-Specific Styles', 'https://semopenalex.org/location/W42883368242', 'https://semopenalex.org/location/W21415620721', 'https://semopenalex.org/location/W43949732451', 'https://semopenalex.org/location/W28086033751', 'https://semopenalex.org/location/W42253888061', 'https://semopenalex.org/location/W43852928981', 'Overview of the NLPCC 2015 Shared Task: Weibo-Oriented Chinese News Summarization', 'SituatedGen: Incorporating Geographical and Temporal Contexts into Generative Commonsense Reasoning', 'WordRank-Based Lexical Signatures for Finding Lost or Related Web Pages', 'A practical system for harvesting and monitoring hot topics on the web', 'https://semopenalex.org/location/W682814491', 'BiCWS: Mining Cognitive Differences from Bilingual Web Search Results', 'https://semopenalex.org/location/W27566762001', 'Learning to Recommend Quotes for Writing', 'https://semopenalex.org/location/W49460081', 'Multi-document summarization using cluster-based link analysis', 'https://semopenalex.org/location/W31746000991', 'Evaluating Self-Generated Documents for Enhancing Retrieval-Augmented  Generation with Large Language Models', 'https://semopenalex.org/location/W43875611323', 'https://semopenalex.org/location/W32130735991', 'A New Benchmark and Reverse Validation Method for Passage-level Hallucination Detection', 'https://semopenalex.org/location/W43924266211', 'https://semopenalex.org/location/W43895204022', 'Evaluating Factuality in Cross-lingual Summarization', 'https://semopenalex.org/location/W20837783641', 'https://semopenalex.org/location/W29631289872', 'https://semopenalex.org/location/W32125749963', 'https://semopenalex.org/location/W15021839891', 'Semantic Dependency Parsing via Book Embedding', 'Joint Decoding of Tree Transduction Models for Sentence Compression', 'https://semopenalex.org/location/W43626796313', 'https://semopenalex.org/location/W20827587511', 'History Matters: Temporal Knowledge Editing in Large Language Model', 'https://semopenalex.org/location/W31848521942', 'Diversifying Neural Text Generation with Part-of-Speech Guided Softmax and Sampling', 'https://semopenalex.org/location/W32136239431', 'https://semopenalex.org/location/W31055268741', 'https://semopenalex.org/location/W27990449701', 'https://semopenalex.org/location/W25624397971', 'https://semopenalex.org/location/W19667458141', 'https://semopenalex.org/location/W29790296041', 'https://semopenalex.org/location/W43831757962', 'Evaluating and Mitigating Number Hallucinations in Large Vision-Language  Models: A Consistency Perspective', 'https://semopenalex.org/location/W42838066501', 'https://semopenalex.org/location/W44055623831', 'IGSQL: Database Schema Interaction Graph Based Neural Model for Context-Dependent Text-to-SQL Generation', 'Cross-Lingual Sentiment Classification with Bilingual Document Representation Learning', 'https://semopenalex.org/location/W43626796311', 'https://semopenalex.org/location/W43925385321', 'https://semopenalex.org/location/W8277644471', 'https://semopenalex.org/location/W21676608641', 'Single document keyphrase extraction using neighborhood knowledge', 'https://semopenalex.org/location/W1014155901', 'Towards a Neural Network Approach to Abstractive Multi-Document Summarization', 'WIND: Weighting Instances Differentially for Model-Agnostic Domain Adaptation', 'https://semopenalex.org/location/W43799335312', 'CRF-based Experiments for Cross-Domain Chinese Word Segmentation at CIPS-SIGHAN-2010', 'https://semopenalex.org/location/W42837164642', 'Asking the Crowd: Question Analysis, Evaluation and Generation for Open Discussion on Online Forums', 'https://semopenalex.org/location/W23572746651', 'A Measure Based on Optimal Matching in Graph Theory for Document Similarity', 'Document Similarity Search Based on Generic Summaries', 'https://semopenalex.org/location/W43855708741', 'https://semopenalex.org/location/W27986003981', 'https://semopenalex.org/location/W25577493911', 'https://semopenalex.org/location/W31333763861', 'https://semopenalex.org/location/W16226003861', 'https://semopenalex.org/location/W30352029331', 'https://semopenalex.org/location/W29533315241', 'https://semopenalex.org/location/W20742767501', 'https://semopenalex.org/location/W44047807402', 'https://semopenalex.org/location/W44010431251', 'https://semopenalex.org/location/W28961243511', 'https://semopenalex.org/location/W22505462022', 'A Simple Information-Based Approach to Unsupervised Domain-Adaptive Aspect-Based Sentiment Analysis', 'https://semopenalex.org/location/W43855723241', 'https://semopenalex.org/location/W43063531622', 'A Neural Approach to Pun Generation', 'A Data-Driven, Factorization Parser for CCG Dependency Structures', 'Interactive Multi-Grained Joint Model for Targeted Sentiment Analysis', 'Findings of the Association for Computational Linguistics: ACL 2023', 'https://semopenalex.org/location/W322535301', 'Automatic Text Simplification&lt;i&gt;Horacio Saggion&lt;/i&gt; (Universitat Pompeu Fabra) Morgan &amp;amp; Claypool (Synthesis Lectures on Human Language Technologies, edited by Graeme Hirst, volume 37), 2017, xvi+121 pp; paperback, ISBN 978-1-62705-868-1; ebook, ISBN 978-1-62705-869-8; doi:10.2200/S00700ED1V01Y201602HLT032', 'https://semopenalex.org/location/W43895188332', 'PKUTM participation at TAC 2011 Summarization Track.', 'https://semopenalex.org/location/W1038438251', 'https://semopenalex.org/location/W22947499631', 'Missing Information, Unresponsive Authors, Experimental Flaws: The Impossibility of Assessing the Reproducibility of Previous Human Evaluations in NLP', 'https://semopenalex.org/location/W43916023241', 'https://semopenalex.org/location/W32002855301', 'https://semopenalex.org/location/W28864741021', 'https://semopenalex.org/location/W43092020842', 'Controllable Unsupervised Text Attribute Transfer via Editing Entangled Latent Representation', 'https://semopenalex.org/location/W29985189891', 'S2ORM', 'BAB-QA: A New Neural Model for Emotion Detection in Multi-party Dialogue', 'https://semopenalex.org/location/W43210141363', 'https://semopenalex.org/location/W42883368243', 'Learning Bilingual Embedding Model for Cross-Language Sentiment Classification', 'Multimodal Transformer for Multimodal Machine Translation', 'https://semopenalex.org/location/W31747592141', 'https://semopenalex.org/location/W32114636871', 'https://semopenalex.org/location/W44035793721', 'https://semopenalex.org/location/W43617566021', 'PaCoST: Paired Confidence Significance Testing for Benchmark  Contamination Detection in Large Language Models', 'https://semopenalex.org/location/W530687281', 'https://semopenalex.org/location/W28887876782', 'https://semopenalex.org/location/W42211412063', 'https://semopenalex.org/location/W21210801631', 'Improving Grammatical Error Correction with Data Augmentation by Editing Latent Representation', 'https://semopenalex.org/location/W42253888062', 'https://semopenalex.org/location/W24246716131', 'https://semopenalex.org/location/W28887876781', 'https://semopenalex.org/location/W31751954631', 'Domain-Adaptive Neural Automated Essay Scoring', 'Automatic Generation of Related Work Sections in Scientific Papers: An Optimization Approach', 'Heterogeneous Graph Transformer for Graph-to-Sequence Learning', 'PosterBot: A System for Generating Posters of Scientific Papers with Neural Models', 'DivGAN: Towards Diverse Paraphrase Generation via Diversified Generative Adversarial Network', 'Overview of the NLPCC 2018 Shared Task: Grammatical Error Correction', 'https://semopenalex.org/location/W27665803441', 'ParaSCI: A Large Scientific Paraphrase Dataset for Longer Paraphrase Generation', 'BrailleSUM: A News Summarization System for the Blind and Visually Impaired People', 'https://semopenalex.org/location/W28871614501', 'https://semopenalex.org/location/W8277644472', 'A New Re-ranking Metho</t>
-  </si>
-  <si>
-    <t>['Glacier Monitoring Using Frequency Domain Offset Tracking Applied to Sentinel-1 Images: A Product Performance Comparison', 'https://semopenalex.org/location/W29127815873', 'A Novel Tool for Unsupervised Flood Mapping Using Sentinel-1 Images', 'https://semopenalex.org/location/W43877636401', 'Correlation of the Fields Scattered by a Fractal Surface at Two Closely Spaced Receivers', 'https://semopenalex.org/location/W42069686492', 'https://semopenalex.org/location/W42878909881', 'https://semopenalex.org/location/W31848768412', 'https://semopenalex.org/location/W44022614201', 'A comparative sensitivity analysis of scattering-based despeckling algorithms', 'https://semopenalex.org/location/W29881205341', 'https://semopenalex.org/location/W31993907601', 'https://semopenalex.org/location/W29282537721', 'https://semopenalex.org/location/W42052019421', 'Feature Extraction From Multitemporal SAR Images Using Selforganizing Map Clustering and Object-Based Image Analysis', 'Multitemporal synthetic aperture radar for urban planning and critical infrastructure monitoring', 'Closed-Form Anisotropic Polarimetric Two-Scale Model for Fast Evaluation of Sea Surface Backscattering', 'Small Reservoirs Extraction in Semiarid Regions Using Multitemporal Synthetic Aperture Radar Images', 'https://semopenalex.org/location/W43878030641', 'https://semopenalex.org/location/W28914311983', 'Scattering Along the Specular Direction from the Sea Modeled as a Fractal Surface', 'Using GEOBIA for feature extraction from multitemporal SAR images: Preliminary results', 'Maritime Surveillance Using Spaceborne GNSS-Reflectometry: The Role of the Scattering Configuration and Receiving Polarization Channel', 'https://semopenalex.org/location/W27660924161', 'Bistatic Scattering From Anisotropic Rough Surfaces via a Closed-Form Two-Scale Model', 'Formation-Flying SAR Receivers in Far-From-Transmitter Geometry: Signal Model and Processing Scheme', 'https://semopenalex.org/location/W44022604271', 'Coprime synthetic aperture radars', 'https://semopenalex.org/location/W44022629541', 'Sensitivity analysis of a scattering-based nonlocal means Despeckling Algorithm', 'https://semopenalex.org/location/W32072007311', 'https://semopenalex.org/location/W31848768411', 'https://semopenalex.org/location/W43878017851', 'https://semopenalex.org/location/W29561442231', 'https://semopenalex.org/location/W27762611981', 'https://semopenalex.org/location/W29018988831', 'https://semopenalex.org/location/W29488924392', 'https://semopenalex.org/location/W29488924393', 'https://semopenalex.org/location/W29127815871', 'https://semopenalex.org/location/W25885227232', 'https://semopenalex.org/location/W43862079901', 'Baseline Decorrelation in Bistatic Interferometric SAR Systems Over Bare Soil Surfaces', 'https://semopenalex.org/location/W43878017971', 'Acquisition modes', 'Simulation of GNSS-R Signals in Arbitrary Viewing Geometry with a Closed-Form Bistatic Two-Scale Model', 'https://semopenalex.org/location/W44022614261', 'https://semopenalex.org/location/W27563590741', 'https://semopenalex.org/location/W32115469181', 'https://semopenalex.org/location/W43906783971', 'Time-Domain and Monostatic-like Frequency-Domain Methods for Bistatic SAR Simulation', 'https://semopenalex.org/location/W43917597611', 'https://semopenalex.org/location/W42069686491', 'Electromagnetic Scattering from Fractional Brownian Motion Surfaces via the Small Slope Approximation', 'https://semopenalex.org/location/W43129684911', 'https://semopenalex.org/location/W28855740753', 'Pol-SARAS: A Fully Polarimetric SAR Raw Signal Simulator for Extended Soil Surfaces', 'Integrated Infrastructure Monitoring Procedure for Road Network Management', 'https://semopenalex.org/location/W43878728991', 'Unsupervised Rapid Flood Mapping Using Sentinel-1 GRD SAR Images', 'Polarimetric Two-Scale Model for the Evaluation of Bistatic Scattering from Anisotropic Sea Surfaces', 'Ambiguity problems and their mitigation', 'A new convenient tool for ice sheets exploration the fractal dimension', 'https://semopenalex.org/location/W43225028851', 'https://semopenalex.org/location/W26095320801', 'Introduction', 'https://semopenalex.org/location/W31325075201', 'A fully convolutional neural network for low-complexity single-stage ship detection in Sentinel-1 SAR images', 'Addressing ices in the solar system via their fractal dimension measurement', 'https://semopenalex.org/location/W29488924391', 'An Analytical Formulation for the Correlation of Surface-Scattered Fields at Two Bistatic Radar Receivers', 'https://semopenalex.org/location/W27762611982', 'https://semopenalex.org/location/W31848768413', 'https://semopenalex.org/location/W25885227231', 'https://semopenalex.org/location/W43917537921', 'https://semopenalex.org/location/W27553009891', 'Coprime Synthetic Aperture Radar: State of the Art and Application to Ship Detection', 'https://semopenalex.org/location/W27908694951', 'https://semopenalex.org/location/W27747519831', 'https://semopenalex.org/location/W28914311981', 'Urban Area Mapping Using Multitemporal SAR Images in Combination with Self-Organizing Map Clustering and Object-Based Image Analysis', 'https://semopenalex.org/location/W31128765681', 'https://semopenalex.org/location/W27625582821', 'Analytical Evaluation of the Baseline Decorrelation in Bistatic Interferometric SAR Systems', "Deciphering Earth's Movements: Unveiling Subsidence and Displacement in Capo Colonna Through SAR and CGPS", 'Cardinal Effect in Bistatic SAR Imagery: Analysis and Physical Interpretation', 'https://semopenalex.org/location/W29127815872', 'An Analytical Formulation of the Correlation of GNSS-R Signals', 'https://semopenalex.org/location/W27908694952', 'https://semopenalex.org/location/W30943681811', 'Integration of SAR and GEOBIA for the Analysis of Time-Series Data', 'Efficient Simulation of Extended-Scene SAR Raw Signals with Any Acquisition Mode', 'Despeckling of Multifrequency SAR Data Using Electromagnetic Scattering Models', 'https://semopenalex.org/location/W31291607332', 'https://semopenalex.org/location/W31576231201', 'The Role of Skin in mm-Wave Exposure of Human Body', 'https://semopenalex.org/location/W28855740751', 'https://semopenalex.org/location/W42057164411', 'https://semopenalex.org/location/W29018743401', 'Formation-Flying SAR Receivers in FAR-from-Transmitter Geometry: X-Band SAR Antenna Design', 'https://semopenalex.org/location/W28855740752', 'Efficient Processing for Far-From-Transmitter Formation-Flying SAR Receivers', 'Analytical Formulation of Scattering From Anisotropic Power-Law Spectrum Surfaces: Getting Rid of the Cutoff Wavenumber', 'https://semopenalex.org/location/W32050064891', 'A Unified Formulation of SAR Raw Signals From Extended Scenes for All Acquisition Modes With Application to Simulation', 'Hydrogeological characterization of a closed MSW landfill using multivariate statistical analysis and groundwater numerical modelling', 'Assessing Performance of Multitemporal SAR Image Despeckling Filters via a Benchmarking Tool', 'https://semopenalex.org/location/W43878704031', 'https://semopenalex.org/location/W43878697331', 'Design of Low-Cost Active Reflectors for Advanced InSAR Applications: First Results', 'https://semopenalex.org/location/W29011861951', 'https://semopenalex.org/location/W27721700481', 'Remote Sensing for Monitoring Biodiversity in Urban Environment', 'https://semopenalex.org/location/W28914311982', 'https://semopenalex.org/location/W43132449201', 'A Novel Analytical Formulation of the Correlation of GNSS-R Signals Scattered by a Natural Fractal Surface', 'https://semopenalex.org/location/W29018043391', 'https://semopenalex.org/location/W29031449731', 'https://semopenalex.org/location/W30036652921', 'https://semopenalex.org/location/W28099006691', 'https://semopenalex.org/location/W32075299251', 'SAR Radiometric Calibration Based on Differential Geometry: From Theory to Experimentation on SAOCOM Imagery', 'Two-Scale Model for the Evaluation of Sea-Surface Scattering in GNSS-R Ship-Detection Applications', 'https://semopenalex.org/location/W43827525081', 'Polarimetric Two-Scale Model for Rough Surface Bistatic Scattering Evaluation', 'https://semopenalex.org/location/W44042941271', 'Scattering-based Despeckling of Multi-frequency SAR Data', 'https://semopenalex.org/location/W32057021671', 'Polarimetric Two-Scale Model for Soil Moisture Estimation from Hybrid Compact Polarimetry SAR Data', 'https://semopenalex.org/location/W27746187661', 'https://semopenalex.org/location/W30935297031', 'RGB SAR product exploiting multitemporal: General processing and applications', 'https://semopenalex.org/location/W43815923961', 'Link Budget Analysis for GNSS-R Sea Surface Return in Arbitrary Acquisition Geometries Using BA-PTSM', 'Retrieval of high-resolution topography of the Titan’ surface by using Cassini SAR data', 'Fractal-Based Local Range Slope Estimation from Single SAR Image with Applications to SAR Despeckling and Topographic Mapping', 'Mapping small reservoirs in semi-arid regions using multitemporal SAR: Methods and applications', 'Spaceborne GNSS-Reflectometry for Ship-Detection Applications: Impact of Acquisition Geometry and Polarization', 'A fully polarimetric SAR raw signal simulator', 'A New Tool for Road Network Deformations Monitoring Through Space-Born SAR Data and In-Situ Instruments', 'https://semopenalex.org/location/W27632159761', 'https://semopenalex.org/location/W27903991441', 'Sea state and wind speed', 'https://semopenalex.org/location/W42829188311', 'https://semopenalex.org/location/W31291607331', 'Planning 5G Networks Under EMF Constraints: State of the Art and Vision', 'Electromagnetic Scattering from a Canonical Target over an Anisotropic Rough Surface using Geometrical Optics', 'https://semopenalex.org/location/W42059632101', 'Link Budget Analysis for the Modeling of GNSS-R Sea Surface Returns in Far-from-Specular Acquisition Geometries', 'https://semopenalex.org/location/W29006840811', 'X-Band SAR Antenna Design for a CubeSat Formation-Flying Remote Sensing Mission', 'Closed-form Polarimetric Two-Scale Model for sea scattering evaluation', 'https://semopenalex.org/location/W29014813671', 'Physical models for evaluating the interferometric coherence of potential persistent scatterers', 'Flood Detection with SAR: A Review of Techniques and Datasets', 'https://semopenalex.org/location/W26132134601', 'https://semopenalex.org/location/W30884119801', 'Bistatic scattering from a canonical building', 'https://semopenalex.org/location/W27778336261', 'Earth Environmental Monitoring Using Multi-Temporal Synthetic Aperture Radar: A Critical Review of Selected Applications', 'The Role of Resolution in the Estimation of Fractal Dimension Maps From SAR Data', 'Long-Term Satellite Monitoring of the Slumgullion Landslide Using Space-Borne Synthetic Aperture Radar Sub-Pixel Offset Tracking', 'https://semopenalex.org/location/W27749247961', 'https://semopenalex.org/location/W31292473171', 'https://semopenalex.org/location/W42056663831', 'Benchmarking Framework for Multitemporal SAR Despeckling', 'Railway Bridge Monitoring with Sar: A Case Study', 'https://semopenalex.org/location/W44002082621']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/location/W44027563071', 'https://semopenalex.org/location/W43872509461', 'https://semopenalex.org/location/W43904891721', 'Immunity Vanishing Act: Epidemic Variant and Immunity Analysis via Evolutionary Computation', 'https://semopenalex.org/location/W44028121901', 'All lockdowns are not equal: Reducing epidemic impact through evolutionary computation', 'https://semopenalex.org/location/W44032105491', 'https://semopenalex.org/location/W43861716341', 'https://semopenalex.org/location/W44028121881', 'Freezing of gait in Parkinson’s disease: Classification using computational intelligence', 'Driving Evolution Towards Discovery of Patterns in Sets of Weakly-Conserved DNA Sequences', 'Network Induction Issues', 'Conference Report on 2022 IEEE Conference on Computational Intelligence in Bioinformatics and Computational Biology (IEEE CIBCB 2022) [Conference Report]', 'https://semopenalex.org/location/W44028122871', 'https://semopenalex.org/location/W43861716342', 'https://semopenalex.org/location/W43912337582', 'https://semopenalex.org/location/W43789796561', 'Comparison of Representations to Evolve Weighted Contact Networks with Epidemic Properties', 'https://semopenalex.org/location/W43872514871', 'https://semopenalex.org/location/W44028123391', 'Graph Compression', 'From Bits to Bases: Evolving a Versatile Construct for Biological Sequence and Network Data', 'https://semopenalex.org/location/W43912337581', 'A multi-objective genetic algorithm for compression of weighted graphs to simplify epidemic analysis', '2022 IEEE conference on computational intelligence in bioinformatics and computational biology (IEEE CIBCB, 2022)', 'Evolutionary Computation', 'Network Induction', 'Generating Models of Human Gait in Patients with Parkinson’s Disease using Genetic Programming', 'https://semopenalex.org/location/W44028127321', 'Promoting Diversity in the Evolution of Biological Sequence Data', 'https://semopenalex.org/location/W44028130911', 'Introduction', 'What Drives Evolution of Self-Driving Automata?', 'https://semopenalex.org/location/W44032105271', 'https://semopenalex.org/location/W43789796562', 'AI Versus Epidemics', 'https://semopenalex.org/location/W43900150231', 'https://semopenalex.org/location/W44014165061', 'Dungeons, Dragons, and Data Breaches: Analyzing AI Attacks on Various Network Configurations', 'https://semopenalex.org/location/W43190545381', 'https://semopenalex.org/location/W43791408481', 'Vaccine Distribution', 'https://semopenalex.org/location/W44032122871']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/authorship/W2035561336A5027830035', 'https://semopenalex.org/authorship/W2162485250A5027830035', 'https://semopenalex.org/authorship/W2246672683A5027830035', 'https://semopenalex.org/authorship/W4298871721A5027830035', 'https://semopenalex.org/authorship/W2145983295A5027830035', 'https://semopenalex.org/authorship/W2025458350A5027830035', 'https://semopenalex.org/authorship/W4301512502A5027830035', 'https://semopenalex.org/authorship/W2956308890A5027830035', 'https://semopenalex.org/authorship/W2223218801A5027830035', 'https://semopenalex.org/authorship/W2113885710A5017511611', 'https://semopenalex.org/authorship/W266384355A5027830035', 'https://semopenalex.org/authorship/W2099441560A5027830035', 'https://semopenalex.org/authorship/W1624008340A5017511611', 'https://semopenalex.org/authorship/W1820714040A5027830035', 'https://semopenalex.org/authorship/W2106293056A5027830035', 'https://semopenalex.org/authorship/W4405562746A5027830035', 'https://semopenalex.org/authorship/W8218751A5027830035', 'https://semopenalex.org/authorship/W2806144920A5017511611', 'https://semopenalex.org/authorship/W2130794128A5027830035', 'https://semopenalex.org/authorship/W4300434862A5027830035', 'https://semopenalex.org/authorship/W2021144192A5027830035', 'https://semopenalex.org/authorship/W2761218667A5027830035', 'https://semopenalex.org/authorship/W2920910927A5027830035', 'https://semopenalex.org/authorship/W2476684204A5027830035', 'https://semopenalex.org/authorship/W1883544968A5027830035', 'https://semopenalex.org/authorship/W2568027424A5027830035', 'https://semopenalex.org/authorship/W2134429331A5027830035', 'https://semopenalex.org/authorship/W2293217651A5017511611', 'https://semopenalex.org/authorship/W2159784132A5027830035', 'https://semopenalex.org/authorship/W2155484207A5027830035', 'https://semopenalex.org/authorship/W1828712802A5027830035', 'https://semopenalex.org/authorship/W2101633987A5017511611', 'https://semopenalex.org/authorship/W1976082632A5027830035', 'https://semopenalex.org/authorship/W2120659763A5027830035', 'https://semopenalex.org/authorship/W2500060407A5027830035', 'https://semopenalex.org/authorship/W4200630260A5027830035', 'https://semopenalex.org/authorship/W2955178723A5017511611', 'https://semopenalex.org/authorship/W2142005762A5027830035', 'https://semopenalex.org/authorship/W4309830289A5027830035', 'https://semopenalex.org/authorship/W4394744533A5027830035', 'https://semopenalex.org/authorship/W2114059901A5027830035', 'https://semopenalex.org/authorship/W2133913871A5027830035', 'https://semopenalex.org/authorship/W2147993784A5027830035', 'https://semopenalex.org/authorship/W2135428614A5027830035', 'https://semopenalex.org/authorship/W4309877015A5027830035', 'https://semopenalex.org/authorship/W2806925689A5027830035', 'https://semopenalex.org/authorship/W1943126751A5027830035', 'https://semopenalex.org/authorship/W2170015373A5027830035', 'https://semopenalex.org/authorship/W2950247931A5027830035', 'https://semopenalex.org/authorship/W2013218112A5027830035', 'https://semopenalex.org/authorship/W4401750498A5027830035', 'https://semopenalex.org/authorship/W2755327666A5017511611', 'https://semopenalex.org/authorship/W989118312A5027830035', 'https://semopenalex.org/authorship/W2017148819A5027830035', 'https://semopenalex.org/authorship/W2100814254A5017511611', 'https://semopenalex.org/authorship/W2013030361A5027830035', 'https://semopenalex.org/authorship/W4388638199A5017511611', 'https://semopenalex.org/authorship/W2003410902A5027830035', 'https://semopenalex.org/authorship/W2126409288A5027830035', 'https://semopenalex.org/authorship/W2673901561A5027830035', 'https://semopenalex.org/authorship/W2163547689A5027830035', 'https://semopenalex.org/authorship/W2003520411A5027830035', 'https://semopenalex.org/authorship/W2063650998A5027830035', 'https://semopenalex.org/authorship/W4224247224A5027830035', 'https://semopenalex.org/authorship/W2100556278A5027830035', 'https://semopenalex.org/authorship/W2109988731A5027830035', 'https://semopenalex.org/authorship/W2136275432A5027830035', 'https://semopenalex.org/authorship/W2161770118A5027830035', 'https://semopenalex.org/authorship/W2117127275A5027830035', 'https://semopenalex.org/authorship/W2043499328A5027830035', 'https://semopenalex.org/authorship/W1984186332A5027830035', 'https://semopenalex.org/authorship/W1984118997A5027830035', 'https://semopenalex.org/authorship/W2189600142A5027830035', 'https://semopenalex.org/authorship/W2241683853A5017511611', 'https://semopenalex.org/authorship/W1895161527A5027830035', 'https://semopenalex.org/authorship/W2963612078A5027830035', 'https://semopenalex.org/authorship/W1984896113A5027830035', 'https://semopenalex.org/authorship/W1999564901A5027830035', 'https://semopenalex.org/authorship/W2166805843A5017511611', 'https://semopenalex.org/authorship/W2187527650A5027830035', 'https://semopenalex.org/authorship/W2587913063A5027830035', 'https://semopenalex.org/authorship/W2007670367A5017511611', 'https://semopenalex.org/authorship/W2115645605A5027830035', 'https://semopenalex.org/authorship/W2152599017A5027830035', 'https://semopenalex.org/authorship/W4386362571A5027830035', 'https://semopenalex.org/authorship/W3005113692A5027830035', 'https://semopenalex.org/authorship/W2763660685A5027830035', 'https://semopenalex.org/authorship/W2170329684A5027830035', 'https://semopenalex.org/authorship/W2166862038A5027830035', 'https://semopenalex.org/authorship/W2883797206A5017511611', 'https://semopenalex.org/authorship/W2133118701A5027830035', 'https://semopenalex.org/authorship/W2111128642A5027830035', 'https://semopenalex.org/authorship/W2981712458A5017511611', 'https://semopenalex.org/authorship/W2890986802A5027830035', 'https://semopenalex.org/authorship/W2055834582A5027830035', 'https://semopenalex.org/authorship/W4388829566A5027830035', 'https://semopenalex.org/authorship/W2149213383A5017511611', 'https://semopenalex.org/authorship/W2134671262A5027830035', 'https://semopenalex.org/authorship/W2397071937A5027830035', 'https://semopenalex.org/authorship/W1980527047A5027830035', 'https://semopenalex.org/authorship/W2162281264A5027830035', 'https://semopenalex.org/authorship/W1968153028A5027830035', 'https://semopenalex.org/authorship/W2903667675A5027830035', 'https://semopenalex.org/authorship/W2112866668A5027830035', 'https://semopenalex.org/authorship/W4221012413A5027830035', 'https://semopenalex.org/authorship/W1971056102A5017511611', 'https://semopenalex.org/authorship/W2024240534A5027830035', 'https://semopenalex.org/authorship/W1785723168A5027830035', 'https://semopenalex.org/authorship/W2122768752A5027830035', 'https://semopenalex.org/authorship/W2163889321A5027830035', 'https://semopenalex.org/authorship/W2100527158A5027830035', 'https://semopenalex.org/authorship/W2437887498A5027830035', 'https://semopenalex.org/authorship/W2019064108A5027830035', 'https://semopenalex.org/authorship/W2085150116A5027830035', 'https://semopenalex.org/authorship/W2182338449A5027830035', 'https://semopenalex.org/authorship/W3046488911A5027830035', 'https://semopenalex.org/authorship/W1818779082A5027830035', 'https://semopenalex.org/authorship/W3204100703A5027830035', 'https://semopenalex.org/authorship/W2126230854A5027830035', 'https://semopenalex.org/authorship/W4289306231A5027830035', 'https://semopenalex.org/authorship/W2189224346A5027830035', 'https://semopenalex.org/authorship/W2020196086A5027830035', 'https://semopenalex.org/authorship/W2316293614A5027830035', 'https://semopenalex.org/authorship/W2025968816A5027830035', 'https://semopenalex.org/authorship/W2116018884A5027830035', 'https://semopenalex.org/authorship/W4226253448A5017511611', 'https://semopenalex.org/authorship/W2068189057A5027830035', 'https://semopenalex.org/authorship/W2057477395A5027830035', 'https://semopenalex.org/authorship/W3115993754A5027830035', 'https://semopenalex.org/authorship/W3214000901A5027830035', 'https://semopenalex.org/authorship/W2075899871A5027830035', 'https://semopenalex.org/authorship/W2148267424A5027830035', 'https://semopenalex.org/authorship/W1994628498A5027830035', 'https://semopenalex.org/authorship/W2756070092A5017511611', 'https://semopenalex.org/authorship/W3088822975A5027830035', 'https://semopenalex.org/authorship/W2148907823A5027830035', 'https://semopenalex.org/authorship/W4243966075A5027830035', 'https://semopenalex.org/authorship/W2591258888A5027830035', 'https://semopenalex.org/authorship/W2138395721A5027830035', 'https://semopenalex.org/authorship/W2065628492A5027830035', 'https://semopenalex.org/authorship/W2072116332A5027830035', 'https://semopenalex.org/authorship/W1602846904A5027830035', 'https://semopenalex.org/authorship/W1552869711A5027830035', 'https://semopenalex.org/authorship/W2939804650A5017511611', 'https://semopenalex.org/authorship/W2182254337A5027830035', 'https://semopenalex.org/authorship/W2764441237A5027830035', 'https://semopenalex.org/authorship/W2140316862A5027830035', 'https://semopenalex.org/authorship/W2018627313A5027830035', 'https://semopenalex.org/authorship/W2118103599A5027830035', 'https://semopenalex.org/authorship/W4381304944A5027830035', 'https://semopenalex.org/authorship/W3168228747A5027830035', 'https://semopenalex.org/authorship/W2397760318A5017511611', 'https://semopenalex.org/authorship/W2745032981A5017511611', 'https://semopenalex.org/authorship/W2141592093A5027830035', 'https://semopenalex.org/authorship/W4379232433A5027830035', 'https://semopenalex.org/authorship/W2130502393A5027830035', 'https://semopenalex.org/authorship/W4256256581A5027830035', 'https://semopenalex.org/authorship/W2949402315A5027830035', 'https://semopenalex.org/authorship/W3130481183A5017511611', 'https://semopenalex.org/authorship/W1997019093A5017511611', 'https://semopenalex.org/authorship/W4288596410A5027830035', 'https://semopenalex.org/authorship/W2085980614A5027830035', 'https://semopenalex.org/authorship/W3106343576A5027830035', 'https://semopenalex.org/authorship/W4386728290A5027830035', 'https://semopenalex.org/authorship/W2035930173A5027830035', 'https://semopenalex.org/authorship/W4377043292A5027830035', 'https://semopenalex.org/authorship/W2805042680A5027830035', 'https://semopenalex.org/authorship/W3103915668A5027830035', 'https://semopenalex.org/authorship/W2902929870A5027830035', 'https://semopenalex.org/authorship/W4402502594A5027830035', 'https://semopenalex.org/authorship/W3012817764A5027830035', 'https://semopenalex.org/authorship/W842176471A5027830035', 'https://semopenalex.org/authorship/W2541647902A5027830035', 'https://semopenalex.org/authorship/W2060717066A5017511611', 'https://semopenalex.org/authorship/W2977723824A5027830035', 'https://semopenalex.org/authorship/W3003820456A5027830035', 'https://semopenalex.org/authorship/W610096311A5027830035', 'https://semopenalex.org/authorship/W2129001064A5027830035', 'https://semopenalex.org/authorship/W1909031490A5027830035', 'https://semopenalex.org/authorship/W2129898633A5027830035', 'https://semopenalex.org/authorship/W2918802163A5027830035', 'https://semopenalex.org/authorship/W4388235556A5027830035', 'https://semopenalex.org/authorship/W1984769758A5027830035', 'https://semopenalex.org/authorship/W4396898129A5027830035', 'https://semopenalex.org/authorship/W4226267095A5027830035', 'https://semopenalex.org/authorship/W1507181737A5027830035', 'https://semopenalex.org/authorship/W2140311422A5027830035', 'https://semopenalex.org/authorship/W2148131061A5027830035', 'https://semopenalex.org/authorship/W3048660463A5027830035', 'https://semopenalex.org/authorship/W2143053621A5027830035', 'https://semopenalex.org/authorship/W4226163818A5027830035', 'https://semopenalex.org/authorship/W2243109900A5027830035', 'https://semopenalex.org/authorship/W2087217507A5027830035', 'https://semopenalex.org/authorship/W4283215612A5027830035', 'https://semopenalex.org/authorship/W4300799299A5027830035', 'https://semopenalex.org/authorship/W2119248338A5027830035', 'https://semopenalex.org/authorship/W4400686367A5027830035', 'https://semopenalex.org/authorship/W3098360176A5027830035', 'https://semopenalex.org/authorship/W4376141221A5017511611', 'https://semopenalex.org/authorship/W2159202008A5027830035', 'https://semopenalex.org/authorship/W1867432869A5027830035', 'https://semopenalex.org/authorship/W2152477879A5017511611', 'https://semopenalex.org/authorship/W2122128429A5027830035', 'https://semopenalex.org/authorship/W2400256934A5027830035', 'https://semopenalex.org/authorship/W3009810166A5027830035', 'https://semopenalex.org/authorship/W2039909063A5027830035', 'https://semopenalex.org/authorship/W2958959679A5027830035', 'https://semopenalex.org/authorship/W2112902331A5027830035', 'https://semopenalex.org/authorship/W1571761681A5027830035', 'https://semopenalex.org/authorship/W2162965487A5027830035', 'https://semopenalex.org/authorship/W2165066371A5017511611', 'https://semopenalex.org/authorship/W2149742409A5027830035', 'https://semopenalex.org/authorship/W2092230235A5027830035', 'https://semopenalex.org/authorship/W2099205567A5027830035', 'https://semopenalex.org/authorship/W2988564852A5027830035', 'https://semopenalex.org/authorship/W2141480726A5027830035', 'https://semopenalex.org/authorship/W2100279715A5017511611', 'https://semopenalex.org/authorship/W2124699087A5017511611', 'https://semopenalex.org/authorship/W2143728623A5027830035', 'https://semopenalex.org/authorship/W2171258724A5027830035', 'https://semopenalex.org/authorship/W1940162557A5027830035', 'https://semopenalex.org/authorship/W4402699738A5027830035', 'https://semopenalex.org/authorship/W4301499895A5027830035', 'https://semopenalex.org/authorship/W1975277950A5027830035', 'https://semopenalex.org/authorship/W1774599862A5017511611', 'https://semopenalex.org/authorship/W2283163132A5027830035', 'https://semopenalex.org/authorship/W3183317559A5027830035', 'https://semopenalex.org/authorship/W4307934118A5027830035', 'https://semopenalex.org/authorship/W609082053A5027830035', 'https://semopenalex.org/authorship/W4282004224A5027830035', 'https://semopenalex.org/authorship/W2155624091A5027830035', 'https://semopenalex.org/authorship/W2097084589A5027830035', 'https://semopenalex.org/authorship/W2106903616A5027830035', 'https://semopenalex.org/authorship/W1975302208A5027830035', 'https://semopenalex.org/authorship/W2185477524A5027830035', 'https://semopenalex.org/authorship/W2108862142A5027830035', 'https://semopenalex.org/authorship/W2572859442A5027830035', 'https://semopenalex.org/authorship/W3002449320A5027830035', 'https://semopenalex.org/authorship/W2143780518A5017511611', 'https://semopenalex.org/authorship/W2123832893A5027830035', 'https://semopenalex.org/authorship/W3015454417A5017511611', 'https://semopenalex.org/authorship/W4390050192A5027830035', 'https://semopenalex.org/authorship/W2095121969A5027830035', 'https://semopenalex.org/authorship/W2158537680A5017511611', 'https://semopenalex.org/authorship/W4386728259A5027830035', 'https://semopenalex.org/authorship/W2952777161A5027830035', 'https://semopenalex.org/authorship/W3166787465A5027830035', 'https://semopenalex.org/authorship/W4223588778A5027830035', 'https://semopenalex.org/authorship/W2701634507A5017511611', 'https://semopenalex.org/authorship/W2308119766A5027830035', 'https://semopenalex.org/authorship/W2938524150A5027830035', 'https://semopenalex.org/authorship/W125371902A5027830035', 'https://semopenalex.org/authorship/W2027160844A5027830035', 'https://semopenalex.org/authorship/W2146189427A5017511611', 'https://semopenalex.org/authorship/W4287551966A5027830035', 'https://semopenalex.org/authorship/W1989616605A5027830035', 'https://semopenalex.org/authorship/W4386352568A5027830035', 'https://semopenalex.org/authorship/W3012587348A5027830035', 'https://semopenalex.org/authorship/W2395280900A5027830035', 'https://semopenalex.org/authorship/W2127722806A5027830035', 'https://semopenalex.org/authorship/W2125523397A5027830035', 'https://semopenalex.org/authorship/W1981586887A5027830035', 'https://semopenalex.org/authorship/W2963482739A5027830035', 'https://semopenalex.org/authorship/W2034340815A5027830035', 'https://semopenalex.org/authorship/W2150474553A5027830035', 'https://semopenalex.org/authorship/W6747142A5027830035', 'https://semopenalex.org/authorship/W2064969586A5027830035', 'https://semopenalex.org/authorship/W2002799652A5027830035', 'https://semopenalex.org/authorship/W2106233876A5027830035', 'https://semopenalex.org/authorship/W4386081510A5027830035', 'https://semopenalex.org/authorship/W2908750658A5027830035', 'https://semopenalex.org/authorship/W2078203941A5027830035', 'https://semopenalex.org/authorship/W2111934195A5027830035', 'https://semopenalex.org/authorship/W2059944861A5027830035', 'https://semopenalex.org/authorship/W2100860054A5027830035', 'https://semopenalex.org/authorship/W2055673378A5027830035', 'https://semopenalex.org/authorship/W4403704152A5027830035', 'https://semopenalex.org/authorship/W2066062210A5027830035', 'https://semopenalex.org/authorship/W2566922557A5027830035', 'https://semopenalex.org/authorship/W2143075489A5017511611', 'https://semopenalex.org/authorship/W4322832362A5017511611', 'https://semopenalex.org/authorship/W2970497931A5017511611', 'https://semopenalex.org/authorship/W4288482042A5027830035', 'https://semopenalex.org/authorship/W1855265535A5027830035', 'https://semopenalex.org/authorship/W4224949960A5027830035', 'https://semopenalex.org/authorship/W1989282861A5027830035', 'https://semopenalex.org/authorship/W4309129028A5027830035', 'https://semopenalex.org/authorship/W2108634960A5027830035', 'https://semopenalex.org/authorship/W2121529688A5027830035', 'https://semopenalex.org/authorship/W2012992134A5027830035', 'https://semopenalex.org/authorship/W2168793726A5027830035', 'https://semopenalex.org/authorship/W1964384820A5027830035', 'https://semopenalex.org/authorship/W2097076848A5027830035', 'https://semopenalex.org/authorship/W2117368578A5027830035', 'https://semopenalex.org/authorship/W2171540325A5027830035', 'https://semopenalex.org/authorship/W2106738903A5027830035', 'https://semopenalex.org/authorship/W2001708147A5027830035', 'https://semopenalex.org/authorship/W2021426840A5027830035', 'https://semopenalex.org/authorship/W4297229624A5027830035', 'https://semopenalex.org/authorship/W4393531447A5027830035', 'https://semopenalex.org/authorship/W2138621265A5017511611', 'https://semopenalex.org/authorship/W4397026396A5027830035', 'https://semopenalex.org/authorship/W1951572853A5027830035', 'https://semopenalex.org/authorship/W2618462601A5027830035', 'https://semopenalex.org/authorship/W2280892290A5027830035', 'https://semopenalex.org/authorship/W3200113339A5017511611', 'https://semopenalex.org/authorship/W2050578629A5027830035', 'https://semopenalex.org/authorship/W2109495528A5027830035', 'https://semopenalex.org/authorship/W2166500461A5027830035', 'https://semopenalex.org/authorship/W2025132922A5017511611', 'https://semopenalex.org/authorship/W2160616608A5017511611', 'https://semopenalex.org/authorship/W2182267970A5027830035', 'https://semopenalex.org/authorship/W2746198904A5027830035', 'https://semopenalex.org/authorship/W2129299867A5027830035', 'https://semopenalex.org/authorship/W2158228464A5027830035', 'https://semopenalex.org/authorship/W2131752107A5027830035', 'https://semopenalex.org/authorship/W619554517A5027830035', 'https://semopenalex.org/authorship/W2102549524A5017511611', 'https://semopenalex.org/authorship/W2512503502A5017511611', 'https://semopenalex.org/authorship/W4243743111A5027830035', 'https://semopenalex.org/authorship/W2115596980A5027830035', 'https://semopenalex.org/authorship/W3162654685A5027830035', 'https://semopenalex.org/authorship/W2998913556A5027830035', 'https://semopenalex.org/authorship/W4287903453A5027830035', 'https://semopenalex.org/authorship/W2076199721A5027830035', 'https://semopenalex.org/authorship/W2155252144A5027830035', 'https://semopenalex.org/authorship/W3158448776A5027830035', 'https://semopenalex.org/authorship/W2697509747A5017511611', 'https://semopenalex.org/authorship/W1987895141A5027830035', 'https://semopenalex.org/authorship/W4388567240A5027830035', 'https://semopenalex.org/authorship/W4255556357A5027830035', 'https://semopenalex.org/authorship/W2159063898A5027830035', 'https://semopenalex.org/authorship/W2142780243A5017511611', 'https://semopenalex.org/authorship/W2077024675A5027830035', 'https://semopenalex.org/authorship/W4300587259A5027830035', 'https://semopenalex.org/authorship/W3203864625A5027830035', 'https://semopenalex.org/authorship/W2978037608A5027830035', 'https://semopenalex.org/authorship/W4312819449A5027830035', 'https://semopenalex.org/authorship/W2014068777A5017511611', 'https://semopenalex.org/authorship/W4362607752A5027830035', 'https://semopenalex.org/authorship/W1783191689A5027830035', 'https://semopenalex.org/authorship/W2291045170A5027830035', 'https://semopenalex.org/authorship/W2124699087A5027830035', 'https://semopenalex.org/authorship/W3085042870A5027830035', 'https://semopenalex.org/authorship/W3190979825A5027830035', 'https://semopenalex.org/authorship/W2120952077A5027830035', 'https://semopenalex.org/authorship/W2185641310A5027830035', 'https://semopenalex.org/authorship/W2103637183A5027830035', 'https://semopenalex.org/authorship/W2035640322A5027830035', 'https://semopenalex.org/authorship/W3162627549A5027830035', 'https://semopenalex.org/authorship/W855221475A5027830035', 'https://semopenalex.org/authorship/W1999197804A5027830035', 'https://semopenalex.org/authorship/W2152599017A5017511611', 'https://semopenalex.org/authorship/W2126535187A5027830035', 'https://semopenalex.org/authorship/W4386362810A5027830035', 'https://semopenalex.org/authorship/W2287663230A5027830035', 'https://semopenalex.org/authorship/W2050921210A5027830035', 'https://semopenalex.org/authorship/W4297966944A5027830035', 'https://semopenalex.org/authorship/W2786494993A5027830035', 'https://semopenalex.org/authorship/W2131459843A5027830035', 'https://semopenalex.org/authorship/W2158368814A5017511611', 'https://semopenalex.org/authorship/W2118345904A5027830035', 'https://semopenalex.org/authorship/W2084295409A5027830035', 'https://semopenalex.org/authorship/W2149513726A5027830035', 'https://semopenalex.org/authorship/W2129361591A5027830035', 'https://semopenalex.org/authorship/W2151042992A5027830035', 'https://semopenalex.org/authorship/W2030004233A5017511611', 'https://semopenalex.org/authorship/W1764115161A5027830035', 'https://semopenalex.org/authorship/W2164697291A5027830035', 'https://semopenalex.org/authorship/W3093907665A5027830035', 'https://semopenalex.org/authorship/W4225966372A5027830035', 'https://semopenalex.org/authorship/W4400242511A5027830035', 'https://semopenalex.org/authorship/W2041220458A5027830035', 'https://semopenalex.org/authorship/W2114379490A5027830035', 'https://semopenalex.org/authorship/W1814362492A5027830035', 'https://semopenalex.org/authorship/W3196466252A5027830035', 'https://semopenalex.org/authorship/W4249394463A5027830035', 'https://semopenalex.org/authorship/W605016662A5027830035', 'https://semopenalex.org/authorship/W1984866494A5027830035', 'https://semopenalex.org/authorship/W4256384691A5027830035', 'https://semopenalex.org/authorship/W3015796941A5027830035', 'https://semopenalex.org/authorship/W2168665985A5027830035', 'https://semopenalex.org/authorship/W2950434959A5027830035', 'https://semopenalex.org/authorship/W4288374763A5027830035', 'https://semopenalex.org/authorship/W2988626048A5027830035', 'https://semopenalex.org/authorship/W4304701022A5027830035', 'https://semopenalex.org/authorship/W3164197023A5027830035', 'https://semopenalex.org/authorship/W2160492008A5027830035', 'https://semopenalex.org/authorship/W3155241911A5027830035', 'https://semopenalex.org/authorship/W3106431100A5027830035', 'https://semopenalex.org/authorship/W4205889589A5027830035', 'https://semopenalex.org/authorship/W2143711974A5017511611', 'https://semopenalex.org/authorship/W2164044612A5027830035', 'https://semopenalex.org/authorship/W1778342465A5027830035', 'https://semopenalex.org/authorship/W2104561024A5027830035', 'https://semopenalex.org/authorship/W1492310094A5027830035', 'https://semopenalex.org/authorship/W1945620949A5027830035', 'https://semopenalex.org/authorship/W2104882822A5027830035', 'https://semopenalex.org/authorship/W2073431334A5027830035', 'https://semopenalex.org/authorship/W4200629809A5027830035', 'https://semopenalex.org/authorship/W2945382159A5027830035', 'https://semopenalex.org/authorship/W2136390628A5027830035', 'https://semopenalex.org/authorship/W2150591965A5027830035', 'https://semopenalex.org/authorship/W1564509605A5027830035', 'https://semopenalex.org/authorship/W2122776646A5027830035', 'https://semopenalex.org/authorship/W2101094458A5027830035', 'https://semopenalex.org/authorship/W1881094281A5027830035', 'https://semopenalex.org/authorship/W2147674767A5027830035', 'https://semopenalex.org/authorship/W2108934479A5017511611', 'https://semopenalex.org/authorship/W2618786793A5017511611', 'https://semopenalex.org/authorship/W2145173682A5027830035', 'https://semopenalex.org/authorship/W2152477879A5027830035', 'https://semopenalex.org/authorship/W2130561641A5027830035', 'https://semopenalex.org/authorship/W2153058280A5027830035', 'https://semopenalex.org/authorship/W2018384246A5027830035', 'https://semopenalex.org/authorship/W1814798360A5027830035', 'https://semopenalex.org/authorship/W2145876651A5027830035', 'https://semopenalex.org/authorship/W2082792607A5027830035', 'https://semopenalex.org/authorship/W2145568341A5027830035', 'https://semopenalex.org/authorship/W2021159593A5027830035', 'https://semopenalex.org/authorship/W4394868342A5017511611', 'https://semopenalex.org/authorship/W2982533818A5027830035', 'https://semopenalex.org/authorship/W1972847653A5017511611', 'https://semopenalex.org/authorship/W4247814650A5027830035', 'https://semopenalex.org/authorship/W2167460076A5027830035', 'https://semopenalex.org/authorship/W4284707241A5027830035', 'https://semopenalex.org/authorship/W2112567022A5027830035', 'https://semopenalex.org/authorship/W2065530904A5027830035', 'https://semopenalex.org/authorship/W2164511982A5027830035', 'https://semopenalex.org/authorship/W3084462124A5017511611', 'https://semopenalex.org/authorship/W1585966427A5027830035', 'https://semopenalex.org/authorship/W2811277086A5027830035', 'https://semopenalex.org/authorship/W2128254445A5027830035', 'https://semopenalex.org/authorship/W4294643449A5017511611', 'https://semopenalex.org/authorship/W2293728320A5017511611', 'https://semopenalex.org/authorship/W1808004798A5027830035', 'https://semopenalex.org/authorship/W2027156706A5027830035', 'https://semopenalex.org/authorship/W2150869369A5027830035', 'https://semopenalex.org/authorship/W2030004233A5027830035', 'https://semopenalex.org/authorship/W2162696202A5027830035', 'https://semopenalex.org/authorship/W4309321321A5017511611', 'https://semopenalex.org/authorship/W2242734504A5027830035', 'https://semopenalex.org/authorship/W3163624263A5027830035', 'https://semopenalex.org/authorship/W2137966369A5027830035', 'https://semopenalex.org/authorship/W2126043778A5027830035', 'https://semopenalex.org/authorship/W2098408658A5027830035', 'https://semopenalex.org/authorship/W1843753733A5027830035', 'https://semopenalex.org/authorship/W4386728284A5027830035', 'https://semopenalex.org/authorship/W2113689008A5027830035', 'https://semopenalex.org/authorship/W2097494906A5027830035', 'https://semopenalex.org/authorship/W4402559984A5027830035', 'https://semopenalex.org/authorship/W2170432288A5017511611', 'https://semopenalex.org/authorship/W4285201772A5017511611', 'https://semopenalex.org/authorship/W3123138559A5027830035', 'https://semopenalex.org/authorship/W4242495832A5027830035', 'https://semopenalex.org/authorship/W4386728227A5027830035', 'https://semopenalex.org/authorship/W2184393924A5027830035', 'https://semopenalex.org/authorship/W3183518399A5027830035', 'https://semopenalex.org/authorship/W2146692894A5027830035', 'https://semopenalex.org/authorship/W4389138629A5027830035', 'https://semopenalex.org/authorship/W2963927825A5027830035', 'https://semopenalex.org/authorship/W2018680103A5027830035', 'https://semopenalex.org/authorship/W1963919043A5027830035', 'https://semopenalex.org/authorship/W1991118037A5027830035', 'https://semopenalex.org/authorship/W2337742825A5027830035', 'https://semopenalex.org/authorship/W205233311A5027830035', 'https://semopenalex.org/authorship/W2241753404A5027830035', 'https://semopenalex.org/authorship/W2099998345A5027830035', 'https://semopenalex.org/authorship/W2166197815A5017511611', 'https://semopenalex.org/authorship/W2138556535A5027830035', 'https://semopenalex.org/authorship/W656907390A5027830035', 'https://semopenalex.org/authorship/W2898681335A5027830035', 'https://semopenalex.org/authorship/W1891629850A5027830035', 'https://semopenalex.org/authorship/W1861730306A5027830035', 'https://semopenalex.org/authorship/W2150042449A5027830035', 'https://semopenalex.org/authorship/W2007101240A5027830035', 'https://semopenalex.org/authorship/W2115811215A5027830035', 'https://semopenalex.org/authorship/W2101522113A5017511611', 'https://semopenalex.org/authorship/W4298181338A5027830035', 'https://semopenalex.org/authorship/W2327976118A5027830035', 'https://semopenalex.org/authorship/W2111182668A5027830035', 'https://semopenalex.org/authorship/W3022662194A5017511611', 'https://semopenalex.org/authorship/W2805259552A5027830035', 'https://semopenalex.org/authorship/W2135940404A5027830035', 'https://semopenalex.org/authorship/W2939947188A5027830035', 'https://semopenalex.org/authorship/W1946393290A5027830035', 'https://semopenalex.org/authorship/W2165331646A5027830035', 'https://semopenalex.org/authorship/W4383472744A5027830035', 'https://semopenalex.org/authorship/W2046546110A5027830035', 'https://semopenalex.org/authorship/W3107843792A5027830035', 'https://semopenalex.org/authorship/W606515514A5027830035', 'https://semopenalex.org/authorship/W2006798507A5027830035', 'https://semopenalex.org/authorship/W2185221298A5027830035', 'https://semopenalex.org/authorship/W2129518598A5027830035', 'https://semopenalex.org/authorship/W2334675349A5027830035', 'https://semopenalex.org/authorship/W615388181A5027830035', 'https://semopenalex.org/authorship/W2144570150A5027830035', 'https://semopenalex.org/authorship/W2487376240A5027830035', 'https://semopenalex.org/authorship/W2066478156A5027830035', 'https://semopenalex.org/authorship/W2117161818A5027830035', 'https://semopenalex.org/authorship/W4292214108A5027830035', 'https://semopenalex.org/authorship/W2100556278A5017511611', 'https://semopenalex.org/authorship/W2383111726A5027830035', 'https://semopenalex.org/authorship/W2162969215A5027830035', 'https://semopenalex.org/authorship/W2117083020A5027830035', 'https://semopenalex.org/authorship/W2594176303A5027830035', 'https://semopenalex.org/authorship/W4233630823A5027830035', 'https://semopenalex.org/authorship/W2075769341A5027830035', 'https://semopenalex.org/authorship/W2169931542A5027830035', 'https://semopenalex.org/authorship/W2950767750A5027830035', 'https://semopenalex.org/authorship/W1982263943A5027830035', 'https://semopenalex.org/authorship/W2007454648A5027830035', 'https://semopenalex.org/authorship/W2142195632A5027830035', 'https://semopenalex.org/authorship/W1965141814A5027830035', 'https://semopenalex.org/authorship/W2110043300A5017511611', 'https://semopenalex.org/authorship/W2021186270A5027830035', 'https://semopenalex.org/authorship/W2615249850A5027830035', 'https://semopenalex.org/authorship/W2039091249A5027830035', 'https://semopenalex.org/authorship/W2979998822A5027830035', 'https://semopenalex.org/authorship/W2172643935A5027830035', 'https://semopenalex.org/authorship/W4244875117A5027830035', 'https://semopenalex.org/authorship/W2557336675A5027830035', 'https://semopenalex.org/authorship/W2970159846A5017511611', 'https://semopenalex.org/authorship/W2086931264A5017511611', 'https://semopenalex.org/authorship/W1990472383A5027830035', 'https://semopenalex.org/authorship/W2486186027A5027830035', 'https://semopenalex.org/authorship/W1825244231A5027830035', 'https://semopenalex.org/authorship/W2277416294A5027830035', 'https://semopenalex.org/authorship/W1824121449A5027830035', 'https://semopenalex.org/authorship/W2763756011A5027830035', 'https://semopenalex.org/authorship/W3036970724A5027830035', 'https://semopenalex.org/authorship/W2102302018A5027830035', 'https://semopenalex.org/authorship/W1993842801A5027830035', 'https://semopenalex.org/authorship/W2017812570A5017511611', 'https://semopenalex.org/authorship/W1997019093A5027830035', 'https://semopenalex.org/authorship/W1993524608A5027830035', 'https://semopenalex.org/authorship/W4299390071A5027830035', 'https://semopenalex.org/aut</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/authorship/W4312605566A5019693610', 'https://semopenalex.org/authorship/W2913594206A5056183585', 'https://semopenalex.org/authorship/W2795581336A5019693610', 'https://semopenalex.org/authorship/W2899305210A5056183585', 'https://semopenalex.org/authorship/W3143959337A5056183585', 'https://semopenalex.org/authorship/W2346980133A5056183585', 'https://semopenalex.org/authorship/W2108911539A5056183585', 'https://semopenalex.org/authorship/W2986358413A5056183585', 'https://semopenalex.org/authorship/W2515389026A5019693610', 'https://semopenalex.org/authorship/W2528963299A5056183585', 'https://semopenalex.org/authorship/W2901616108A5019693610', 'https://semopenalex.org/authorship/W4224279084A5056183585', 'https://semopenalex.org/authorship/W4324150573A5056183585', 'https://semopenalex.org/authorship/W2154752229A5056183585', 'https://semopenalex.org/authorship/W4402722090A5056183585', 'https://semopenalex.org/authorship/W2054886944A5056183585', 'https://semopenalex.org/authorship/W4392429145A5019693610', 'https://semopenalex.org/authorship/W2978280554A5056183585', 'https://semopenalex.org/authorship/W3117330688A5019693610', 'https://semopenalex.org/authorship/W2962975962A5056183585', 'https://semopenalex.org/authorship/W3030735111A5019693610', 'https://semopenalex.org/authorship/W3162832522A5056183585', 'https://semopenalex.org/authorship/W2973132733A5056183585', 'https://semopenalex.org/authorship/W3165155612A5019693610', 'https://semopenalex.org/authorship/W2899470128A5056183585', 'https://semopenalex.org/authorship/W4233748389A5056183585', 'https://semopenalex.org/authorship/W2789478762A5056183585', 'https://semopenalex.org/authorship/W4225473762A5056183585', 'https://semopenalex.org/authorship/W4319452484A5019693610', 'https://semopenalex.org/authorship/W2946308339A5056183585', 'https://semopenalex.org/authorship/W2885122621A5056183585', 'https://semopenalex.org/authorship/W4399126764A5056183585', 'https://semopenalex.org/authorship/W4214504130A5056183585', 'https://semopenalex.org/authorship/W2752561456A5056183585', 'https://semopenalex.org/authorship/W2461856634A5019693610', 'https://semopenalex.org/authorship/W3033704563A5056183585', 'https://semopenalex.org/authorship/W2725971658A5056183585', 'https://semopenalex.org/authorship/W3163327897A5056183585', 'https://semopenalex.org/authorship/W3182364466A5056183585', 'https://semopenalex.org/authorship/W2518694405A5019693610', 'https://semopenalex.org/authorship/W2288812598A5056183585', 'https://semopenalex.org/authorship/W4307204790A5019693610', 'https://semopenalex.org/authorship/W2775793881A5056183585', 'https://semopenalex.org/authorship/W4391423303A5019693610', 'https://semopenalex.org/authorship/W4366588423A5056183585', 'https://semopenalex.org/authorship/W4310446060A5019693610', 'https://semopenalex.org/authorship/W2978422619A5056183585', 'https://semopenalex.org/authorship/W2019487042A5056183585', 'https://semopenalex.org/authorship/W1985504739A5056183585', 'https://semopenalex.org/authorship/W3062298123A5056183585', 'https://semopenalex.org/authorship/W4211095911A5056183585', 'https://semopenalex.org/authorship/W1553133540A5056183585', 'https://semopenalex.org/authorship/W2968884122A5056183585', 'https://semopenalex.org/authorship/W3034123328A5056183585', 'https://semopenalex.org/authorship/W2921194733A5056183585', 'https://semopenalex.org/authorship/W4287729941A5056183585', 'https://semopenalex.org/authorship/W1834136374A5056183585', 'https://semopenalex.org/authorship/W3201213010A5056183585', 'https://semopenalex.org/authorship/W862033376A5056183585', 'https://semopenalex.org/authorship/W4211259494A5056183585', 'https://semopenalex.org/authorship/W4404915142A5056183585', 'https://semopenalex.org/authorship/W4366598255A5056183585', 'https://semopenalex.org/authorship/W3186694431A5019693610', 'https://semopenalex.org/authorship/W1771936601A5056183585', 'https://semopenalex.org/authorship/W3121775658A5019693610', 'https://semopenalex.org/authorship/W4307475355A5056183585', 'https://semopenalex.org/authorship/W4251839844A5056183585', 'https://semopenalex.org/authorship/W2725971658A5019693610', 'https://semopenalex.org/authorship/W2795503716A5019693610', 'https://semopenalex.org/authorship/W2346600598A5056183585', 'https://semopenalex.org/authorship/W2273076933A5056183585', 'https://semopenalex.org/authorship/W2978827769A5019693610', 'https://semopenalex.org/authorship/W2762577600A5019693610', 'https://semopenalex.org/authorship/W2557881781A5019693610', 'https://semopenalex.org/authorship/W3163078982A5019693610', 'https://semopenalex.org/authorship/W4324151651A5056183585', 'https://semopenalex.org/authorship/W3196785132A5019693610', 'https://semopenalex.org/authorship/W3119309106A5019693610', 'https://semopenalex.org/authorship/W4389891943A5019693610', 'https://semopenalex.org/authorship/W4393067517A5056183585', 'https://semopenalex.org/authorship/W2942324097A5056183585', 'https://semopenalex.org/authorship/W2012358521A5056183585', 'https://semopenalex.org/authorship/W4386163788A5019693610', 'https://semopenalex.org/authorship/W4230032809A5056183585', 'https://semopenalex.org/authorship/W3029899401A5056183585', 'https://semopenalex.org/authorship/W2263778529A5056183585', 'https://semopenalex.org/authorship/W4312572845A5019693610', 'https://semopenalex.org/authorship/W4393752214A5056183585', 'https://semopenalex.org/authorship/W3161959528A5056183585', 'https://semopenalex.org/authorship/W4387421144A5056183585', 'https://semopenalex.org/authorship/W1704771702A5056183585', 'https://semopenalex.org/authorship/W4394883037A5019693610', 'https://semopenalex.org/authorship/W2344158693A5056183585', 'https://semopenalex.org/authorship/W2519914856A5056183585', 'https://semopenalex.org/authorship/W3161889270A5056183585', 'https://semopenalex.org/authorship/W3096658838A5056183585', 'https://semopenalex.org/authorship/W2752031858A5019693610', 'https://semopenalex.org/authorship/W3194688439A5019693610', 'https://semopenalex.org/authorship/W4366549587A5019693610', 'https://semopenalex.org/authorship/W2072697691A5056183585', 'https://semopenalex.org/authorship/W4213455276A5056183585', 'https://semopenalex.org/authorship/W2977979696A5056183585', 'https://semopenalex.org/authorship/W3110075456A5056183585', 'https://semopenalex.org/authorship/W3030577208A5056183585', 'https://semopenalex.org/authorship/W2791540051A5056183585', 'https://semopenalex.org/authorship/W2754101670A5019693610', 'https://semopenalex.org/authorship/W3028790862A5056183585', 'https://semopenalex.org/authorship/W2037697732A5056183585', 'https://semopenalex.org/authorship/W2024357873A5019693610', 'https://semopenalex.org/authorship/W3161202338A5019693610', 'https://semopenalex.org/authorship/W2082538501A5056183585', 'https://semopenalex.org/authorship/W4229043996A5019693610', 'https://semopenalex.org/authorship/W2465877051A5056183585', 'https://semopenalex.org/authorship/W4389897704A5019693610', 'https://semopenalex.org/authorship/W1975028026A5056183585', 'https://semopenalex.org/authorship/W3142764819A5056183585', 'https://semopenalex.org/authorship/W2401872729A5019693610', 'https://semopenalex.org/authorship/W3022986551A5019693610', 'https://semopenalex.org/authorship/W2159491375A5056183585', 'https://semopenalex.org/authorship/W4401406766A5019693610', 'https://semopenalex.org/authorship/W4200525013A5056183585', 'https://semopenalex.org/authorship/W4396832885A5056183585', 'https://semopenalex.org/authorship/W3204393727A5056183585', 'https://semopenalex.org/authorship/W3033866035A5056183585', 'https://semopenalex.org/authorship/W3206712787A5056183585', 'https://semopenalex.org/authorship/W2913475584A5056183585', 'https://semopenalex.org/authorship/W2898822823A5056183585', 'https://semopenalex.org/authorship/W2768260654A5056183585', 'https://semopenalex.org/authorship/W3096988350A5056183585', 'https://semopenalex.org/authorship/W3130372017A5056183585', 'https://semopenalex.org/authorship/W1993984611A5019693610', 'https://semopenalex.org/authorship/W2898820983A5056183585', 'https://semopenalex.org/authorship/W4210768549A5056183585', 'https://semopenalex.org/authorship/W2972889118A5056183585', 'https://semopenalex.org/authorship/W2902941289A5056183585', 'https://semopenalex.org/authorship/W4404026276A5019693610', 'https://semopenalex.org/authorship/W4241528240A5019693610', 'https://semopenalex.org/authorship/W4366583171A5019693610', 'https://semopenalex.org/authorship/W2977911811A5056183585', 'https://semopenalex.org/authorship/W1710215999A5056183585', 'https://semopenalex.org/authorship/W3009160614A5019693610', 'https://semopenalex.org/authorship/W2611151946A5019693610', 'https://semopenalex.org/authorship/W4383220643A5056183585', 'https://semopenalex.org/authorship/W2789478762A5019693610', 'https://semopenalex.org/authorship/W1246643588A5019693610', 'https://semopenalex.org/authorship/W2520077052A5019693610', 'https://semopenalex.org/authorship/W3028180736A5056183585', 'https://semopenalex.org/authorship/W2346027641A5019693610', 'https://semopenalex.org/authorship/W2898145840A5056183585', 'https://semopenalex.org/authorship/W4404873047A5019693610', 'https://semopenalex.org/authorship/W1568803211A5056183585', 'https://semopenalex.org/authorship/W2602429360A5056183585', 'https://semopenalex.org/authorship/W4221065578A5056183585', 'https://semopenalex.org/authorship/W3200245219A5056183585', 'https://semopenalex.org/authorship/W4387606708A5019693610', 'https://semopenalex.org/authorship/W2110284634A5056183585', 'https://semopenalex.org/authorship/W2972759039A5056183585', 'https://semopenalex.org/authorship/W2977597077A5056183585', 'https://semopenalex.org/authorship/W2940716241A5019693610', 'https://semopenalex.org/authorship/W4393908582A5056183585', 'https://semopenalex.org/authorship/W2007978709A5056183585', 'https://semopenalex.org/authorship/W4402722131A5019693610', 'https://semopenalex.org/authorship/W2811468211A5056183585', 'https://semopenalex.org/authorship/W2087800309A5019693610', 'https://semopenalex.org/authorship/W2972600126A5056183585', 'https://semopenalex.org/authorship/W3193717464A5056183585', 'https://semopenalex.org/authorship/W3047192924A5056183585', 'https://semopenalex.org/authorship/W2063007215A5056183585', 'https://semopenalex.org/authorship/W2944843734A5019693610', 'https://semopenalex.org/authorship/W3035628382A5019693610', 'https://semopenalex.org/authorship/W3198359754A5019693610', 'https://semopenalex.org/authorship/W3184531492A5056183585', 'https://semopenalex.org/authorship/W2033617925A5056183585', 'https://semopenalex.org/authorship/W4324152586A5056183585', 'https://semopenalex.org/authorship/W2551155618A5056183585', 'https://semopenalex.org/authorship/W2033680836A5056183585', 'https://semopenalex.org/authorship/W3197280612A5056183585', 'https://semopenalex.org/authorship/W2119929248A5056183585', 'https://semopenalex.org/authorship/W2075286904A5019693610', 'https://semopenalex.org/authorship/W4406805368A5019693610', 'https://semopenalex.org/authorship/W2605978692A5056183585', 'https://semopenalex.org/authorship/W4394825420A5019693610', 'https://semopenalex.org/authorship/W4309619903A5019693610', 'https://semopenalex.org/authorship/W2068367136A5056183585', 'https://semopenalex.org/authorship/W1965526182A5056183585', 'https://semopenalex.org/authorship/W3201451193A5019693610', 'https://semopenalex.org/authorship/W3206366132A5019693610', 'https://semopenalex.org/authorship/W2409578015A5019693610', 'https://semopenalex.org/authorship/W3171875220A5019693610', 'https://semopenalex.org/authorship/W2519730427A5019693610', 'https://semopenalex.org/authorship/W2753363725A5056183585', 'https://semopenalex.org/authorship/W4386929049A5019693610', 'https://semopenalex.org/authorship/W2921533080A5056183585', 'https://semopenalex.org/authorship/W2898667062A5056183585', 'https://semopenalex.org/authorship/W2318574332A5019693610', 'https://semopenalex.org/authorship/W3094759305A5056183585', 'https://semopenalex.org/authorship/W3000816869A5019693610', 'https://semopenalex.org/authorship/W3005470382A5056183585', 'https://semopenalex.org/authorship/W2752490344A5019693610', 'https://semopenalex.org/authorship/W2576215493A5056183585', 'https://semopenalex.org/authorship/W1484203263A5056183585', 'https://semopenalex.org/authorship/W2968293343A5056183585', 'https://semopenalex.org/authorship/W4292261957A5056183585', 'https://semopenalex.org/authorship/W1751138515A5019693610', 'https://semopenalex.org/authorship/W4283397308A5019693610', 'https://semopenalex.org/authorship/W2793897377A5056183585', 'https://semopenalex.org/authorship/W4393877125A5056183585', 'https://semopenalex.org/authorship/W2537880674A5056183585', 'https://semopenalex.org/authorship/W2973046614A5056183585', 'https://semopenalex.org/authorship/W2613908791A5056183585', 'https://semopenalex.org/authorship/W4294891921A5056183585', 'https://semopenalex.org/authorship/W2942324097A5019693610', 'https://semopenalex.org/authorship/W4366583934A5019693610', 'https://semopenalex.org/authorship/W2165066165A5056183585', 'https://semopenalex.org/authorship/W3178374478A5056183585', 'https://semopenalex.org/authorship/W2897414246A5056183585', 'https://semopenalex.org/authorship/W2966384546A5056183585', 'https://semopenalex.org/authorship/W3090583924A5019693610', 'https://semopenalex.org/authorship/W3196772354A5056183585', 'https://semopenalex.org/authorship/W4393067390A5056183585', 'https://semopenalex.org/authorship/W2519558346A5056183585', 'https://semopenalex.org/authorship/W2139733095A5019693610', 'https://semopenalex.org/authorship/W1877041815A5056183585', 'https://semopenalex.org/authorship/W2169202944A5019693610', 'https://semopenalex.org/authorship/W3215451397A5019693610', 'https://semopenalex.org/authorship/W2149683870A5019693610', 'https://semopenalex.org/authorship/W2092202628A5056183585', 'https://semopenalex.org/authorship/W1998431265A5019693610', 'https://semopenalex.org/authorship/W3095740806A5056183585', 'https://semopenalex.org/authorship/W4366597679A5056183585', 'https://semopenalex.org/authorship/W2548042282A5056183585', 'https://semopenalex.org/authorship/W4393908582A5019693610', 'https://semopenalex.org/authorship/W2294361658A5056183585', 'https://semopenalex.org/authorship/W3110591323A5056183585', 'https://semopenalex.org/authorship/W2080327955A5019693610', 'https://semopenalex.org/authorship/W2798335699A5056183585', 'https://semopenalex.org/authorship/W1860259465A5056183585', 'https://semopenalex.org/authorship/W2131570437A5056183585', 'https://semopenalex.org/authorship/W3161974712A5019693610', 'https://semopenalex.org/authorship/W4389256452A5019693610', 'https://semopenalex.org/authorship/W3007521088A5019693610', 'https://semopenalex.org/authorship/W2903849727A5019693610', 'https://semopenalex.org/authorship/W2610676428A5056183585', 'https://semopenalex.org/authorship/W4315777028A5056183585', 'https://semopenalex.org/authorship/W3141512745A5056183585', 'https://semopenalex.org/authorship/W3206712787A5019693610', 'https://semopenalex.org/authorship/W2567779880A5056183585', 'https://semopenalex.org/authorship/W2976524236A5056183585', 'https://semopenalex.org/authorship/W791468510A5056183585', 'https://semopenalex.org/authorship/W2973140914A5056183585', 'https://semopenalex.org/authorship/W2901616108A5056183585', 'https://semopenalex.org/authorship/W3033839905A5056183585', 'https://semopenalex.org/authorship/W2904910662A5019693610', 'https://semopenalex.org/authorship/W2089266363A5056183585', 'https://semopenalex.org/authorship/W2755506150A5019693610', 'https://semopenalex.org/authorship/W3203088685A5019693610', 'https://semopenalex.org/authorship/W4366547357A5056183585', 'https://semopenalex.org/authorship/W3126826400A5019693610', 'https://semopenalex.org/authorship/W2294561329A5019693610', 'https://semopenalex.org/authorship/W2078369692A5056183585', 'https://semopenalex.org/authorship/W2520077052A5056183585', 'https://semopenalex.org/authorship/W1522158218A5056183585', 'https://semopenalex.org/authorship/W4238249729A5056183585', 'https://semopenalex.org/authorship/W3188766356A5019693610', 'https://semopenalex.org/authorship/W4391210282A5056183585', 'https://semopenalex.org/authorship/W2929751249A5019693610', 'https://semopenalex.org/authorship/W4308467568A5056183585', 'https://semopenalex.org/authorship/W2898627444A5019693610', 'https://semopenalex.org/authorship/W3163921267A5056183585', 'https://semopenalex.org/authorship/W2090841027A5019693610', 'https://semopenalex.org/authorship/W3190617503A5056183585', 'https://semopenalex.org/authorship/W3188420011A5056183585', 'https://semopenalex.org/authorship/W2060118520A5019693610', 'https://semopenalex.org/authorship/W2114418543A5056183585', 'https://semopenalex.org/authorship/W2061583538A5056183585', 'https://semopenalex.org/authorship/W3032662532A5019693610', 'https://semopenalex.org/authorship/W3037695612A5019693610', 'https://semopenalex.org/authorship/W2561633795A5056183585', 'https://semopenalex.org/authorship/W4404569483A5019693610', 'https://semopenalex.org/authorship/W2755164339A5019693610', 'https://semopenalex.org/authorship/W4312282153A5056183585', 'https://semopenalex.org/authorship/W4220905243A5056183585', 'https://semopenalex.org/authorship/W2753671526A5056183585', 'https://semopenalex.org/authorship/W4377250056A5056183585', 'https://semopenalex.org/authorship/W2137846113A5056183585', 'https://semopenalex.org/authorship/W4312841490A5019693610', 'https://semopenalex.org/authorship/W4225133274A5019693610', 'https://semopenalex.org/authorship/W2129488573A5019693610', 'https://semopenalex.org/authorship/W4256454723A5056183585', 'https://semopenalex.org/authorship/W4241289669A5019693610', 'https://semopenalex.org/authorship/W1524596993A5056183585', 'https://semopenalex.org/authorship/W4393877125A5019693610', 'https://semopenalex.org/authorship/W2972702127A5056183585', 'https://semopenalex.org/authorship/W2072490274A5019693610', 'https://semopenalex.org/authorship/W2088270376A5056183585', 'https://semopenalex.org/authorship/W4214593503A5056183585', 'https://semopenalex.org/authorship/W2625122753A5019693610', 'https://semopenalex.org/authorship/W2975736083A5056183585', 'https://semopenalex.org/authorship/W2091382943A5019693610', 'https://semopenalex.org/authorship/W3177151358A5056183585', 'https://semopenalex.org/authorship/W2921058600A5056183585', 'https://semopenalex.org/authorship/W3162177365A5056183585', 'https://semopenalex.org/authorship/W2752493326A5056183585', 'https://semopenalex.org/authorship/W4366967286A5019693610', 'https://semopenalex.org/authorship/W4200018492A5019693610', 'https://semopenalex.org/authorship/W4200616097A5056183585', 'https://semopenalex.org/authorship/W2139733095A5056183585', 'https://semopenalex.org/authorship/W4287071181A5019693610', 'https://semopenalex.org/authorship/W3193396842A5056183585', 'https://semopenalex.org/authorship/W1510660243A5056183585', 'https://semopenalex.org/authorship/W3084729599A5019693610', 'https://semopenalex.org/authorship/W4404373433A5056183585', 'https://semopenalex.org/authorship/W2611685970A5056183585', 'https://semopenalex.org/authorship/W2293208404A5019693610', 'https://semopenalex.org/authorship/W3204110051A5056183585', 'https://semopenalex.org/authorship/W2108512685A5056183585', 'https://semopenalex.org/authorship/W4224242333A5056183585', 'https://semopenalex.org/authorship/W2017727997A5056183585', 'https://semopenalex.org/authorship/W3202016550A5056183585', 'https://semopenalex.org/authorship/W3135072684A5056183585', 'https://semopenalex.org/authorship/W2121082751A5056183585', 'https://semopenalex.org/authorship/W1993514406A5056183585', 'https://semopenalex.org/authorship/W4210450354A5019693610', 'https://semopenalex.org/authorship/W2736312195A5056183585', 'https://semopenalex.org/authorship/W2903417746A5056183585', 'https://semopenalex.org/authorship/W2054886944A5019693610', 'https://semopenalex.org/authorship/W4324150147A5056183585', 'https://semopenalex.org/authorship/W4225088745A5019693610', 'https://semopenalex.org/authorship/W2944843734A5056183585', 'https://semopenalex.org/authorship/W3183940262A5019693610', 'https://semopenalex.org/authorship/W4230967253A5019693610', 'https://semopenalex.org/authorship/W2177601947A5019693610', 'https://semopenalex.org/authorship/W3112877194A5019693610', 'https://semopenalex.org/authorship/W4239396382A5056183585', 'https://semopenalex.org/authorship/W4404977899A5056183585', 'https://semopenalex.org/authorship/W2909558410A5019693610', 'https://semopenalex.org/authorship/W3095367321A5019693610', 'https://semopenalex.org/authorship/W2133951180A5056183585', 'https://semopenalex.org/authorship/W2598459295A5056183585', 'https://semopenalex.org/authorship/W2102667737A5056183585', 'https://semopenalex.org/authorship/W4234952088A5056183585', 'https://semopenalex.org/authorship/W1976594634A5056183585', 'https://semopenalex.org/authorship/W2024357873A5056183585', 'https://semopenalex.org/authorship/W3160199101A5019693610', 'https://semopenalex.org/authorship/W4214684069A5056183585', 'https://semopenalex.org/authorship/W3011317564A5019693610', 'https://semopenalex.org/authorship/W2052607251A5056183585', 'https://semopenalex.org/authorship/W2752493326A5019693610', 'https://semopenalex.org/authorship/W3028614762A5056183585', 'https://semopenalex.org/authorship/W2896178739A5056183585', 'https://semopenalex.org/authorship/W2520661109A5056183585', 'https://semopenalex.org/authorship/W4379033872A5019693610', 'https://semopenalex.org/authorship/W3015284588A5056183585', 'https://semopenalex.org/authorship/W4361189030A5056183585', 'https://semopenalex.org/authorship/W2610780371A5056183585', 'https://semopenalex.org/authorship/W4385856456A5056183585', 'https://semopenalex.org/authorship/W2102905932A5056183585', 'https://semopenalex.org/authorship/W2790187313A5056183585', 'https://semopenalex.org/authorship/W2519250278A5056183585', 'https://semopenalex.org/authorship/W2067004171A5056183585', 'https://semopenalex.org/authorship/W2888386951A5056183585', 'https://semopenalex.org/authorship/W3030149602A5056183585', 'https://semopenalex.org/authorship/W2981708234A5019693610', 'https://semopenalex.org/authorship/W2152557601A5056183585', 'https://semopenalex.org/authorship/W2899389394A5019693610', 'https://semopenalex.org/authorship/W2774467220A5056183585', 'https://semopenalex.org/authorship/W1985142918A5056183585', 'https://semopenalex.org/authorship/W2008208122A5019693610', 'https://semopenalex.org/authorship/W3181801907A5056183585', 'https://semopenalex.org/authorship/W3003369003A5056183585', 'https://semopenalex.org/authorship/W3031395001A5019693610', 'https://semopenalex.org/authorship/W3112090964A5056183585', 'https://semopenalex.org/authorship/W2610274107A5056183585', 'https://semopenalex.org/authorship/W2079488626A5056183585', 'https://semopenalex.org/authorship/W4393752214A5019693610', 'https://semopenalex.org/authorship/W3163521409A5019693610', 'https://semopenalex.org/authorship/W2136876773A5056183585', 'https://semopenalex.org/authorship/W2410138785A5019693610', 'https://semopenalex.org/authorship/W2973016298A5056183585', 'https://semopenalex.org/authorship/W1981715407A5019693610', 'https://semopenalex.org/authorship/W3033480106A5056183585', 'https://semopenalex.org/authorship/W2920869031A5019693610', 'https://semopenalex.org/authorship/W4399763801A5019693610', 'https://semopenalex.org/authorship/W2057014910A5056183585', 'https://semopenalex.org/authorship/W2156243282A5056183585', 'https://semopenalex.org/authorship/W2055070571A5019693610', 'https://semopenalex.org/authorship/W2602397751A5056183585', 'https://semopenalex.org/authorship/W3095347735A5056183585', 'https://semopenalex.org/authorship/W2591593006A5056183585', 'https://semopenalex.org/authorship/W2798335699A5019693610', 'https://semopenalex.org/authorship/W2751622533A5056183585', 'https://semopenalex.org/authorship/W4245844025A5019693610', 'https://semopenalex.org/authorship/W2750727230A5056183585', 'https://semopenalex.org/authorship/W4224305168A5056183585', 'https://semopenalex.org/authorship/W2810881717A5056183585', 'https://semopenalex.org/authorship/W2899333601A5056183585', 'https://semopenalex.org/authorship/W2057014910A5019693610', 'https://semopenalex.org/authorship/W3160545975A5019693610', 'https://semopenalex.org/authorship/W3035727063A5056183585', 'https://semopenalex.org/authorship/W4242142265A5056183585', 'https://semopenalex.org/authorship/W3003204379A5019693610', 'https://semopenalex.org/authorship/W2753801751A5056183585', 'https://semopenalex.org/authorship/W4224255688A5056183585', 'https://semopenalex.org/authorship/W4400189062A5019693610', 'https://semopenalex.org/authorship/W4400430993A5019693610', 'https://semopenalex.org/authorship/W2972419497A5056183585', 'https://semopenalex.org/authorship/W2752042616A5056183585', 'https://semopenalex.org/authorship/W2256119246A5056183585', 'https://semopenalex.org/authorship/W2895512277A5056183585', 'https://semopenalex.org/authorship/W2519458229A5056183585', 'https://semopenalex.org/authorship/W2902563098A5056183585', 'https://semopenalex.org/authorship/W3163085734A5019693610', 'https://semopenalex.org/authorship/W2737450254A5056183585', 'https://semopenalex.org/authorship/W2187647369A5056183585', 'https://semopenalex.org/authorship/W2346600598A5019693610', 'https://semopenalex.org/authorship/W2513683703A5056183585', 'https://semopenalex.org/authorship/W2088502162A5056183585', 'https://semopenalex.org/authorship/W2752658305A5056183585', 'https://semopenalex.org/authorship/W4232727837A5056183585', 'https://semopenalex.org/authorship/W2942738233A5019693610', 'https://semopenalex.org/authorship/W4393102879A5056183585', 'https://semopenalex.org/authorship/W3024164567A5019693610', 'https://semopenalex.org/authorship/W2977617583A5056183585', 'https://semopenalex.org/authorship/W4324154015A5056183585', 'https://semopenalex.org/authorship/W4239396382A5019693610', 'https://semopenalex.org/authorship/W3121062173A5019693610', 'https://semopenalex.org/authorship/W3032857618A5056183585', 'https://semopenalex.org/authorship/W4379879736A5019693610', 'https://semopenalex.org/authorship/W4387085789A5019693610', 'https://semopenalex.org/authorship/W1982984133A5019693610', 'https://semopenalex.org/authorship/W3043824623A5056183585', 'https://semopenalex.org/authorship/W2738622408A5056183585', 'https://semopenalex.org/authorship/W3091007149A5019693610', 'https://semopenalex.org/authorship/W2751429127A5056183585', 'https://semopenalex.org/authorship/W3036463368A5056183585', 'https://semopenalex.org/authorship/W2520352456A5056183585', 'https://semopenalex.org/authorship/W4312646439A5056183585']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/authorship/W2132364404A5056164318', 'https://semopenalex.org/authorship/W2036165062A5051587506', 'https://semopenalex.org/authorship/W4396894716A5051587506', 'https://semopenalex.org/authorship/W2809782991A5056164318', 'https://semopenalex.org/authorship/W4405120549A5051587506', 'https://semopenalex.org/authorship/W1979289740A5056164318', 'https://semopenalex.org/authorship/W1995950498A5051587506', 'https://semopenalex.org/authorship/W4253850266A5051587506', 'https://semopenalex.org/authorship/W2210223524A5051587506', 'https://semopenalex.org/authorship/W2122571865A5051587506', 'https://semopenalex.org/authorship/W2398987072A5051587506', 'https://semopenalex.org/authorship/W2062957328A5056164318', 'https://semopenalex.org/authorship/W2219017076A5051587506', 'https://semopenalex.org/authorship/W2903213374A5051587506', 'https://semopenalex.org/authorship/W2805153701A5056164318', 'https://semopenalex.org/authorship/W2941373095A5056164318', 'https://semopenalex.org/authorship/W1999508547A5051587506', 'https://semopenalex.org/authorship/W4240245530A5051587506', 'https://semopenalex.org/authorship/W1990091852A5051587506', 'https://semopenalex.org/authorship/W1965382252A5056164318', 'https://semopenalex.org/authorship/W4393146711A5051587506', 'https://semopenalex.org/authorship/W2161850606A5051587506', 'https://semopenalex.org/authorship/W1986827696A5051587506', 'https://semopenalex.org/authorship/W2903194584A5051587506', 'https://semopenalex.org/authorship/W4386814402A5056164318', 'https://semopenalex.org/authorship/W2112979372A5051587506', 'https://semopenalex.org/authorship/W4253131601A5051587506', 'https://semopenalex.org/authorship/W1995308547A5051587506', 'https://semopenalex.org/authorship/W2111759980A5051587506', 'https://semopenalex.org/authorship/W4249963731A5051587506', 'https://semopenalex.org/authorship/W2165818457A5056164318', 'https://semopenalex.org/authorship/W2109705305A5056164318', 'https://semopenalex.org/authorship/W2116314971A5051587506', 'https://semopenalex.org/authorship/W2560712448A5056164318', 'https://semopenalex.org/authorship/W2144918660A5051587506', 'https://semopenalex.org/authorship/W4249594017A5051587506', 'https://semopenalex.org/authorship/W2035518282A5056164318', 'https://semopenalex.org/authorship/W1633573314A5051587506', 'https://semopenalex.org/authorship/W2043269074A5051587506', 'https://semopenalex.org/authorship/W2070215238A5051587506', 'https://semopenalex.org/authorship/W1982314073A5056164318', 'https://semopenalex.org/authorship/W2074193071A5051587506', 'https://semopenalex.org/authorship/W2162338867A5056164318', 'https://semopenalex.org/authorship/W2031625065A5051587506', 'https://semopenalex.org/authorship/W2004738891A5051587506', 'https://semopenalex.org/authorship/W2062243122A5051587506', 'https://semopenalex.org/authorship/W2064672353A5051587506', 'https://semopenalex.org/authorship/W2293459815A5056164318', 'https://semopenalex.org/authorship/W2042756792A5051587506', 'https://semopenalex.org/authorship/W2411894725A5056164318', 'https://semopenalex.org/authorship/W3130320973A5056164318', 'https://semopenalex.org/authorship/W2112535726A5056164318', 'https://semopenalex.org/authorship/W1577463177A5051587506', 'https://semopenalex.org/authorship/W2666172191A5051587506', 'https://semopenalex.org/authorship/W2025546942A5056164318', 'https://semopenalex.org/authorship/W2104408001A5051587506', 'https://semopenalex.org/authorship/W2754948093A5051587506', 'https://semopenalex.org/authorship/W1501172792A5056164318', 'https://semopenalex.org/authorship/W2512795596A5056164318', 'https://semopenalex.org/authorship/W2625986270A5051587506', 'https://semopenalex.org/authorship/W4401943800A5056164318', 'https://semopenalex.org/authorship/W2129869483A5051587506', 'https://semopenalex.org/authorship/W2039163755A5051587506', 'https://semopenalex.org/authorship/W2171606781A5051587506', 'https://semopenalex.org/authorship/W2060283246A5051587506', 'https://semopenalex.org/authorship/W325059703A5051587506', 'https://semopenalex.org/authorship/W2072776346A5051587506', 'https://semopenalex.org/authorship/W1969516436A5051587506', 'https://semopenalex.org/authorship/W2910014621A5051587506', 'https://semopenalex.org/authorship/W1990193612A5056164318', 'https://semopenalex.org/authorship/W4255531846A5051587506', 'https://semopenalex.org/authorship/W2497743975A5051587506', 'https://semopenalex.org/authorship/W2115899637A5051587506', 'https://semopenalex.org/authorship/W2401687993A5051587506', 'https://semopenalex.org/authorship/W3160200186A5051587506', 'https://semopenalex.org/authorship/W2804376295A5056164318', 'https://semopenalex.org/authorship/W2149899452A5051587506', 'https://semopenalex.org/authorship/W2554047600A5051587506', 'https://semopenalex.org/authorship/W2611767226A5051587506', 'https://semopenalex.org/authorship/W2907364096A5051587506', 'https://semopenalex.org/authorship/W2800308132A5051587506', 'https://semopenalex.org/authorship/W2129869483A5056164318', 'https://semopenalex.org/authorship/W2532447822A5051587506', 'https://semopenalex.org/authorship/W4206683427A5051587506', 'https://semopenalex.org/authorship/W2917706508A5051587506', 'https://semopenalex.org/authorship/W4392713273A5051587506', 'https://semopenalex.org/authorship/W4366964206A5056164318', 'https://semopenalex.org/authorship/W4401578804A5056164318', 'https://semopenalex.org/authorship/W2356144191A5056164318', 'https://semopenalex.org/authorship/W4400946519A5051587506', 'https://semopenalex.org/authorship/W2401583884A5051587506', 'https://semopenalex.org/authorship/W2120355631A5051587506', 'https://semopenalex.org/authorship/W67894965A5051587506', 'https://semopenalex.org/authorship/W2895854254A5051587506', 'https://semopenalex.org/authorship/W2024612964A5051587506', 'https://semopenalex.org/authorship/W2748533023A5051587506', 'https://semopenalex.org/authorship/W2240362173A5051587506', 'https://semopenalex.org/authorship/W3107887875A5051587506', 'https://semopenalex.org/authorship/W2968293641A5056164318', 'https://semopenalex.org/authorship/W4316659889A5051587506', 'https://semopenalex.org/authorship/W1991853935A5051587506', 'https://semopenalex.org/authorship/W2895967513A5051587506', 'https://semopenalex.org/authorship/W2789263069A5056164318', 'https://semopenalex.org/authorship/W2413288731A5051587506', 'https://semopenalex.org/authorship/W2135598717A5056164318', 'https://semopenalex.org/authorship/W2184299809A5051587506', 'https://semopenalex.org/authorship/W1608276691A5051587506', 'https://semopenalex.org/authorship/W2028566173A5056164318', 'https://semopenalex.org/authorship/W2947626283A5056164318', 'https://semopenalex.org/authorship/W3089291192A5051587506', 'https://semopenalex.org/authorship/W196228518A5056164318', 'https://semopenalex.org/authorship/W2080817506A5056164318', 'https://semopenalex.org/authorship/W2883856658A5051587506', 'https://semopenalex.org/authorship/W3092453362A5051587506', 'https://semopenalex.org/authorship/W2123532445A5051587506', 'https://semopenalex.org/authorship/W2204033782A5051587506', 'https://semopenalex.org/authorship/W2981465620A5051587506', 'https://semopenalex.org/authorship/W2945691872A5056164318', 'https://semopenalex.org/authorship/W857122145A5051587506', 'https://semopenalex.org/authorship/W2761828172A5051587506', 'https://semopenalex.org/authorship/W2496039851A5051587506', 'https://semopenalex.org/authorship/W2073709132A5051587506', 'https://semopenalex.org/authorship/W2102190590A5051587506', 'https://semopenalex.org/authorship/W2188799909A5051587506', 'https://semopenalex.org/authorship/W979651393A5051587506', 'https://semopenalex.org/authorship/W4367360032A5051587506', 'https://semopenalex.org/authorship/W2011410844A5051587506', 'https://semopenalex.org/authorship/W2150998397A5051587506', 'https://semopenalex.org/authorship/W2885100636A5051587506', 'https://semopenalex.org/authorship/W2744837872A5051587506', 'https://semopenalex.org/authorship/W2062904953A5051587506', 'https://semopenalex.org/authorship/W4392942581A5051587506', 'https://semopenalex.org/authorship/W2473052796A5051587506', 'https://semopenalex.org/authorship/W2606501011A5056164318', 'https://semopenalex.org/authorship/W2496567738A5051587506', 'https://semopenalex.org/authorship/W48804293A5051587506', 'https://semopenalex.org/authorship/W2288294525A5051587506', 'https://semopenalex.org/authorship/W2596027452A5051587506', 'https://semopenalex.org/authorship/W1422159917A5051587506', 'https://semopenalex.org/authorship/W2230115501A5051587506', 'https://semopenalex.org/authorship/W4392577068A5051587506', 'https://semopenalex.org/authorship/W2138922641A5051587506', 'https://semopenalex.org/authorship/W2134444560A5051587506', 'https://semopenalex.org/authorship/W2527344267A5051587506', 'https://semopenalex.org/authorship/W2076330335A5051587506', 'https://semopenalex.org/authorship/W2094708864A5056164318', 'https://semopenalex.org/authorship/W2515896452A5056164318', 'https://semopenalex.org/authorship/W2288534976A5051587506', 'https://semopenalex.org/authorship/W2138291705A5051587506', 'https://semopenalex.org/authorship/W2163138922A5051587506', 'https://semopenalex.org/authorship/W2550712691A5051587506', 'https://semopenalex.org/authorship/W2786601708A5051587506', 'https://semopenalex.org/authorship/W1514325539A5051587506', 'https://semopenalex.org/authorship/W1538415416A5056164318', 'https://semopenalex.org/authorship/W4231226382A5051587506', 'https://semopenalex.org/authorship/W2144750318A5056164318', 'https://semopenalex.org/authorship/W2079895649A5056164318', 'https://semopenalex.org/authorship/W4401021691A5051587506', 'https://semopenalex.org/authorship/W4376526615A5051587506', 'https://semopenalex.org/authorship/W3021203574A5051587506', 'https://semopenalex.org/authorship/W146617261A5051587506', 'https://semopenalex.org/authorship/W565256208A5051587506', 'https://semopenalex.org/authorship/W2015849174A5051587506', 'https://semopenalex.org/authorship/W2058904901A5056164318', 'https://semopenalex.org/authorship/W1933806665A5051587506', 'https://semopenalex.org/authorship/W2029131637A5051587506', 'https://semopenalex.org/authorship/W2172143183A5051587506', 'https://semopenalex.org/authorship/W2145502705A5051587506', 'https://semopenalex.org/authorship/W1584206897A5056164318', 'https://semopenalex.org/authorship/W2072209700A5051587506', 'https://semopenalex.org/authorship/W4405094102A5056164318', 'https://semopenalex.org/authorship/W2001905011A5051587506', 'https://semopenalex.org/authorship/W2092005371A5051587506', 'https://semopenalex.org/authorship/W2166217821A5051587506', 'https://semopenalex.org/authorship/W2081189334A5051587506', 'https://semopenalex.org/authorship/W3179020455A5051587506', 'https://semopenalex.org/authorship/W4250489070A5051587506', 'https://semopenalex.org/authorship/W2139454561A5051587506', 'https://semopenalex.org/authorship/W1544524730A5056164318', 'https://semopenalex.org/authorship/W3013997466A5051587506', 'https://semopenalex.org/authorship/W2747040169A5051587506', 'https://semopenalex.org/authorship/W2106211998A5051587506', 'https://semopenalex.org/authorship/W2804891820A5051587506', 'https://semopenalex.org/authorship/W3157167113A5051587506', 'https://semopenalex.org/authorship/W1791684062A5051587506', 'https://semopenalex.org/authorship/W2139436497A5051587506', 'https://semopenalex.org/authorship/W2755469263A5051587506', 'https://semopenalex.org/authorship/W2024012113A5051587506', 'https://semopenalex.org/authorship/W4296365397A5051587506', 'https://semopenalex.org/authorship/W2111424373A5051587506', 'https://semopenalex.org/authorship/W2068524892A5051587506', 'https://semopenalex.org/authorship/W2068973986A5051587506', 'https://semopenalex.org/authorship/W160837981A5051587506', 'https://semopenalex.org/authorship/W3095131015A5051587506', 'https://semopenalex.org/authorship/W2742916377A5051587506', 'https://semopenalex.org/authorship/W2089241417A5051587506', 'https://semopenalex.org/authorship/W2954164432A5051587506', 'https://semopenalex.org/authorship/W1544524730A5051587506', 'https://semopenalex.org/authorship/W1494162500A5056164318', 'https://semopenalex.org/authorship/W102421301A5051587506', 'https://semopenalex.org/authorship/W2077200079A5051587506', 'https://semopenalex.org/authorship/W1857000584A5051587506', 'https://semopenalex.org/authorship/W2095834672A5051587506', 'https://semopenalex.org/authorship/W1974886156A5051587506', 'https://semopenalex.org/authorship/W1860740456A5056164318', 'https://semopenalex.org/authorship/W2159662334A5051587506', 'https://semopenalex.org/authorship/W2044900380A5051587506', 'https://semopenalex.org/authorship/W2559559327A5056164318', 'https://semopenalex.org/authorship/W3016161880A5051587506', 'https://semopenalex.org/authorship/W4396665589A5056164318', 'https://semopenalex.org/authorship/W2513883066A5051587506', 'https://semopenalex.org/authorship/W2401381263A5056164318', 'https://semopenalex.org/authorship/W3042004637A5051587506', 'https://semopenalex.org/authorship/W1177607589A5051587506', 'https://semopenalex.org/authorship/W2569889271A5051587506', 'https://semopenalex.org/authorship/W1584206897A5051587506', 'https://semopenalex.org/authorship/W3200674364A5051587506', 'https://semopenalex.org/authorship/W2786657846A5051587506', 'https://semopenalex.org/authorship/W2171510346A5051587506', 'https://semopenalex.org/authorship/W2501830935A5051587506', 'https://semopenalex.org/authorship/W2950468099A5051587506', 'https://semopenalex.org/authorship/W48804293A5056164318', 'https://semopenalex.org/authorship/W2557110996A5056164318', 'https://semopenalex.org/authorship/W1494063694A5051587506', 'https://semopenalex.org/authorship/W4321614042A5056164318', 'https://semopenalex.org/authorship/W2034050419A5051587506', 'https://semopenalex.org/authorship/W2571158126A5051587506', 'https://semopenalex.org/authorship/W2063650982A5051587506', 'https://semopenalex.org/authorship/W4205212276A5051587506', 'https://semopenalex.org/authorship/W2982452767A5051587506', 'https://semopenalex.org/authorship/W3136727059A5056164318', 'https://semopenalex.org/authorship/W2542642724A5051587506', 'https://semopenalex.org/authorship/W4294672395A5051587506', 'https://semopenalex.org/authorship/W4285408205A5051587506', 'https://semopenalex.org/authorship/W2061231005A5051587506', 'https://semopenalex.org/authorship/W2883395494A5056164318', 'https://semopenalex.org/authorship/W1999149743A5051587506', 'https://semopenalex.org/authorship/W4252093019A5051587506', 'https://semopenalex.org/authorship/W1998201483A5051587506', 'https://semopenalex.org/authorship/W2290200834A5051587506', 'https://semopenalex.org/authorship/W2896727063A5056164318', 'https://semopenalex.org/authorship/W2768649200A5051587506', 'https://semopenalex.org/authorship/W4392188385A5051587506', 'https://semopenalex.org/authorship/W2550667658A5051587506', 'https://semopenalex.org/authorship/W4376630019A5051587506', 'https://semopenalex.org/authorship/W1654176175A5051587506', 'https://semopenalex.org/authorship/W2803258972A5051587506', 'https://semopenalex.org/authorship/W1908879184A5051587506', 'https://semopenalex.org/authorship/W2056096508A5051587506', 'https://semopenalex.org/authorship/W4206307909A5051587506', 'https://semopenalex.org/authorship/W2075578427A5056164318', 'https://semopenalex.org/authorship/W52623672A5056164318', 'https://semopenalex.org/authorship/W2142079724A5056164318', 'https://semopenalex.org/authorship/W4205613083A5056164318', 'https://semopenalex.org/authorship/W2088723639A5051587506', 'https://semopenalex.org/authorship/W2156138095A5051587506', 'https://semopenalex.org/authorship/W2901316497A5051587506', 'https://semopenalex.org/authorship/W1990019789A5051587506', 'https://semopenalex.org/authorship/W2002312562A5051587506', 'https://semopenalex.org/authorship/W3187351556A5051587506', 'https://semopenalex.org/authorship/W4210325270A5051587506', 'https://semopenalex.org/authorship/W2077737077A5051587506', 'https://semopenalex.org/authorship/W2538630038A5056164318', 'https://semopenalex.org/authorship/W2478910470A5051587506', 'https://semopenalex.org/authorship/W2165377954A5051587506', 'https://semopenalex.org/authorship/W1840794446A5051587506', 'https://semopenalex.org/authorship/W2163180953A5051587506', 'https://semopenalex.org/authorship/W2170201418A5051587506', 'https://semopenalex.org/authorship/W143942840A5051587506', 'https://semopenalex.org/authorship/W2966031361A5051587506', 'https://semopenalex.org/authorship/W4206807237A5051587506', 'https://semopenalex.org/authorship/W41465441A5051587506', 'https://semopenalex.org/authorship/W2044237546A5051587506', 'https://semopenalex.org/authorship/W49790452A5051587506', 'https://semopenalex.org/authorship/W1573590416A5051587506', 'https://semopenalex.org/authorship/W2246286794A5051587506', 'https://semopenalex.org/authorship/W2516286998A5051587506', 'https://semopenalex.org/authorship/W3004301528A5056164318', 'https://semopenalex.org/authorship/W149383384A5051587506', 'https://semopenalex.org/authorship/W2029818237A5056164318', 'https://semopenalex.org/authorship/W4285216643A5056164318', 'https://semopenalex.org/authorship/W158943908A5051587506', 'https://semopenalex.org/authorship/W1973148750A5051587506', 'https://semopenalex.org/authorship/W2170913025A5051587506', 'https://semopenalex.org/authorship/W4401808601A5051587506', 'https://semopenalex.org/authorship/W1933806665A5056164318', 'https://semopenalex.org/authorship/W2610600517A5051587506', 'https://semopenalex.org/authorship/W2407231546A5051587506', 'https://semopenalex.org/authorship/W3157283285A5056164318', 'https://semopenalex.org/authorship/W2167521347A5056164318', 'https://semopenalex.org/authorship/W4230332361A5051587506', 'https://semopenalex.org/authorship/W3096110661A5051587506', 'https://semopenalex.org/authorship/W2923039095A5051587506', 'https://semopenalex.org/authorship/W1922706319A5051587506', 'https://semopenalex.org/authorship/W3017031701A5051587506', 'https://semopenalex.org/authorship/W2147456231A5051587506', 'https://semopenalex.org/authorship/W2041108261A5056164318', 'https://semopenalex.org/authorship/W4390512166A5051587506', 'https://semopenalex.org/authorship/W3097508557A5051587506', 'https://semopenalex.org/authorship/W33403252A5051587506', 'https://semopenalex.org/authorship/W3211349420A5056164318', 'https://semopenalex.org/authorship/W2130803541A5051587506', 'https://semopenalex.org/authorship/W2586727473A5051587506', 'https://semopenalex.org/authorship/W1608886591A5056164318', 'https://semopenalex.org/authorship/W2131405606A5056164318', 'https://semopenalex.org/authorship/W2153457047A5051587506', 'https://semopenalex.org/authorship/W4306173842A5051587506', 'https://semopenalex.org/authorship/W2291113318A5056164318', 'https://semopenalex.org/authorship/W2495352272A5051587506', 'https://semopenalex.org/authorship/W2120216356A5051587506', 'https://semopenalex.org/authorship/W2024786226A5051587506', 'https://semopenalex.org/authorship/W2170201418A5056164318', 'https://semopenalex.org/authorship/W3162144158A5051587506', 'https://semopenalex.org/authorship/W2124703480A5051587506', 'https://semopenalex.org/authorship/W2162066092A5051587506', 'https://semopenalex.org/authorship/W2170741870A5051587506', 'https://semopenalex.org/authorship/W196228518A5051587506', 'https://semopenalex.org/authorship/W2998201073A5051587506', 'https://semopenalex.org/authorship/W4253265224A5051587506', 'https://semopenalex.org/authorship/W2130007135A5051587506', 'https://semopenalex.org/authorship/W2794572176A5056164318', 'https://semopenalex.org/authorship/W2945300184A5056164318', 'https://semopenalex.org/authorship/W4252463735A5051587506', 'https://semopenalex.org/authorship/W1857000584A5056164318', 'https://semopenalex.org/authorship/W3206895939A5051587506', 'https://semopenalex.org/authorship/W1969462495A5051587506', 'https://semopenalex.org/authorship/W3085760006A5056164318', 'https://semopenalex.org/authorship/W1448329507A5051587506', 'https://semopenalex.org/authorship/W4387450689A5051587506', 'https://semopenalex.org/authorship/W2754307650A5051587506', 'https://semopenalex.org/authorship/W2137861763A5056164318', 'https://semopenalex.org/authorship/W2012912450A5056164318', 'https://semopenalex.org/authorship/W1986540981A5056164318', 'https://semopenalex.org/authorship/W2095968352A5051587506', 'https://semopenalex.org/authorship/W3118215277A5051587506', 'https://semopenalex.org/authorship/W1943042767A5056164318', 'https://semopenalex.org/authorship/W652412083A5051587506', 'https://semopenalex.org/authorship/W2080996134A5051587506', 'https://semopenalex.org/authorship/W2150298155A5051587506', 'https://semopenalex.org/authorship/W3206640136A5051587506', 'https://semopenalex.org/authorship/W2078326945A5051587506', 'https://semopenalex.org/authorship/W2144750318A5051587506', 'https://semopenalex.org/authorship/W2413863213A5051587506', 'https://semopenalex.org/authorship/W2929921254A5051587506', 'https://semopenalex.org/authorship/W4286571613A5051587506', 'https://semopenalex.org/authorship/W2147139299A5051587506', 'https://semopenalex.org/authorship/W2066111880A5051587506', 'https://semopenalex.org/authorship/W2041334917A5051587506', 'https://semopenalex.org/authorship/W2128563460A5051587506', 'https://semopenalex.org/authorship/W2109186457A5056164318', 'https://semopenalex.org/authorship/W4404030648A5051587506', 'https://semopenalex.org/authorship/W2034179412A5051587506', 'https://semopenalex.org/authorship/W2484374542A5051587506', 'https://semopenalex.org/authorship/W3095279071A5051587506', 'https://semopenalex.org/authorship/W1481133633A5051587506', 'https://semopenalex.org/authorship/W2293958373A5056164318', 'https://semopenalex.org/authorship/W4389321773A5056164318', 'https://semopenalex.org/authorship/W2188362632A5051587506', 'https://semopenalex.org/authorship/W2475285031A5051587506', 'https://semopenalex.org/authorship/W4237620799A5056164318', 'https://semopenalex.org/authorship/W1985701940A5056164318', 'https://semopenalex.org/authorship/W1999134690A5051587506', 'https://semopenalex.org/authorship/W2139255754A5051587506', 'https://semopenalex.org/authorship/W2111277352A5051587506', 'https://semopenalex.org/authorship/W2612784784A5051587506', 'https://semopenalex.org/authorship/W2138320177A5056164318', 'https://semopenalex.org/authorship/W1569686365A5056164318', 'https://semopenalex.org/authorship/W2098948701A5051587506', 'https://semopenalex.org/authorship/W2111964097A5056164318', 'https://semopenalex.org/authorship/W4394742902A5056164318', 'https://semopenalex.org/authorship/W214032606A5056164318', 'https://semopenalex.org/authorship/W2138433001A5051587506', 'https://semopenalex.org/authorship/W2756387886A5051587506', 'https://semopenalex.org/authorship/W2625256202A5051587506', 'https://semopenalex.org/authorship/W2140805995A5051587506', 'https://semopenalex.org/authorship/W25440647A5051587506', 'https://semopenalex.org/authorship/W2903545243A5051587506', 'https://semopenalex.org/authorship/W2412127048A5051587506', 'https://semopenalex.org/authorship/W2145747218A5051587506', 'https://semopenalex.org/authorship/W4289655844A5051587506', 'https://semopenalex.org/authorship/W2092477317A5056164318', 'https://semopenalex.org/authorship/W4237745095A5051587506', 'https://semopenalex.org/authorship/W328613600A5051587506', 'https://semopenalex.org/authorship/W4402830551A5051587506', 'https://semopenalex.org/authorship/W2620890574A5056164318', 'https://semopenalex.org/authorship/W2016989291A5051587506', 'https://semopenalex.org/authorship/W1506027738A5051587506', 'https://semopenalex.org/authorship/W2004738891A5056164318', 'https://semopenalex.org/authorship/W4404030068A5051587506', 'https://semopenalex.org/authorship/W2967876484A5051587506', 'https://semopenalex.org/authorship/W2624802634A5051587506', 'https://semopenalex.org/authorship/W1517253300A5051587506', 'https://semopenalex.org/authorship/W12268595A5051587506', 'https://semopenalex.org/authorship/W2103224970A5051587506', 'https://semopenalex.org/authorship/W402024038A5051587506', 'https://semopenalex.org/authorship/W2052982204A5051587506', 'https://semopenalex.org/authorship/W2608491785A5051587506', 'https://semopenalex.org/authorship/W2163881253A5051587506', 'https://semopenalex.org/authorship/W1587236616A5051587506', 'https://semopenalex.org/authorship/W2751662694A5056164318', 'https://semopenalex.org/authorship/W2965366155A5051587506', 'https://semopenalex.org/authorship/W4285815179A5056164318', 'https://semopenalex.org/authorship/W1967677932A5051587506', 'https://semopenalex.org/authorship/W2271801361A5056164318', 'https://semopenalex.org/authorship/W1520936229A5051587506', 'https://semopenalex.org/authorship/W2785105341A5051587506', 'https://semopenalex.org/authorship/W4391156256A5051587506', 'https://semopenalex.org/authorship/W2890543403A5056164318', 'https://semopenalex.org/authorship/W2146033518A5051587506', 'https://semopenalex.org/authorship/W2995911827A5051587506', 'https://semopenalex.org/authorship/W2564132746A5051587506', 'https://semopenalex.org/authorship/W2070269076A5051587506', 'https://semopenalex.org/authorship/W2155718231A5051587506', 'https://semopenalex.org/authorship/W1608886591A5051587506', 'https://semopenalex.org/authorship/W4400238477A5051587506', 'https://semopenalex.org/authorship/W2132053703A5051587506', 'https://semopenalex.org/authorship/W2154510046A5056164318', 'https://semopenalex.org/authorship/W1860740456A5051587506', 'https://semopenalex.org/authorship/W2786606238A5051587506', 'https://semopenalex.org/authorship/W1574380960A5051587506', 'https://semopenalex.org/authorship/W2124560301A5051587506', 'https://semopenalex.org/authorship/W1526915766A5056164318', 'https://semopenalex.org/authorship/W2405266982A5056164318', 'https://semopenalex.org/authorship/W2014241426A5051587506', 'https://semopenalex.org/authorship/W1923826352A5051587506', 'https://semopenalex.org/authorship/W4401579183A5056164318', 'https://semopenalex.org/authorship/W2475545374A5051587506', 'https://semopenalex.org/authorship/W2945412056A5051587506', 'https://semopenalex.org/authorship/W1531223514A5051587506', 'https://semopenalex.org/authorship/W2064476539A5051587506', 'https://semopenalex.org/authorship/W4253855517A5051587506', 'https://semopenalex.org/authorship/W2212338561A5051587506', 'https://semopenalex.org/authorship/W2108876125A5056164318', 'https://semopenalex.org/authorship/W2275014257A5051587506', 'https://semopenalex.org/authorship/W2134768851A5051587506', 'https://semopenalex.org/authorship/W4238734812A5051587506', 'https://semopenalex.org/authorship/W2023972619A5051587506', 'https://semopenalex.org/authorship/W2289149676A5051587506', 'https://semopenalex.org/authorship/W2024336304A5051587506', 'https://semopenalex.org/authorship/W2091944075A5051587506', 'https://semopenalex.org/authorship/W3196495759A5051587506', 'https://semopenalex.org/authorship/W2085435476A5051587506', 'https://semopenalex.org/authorship/W2160391119A5056164318', 'https://semopenalex.org/authorship/W1943042767A5051587506', 'https://semopenalex.org/authorship/W2065803961A5051587506', 'https://semopenalex.org/authorship/W2161966477A5051587506', 'https://semopenalex.org/authorship/W2340283416A5051587506', 'https://semopenalex.org/authorship/W2289584941A5051587506', 'https://semopenalex.org/authorship/W1419972110A5051587506', 'https://semopenalex.org/authorship/W2127414738A5051587506', 'https://semopenalex.org/authorship/W4233681091A5051587506', 'https://semopenalex.org/authorship/W4400946621A5051587506', 'https://semopenalex.org/authorship/W72692433A5051587506', 'https://semopenalex.org/authorship/W2948995623A5051587506', 'https://semopenalex.org/authorship/W858120236A5051587506', 'https://semopenalex.org/authorship/W2044431283A5056164318', 'https://semopenalex.org/authorship/W2293095660A5051587506', 'https://semopenalex.org/authorship/W2058293659A5051587506', 'https://semopenalex.org/authorship/W2144253537A5051587506', 'https://semopenalex.org/authorship/W2146520711A5051587506', 'https://semopenalex.org/authorship/W2886396839A5051587506', 'https://semopenalex.org/authorship/W2768928198A5056164318', 'https://semopenalex.org/authorship/W1994278842A5051587506', 'https://semopenalex.org/authorship/W1991026653A5051587506', 'https://semopenalex.org/authorship/W139668830A5056164318', 'https://semopenalex.org/authorship/W2203509984A5051587506', 'https://semopenalex.org/authorship/W2136654140A5051587506', 'https://semopenalex.org/authorship/W2148646851A5051587506', 'https://semopenalex.org/authorship/W1508821613A5056164318', 'https://semopenalex.org/authorship/W2146002591A5051587506', 'https://semopenalex.org/authorship/W2166520679A5051587506', 'https://semopenalex.org/authorship/W2072553352A5051587506', 'https://semopenalex.org/authorship/W2124054384A5051587506', 'https://semopenalex.org/authorship/W3027319226A5056164318', 'https://semopenalex.org/authorship/W2961776981A5051587506', 'https://semopenalex.org/authorship/W4390187585A5051587506', 'https://semopenalex.org/authorship/W2480965638A5056164318', 'https://semopenalex.org/authorship/W4210708907A5051587506', 'https://semopenalex.org/authorship/W4405935629A5051587506', 'https://semopenalex.org/authorship/W2062957328A5051587506', 'https://semopenalex.org/authorship/W2888177496A5056164318', 'https://semopenalex.org/authorship/W2142484380A5051587506', 'https://semopenalex.org/authorship/W2755359845A5051587506', 'https://semopenalex.org/authorship/W2935942569A5051587506', 'https://semopenalex.org/authorship/W1489534528A5051587506', 'https://semopenalex.org/authorship/W2159139699A5051587506', 'https://semopenalex.org/authorship/W2125143433A5051587506', 'https://semopenalex.org/authorship/W1518248903A5051587506', 'https://semopenalex.org/authorship/W4390188024A5051587506', 'https://semopenalex.org/authorship/W2107191431A5056164318', 'https://semopenalex.org/authorship/W1978851795A5051587506', 'https://semopenalex.org/authorship/W4285503152A5051587506', 'https://semopenalex.org/authorship/W2334327213A5051587506', 'https://semopenalex.org/authorship/W2538630038A5051587506', 'https://semopenalex.org/authorship/W1973125618A5051587506', 'https://semopenalex.org/authorship/W2108304242A5051587506', 'https://semopenalex.org/authorship/W2906163189A5051587506', 'https://semopenalex.org/authorship/W2033725854A5056164318', 'https://semopenalex.org/authorship/W1971283588A5051587506', 'https://semopenalex.org/authorship/W2983014989A5056164318', 'https://semopenalex.org/authorship/W1488510230A5051587506', 'https://semopenalex.org/authorship/W4367360059A5056164318', 'https://semopenalex.org/authorship/W2576879514A5051587506', 'https://semopenalex.org/authorship/W2341007259A5051587506', 'https://semopenalex.org/authorship/W2789144447A5056164318', 'https://semopenalex.org/authorship/W2019708772A5056164318', 'https://semopenalex.org/authorship/W4385626270A5051587506', 'https://semopenalex.org/authorship/W2615205062A5051587506', 'https://semopenalex.org/authorship/W2401333290A5051587506', 'https://semopenalex.org/authorship/W2903177638A5051587506', 'https://semopenalex.org/authorship/W3206850855A5051587506', 'https://semopenalex.org/authorship/W4244005678A5051587506', 'https://semopenalex.org/authorship/W2494421230A5051587506', 'https://semopenalex.org/authorship/W2125308824A5051587506', 'https://semopenalex.org/authorship/W2295164153A5051587506', 'https://semopenalex.org/authorship/W2397834607A5051587506', 'https://semopenalex.org/authorship/W3132353162A5051587506', 'https://semopenalex.org/authorship/W1910867531A5051587506', 'https://semopenalex.org/authorship/W1967568969A5051587506', 'https://semopenalex.org/authorship/W2166211129A5051587506', 'https://semopenalex.org/authorship/W4365802790A5051587506', 'https://semopenalex.org/authorship/W2967954143A5051587506', 'https://semopenalex.org/authorship/W2079466034A5051587506', 'https://semopenalex.org/authorship/W2166826477A5051587506', 'https://semopenalex.org/authorship/W2612282432A5056164318', 'https://semopenalex.org/authorship/W1823956242A5051587506', 'https://semopenalex.org/authorship/W2769445687A5056164318', 'https://semopenalex.org/authorship/W1870822388A5051587506', 'https://semopenalex.org/authorship/W2112107898A5056164318', 'https://semopenalex.org/authorship/W3175708501A5051587506', 'https://semopenalex.org/authorship/W1999631843A5051587506', 'https://semopenalex.org/authorship/W2032099346A5051587506', 'https://semopenalex.org/authorship/W2034507787A5051587506', 'https://semopenalex.org/authorship/W2158569759A5051587506', 'https://semopenalex.org/authorship/W2084854878A5051587506', 'https://semopenalex.org/authorship/W2730743430A5051587506', 'https://semopenalex.org/authorship/W2579158977A5056164318', 'https://semopenalex.org/authorship/W2028754220</t>
+    <t>['https://semopenalex.org/authorship/W2397277866A5086727894', 'https://semopenalex.org/authorship/W2780277126A5086727894', 'https://semopenalex.org/authorship/W4293863370A5086727894', 'https://semopenalex.org/authorship/W2903944530A5086727894', 'https://semopenalex.org/authorship/W2996342798A5086727894', 'https://semopenalex.org/authorship/W3134422373A5086727894', 'https://semopenalex.org/authorship/W3158463786A5086727894', 'https://semopenalex.org/authorship/W3048792033A5086727894', 'https://semopenalex.org/authorship/W2226359063A5086727894', 'https://semopenalex.org/authorship/W2974444355A5086727894', 'https://semopenalex.org/authorship/W2788968669A5086727894', 'https://semopenalex.org/authorship/W1999760195A5086727894', 'https://semopenalex.org/authorship/W2792290921A5086727894', 'https://semopenalex.org/authorship/W2897762537A5086727894', 'https://semopenalex.org/authorship/W4206136166A5086727894', 'https://semopenalex.org/authorship/W2996971450A5086727894', 'https://semopenalex.org/authorship/W2100407406A5086727894', 'https://semopenalex.org/authorship/W2844810377A5086727894', 'https://semopenalex.org/authorship/W2979701877A5086727894', 'https://semopenalex.org/authorship/W4406267825A5086727894', 'https://semopenalex.org/authorship/W2772966323A5086727894', 'https://semopenalex.org/authorship/W2805460435A5086727894', 'https://semopenalex.org/authorship/W4238294234A5086727894', 'https://semopenalex.org/authorship/W3205075200A5086727894', 'https://semopenalex.org/authorship/W4390737683A5086727894', 'https://semopenalex.org/authorship/W2948196949A5086727894', 'https://semopenalex.org/authorship/W4396568545A5086727894', 'https://semopenalex.org/authorship/W4367671449A5086727894', 'https://semopenalex.org/authorship/W2957110867A5086727894', 'https://semopenalex.org/authorship/W3202715770A5086727894']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/location/W25305687642', 'https://semopenalex.org/location/W28000505381', 'https://semopenalex.org/location/W25305687641', 'https://semopenalex.org/location/W42309685121', 'https://semopenalex.org/location/W43791159661', 'https://semopenalex.org/location/W29837826201', 'https://semopenalex.org/location/W32147435071', 'https://semopenalex.org/location/W14838732894', 'https://semopenalex.org/location/W30127488011', 'https://semopenalex.org/location/W20243484451', 'https://semopenalex.org/location/W27956841612', 'https://semopenalex.org/location/W44050344991', 'https://semopenalex.org/location/W27862507821', 'https://semopenalex.org/location/W29000605871', 'https://semopenalex.org/location/W43829818882', 'https://semopenalex.org/location/W15068103471', 'https://semopenalex.org/location/W21429592102', 'https://semopenalex.org/location/W31662312682', 'https://semopenalex.org/location/W31900260261', 'https://semopenalex.org/location/W30455856361', 'https://semopenalex.org/location/W23977394001', 'https://semopenalex.org/location/W30915935821', 'https://semopenalex.org/location/W43068956173', 'https://semopenalex.org/location/W32147435072', 'https://semopenalex.org/location/W30497024891', 'https://semopenalex.org/location/W31871691351', 'https://semopenalex.org/location/W30426697023', 'https://semopenalex.org/location/W44051774161', 'https://semopenalex.org/location/W42383839001', 'https://semopenalex.org/location/W28970790371', 'https://semopenalex.org/location/W30365122661', 'https://semopenalex.org/location/W21311253521', 'https://semopenalex.org/location/W28078943081', 'https://semopenalex.org/location/W24710522091', 'https://semopenalex.org/location/W6149025581', 'https://semopenalex.org/location/W30458346031', 'https://semopenalex.org/location/W30401575511', 'https://semopenalex.org/location/W30919516801', 'https://semopenalex.org/location/W21285198911', 'https://semopenalex.org/location/W42833253261', 'https://semopenalex.org/location/W30882384051', 'https://semopenalex.org/location/W24669668731', 'https://semopenalex.org/location/W28060387991', 'https://semopenalex.org/location/W29649262091', 'https://semopenalex.org/location/W43068956172', 'https://semopenalex.org/location/W43068956175', 'https://semopenalex.org/location/W21660939901', 'https://semopenalex.org/location/W29511010961', 'https://semopenalex.org/location/W25986997551', 'https://semopenalex.org/location/W29951453521', 'https://semopenalex.org/location/W29468737141', 'https://semopenalex.org/location/W25122530981', 'https://semopenalex.org/location/W30888177051', 'https://semopenalex.org/location/W29454079491', 'https://semopenalex.org/location/W43887990101', 'https://semopenalex.org/location/W43811573001', 'https://semopenalex.org/location/W43861592451', 'https://semopenalex.org/location/W44035980142', 'https://semopenalex.org/location/W29414042091', 'https://semopenalex.org/location/W30482369121', 'https://semopenalex.org/location/W42051370691', 'https://semopenalex.org/location/W27676589071', 'https://semopenalex.org/location/W25627600741', 'https://semopenalex.org/location/W31656415443', 'https://semopenalex.org/location/W29421282431', 'https://semopenalex.org/location/W43855562551', 'https://semopenalex.org/location/W42262443241', 'https://semopenalex.org/location/W30345383281', 'https://semopenalex.org/location/W43856175291', 'https://semopenalex.org/location/W43854027001', 'https://semopenalex.org/location/W43823653861', 'https://semopenalex.org/location/W42932502961', 'https://semopenalex.org/location/W43902058871', 'https://semopenalex.org/location/W30032445501', 'https://semopenalex.org/location/W43063173041', 'https://semopenalex.org/location/W42909435511', 'https://semopenalex.org/location/W43869518061', 'https://semopenalex.org/location/W29421075031', 'https://semopenalex.org/location/W30376855032', 'https://semopenalex.org/location/W18774675621', 'https://semopenalex.org/location/W30455098671', 'https://semopenalex.org/location/W15969306701', 'https://semopenalex.org/location/W25862769561', 'https://semopenalex.org/location/W30886117901', 'https://semopenalex.org/location/W30426697021', 'https://semopenalex.org/location/W30948193224', 'https://semopenalex.org/location/W30948193221', 'https://semopenalex.org/location/W30052490041', 'https://semopenalex.org/location/W32088965581', 'https://semopenalex.org/location/W28884399821', 'https://semopenalex.org/location/W26115059681', 'https://semopenalex.org/location/W31803441821', 'https://semopenalex.org/location/W31628635341', 'https://semopenalex.org/location/W43926169801', 'https://semopenalex.org/location/W43046919621', 'https://semopenalex.org/location/W30891714731', 'https://semopenalex.org/location/W28087319251', 'https://semopenalex.org/location/W14838732893', 'https://semopenalex.org/location/W30376855031', 'https://semopenalex.org/location/W27630405051', 'https://semopenalex.org/location/W27654696761', 'https://semopenalex.org/location/W43061604711', 'https://semopenalex.org/location/W42265388351', 'https://semopenalex.org/location/W30885348461', 'https://semopenalex.org/location/W30044603271', 'https://semopenalex.org/location/W43868591711', 'https://semopenalex.org/location/W30948193222', 'https://semopenalex.org/location/W29054320151', 'https://semopenalex.org/location/W26018933081', 'https://semopenalex.org/location/W42474583511', 'https://semopenalex.org/location/W21429592101', 'https://semopenalex.org/location/W30955984631', 'https://semopenalex.org/location/W26266951001', 'https://semopenalex.org/location/W43882799971', 'https://semopenalex.org/location/W23999023701', 'https://semopenalex.org/location/W42856043091', 'https://semopenalex.org/location/W12015545801', 'https://semopenalex.org/location/W27530325001', 'https://semopenalex.org/location/W42312112621', 'https://semopenalex.org/location/W43105296071', 'https://semopenalex.org/location/W21902780251', 'https://semopenalex.org/location/W29946198511', 'https://semopenalex.org/location/W29888192761', 'https://semopenalex.org/location/W43124462061', 'https://semopenalex.org/location/W44052325641', 'https://semopenalex.org/location/W25391549851', 'https://semopenalex.org/location/W27555683841', 'https://semopenalex.org/location/W31749439391', 'https://semopenalex.org/location/W29655391521', 'https://semopenalex.org/location/W43887990103', 'https://semopenalex.org/location/W29859817821', 'https://semopenalex.org/location/W29566225572', 'https://semopenalex.org/location/W30426697022', 'https://semopenalex.org/location/W27396165181', 'https://semopenalex.org/location/W22938731501', 'https://semopenalex.org/location/W31656415442', 'https://semopenalex.org/location/W29946198512', 'https://semopenalex.org/location/W43998794571', 'https://semopenalex.org/location/W29131890991', 'https://semopenalex.org/location/W31033840591', 'https://semopenalex.org/location/W29566225571', 'https://semopenalex.org/location/W28080081831', 'https://semopenalex.org/location/W25077834181', 'https://semopenalex.org/location/W23912393001', 'https://semopenalex.org/location/W43063169091', 'https://semopenalex.org/location/W44035980141', 'https://semopenalex.org/location/W20222792351', 'https://semopenalex.org/location/W30897530231', 'https://semopenalex.org/location/W27920797361', 'https://semopenalex.org/location/W22774936731', 'https://semopenalex.org/location/W14838732891', 'https://semopenalex.org/location/W29640826022', 'https://semopenalex.org/location/W28967664061', 'https://semopenalex.org/location/W43061604713', 'https://semopenalex.org/location/W19698391981', 'https://semopenalex.org/location/W43211235011', 'https://semopenalex.org/location/W21034674991', 'https://semopenalex.org/location/W31006266141', 'https://semopenalex.org/location/W43068956176', 'https://semopenalex.org/location/W31452592371', 'https://semopenalex.org/location/W43666671821', 'https://semopenalex.org/location/W29315761321', 'https://semopenalex.org/location/W2926427961', 'https://semopenalex.org/location/W14838732892', 'https://semopenalex.org/location/W22786769011', 'https://semopenalex.org/location/W27703789261', 'https://semopenalex.org/location/W30948193223', 'https://semopenalex.org/location/W21285198914', 'https://semopenalex.org/location/W21285198912', 'https://semopenalex.org/location/W25842933981', 'https://semopenalex.org/location/W29640826021', 'https://semopenalex.org/location/W31471774571', 'https://semopenalex.org/location/W28844284181', 'https://semopenalex.org/location/W30827033561', 'https://semopenalex.org/location/W26115059682', 'https://semopenalex.org/location/W43068956177', 'https://semopenalex.org/location/W32107593731', 'https://semopenalex.org/location/W29581194931', 'https://semopenalex.org/location/W22966118231', 'https://semopenalex.org/location/W21429592103', 'https://semopenalex.org/location/W44009098861', 'https://semopenalex.org/location/W44027636231', 'https://semopenalex.org/location/W43233386271', 'https://semopenalex.org/location/W1079679441', 'https://semopenalex.org/location/W29843174051', 'https://semopenalex.org/location/W27956841611', 'https://semopenalex.org/location/W30950014991', 'https://semopenalex.org/location/W44068680961', 'https://semopenalex.org/location/W31662312681', 'https://semopenalex.org/location/W18172888851', 'https://semopenalex.org/location/W43931850291', 'https://semopenalex.org/location/W32174702571', 'https://semopenalex.org/location/W28832165761', 'https://semopenalex.org/location/W31656678471', 'https://semopenalex.org/location/W27940330211', 'https://semopenalex.org/location/W30052490042', 'https://semopenalex.org/location/W22190572501', 'https://semopenalex.org/location/W29784152661', 'https://semopenalex.org/location/W30801908571', 'https://semopenalex.org/location/W43068956171', 'https://semopenalex.org/location/W30948193225', 'https://semopenalex.org/location/W43870462191', 'https://semopenalex.org/location/W27487378811', 'https://semopenalex.org/location/W7665864621', 'https://semopenalex.org/location/W32072432981', 'https://semopenalex.org/location/W31515741391', 'https://semopenalex.org/location/W32163023621', 'https://semopenalex.org/location/W43887990102', 'https://semopenalex.org/location/W22465567601', 'https://semopenalex.org/location/W28080081832', 'https://semopenalex.org/location/W21263891551', 'https://semopenalex.org/location/W29781601891', 'https://semopenalex.org/location/W28959508741', 'https://semopenalex.org/location/W42000397651', 'https://semopenalex.org/location/W19231700931', 'https://semopenalex.org/location/W42930562941', 'https://semopenalex.org/location/W22261468281', 'https://semopenalex.org/location/W29916244791', 'https://semopenalex.org/location/W44068802951', 'https://semopenalex.org/location/W42209538491', 'https://semopenalex.org/location/W25193597391', 'https://semopenalex.org/location/W32072432982', 'https://semopenalex.org/location/W32135727241', 'https://semopenalex.org/location/W44035165841', 'https://semopenalex.org/location/W29664832071', 'https://semopenalex.org/location/W43061604712', 'https://semopenalex.org/location/W30032445502', 'https://semopenalex.org/location/W30052490043', 'https://semopenalex.org/location/W30849226791', 'https://semopenalex.org/location/W42261851681', 'https://semopenalex.org/location/W22435911181', 'https://semopenalex.org/location/W31656415441', 'https://semopenalex.org/location/W43129933041', 'https://semopenalex.org/location/W42210492031', 'https://semopenalex.org/location/W32019820662', 'https://semopenalex.org/location/W28837227301', 'https://semopenalex.org/location/W43924539111', 'https://semopenalex.org/location/W21285198913', 'https://semopenalex.org/location/W42059472451', 'https://semopenalex.org/location/W43068956174', 'https://semopenalex.org/location/W24778492681', 'https://semopenalex.org/location/W43061604714', 'https://semopenalex.org/location/W30956804081', 'https://semopenalex.org/location/W43833402031', 'https://semopenalex.org/location/W18955604291', 'https://semopenalex.org/location/W32019820661', 'https://semopenalex.org/location/W22966755681', 'https://semopenalex.org/location/W32083490971', 'https://semopenalex.org/location/W15375095501', 'https://semopenalex.org/location/W18770595181', 'https://semopenalex.org/location/W43870462192', 'https://semopenalex.org/location/W43829818881']</t>
+  </si>
+  <si>
+    <t>['The Great Importance of Cross-Document Relationships for Multi-document Summarization', 'Routing Enforced Generative Model for Recipe Generation', 'https://semopenalex.org/location/W23572746651', 'https://semopenalex.org/location/W31333763863', 'https://semopenalex.org/location/W26149051672', 'Using bilingual knowledge and ensemble techniques for unsupervised Chinese sentiment analysis', 'https://semopenalex.org/location/W42976309841', 'QuoteRec', 'Towards Constructing Sports News from Live Text Commentary', 'https://semopenalex.org/location/W43855741921', 'Evaluating Factuality in Cross-lingual Summarization', 'Massive Styles Transfer with Limited Labeled Data', 'https://semopenalex.org/location/W30356479091', 'A Data-Driven, Factorization Parser for CCG Dependency Structures', "&lt;scp&gt;WL&lt;/scp&gt;‐index: Leveraging citation mention number to quantify an individual's scientific impact", 'Document-Based HITS Model for Multi-document Summarization', 'https://semopenalex.org/location/W44047828401', 'https://semopenalex.org/location/W30034461822', 'Video Paragraph Captioning as a Text Summarization Task', 'https://semopenalex.org/location/W21484376701', 'Point Precisely: Towards Ensuring the Precision of Data in Generated Texts Using Delayed Copy Mechanism', 'EUSUM', 'CC-Riddle: A Question Answering Dataset of Chinese Character Riddles', 'Learning a Product Relevance Model from Click-Through Data in E-Commerce', 'Named Entity Resolution in Chinese News Comments on the Web', 'Document Similarity Search Based on Manifold-Ranking of TextTiles', 'S2ORM', 'TimedTextRank', 'https://semopenalex.org/location/W21415620721', 'https://semopenalex.org/location/W27710802441', 'MC-MKE: A Fine-Grained Multimodal Knowledge Editing Benchmark  Emphasizing Modality Consistency', 'https://semopenalex.org/location/W30342392641', 'https://semopenalex.org/location/W43916023241', 'https://semopenalex.org/location/W31032919081', 'https://semopenalex.org/location/W19947926601', 'Towards a Novel Association Measure via Web Search Results Mining', 'https://semopenalex.org/location/W43066765701', 'Recent advances in document summarization', 'https://semopenalex.org/location/W15021839891', 'Adversarial Text Generation via Sequence Contrast Discrimination', 'https://semopenalex.org/location/W15379794301', 'Phrase-based Compressive Cross-Language Summarization', 'https://semopenalex.org/location/W29517811211', 'https://semopenalex.org/location/W1192140891', 'https://semopenalex.org/location/W22510249081', 'https://semopenalex.org/location/W31607062801', 'https://semopenalex.org/location/W31770344582', 'https://semopenalex.org/location/W22947499631', 'AKMiner: Domain-Specific Knowledge Graph Mining from Academic Literatures', 'https://semopenalex.org/location/W25624397971', 'https://semopenalex.org/location/W42882874653', 'https://semopenalex.org/location/W19875310391', 'Semantic Dependency Parsing via Book Embedding', 'https://semopenalex.org/location/W24007992601', 'Tweet Timeline Generation with Determinantal Point Processes', 'https://semopenalex.org/location/W42261619781', 'https://semopenalex.org/location/W25090054321', 'https://semopenalex.org/location/W31746799441', 'A New Re-ranking Method for Generic Chinese Text Summarization and Its Evaluation', 'Social Biases in Automatic Evaluation Metrics for NLG', 'AMRec: an intelligent system for academic method recommendation', 'Exploiting neighborhood knowledge for single document summarization and keyphrase extraction', 'https://semopenalex.org/location/W31747592141', 'https://semopenalex.org/location/W29980564851', 'https://semopenalex.org/location/W25576652171', 'Semantic Parsing for English as a Second Language', 'Is Summary Useful or Not? An Extrinsic Human Evaluation of Text Summaries on Downstream Tasks', 'CodeQA: A Question Answering Dataset for Source Code Comprehension', 'https://semopenalex.org/location/W43874281231', 'https://semopenalex.org/location/W28991688921', 'https://semopenalex.org/location/W30347733621', 'https://semopenalex.org/location/W32138258991', 'https://semopenalex.org/location/W18981012602', 'Homophonic Pun Generation with Lexically Constrained Rewriting', 'https://semopenalex.org/location/W32137654601', 'Automatic Text Simplification', 'https://semopenalex.org/location/W29063600401', 'https://semopenalex.org/location/W31848521944', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering Task-Specific Styles', 'Single document keyphrase extraction using neighborhood knowledge', 'https://semopenalex.org/location/W43895204022', 'Comparing Knowledge-Intensive and Data-Intensive Models for English Resource Semantic Parsing', 'https://semopenalex.org/location/W28871614501', 'https://semopenalex.org/location/W20498562311', 'https://semopenalex.org/location/W15005290131', 'https://semopenalex.org/location/W42869677631', 'https://semopenalex.org/location/W25115328441', 'Leveraging Diverse Lexical Chains to Construct Essays for Chinese College Entrance Examination', 'https://semopenalex.org/location/W27990449701', 'https://semopenalex.org/location/W30352029331', 'https://semopenalex.org/location/W43784652742', 'Overview of Baidu Cup 2016: Challenge on Entity Search', 'https://semopenalex.org/location/W32137654602', 'https://semopenalex.org/location/W30833650751', 'A practical system for harvesting and monitoring hot topics on the web', 'Towards a unified approach to document similarity search using manifold-ranking of blocks', 'https://semopenalex.org/location/W27591811581', 'Sentiment Analysis of Peer Review Texts for Scholarly Papers', 'Neural Maximum Subgraph Parsing for Cross-Domain Semantic Dependency Analysis', 'https://semopenalex.org/location/W42242380072', 'Improved affinity graph based multi-document summarization', 'A Syntax-Guided Grammatical Error Correction Model with Dependency Tree Correction', 'Human-like Summarization Evaluation with ChatGPT', 'Cross-Language Opinion Target Extraction in Review Texts', 'https://semopenalex.org/location/W29985189891', 'https://semopenalex.org/location/W1540197011', 'https://semopenalex.org/location/W16557712492', 'https://semopenalex.org/location/W31746000991', 'https://semopenalex.org/location/W31990421561', 'https://semopenalex.org/location/W42869677632', 'https://semopenalex.org/location/W43875596752', 'https://semopenalex.org/location/W29872059511', 'Revisiting Pivot-Based Paraphrase Generation: Language Is Not the Only Optional Pivot', 'Automatic Text Simplification&lt;i&gt;Horacio Saggion&lt;/i&gt; (Universitat Pompeu Fabra) Morgan &amp;amp; Claypool (Synthesis Lectures on Human Language Technologies, edited by Graeme Hirst, volume 37), 2017, xvi+121 pp; paperback, ISBN 978-1-62705-868-1; ebook, ISBN 978-1-62705-869-8; doi:10.2200/S00700ED1V01Y201602HLT032', 'https://semopenalex.org/location/W29894899231', 'Proceedings of the 61st Annual Meeting of the Association for Computational Linguistics (Volume 1: Long Papers)', 'https://semopenalex.org/location/W43855706661', 'https://semopenalex.org/location/W43135339181', 'https://semopenalex.org/location/W32085278861', 'Manifold-ranking based topic-focused multi-document summarization', 'https://semopenalex.org/location/W32125749963', 'https://semopenalex.org/location/W43068023853', 'How to Avoid Sentences Spelling Boring? Towards a Neural Approach to Unsupervised Metaphor Generation', 'Improving Word Embeddings for Antonym Detection Using Thesauri and SentiWordNet', 'Grammatical Relations in Chinese: GB-Ground Extraction and Data-Driven Parsing', 'Stabilization/solidification of lead- and cadmium-containing tailings for cemented paste backfill by using clinker-free binders', 'https://semopenalex.org/location/W31333763861', 'Multi-Domain Sentiment Classification Based on Domain-Aware Embedding and Attention', 'https://semopenalex.org/location/W30431573303', 'Parsing Chinese Sentences with Grammatical Relations', 'https://semopenalex.org/location/W14478392231', 'https://semopenalex.org/location/W29517811212', 'https://semopenalex.org/location/W29740710332', 'Towards a Universal Sentiment Classifier in Multiple languages', 'Generating Diverse and Descriptive Image Captions Using Visual Paraphrases', 'https://semopenalex.org/location/W15483875481', 'https://semopenalex.org/location/W1785624211', 'https://semopenalex.org/location/W30342096831', 'Compressive document summarization via sparse optimization', 'PPSGen: learning to generate presentation slides for academic papers', 'Overview of the NLPCC-ICCPOL 2016 Shared Task: Sports News Generation from Live Webcast Scripts', 'https://semopenalex.org/location/W30984117503', 'An Empirical Study of Automatic Post-Editing', 'Describe Images in a Boring Way: Towards Cross-Modal Sarcasm Generation', 'Combining Content and Context Similarities for Image Retrieval', 'https://semopenalex.org/location/W30343783231', 'https://semopenalex.org/location/W42837839231', 'Towards Automatic Construction of News Overview Articles by News Synthesis', 'TransModality: An End2End Fusion Method with Transformer for Multimodal Sentiment Analysis', 'https://semopenalex.org/location/W8277644471', 'https://semopenalex.org/location/W31531285152', 'https://semopenalex.org/location/W28991688922', 'https://semopenalex.org/location/W43938519781', 'Reducing Approximation and Estimation Errors for Chinese Lexical Processing with Heterogeneous Annotations', 'ATSUM: Extracting Attractive Summaries for News Propagation on Microblogs', 'https://semopenalex.org/location/W14993440701', 'https://semopenalex.org/location/W30431573302', 'https://semopenalex.org/location/W42838066501', 'Content Selection for Real-time Sports News Construction from Commentary Texts', 'https://semopenalex.org/location/W43875611321', 'https://semopenalex.org/location/W43063531621', 'Dependency-based Mixture Language Models', 'https://semopenalex.org/location/W43098001051', 'https://semopenalex.org/location/W42264767652', 'https://semopenalex.org/location/W21326438521', 'https://semopenalex.org/location/W43855702241', 'https://semopenalex.org/location/W44026716922', 'A Neural Network Approach to Quote Recommendation in Writings', 'https://semopenalex.org/location/W15387621891', 'https://semopenalex.org/location/W29640107141', 'TransSum: Translating Aspect and Sentiment Embeddings for Self-Supervised Opinion Summarization', 'https://semopenalex.org/location/W43855713642', 'https://semopenalex.org/location/W43092020842', 'Overview of the NLPCC 2018 Shared Task: Grammatical Error Correction', 'https://semopenalex.org/location/W43784652743', 'https://semopenalex.org/location/W32114636871', 'https://semopenalex.org/location/W27986003981', 'https://semopenalex.org/location/W27871759461', 'Better AMR-To-Text Generation with Graph Structure Reconstruction', 'https://semopenalex.org/location/W27414383491', 'Visualizing timelines', 'Automatic Generation of Citation Texts in Scholarly Papers: A Pilot Study', 'On the Helpfulness of Document Context to Sentence Simplification', 'Learning to Explain Ambiguous Headlines of Online News', 'https://semopenalex.org/location/W20527844861', 'https://semopenalex.org/location/W22506227611', 'https://semopenalex.org/location/W29835618061', 'https://semopenalex.org/location/W43875611322', 'Effects of Additional Ring-Fusion Site on Dual Reactivity Based Dynamic Covalent Chemistry', 'https://semopenalex.org/location/W43855706662', 'PaCoST: Paired Confidence Significance Testing for Benchmark  Contamination Detection in Large Language Models', 'https://semopenalex.org/location/W19838737911', 'https://semopenalex.org/location/W42211412063', 'https://semopenalex.org/location/W22512270291', 'https://semopenalex.org/location/W43801365213', 'PKUSUMSUM : A Java Platform for Multilingual Document Summarization', 'RST Discourse Parsing as Text-to-Text Generation', 'A Neural Approach to Irony Generation', 'https://semopenalex.org/location/W15006269141', 'New Datasets and Controllable Iterative Data Augmentation Method for Code-switching ASR Error Correction', 'Incorporating Cross-Document Relationships Between Sentences for Single Document Summarizations', 'https://semopenalex.org/location/W27403899911', 'https://semopenalex.org/location/W31678084402', 'https://semopenalex.org/location/W28910358391', 'https://semopenalex.org/location/W29630087172', 'https://semopenalex.org/location/W27566397301', 'https://semopenalex.org/location/W43066765703', 'Block-Based Similarity Search on the Web Using Manifold-Ranking', 'https://semopenalex.org/location/W42964147591', 'https://semopenalex.org/location/W42339074421', 'https://semopenalex.org/location/W42909481091', 'https://semopenalex.org/location/W42257837861', 'https://semopenalex.org/location/W29723392301', 'Domain-Adaptive Neural Automated Essay Scoring', 'https://semopenalex.org/location/W42260991372', 'https://semopenalex.org/location/W31761057411', 'DivGAN: Towards Diverse Paraphrase Generation via Diversified Generative Adversarial Network', 'https://semopenalex.org/location/W31227944381', 'https://semopenalex.org/location/W31037018011', 'Overview of the NLPCC 2023 Shared Task: Chinese Spelling Check', 'Automatic Slides Generation for Scholarly Papers: A Fine-Grained Dataset and Baselines (Student Abstract)', 'https://semopenalex.org/location/W21321415111', 'Learning information diffusion process on the web', 'https://semopenalex.org/location/W25985692201', 'https://semopenalex.org/location/W43801365211', 'https://semopenalex.org/location/W42261619782', 'Recent advances of neural text generation: Core tasks, datasets, models and challenges', 'https://semopenalex.org/location/W32114636872', 'https://semopenalex.org/location/W43897135851', 'https://semopenalex.org/location/W22505462022', 'https://semopenalex.org/location/W30879979901', 'Proceedings of the 61st Annual Meeting of the Association for Computational Linguistics (Volume 2: Short Papers)', 'https://semopenalex.org/location/W27867448431', 'https://semopenalex.org/location/W18981012601', 'https://semopenalex.org/location/W43929046831', 'https://semopenalex.org/location/W43868757901', 'https://semopenalex.org/location/W31770344583', 'Defining and Detecting Vulnerability in Human Evaluation Guidelines: A Preliminary Study Towards Reliable NLG Evaluation', 'https://semopenalex.org/location/W24236365061', 'Automated Chess Commentator Powered by Neural Chess Engine', 'Structure-Aware Pre-Training for Table-to-Text Generation', 'https://semopenalex.org/location/W31006826081', 'Neural Comment Generation for Source Code with Auxiliary Code Classification Task', 'https://semopenalex.org/location/W44039954721', 'BiCWS: Mining Cognitive Differences from Bilingual Web Search Results', 'A Measure Based on Optimal Matching in Graph Theory for Document Similarity', 'https://semopenalex.org/location/W43799335313', 'https://semopenalex.org/location/W29521434102', 'https://semopenalex.org/location/W29631289871', 'https://semopenalex.org/location/W43233667202', 'https://semopenalex.org/location/W31747592142', 'Missing Information, Unresponsive Authors, Experimental Flaws: The Impossibility of Assessing the Reproducibility of Previous Human Evaluations in NLP', 'CMiner: Opinion Extraction and Summarization for Chinese Microblogs', 'https://semopenalex.org/location/W42883741952', 'https://semopenalex.org/location/W42976309843', 'https://semopenalex.org/location/W44026719331', 'https://semopenalex.org/location/W43925385321', 'https://semopenalex.org/location/W25128623461', 'https://semopenalex.org/location/W15323504681', 'https://semopenalex.org/location/W43683042411', 'https://semopenalex.org/location/W26149051671', 'https://semopenalex.org/location/W29533315241', 'How Do Seq2Seq Models Perform on End-to-End Data-to-Text Generation?', 'DSGram: Dynamic Weighting Sub-Metrics for Grammatical Error Correction  in the Era of Large Language Models', 'Automatic Text Simplification Horacio Saggion (Universitat Pompeu Fabra) Morgan &amp; Claypool (Synthesis Lectures on Human Language Technologies, edited by Graeme Hirst, volume 37), 2017, xvi+121 pp; paperback, ISBN 978-1-62705-868-1; hardcover, ISBN 978-1-68173-214-5, $69.95; ebook, ISBN 978-1-62705-869-8, $39.96; doi: 10.2200/S00700ED1V01Y201602HLT032.', 'Neural Text Generation with Part-of-Speech Guided Softmax.', 'https://semopenalex.org/location/W20756591941', 'PKUTM at TREC 2010 Blog Track', 'Guiding Abstractive Dialogue Summarization with Content Planning', 'https://semopenalex.org/location/W29174748341', 'https://semopenalex.org/location/W30127214842', 'https://semopenalex.org/location/W43895240061', 'https://semopenalex.org/location/W20806564951', 'https://semopenalex.org/location/W43873157802', 'https://semopenalex.org/location/W16226003861', 'https://semopenalex.org/location/W42883741951', 'Nearest Neighbor Knowledge Distillation for Neural Machine Translation', 'SimpleBERT: A Pre-trained Model That Learns to Generate Simple Words', 'https://semopenalex.org/location/W28864741021', 'WikiIns: A High-Quality Dataset for Controlled Text Editing by Natural Language Instruction', 'https://semopenalex.org/location/W43852928982', 'https://semopenalex.org/location/W32114636873', 'Heterogeneous Graph Transformer for Graph-to-Sequence Learning', 'https://semopenalex.org/location/W42878546701', 'https://semopenalex.org/location/W43210141362', 'Data-driven, PCFG-based and Pseudo-PCFG-based Models for Chinese Dependency Parsing', 'https://semopenalex.org/location/W27987789741', 'https://semopenalex.org/location/W20360909521', 'https://semopenalex.org/location/W43092020843', 'Continual Learning for Neural Machine Translation', 'https://semopenalex.org/location/W43855708741', 'https://semopenalex.org/location/W43855720261', 'https://semopenalex.org/location/W43931470201', 'A Neural Approach to Pun Generation', 'https://semopenalex.org/location/W21415147001', 'https://semopenalex.org/location/W43895194311', 'https://semopenalex.org/location/W42964147593', 'WordRank-Based Lexical Signatures for Finding Lost or Related Web Pages', "x-index: a fantastic new indicator for quantifying a scientist's scientific impact", 'https://semopenalex.org/location/W20713320641', 'https://semopenalex.org/location/W44047823791', 'https://semopenalex.org/location/W27983276441', 'https://semopenalex.org/location/W21327791921', 'https://semopenalex.org/location/W21068657141', 'https://semopenalex.org/location/W43855713641', 'MOVER: Mask, Over-generate and Rank for Hyperbole Generation', 'Clinical challenges and management of primary renal epithelioid angiomyolipoma of duplex kidney with paraneoplastic syndrome', 'https://semopenalex.org/location/W19738942781', 'https://semopenalex.org/location/W43895238911', 'https://semopenalex.org/location/W28988529961', 'https://semopenalex.org/location/W27721872051', 'https://semopenalex.org/location/W31032919082', 'https://semopenalex.org/location/W43994230971', 'https://semopenalex.org/location/W44026716921', 'https://semopenalex.org/location/W43831757962', 'CollabRank', 'Mining and Analyzing the Future Works in Scientific Articles', 'https://semopenalex.org/location/W42133481041', 'https://semopenalex.org/location/W42883368243', 'https://semopenalex.org/location/W42882874652', 'Automatic Labeling of Topic Models Using Text Summaries', 'CrossDial: An Entertaining Dialogue Dataset of Chinese Crosstalk', 'Style-Compress: An LLM-Based Prompt Compression Framework Considering  Task-Specific Styles', 'https://semopenalex.org/location/W682814491', 'https://semopenalex.org/location/W29709013301', 'https://semopenalex.org/location/W31678084401', 'https://semopenalex.org/location/W32130735991', 'https://semopenalex.org/location/W21139822041', 'Jointly Learning to Align and Summarize for Neural Cross-Lingual Summarization', 'A Comprehensive Evaluation and Analysis Study for Chinese Spelling Check', 'https://semopenalex.org/location/W15454762401', 'CTSUM', 'https://semopenalex.org/location/W28961243511', 'Reference Matters: Benchmarking Factual Error Correction for Dialogue Summarization with Fine-grained Evaluation Framework', 'Collaborative Data Cleaning for Sentiment Classification with Noisy Training Corpus', 'Proceedings of the 16th Conference of the European Chapter of the Association for Computational Linguistics: Main Volume', 'https://semopenalex.org/location/W43068023851', 'https://semopenalex.org/location/W31168641881', 'https://semopenalex.org/location/W322535301', 'https://semopenalex.org/location/W27665803442', 'https://semopenalex.org/location/W43920119821', 'Multimodal Transformer for Multimodal Machine Translation', 'https://semopenalex.org/location/W43875596751', 'https://semopenalex.org/location/W43865668652', 'Overview of the NLPCC 2015 Shared Task: Weibo-Oriented Chinese News Summarization', 'https://semopenalex.org/location/W19680356881', 'https://semopenalex.org/location/W15907088031', 'https://semopenalex.org/location/W24246716131', 'Attention-based LSTM Network for Cross-Lingual Sentiment Classification', 'Neural Content Extraction for Poster Generation of Scientific Papers', 'Creative Destruction: Can Language Models Interpret Oxymorons?', 'https://semopenalex.org/location/W26049438881', 'Person resolution in person search results', 'https://semopenalex.org/location/W27983034381', 'Themis: Towards Flexible and Interpretable NLG Evaluation', 'Bridging the Domain Gap: Improve Informal Language Translation via Counterfactual Domain Adaptation', 'https://semopenalex.org/location/W42455043961', 'https://semopenalex.org/location/W32002855301', 'Chinese Spelling Check with Nearest Neighbors', 'https://semopenalex.org/location/W22699315981', 'https://semopenalex.org/location/W31022446661', 'Microscale and macroscale strength behaviors of blast furnace slag- cement based materials: Modeling and analysis', 'https://semopenalex.org/location/W26044438831', 'https://semopenalex.org/location/W30984117501', 'Cm-pmi', 'https://semopenalex.org/location/W43874250801', 'Learning Bilingual Embedding Model for Cross-Language Sentiment Classification', 'https://semopenalex.org/location/W29308733261', 'https://semopenalex.org/location/W42883368241', 'A New Dataset and Empirical Study for Sentence Simplification in Chinese', 'https://semopenalex.org/location/W43996573671', 'https://semopenalex.org/location/W32130735992', 'https://semopenalex.org/location/W22514277782', 'Pushing Paraphrase Away from Original Sentence: A Multi-Round Paraphrase Generation Approach', 'Towards Accurate and Efficient Chinese Part-of-Speech Tagging', 'https://semopenalex.org/location/W43831757961', 'https://semopenalex.org/location/W530687281', 'https://semopenalex.org/location/W44055623831', 'https://semopenalex.org/location/W49460081', 'https://semopenalex.org/location/W43778643422', 'https://semopenalex.org/location/W42964147592', 'https://semopenalex.org/location/W43931526572', 'https://semopenalex.org/location/W44047807401', 'PPSGen: Learning-Based Presentation Slides Generation for Academic Papers', 'https://semopenalex.org/location/W43069682291', 'https://semopenalex.org/location/W43879295153', 'https://semopenalex.org/location/W4026736721', 'https://semopenalex.org/location/W29630087171', 'CRF-based Experiments for Cross-Domain Chinese Word Segmentation at CIPS-SIGHAN-2010', 'https://semopenalex.org/location/W43801365212', 'Abstractive Document Summarization with a Graph-Based Attentional Neural Model', 'https://semopenalex.org/location/W43895204021', 'Parsing for Grammatical Relations via Graph Merging', 'https://semopenalex.org/location/W43799335311', 'https://semopenalex.org/location/W44042613631', 'Analyzing and Evaluating Correlation Measures in NLG Meta-Evaluation', 'https://semopenalex.org/location/W20227410671', 'Document Similarity Search Based on Generic Summaries', 'Learning Diachronic Word Embeddings with Iterative Stable Information Alignment', 'https://semopenalex.org/location/W21288155201', 'https://semopenalex.org/location/W21475099121', 'https://semopenalex.org/location/W44060317991', 'https://semopenalex.org/location/W43855710341', 'https://semopenalex.org/location/W31227944382', 'Harvesting Drug Effectiveness from Social Media', 'https://semopenalex.org/location/W19216503161', 'Visual Information Guided Zero-Shot Paraphrase Generation', 'https://semopenalex.org/location/W43897135852', 'https://semopenalex.org/location/W43859761071', 'Models See Hallucinations: Evaluating the Factuality in Video Captioning', 'Towards a Unified Approach Based on Affinity Graph to Various Multi-document Summarizations', 'https://semopenalex.org/location/W32085278862', 'Automatic Generation of Related Work Sections in Scientific Papers: An Optimization Approach', 'Exploring Context-Aware Evaluation Metrics for Machine Translation', 'Better than Random: Reliable NLG Human Evaluation with Constrained  Active Sampling', 'https://semopenalex.org/location/W43236516122', 'Deep Dependency Substructure-Based Learning for Multidocument Summarization', 'https://semopenalex.org/location/W28887876781', 'https://semopenalex.org/location/W26044829131', 'https://semopenalex.org/location/W43946256851', 'https://semopenalex.org/location/W32125749962', 'Constructing a Family Tree of Ten Indo-European Languages with Delexicalized Cross-linguistic Transfer Patterns', 'https://semopenalex.org/location/W43996953271', 'OpinSummEval: Revisiting Automated Evaluation for Opinion Summarization', 'https://semopenalex.org/location/W43210141363', 'Quasi-Second-Order Parsing for 1-Endpoint-Crossing, Pagenumber-2 Graphs', 'https://semopenalex.org/location/W43066765702', 'Greedy Flipping for Constrained Word Deletion', 'https://semopenalex.org/location/W29009667761', 'https://semopenalex.org/location/W16901060301', 'https://semopenalex.org/location/W42261972352', 'Using Cross-Document Random Walks for Topic-Focused Multi-Document', 'Are all literature citations equally important? Automatic citation strength estimation and its applications', 'Neural Sentence Simplification with Semantic Dependency Information', 'Exploring the Impact of Vision Features in News Image Captioning', 'https://semopenalex.org/location/W43778643423', 'Themis: A Reference-free NLG Evaluation Language Model with Flexibility and Interpretability', 'https://semopenalex.org/location/W29646698731', 'https://semopenalex.org/location/W30357025721', 'https://semopenalex.org/location/W29455336681', 'https://semopenalex.org/location/W31227944383', 'Using only cross-document relationships for both generic and topic-focused multi-document summarizations', 'https://semopenalex.org/location/W27992224531', 'QAVidCap: Enhancing Video Captioning through Question Answering Techniques', 'User Embedding for Scholarly Microblog Recommendation', 'Hierarchical Graph Summarization: Leveraging Hybrid Information through Visible and Invisible Linkage', 'https://semopenalex.org/location/W27398482341', 'https://semopenalex.org/location/W15542701311', 'Representation Learning for Aspect Category Detection in Online Reviews', 'https://semopenalex.org/location/W20203191491', 'https://semopenalex.org/location/W42260991371', 'Pre- and In-Parsing Models for Neural Empty Category Detection', 'https://semopenalex.org/location/W21399281001', 'https://semopenalex.org/location/W27951557541', 'From Neural Sentence Summarization to Headline Generation: A Coarse-to-Fine Approach', 'PKUTM participation at TAC 2011 Summarization Track.', 'https://semopenalex.org/location/W42837164641', 'https://semopenalex.org/location/W28783543041', 'SemSUM: Semantic Dependency Guided Neural Abstractive Summarization', 'https://semopenalex.org/location/W27989648141', 'Learning to Mine Chinese Coordinate Terms Using the Web', 'https://semopenalex.org/location/W43931526571', 'https://semopenalex.org/location/W43879637562', 'https://semopenalex.org/location/W43996572891', 'https://semopenalex.org/location/W31764380051', 'https://semopenalex.org/location/W31848521942', 'A Comprehensive Evaluation of Constrained Text Generation for Large Language Models', 'https://semopenalex.org/location/W43865668651', 'Summarization is (Almost) Dead', 'https://semopenalex.org/location/W43879295151', 'https://semopenalex.org/location/W23497863371', 'Extract Salient Words with WordRank for Effective Similarity Search in Text Data', 'Exploiting syntactic and semantic relationships between terms for opinion retrieval', 'Peking: Profiling Syntactic Tree Parsing Techniques for Semantic Graph Parsing', 'https://semopenalex.org/location/W42852977021', 'https://semopenalex.org/location/W19667458141', 'https://semopenalex.org/location/W24699317431', 'https://semopenalex.org/location/W31636541681', 'https://semopenalex.org/location/W43063531623', 'https://semopenalex.org/location/W21296830771', 'https://semopenalex.org/location/W42261972351', 'https://semopenalex.org/location/W29519376671', 'Multi-Granularity Interaction Network for Extractive and Abstractive Multi-Document Summarization', 'https://semopenalex.org/location/W27566762001', 'Cross-language document summarization via extraction and ranking of multiple summaries', 'T-CVAE: Transformer-Based Conditioned Variational Autoencoder for Story Completion', 'https://semopenalex.org/location/W31333763862', 'https://semopenalex.org/location/W43895188332', 'https://semopenalex.org/location/W29630087173', 'https://semopenalex.org/location/W30355227621', 'Diversifying Neural Text Generation with Part-of-Speech Guided Softmax and Sampling', 'https://semopenalex.org/location/W42883367673', 'https://semopenalex.org/location/W43852928981', 'Emotion Classification in Microblog Texts Using Class Sequential Rules', 'Automated Similarity Metric Generation for Recommendation', 'https://semopenalex.org/location/W21605135101', 'https://semopenalex.org/location/W43880320291', 'MultiSumm: Towards a Unified Model for Multi-Lingual Abstractive Summarization', 'https://semopenalex.org/location/W42260991373', 'https://semopenalex.org/location/W44037528791', 'Graph-Based Multi-Modality Learning for Clinical Decision Support', 'The Impact of Family Care on the Subjective Well-Being of the Elderly: The Mediation Role of General Self-Efficacy and Psychological Resilience', 'https://semopenalex.org/location/W21210801631', 'https://semopenalex.org/location/W31065300841', 'https://semopenalex.org/location/W43778643421', 'Hierarchical Attention Networks for Sentence Ordering', 'https://semopenalex.org/location/W32138258992', 'Beyond topical similarity: a structural similarity measure for retrieving highly similar documents', 'An Improved k-means Algorithm for Documents Clustering', 'https://semopenalex.org/location/W8277644473', 'Parsing to 1-Endpoint-Crossing, Pagenumber-2 Graphs', 'Accurate SHRG-Based Semantic Parsing', 'Interactive Multi-Grained Joint Model for Targeted Sentiment Analysis', 'https://semopenalex.org/location/W43098001053', 'https://semopenalex.org/location/W25772289771', 'https://semopenalex.org/location/W27823823261', 'https://semopenalex.org/location/W44010431251', 'SRRank: Leveraging Semantic Roles for Extractive Multi-Document Summarization', 'Abstractive Multi-Document Summarization via Joint Learning with Single-Document Summarization', 'https://semopenalex.org/location/W30431573301', 'https://semopenalex.org/location/W32137654603', 'https://semopenalex.org/location/W42869677633', 'Semantic Role Labeling for Learner Chinese: the Importance of Syntactic Parsing and L2-L1 Parallel Data', 'https://semopenalex.org/location/W32004422982', 'https://semopenalex.org/location/W43784652741', 'https://semopenalex.org/location/W31670561861', 'https://semopenalex.org/location/W29787076431', 'https://semopenalex.org/location/W43895201081', 'https://semopenalex.org/location/W43924266211', 'https://semopenalex.org/location/W43931470202', 'https://semopenalex.org/location/W43617566021', 'https://semopenalex.org/location/W42264767653', 'SUBTOPIC‐BASED MULTIMODALITY RANKING FOR TOPIC‐FOCUSED MULTIDOCUMENT SUMMARIZATION', 'https://semopenalex.org/location/W32002855302', 'https://semopenalex.org/location/W31135458781', 'https://semopenalex.org/location/W32125749961', 'https://semopenalex.org/location/W43873157801', 'https://semopenalex.org/location/W25577493911', 'https://semopenalex.org/location/W1179362191', 'https://semopenalex.org/location/W43874283711', 'MIL-Decoding: Detoxifying Language Models at Token-Level via Multiple Instance Learning', 'https://semopenalex.org/location/W43868757902', 'https://semopenalex.org/location/W19986665531', 'INS: An Interactive Chinese News Synthesis System', 'https://semopenalex.org/location/W31848521943', 'https://semopenalex.org/location/W22755689011', 'https://semopenalex.org/location/W27936528801', 'https://semopenalex.org/location/W30127214841', 'https://semopenalex.org/locatio</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/location/W28855740753', 'https://semopenalex.org/location/W29014813671', 'https://semopenalex.org/location/W30935297031', 'Analytical Evaluation of the Baseline Decorrelation in Bistatic Interferometric SAR Systems', 'Integrated Infrastructure Monitoring Procedure for Road Network Management', 'Small Reservoirs Extraction in Semiarid Regions Using Multitemporal Synthetic Aperture Radar Images', 'https://semopenalex.org/location/W30884119801', 'Sea state and wind speed', 'https://semopenalex.org/location/W42878909881', 'https://semopenalex.org/location/W44022629541', 'Planning 5G Networks Under EMF Constraints: State of the Art and Vision', 'Maritime Surveillance Using Spaceborne GNSS-Reflectometry: The Role of the Scattering Configuration and Receiving Polarization Channel', 'https://semopenalex.org/location/W27908694951', 'https://semopenalex.org/location/W32075299251', 'https://semopenalex.org/location/W43917537921', 'Integration of SAR and GEOBIA for the Analysis of Time-Series Data', 'https://semopenalex.org/location/W29018988831', 'Sensitivity analysis of a scattering-based nonlocal means Despeckling Algorithm', 'Assessing Performance of Multitemporal SAR Image Despeckling Filters via a Benchmarking Tool', 'Introduction', 'https://semopenalex.org/location/W26132134601', 'Using GEOBIA for feature extraction from multitemporal SAR images: Preliminary results', 'https://semopenalex.org/location/W43129684911', 'https://semopenalex.org/location/W27632159761', 'RGB SAR product exploiting multitemporal: General processing and applications', 'Bistatic scattering from a canonical building', 'https://semopenalex.org/location/W31292473171', 'https://semopenalex.org/location/W29006840811', 'https://semopenalex.org/location/W27553009891', 'Ambiguity problems and their mitigation', 'https://semopenalex.org/location/W32072007311', 'https://semopenalex.org/location/W42069686491', 'Time-Domain and Monostatic-like Frequency-Domain Methods for Bistatic SAR Simulation', 'Analytical Formulation of Scattering From Anisotropic Power-Law Spectrum Surfaces: Getting Rid of the Cutoff Wavenumber', 'An Analytical Formulation of the Correlation of GNSS-R Signals', 'Retrieval of high-resolution topography of the Titan’ surface by using Cassini SAR data', 'https://semopenalex.org/location/W43878017851', 'Link Budget Analysis for GNSS-R Sea Surface Return in Arbitrary Acquisition Geometries Using BA-PTSM', 'https://semopenalex.org/location/W43225028851', 'https://semopenalex.org/location/W29031449731', 'Fractal-Based Local Range Slope Estimation from Single SAR Image with Applications to SAR Despeckling and Topographic Mapping', 'Mapping small reservoirs in semi-arid regions using multitemporal SAR: Methods and applications', 'Polarimetric Two-Scale Model for Rough Surface Bistatic Scattering Evaluation', 'https://semopenalex.org/location/W32057021671', 'https://semopenalex.org/location/W42829188311', 'A new convenient tool for ice sheets exploration the fractal dimension', 'https://semopenalex.org/location/W25885227231', 'Link Budget Analysis for the Modeling of GNSS-R Sea Surface Returns in Far-from-Specular Acquisition Geometries', 'Coprime synthetic aperture radars', 'Electromagnetic Scattering from Fractional Brownian Motion Surfaces via the Small Slope Approximation', 'Benchmarking Framework for Multitemporal SAR Despeckling', 'Efficient Simulation of Extended-Scene SAR Raw Signals with Any Acquisition Mode', 'https://semopenalex.org/location/W27908694952', 'Addressing ices in the solar system via their fractal dimension measurement', 'https://semopenalex.org/location/W29127815873', 'https://semopenalex.org/location/W44042941271', 'Pol-SARAS: A Fully Polarimetric SAR Raw Signal Simulator for Extended Soil Surfaces', 'Long-Term Satellite Monitoring of the Slumgullion Landslide Using Space-Borne Synthetic Aperture Radar Sub-Pixel Offset Tracking', 'Design of Low-Cost Active Reflectors for Advanced InSAR Applications: First Results', 'https://semopenalex.org/location/W42057164411', 'Spaceborne GNSS-Reflectometry for Ship-Detection Applications: Impact of Acquisition Geometry and Polarization', 'https://semopenalex.org/location/W27625582821', 'A fully polarimetric SAR raw signal simulator', 'https://semopenalex.org/location/W31848768411', 'https://semopenalex.org/location/W43878704031', 'Efficient Processing for Far-From-Transmitter Formation-Flying SAR Receivers', 'https://semopenalex.org/location/W27747519831', 'https://semopenalex.org/location/W29127815871', 'https://semopenalex.org/location/W29127815872', 'https://semopenalex.org/location/W29561442231', 'A fully convolutional neural network for low-complexity single-stage ship detection in Sentinel-1 SAR images', 'https://semopenalex.org/location/W43878697331', 'https://semopenalex.org/location/W43878017971', 'https://semopenalex.org/location/W42069686492', 'Scattering-based Despeckling of Multi-frequency SAR Data', 'https://semopenalex.org/location/W30943681811', 'Hydrogeological characterization of a closed MSW landfill using multivariate statistical analysis and groundwater numerical modelling', 'Formation-Flying SAR Receivers in FAR-from-Transmitter Geometry: X-Band SAR Antenna Design', 'Polarimetric Two-Scale Model for Soil Moisture Estimation from Hybrid Compact Polarimetry SAR Data', 'https://semopenalex.org/location/W29488924391', 'https://semopenalex.org/location/W42059632101', 'https://semopenalex.org/location/W43906783971', 'SAR Radiometric Calibration Based on Differential Geometry: From Theory to Experimentation on SAOCOM Imagery', 'Unsupervised Rapid Flood Mapping Using Sentinel-1 GRD SAR Images', 'https://semopenalex.org/location/W32050064891', 'https://semopenalex.org/location/W27903991441', 'The Role of Skin in mm-Wave Exposure of Human Body', 'https://semopenalex.org/location/W29018743401', 'A New Tool for Road Network Deformations Monitoring Through Space-Born SAR Data and In-Situ Instruments', 'https://semopenalex.org/location/W31291607331', 'https://semopenalex.org/location/W29881205341', 'https://semopenalex.org/location/W28914311982', 'Closed-Form Anisotropic Polarimetric Two-Scale Model for Fast Evaluation of Sea Surface Backscattering', 'A Novel Analytical Formulation of the Correlation of GNSS-R Signals Scattered by a Natural Fractal Surface', 'https://semopenalex.org/location/W31128765681', 'A comparative sensitivity analysis of scattering-based despeckling algorithms', 'An Analytical Formulation for the Correlation of Surface-Scattered Fields at Two Bistatic Radar Receivers', 'Urban Area Mapping Using Multitemporal SAR Images in Combination with Self-Organizing Map Clustering and Object-Based Image Analysis', 'Glacier Monitoring Using Frequency Domain Offset Tracking Applied to Sentinel-1 Images: A Product Performance Comparison', 'Electromagnetic Scattering from a Canonical Target over an Anisotropic Rough Surface using Geometrical Optics', 'Physical models for evaluating the interferometric coherence of potential persistent scatterers', 'https://semopenalex.org/location/W29488924392', 'https://semopenalex.org/location/W43878728991', 'https://semopenalex.org/location/W42052019421', 'https://semopenalex.org/location/W31848768413', 'Despeckling of Multifrequency SAR Data Using Electromagnetic Scattering Models', 'https://semopenalex.org/location/W43862079901', 'Multitemporal synthetic aperture radar for urban planning and critical infrastructure monitoring', 'https://semopenalex.org/location/W27660924161', 'Scattering Along the Specular Direction from the Sea Modeled as a Fractal Surface', 'Baseline Decorrelation in Bistatic Interferometric SAR Systems Over Bare Soil Surfaces', 'https://semopenalex.org/location/W31848768412', 'https://semopenalex.org/location/W27721700481', 'https://semopenalex.org/location/W27563590741', 'https://semopenalex.org/location/W27762611981', 'https://semopenalex.org/location/W31291607332', 'https://semopenalex.org/location/W28855740752', 'Feature Extraction From Multitemporal SAR Images Using Selforganizing Map Clustering and Object-Based Image Analysis', 'https://semopenalex.org/location/W44022604271', 'https://semopenalex.org/location/W43878030641', 'https://semopenalex.org/location/W28099006691', 'Formation-Flying SAR Receivers in Far-From-Transmitter Geometry: Signal Model and Processing Scheme', 'https://semopenalex.org/location/W44022614201', 'Flood Detection with SAR: A Review of Techniques and Datasets', 'Two-Scale Model for the Evaluation of Sea-Surface Scattering in GNSS-R Ship-Detection Applications', 'https://semopenalex.org/location/W31325075201', 'https://semopenalex.org/location/W28914311983', 'Coprime Synthetic Aperture Radar: State of the Art and Application to Ship Detection', 'Closed-form Polarimetric Two-Scale Model for sea scattering evaluation', 'https://semopenalex.org/location/W28855740751', 'https://semopenalex.org/location/W44022614261', 'Cardinal Effect in Bistatic SAR Imagery: Analysis and Physical Interpretation', 'Remote Sensing for Monitoring Biodiversity in Urban Environment', 'Simulation of GNSS-R Signals in Arbitrary Viewing Geometry with a Closed-Form Bistatic Two-Scale Model', 'A Novel Tool for Unsupervised Flood Mapping Using Sentinel-1 Images', 'https://semopenalex.org/location/W27778336261', 'https://semopenalex.org/location/W44002082621', 'https://semopenalex.org/location/W29282537721', 'https://semopenalex.org/location/W26095320801', 'https://semopenalex.org/location/W28914311981', 'https://semopenalex.org/location/W31576231201', 'Acquisition modes', 'https://semopenalex.org/location/W27762611982', 'https://semopenalex.org/location/W43132449201', 'https://semopenalex.org/location/W29488924393', 'https://semopenalex.org/location/W43815923961', 'https://semopenalex.org/location/W42056663831', 'A Unified Formulation of SAR Raw Signals From Extended Scenes for All Acquisition Modes With Application to Simulation', 'https://semopenalex.org/location/W27746187661', 'Railway Bridge Monitoring with Sar: A Case Study', 'https://semopenalex.org/location/W29011861951', 'https://semopenalex.org/location/W30036652921', "Deciphering Earth's Movements: Unveiling Subsidence and Displacement in Capo Colonna Through SAR and CGPS", 'Correlation of the Fields Scattered by a Fractal Surface at Two Closely Spaced Receivers', 'https://semopenalex.org/location/W27749247961', 'https://semopenalex.org/location/W25885227232', 'X-Band SAR Antenna Design for a CubeSat Formation-Flying Remote Sensing Mission', 'Bistatic Scattering From Anisotropic Rough Surfaces via a Closed-Form Two-Scale Model', 'https://semopenalex.org/location/W43827525081', 'https://semopenalex.org/location/W43917597611', 'Earth Environmental Monitoring Using Multi-Temporal Synthetic Aperture Radar: A Critical Review of Selected Applications', 'Polarimetric Two-Scale Model for the Evaluation of Bistatic Scattering from Anisotropic Sea Surfaces', 'https://semopenalex.org/location/W31993907601', 'https://semopenalex.org/location/W29018043391', 'The Role of Resolution in the Estimation of Fractal Dimension Maps From SAR Data', 'https://semopenalex.org/location/W32115469181', 'https://semopenalex.org/location/W43877636401']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/location/W44028130911', 'Promoting Diversity in the Evolution of Biological Sequence Data', 'https://semopenalex.org/location/W43872514871', 'AI Versus Epidemics', 'https://semopenalex.org/location/W43900150231', 'https://semopenalex.org/location/W43789796562', 'A multi-objective genetic algorithm for compression of weighted graphs to simplify epidemic analysis', 'From Bits to Bases: Evolving a Versatile Construct for Biological Sequence and Network Data', 'https://semopenalex.org/location/W44028121901', 'https://semopenalex.org/location/W44032105271', 'Driving Evolution Towards Discovery of Patterns in Sets of Weakly-Conserved DNA Sequences', 'Evolutionary Computation', 'Generating Models of Human Gait in Patients with Parkinson’s Disease using Genetic Programming', 'https://semopenalex.org/location/W44028122871', 'Dungeons, Dragons, and Data Breaches: Analyzing AI Attacks on Various Network Configurations', 'https://semopenalex.org/location/W44014165061', 'What Drives Evolution of Self-Driving Automata?', 'https://semopenalex.org/location/W43861716341', 'https://semopenalex.org/location/W43872509461', 'https://semopenalex.org/location/W43190545381', 'https://semopenalex.org/location/W44028127321', 'https://semopenalex.org/location/W44032105491', 'Comparison of Representations to Evolve Weighted Contact Networks with Epidemic Properties', 'https://semopenalex.org/location/W43912337582', 'Vaccine Distribution', 'Introduction', 'Graph Compression', 'https://semopenalex.org/location/W43789796561', 'https://semopenalex.org/location/W44028123391', 'Conference Report on 2022 IEEE Conference on Computational Intelligence in Bioinformatics and Computational Biology (IEEE CIBCB 2022) [Conference Report]', 'https://semopenalex.org/location/W43904891721', 'https://semopenalex.org/location/W44027563071', '2022 IEEE conference on computational intelligence in bioinformatics and computational biology (IEEE CIBCB, 2022)', 'Network Induction', 'Network Induction Issues', 'https://semopenalex.org/location/W43912337581', 'https://semopenalex.org/location/W43791408481', 'https://semopenalex.org/location/W44032122871', 'https://semopenalex.org/location/W44028121881', 'All lockdowns are not equal: Reducing epidemic impact through evolutionary computation', 'Freezing of gait in Parkinson’s disease: Classification using computational intelligence', 'Immunity Vanishing Act: Epidemic Variant and Immunity Analysis via Evolutionary Computation', 'https://semopenalex.org/location/W43861716342']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/authorship/W2182338449A5027830035', 'https://semopenalex.org/authorship/W1021733493A5027830035', 'https://semopenalex.org/authorship/W4401750498A5027830035', 'https://semopenalex.org/authorship/W2166197815A5017511611', 'https://semopenalex.org/authorship/W2025132922A5017511611', 'https://semopenalex.org/authorship/W2164967075A5027830035', 'https://semopenalex.org/authorship/W2902929870A5027830035', 'https://semopenalex.org/authorship/W2950185045A5027830035', 'https://semopenalex.org/authorship/W2102592853A5027830035', 'https://semopenalex.org/authorship/W2143623375A5027830035', 'https://semopenalex.org/authorship/W3103773508A5027830035', 'https://semopenalex.org/authorship/W2785502402A5027830035', 'https://semopenalex.org/authorship/W615388181A5027830035', 'https://semopenalex.org/authorship/W1943126751A5027830035', 'https://semopenalex.org/authorship/W2297506387A5027830035', 'https://semopenalex.org/authorship/W1964384820A5027830035', 'https://semopenalex.org/authorship/W2920551025A5027830035', 'https://semopenalex.org/authorship/W4243743111A5027830035', 'https://semopenalex.org/authorship/W1587379027A5027830035', 'https://semopenalex.org/authorship/W2160172952A5017511611', 'https://semopenalex.org/authorship/W1988343658A5027830035', 'https://semopenalex.org/authorship/W606515514A5027830035', 'https://semopenalex.org/authorship/W2605257447A5027830035', 'https://semopenalex.org/authorship/W4379232433A5027830035', 'https://semopenalex.org/authorship/W2143711974A5017511611', 'https://semopenalex.org/authorship/W2085724005A5027830035', 'https://semopenalex.org/authorship/W609082053A5027830035', 'https://semopenalex.org/authorship/W2018206842A5027830035', 'https://semopenalex.org/authorship/W2336180720A5027830035', 'https://semopenalex.org/authorship/W2025968816A5027830035', 'https://semopenalex.org/authorship/W2116018884A5027830035', 'https://semopenalex.org/authorship/W2140436532A5027830035', 'https://semopenalex.org/authorship/W1996041609A5027830035', 'https://semopenalex.org/authorship/W2048853757A5027830035', 'https://semopenalex.org/authorship/W2064969586A5027830035', 'https://semopenalex.org/authorship/W2908750658A5027830035', 'https://semopenalex.org/authorship/W2963504418A5027830035', 'https://semopenalex.org/authorship/W2121529688A5027830035', 'https://semopenalex.org/authorship/W2152599017A5017511611', 'https://semopenalex.org/authorship/W3104967842A5027830035', 'https://semopenalex.org/authorship/W3088822975A5027830035', 'https://semopenalex.org/authorship/W2545039763A5027830035', 'https://semopenalex.org/authorship/W4311488571A5017511611', 'https://semopenalex.org/authorship/W1748985154A5027830035', 'https://semopenalex.org/authorship/W4304701022A5027830035', 'https://semopenalex.org/authorship/W4289367384A5027830035', 'https://semopenalex.org/authorship/W2101094458A5027830035', 'https://semopenalex.org/authorship/W1972847653A5017511611', 'https://semopenalex.org/authorship/W2618462601A5027830035', 'https://semopenalex.org/authorship/W1797142048A5027830035', 'https://semopenalex.org/authorship/W2159718141A5027830035', 'https://semopenalex.org/authorship/W2150143709A5027830035', 'https://semopenalex.org/authorship/W3015796941A5027830035', 'https://semopenalex.org/authorship/W2141592093A5027830035', 'https://semopenalex.org/authorship/W2118420236A5027830035', 'https://semopenalex.org/authorship/W2663325069A5017511611', 'https://semopenalex.org/authorship/W195512975A5027830035', 'https://semopenalex.org/authorship/W2028525469A5027830035', 'https://semopenalex.org/authorship/W2137313509A5027830035', 'https://semopenalex.org/authorship/W4300434862A5027830035', 'https://semopenalex.org/authorship/W4297229624A5027830035', 'https://semopenalex.org/authorship/W2950707842A5027830035', 'https://semopenalex.org/authorship/W2100279715A5017511611', 'https://semopenalex.org/authorship/W2168665985A5027830035', 'https://semopenalex.org/authorship/W4388235556A5027830035', 'https://semopenalex.org/authorship/W2129859788A5027830035', 'https://semopenalex.org/authorship/W4393531447A5027830035', 'https://semopenalex.org/authorship/W2131752107A5027830035', 'https://semopenalex.org/authorship/W656907390A5027830035', 'https://semopenalex.org/authorship/W2342894014A5027830035', 'https://semopenalex.org/authorship/W1774599862A5017511611', 'https://semopenalex.org/authorship/W2951231774A5027830035', 'https://semopenalex.org/authorship/W2096939401A5027830035', 'https://semopenalex.org/authorship/W1600396855A5027830035', 'https://semopenalex.org/authorship/W2280892290A5027830035', 'https://semopenalex.org/authorship/W3162654685A5027830035', 'https://semopenalex.org/authorship/W4386728259A5027830035', 'https://semopenalex.org/authorship/W2152477879A5017511611', 'https://semopenalex.org/authorship/W2088188946A5027830035', 'https://semopenalex.org/authorship/W2021144192A5027830035', 'https://semopenalex.org/authorship/W2084633773A5027830035', 'https://semopenalex.org/authorship/W2624932408A5027830035', 'https://semopenalex.org/authorship/W2178506535A5027830035', 'https://semopenalex.org/authorship/W842176471A5027830035', 'https://semopenalex.org/authorship/W2114028749A5017511611', 'https://semopenalex.org/authorship/W2103254499A5027830035', 'https://semopenalex.org/authorship/W2939804650A5017511611', 'https://semopenalex.org/authorship/W169488611A5027830035', 'https://semopenalex.org/authorship/W4386728290A5027830035', 'https://semopenalex.org/authorship/W4287551966A5027830035', 'https://semopenalex.org/authorship/W2150591965A5027830035', 'https://semopenalex.org/authorship/W2038042968A5027830035', 'https://semopenalex.org/authorship/W2138114100A5027830035', 'https://semopenalex.org/authorship/W2035899572A5027830035', 'https://semopenalex.org/authorship/W1492310094A5027830035', 'https://semopenalex.org/authorship/W2015282877A5027830035', 'https://semopenalex.org/authorship/W4247141155A5027830035', 'https://semopenalex.org/authorship/W3012587348A5027830035', 'https://semopenalex.org/authorship/W2801854492A5017511611', 'https://semopenalex.org/authorship/W1812922818A5027830035', 'https://semopenalex.org/authorship/W4307786837A5027830035', 'https://semopenalex.org/authorship/W2055673378A5027830035', 'https://semopenalex.org/authorship/W2110043300A5017511611', 'https://semopenalex.org/authorship/W2136497745A5027830035', 'https://semopenalex.org/authorship/W2035640322A5027830035', 'https://semopenalex.org/authorship/W2949908757A5027830035', 'https://semopenalex.org/authorship/W835410257A5027830035', 'https://semopenalex.org/authorship/W2624898243A5027830035', 'https://semopenalex.org/authorship/W2108797761A5027830035', 'https://semopenalex.org/authorship/W4386352568A5027830035', 'https://semopenalex.org/authorship/W1694434332A5027830035', 'https://semopenalex.org/authorship/W4298078907A5027830035', 'https://semopenalex.org/authorship/W2104091137A5027830035', 'https://semopenalex.org/authorship/W2089183963A5027830035', 'https://semopenalex.org/authorship/W2798274156A5027830035', 'https://semopenalex.org/authorship/W3103915668A5027830035', 'https://semopenalex.org/authorship/W2114391062A5027830035', 'https://semopenalex.org/authorship/W2898704942A5027830035', 'https://semopenalex.org/authorship/W2003410902A5027830035', 'https://semopenalex.org/authorship/W2032979218A5017511611', 'https://semopenalex.org/authorship/W4377043292A5027830035', 'https://semopenalex.org/authorship/W2327976118A5027830035', 'https://semopenalex.org/authorship/W2019064108A5027830035', 'https://semopenalex.org/authorship/W4287230780A5027830035', 'https://semopenalex.org/authorship/W2602238908A5027830035', 'https://semopenalex.org/authorship/W2189224346A5027830035', 'https://semopenalex.org/authorship/W2940395492A5017511611', 'https://semopenalex.org/authorship/W2408555870A5017511611', 'https://semopenalex.org/authorship/W1685599524A5027830035', 'https://semopenalex.org/authorship/W2939947188A5027830035', 'https://semopenalex.org/authorship/W2017830666A5027830035', 'https://semopenalex.org/authorship/W4387293163A5027830035', 'https://semopenalex.org/authorship/W2572859442A5027830035', 'https://semopenalex.org/authorship/W2400256934A5027830035', 'https://semopenalex.org/authorship/W2013030361A5027830035', 'https://semopenalex.org/authorship/W4403704152A5027830035', 'https://semopenalex.org/authorship/W2099928373A5027830035', 'https://semopenalex.org/authorship/W2171540875A5027830035', 'https://semopenalex.org/authorship/W2127947685A5027830035', 'https://semopenalex.org/authorship/W2109453625A5027830035', 'https://semopenalex.org/authorship/W2096086749A5027830035', 'https://semopenalex.org/authorship/W2206590685A5027830035', 'https://semopenalex.org/authorship/W2790500092A5027830035', 'https://semopenalex.org/authorship/W8218751A5027830035', 'https://semopenalex.org/authorship/W2155153848A5027830035', 'https://semopenalex.org/authorship/W2115596980A5027830035', 'https://semopenalex.org/authorship/W4237667777A5027830035', 'https://semopenalex.org/authorship/W4249394463A5027830035', 'https://semopenalex.org/authorship/W3137611772A5027830035', 'https://semopenalex.org/authorship/W2035239234A5027830035', 'https://semopenalex.org/authorship/W2129898633A5027830035', 'https://semopenalex.org/authorship/W2131938193A5027830035', 'https://semopenalex.org/authorship/W2130502393A5027830035', 'https://semopenalex.org/authorship/W2124480047A5027830035', 'https://semopenalex.org/authorship/W2068189057A5027830035', 'https://semopenalex.org/authorship/W3098873033A5027830035', 'https://semopenalex.org/authorship/W2078203941A5027830035', 'https://semopenalex.org/authorship/W1881094281A5027830035', 'https://semopenalex.org/authorship/W2890986802A5027830035', 'https://semopenalex.org/authorship/W2100556278A5027830035', 'https://semopenalex.org/authorship/W3085042870A5027830035', 'https://semopenalex.org/authorship/W2185221298A5027830035', 'https://semopenalex.org/authorship/W2030004233A5017511611', 'https://semopenalex.org/authorship/W1778342465A5027830035', 'https://semopenalex.org/authorship/W2152477879A5027830035', 'https://semopenalex.org/authorship/W4292214108A5027830035', 'https://semopenalex.org/authorship/W2033157981A5027830035', 'https://semopenalex.org/authorship/W1696074034A5027830035', 'https://semopenalex.org/authorship/W2945382159A5027830035', 'https://semopenalex.org/authorship/W1969115782A5027830035', 'https://semopenalex.org/authorship/W2117368578A5027830035', 'https://semopenalex.org/authorship/W2140386412A5017511611', 'https://semopenalex.org/authorship/W2765307985A5017511611', 'https://semopenalex.org/authorship/W2149213383A5017511611', 'https://semopenalex.org/authorship/W2152537098A5027830035', 'https://semopenalex.org/authorship/W4400052969A5017511611', 'https://semopenalex.org/authorship/W2982533818A5027830035', 'https://semopenalex.org/authorship/W2722359275A5027830035', 'https://semopenalex.org/authorship/W2112502349A5027830035', 'https://semopenalex.org/authorship/W2005858158A5027830035', 'https://semopenalex.org/authorship/W2791467061A5017511611', 'https://semopenalex.org/authorship/W1585966427A5027830035', 'https://semopenalex.org/authorship/W2970592033A5017511611', 'https://semopenalex.org/authorship/W2223218801A5027830035', 'https://semopenalex.org/authorship/W2146189427A5017511611', 'https://semopenalex.org/authorship/W2126409288A5027830035', 'https://semopenalex.org/authorship/W4225288565A5027830035', 'https://semopenalex.org/authorship/W2143820350A5027830035', 'https://semopenalex.org/authorship/W1565749342A5027830035', 'https://semopenalex.org/authorship/W3118410217A5027830035', 'https://semopenalex.org/authorship/W2128912491A5027830035', 'https://semopenalex.org/authorship/W3112939012A5027830035', 'https://semopenalex.org/authorship/W2143780518A5017511611', 'https://semopenalex.org/authorship/W1992781262A5027830035', 'https://semopenalex.org/authorship/W1564509605A5027830035', 'https://semopenalex.org/authorship/W2161268655A5027830035', 'https://semopenalex.org/authorship/W2126043778A5027830035', 'https://semopenalex.org/authorship/W2611380909A5027830035', 'https://semopenalex.org/authorship/W1967770515A5027830035', 'https://semopenalex.org/authorship/W3036970724A5027830035', 'https://semopenalex.org/authorship/W2167193873A5027830035', 'https://semopenalex.org/authorship/W2952168395A5027830035', 'https://semopenalex.org/authorship/W2970012313A5017511611', 'https://semopenalex.org/authorship/W3106431100A5027830035', 'https://semopenalex.org/authorship/W2102935592A5027830035', 'https://semopenalex.org/authorship/W2082792607A5027830035', 'https://semopenalex.org/authorship/W4406807628A5027830035', 'https://semopenalex.org/authorship/W2785643816A5027830035', 'https://semopenalex.org/authorship/W2594176303A5027830035', 'https://semopenalex.org/authorship/W2170329684A5027830035', 'https://semopenalex.org/authorship/W2037489965A5027830035', 'https://semopenalex.org/authorship/W3097189301A5027830035', 'https://semopenalex.org/authorship/W4379033886A5027830035', 'https://semopenalex.org/authorship/W2007101240A5027830035', 'https://semopenalex.org/authorship/W2185064755A5027830035', 'https://semopenalex.org/authorship/W2048467330A5027830035', 'https://semopenalex.org/authorship/W1984118997A5027830035', 'https://semopenalex.org/authorship/W4397028652A5027830035', 'https://semopenalex.org/authorship/W4396898129A5027830035', 'https://semopenalex.org/authorship/W2026970166A5027830035', 'https://semopenalex.org/authorship/W2806925689A5027830035', 'https://semopenalex.org/authorship/W2158642611A5027830035', 'https://semopenalex.org/authorship/W3129332190A5017511611', 'https://semopenalex.org/authorship/W2057477395A5027830035', 'https://semopenalex.org/authorship/W2108855378A5027830035', 'https://semopenalex.org/authorship/W4402350832A5027830035', 'https://semopenalex.org/authorship/W2106293056A5027830035', 'https://semopenalex.org/authorship/W2097867503A5027830035', 'https://semopenalex.org/authorship/W2099441560A5027830035', 'https://semopenalex.org/authorship/W2129001064A5027830035', 'https://semopenalex.org/authorship/W2147023251A5027830035', 'https://semopenalex.org/authorship/W2141798281A5027830035', 'https://semopenalex.org/authorship/W2439315773A5017511611', 'https://semopenalex.org/authorship/W4394868342A5017511611', 'https://semopenalex.org/authorship/W4244572215A5027830035', 'https://semopenalex.org/authorship/W2155252144A5027830035', 'https://semopenalex.org/authorship/W2279111001A5027830035', 'https://semopenalex.org/authorship/W2958959679A5027830035', 'https://semopenalex.org/authorship/W2185641310A5027830035', 'https://semopenalex.org/authorship/W2060717066A5017511611', 'https://semopenalex.org/authorship/W2159202008A5027830035', 'https://semopenalex.org/authorship/W4389138629A5027830035', 'https://semopenalex.org/authorship/W2293554103A5017511611', 'https://semopenalex.org/authorship/W2940821791A5027830035', 'https://semopenalex.org/authorship/W1976296868A5027830035', 'https://semopenalex.org/authorship/W4400572667A5027830035', 'https://semopenalex.org/authorship/W2955178723A5017511611', 'https://semopenalex.org/authorship/W2112902331A5027830035', 'https://semopenalex.org/authorship/W2096933831A5027830035', 'https://semopenalex.org/authorship/W2032099309A5027830035', 'https://semopenalex.org/authorship/W2077128747A5027830035', 'https://semopenalex.org/authorship/W2140311422A5027830035', 'https://semopenalex.org/authorship/W2134671262A5027830035', 'https://semopenalex.org/authorship/W2103637183A5017511611', 'https://semopenalex.org/authorship/W2136390628A5027830035', 'https://semopenalex.org/authorship/W2127324110A5027830035', 'https://semopenalex.org/authorship/W2158693223A5027830035', 'https://semopenalex.org/authorship/W4312962873A5027830035', 'https://semopenalex.org/authorship/W2767736209A5027830035', 'https://semopenalex.org/authorship/W2119248338A5027830035', 'https://semopenalex.org/authorship/W1989790075A5027830035', 'https://semopenalex.org/authorship/W2127631196A5027830035', 'https://semopenalex.org/authorship/W2792903117A5017511611', 'https://semopenalex.org/authorship/W2114379490A5027830035', 'https://semopenalex.org/authorship/W1993109981A5027830035', 'https://semopenalex.org/authorship/W1764485696A5027830035', 'https://semopenalex.org/authorship/W4386728227A5027830035', 'https://semopenalex.org/authorship/W2977723824A5027830035', 'https://semopenalex.org/authorship/W2141052825A5027830035', 'https://semopenalex.org/authorship/W2182388403A5027830035', 'https://semopenalex.org/authorship/W4288596410A5027830035', 'https://semopenalex.org/authorship/W2140311422A5017511611', 'https://semopenalex.org/authorship/W2120967246A5027830035', 'https://semopenalex.org/authorship/W2164697291A5027830035', 'https://semopenalex.org/authorship/W2148131061A5027830035', 'https://semopenalex.org/authorship/W2141801703A5027830035', 'https://semopenalex.org/authorship/W2243109900A5027830035', 'https://semopenalex.org/authorship/W2078616504A5027830035', 'https://semopenalex.org/authorship/W1667912148A5027830035', 'https://semopenalex.org/authorship/W2098410722A5027830035', 'https://semopenalex.org/authorship/W2164044612A5027830035', 'https://semopenalex.org/authorship/W4386728284A5027830035', 'https://semopenalex.org/authorship/W2013218112A5027830035', 'https://semopenalex.org/authorship/W2053928191A5027830035', 'https://semopenalex.org/authorship/W2027743940A5027830035', 'https://semopenalex.org/authorship/W1987580879A5027830035', 'https://semopenalex.org/authorship/W1882111414A5027830035', 'https://semopenalex.org/authorship/W4290556151A5027830035', 'https://semopenalex.org/authorship/W1764115161A5027830035', 'https://semopenalex.org/authorship/W2950348067A5027830035', 'https://semopenalex.org/authorship/W1984186332A5027830035', 'https://semopenalex.org/authorship/W2117626227A5027830035', 'https://semopenalex.org/authorship/W2103300762A5017511611', 'https://semopenalex.org/authorship/W3005631622A5027830035', 'https://semopenalex.org/authorship/W2811277086A5027830035', 'https://semopenalex.org/authorship/W2144185926A5027830035', 'https://semopenalex.org/authorship/W2167460076A5027830035', 'https://semopenalex.org/authorship/W1814798360A5027830035', 'https://semopenalex.org/authorship/W1984866494A5027830035', 'https://semopenalex.org/authorship/W2155485257A5027830035', 'https://semopenalex.org/authorship/W2153901619A5027830035', 'https://semopenalex.org/authorship/W2611160010A5027830035', 'https://semopenalex.org/authorship/W2108491840A5027830035', 'https://semopenalex.org/authorship/W3164197023A5027830035', 'https://semopenalex.org/authorship/W1758105233A5027830035', 'https://semopenalex.org/authorship/W2618786793A5017511611', 'https://semopenalex.org/authorship/W2120280503A5027830035', 'https://semopenalex.org/authorship/W3002449320A5027830035', 'https://semopenalex.org/authorship/W2161770118A5027830035', 'https://semopenalex.org/authorship/W2102549524A5027830035', 'https://semopenalex.org/authorship/W2162965487A5027830035', 'https://semopenalex.org/authorship/W2066062210A5027830035', 'https://semopenalex.org/authorship/W4301512502A5027830035', 'https://semopenalex.org/authorship/W1787016751A5027830035', 'https://semopenalex.org/authorship/W2040652823A5027830035', 'https://semopenalex.org/authorship/W4315606555A5027830035', 'https://semopenalex.org/authorship/W2139649788A5027830035', 'https://semopenalex.org/authorship/W4310002000A5027830035', 'https://semopenalex.org/authorship/W4322706631A5027830035', 'https://semopenalex.org/authorship/W2988626048A5027830035', 'https://semopenalex.org/authorship/W1971037148A5027830035', 'https://semopenalex.org/authorship/W2135421180A5027830035', 'https://semopenalex.org/authorship/W2166197815A5027830035', 'https://semopenalex.org/authorship/W4231953543A5027830035', 'https://semopenalex.org/authorship/W2130794128A5027830035', 'https://semopenalex.org/authorship/W2020493940A5027830035', 'https://semopenalex.org/authorship/W2918802163A5027830035', 'https://semopenalex.org/authorship/W1968153028A5027830035', 'https://semopenalex.org/authorship/W2098408658A5027830035', 'https://semopenalex.org/authorship/W2140749977A5027830035', 'https://semopenalex.org/authorship/W4297966944A5027830035', 'https://semopenalex.org/authorship/W2138395721A5027830035', 'https://semopenalex.org/authorship/W2107105182A5027830035', 'https://semopenalex.org/authorship/W2166315125A5027830035', 'https://semopenalex.org/authorship/W3179268546A5027830035', 'https://semopenalex.org/authorship/W1812926078A5027830035', 'https://semopenalex.org/authorship/W2065892151A5027830035', 'https://semopenalex.org/authorship/W2136275432A5027830035', 'https://semopenalex.org/authorship/W2294282334A5027830035', 'https://semopenalex.org/authorship/W2150388917A5027830035', 'https://semopenalex.org/authorship/W2978037608A5027830035', 'https://semopenalex.org/authorship/W2101633987A5017511611', 'https://semopenalex.org/authorship/W2162696202A5017511611', 'https://semopenalex.org/authorship/W2073431334A5027830035', 'https://semopenalex.org/authorship/W4309129028A5027830035', 'https://semopenalex.org/authorship/W2143711974A5027830035', 'https://semopenalex.org/authorship/W1984769758A5027830035', 'https://semopenalex.org/authorship/W4232393324A5027830035', 'https://semopenalex.org/authorship/W2110745932A5027830035', 'https://semopenalex.org/authorship/W2101608590A5027830035', 'https://semopenalex.org/authorship/W1990902012A5027830035', 'https://semopenalex.org/authorship/W2184680168A5027830035', 'https://semopenalex.org/authorship/W4255556357A5027830035', 'https://semopenalex.org/authorship/W2104882822A5027830035', 'https://semopenalex.org/authorship/W2195712461A5027830035', 'https://semopenalex.org/authorship/W2171540325A5027830035', 'https://semopenalex.org/authorship/W2007203285A5027830035', 'https://semopenalex.org/authorship/W3092177264A5027830035', 'https://semopenalex.org/authorship/W2143728623A5027830035', 'https://semopenalex.org/authorship/W2143075489A5017511611', 'https://semopenalex.org/authorship/W2122883310A5027830035', 'https://semopenalex.org/authorship/W2092230235A5027830035', 'https://semopenalex.org/authorship/W1940162557A5027830035', 'https://semopenalex.org/authorship/W2999073519A5027830035', 'https://semopenalex.org/authorship/W2148267424A5027830035', 'https://semopenalex.org/authorship/W2952571072A5027830035', 'https://semopenalex.org/authorship/W2963455631A5027830035', 'https://semopenalex.org/authorship/W2109453625A5017511611', 'https://semopenalex.org/authorship/W2463302795A5027830035', 'https://semopenalex.org/authorship/W2162575857A5027830035', 'https://semopenalex.org/authorship/W2697509747A5017511611', 'https://semopenalex.org/authorship/W4304207591A5027830035', 'https://semopenalex.org/authorship/W2056448690A5027830035', 'https://semopenalex.org/authorship/W2184393924A5027830035', 'https://semopenalex.org/authorship/W4297977093A5027830035', 'https://semopenalex.org/authorship/W1773125178A5027830035', 'https://semopenalex.org/authorship/W1993842801A5027830035', 'https://semopenalex.org/authorship/W1975448877A5027830035', 'https://semopenalex.org/authorship/W1996949678A5027830035', 'https://semopenalex.org/authorship/W4393951149A5027830035', 'https://semopenalex.org/authorship/W4309877015A5027830035', 'https://semopenalex.org/authorship/W2125836087A5027830035', 'https://semopenalex.org/authorship/W2114658777A5027830035', 'https://semopenalex.org/authorship/W2122128429A5027830035', 'https://semopenalex.org/authorship/W2127722806A5027830035', 'https://semopenalex.org/authorship/W4392903531A5027830035', 'https://semopenalex.org/authorship/W43334451A5027830035', 'https://semopenalex.org/authorship/W4309321321A5017511611', 'https://semopenalex.org/authorship/W2018680103A5027830035', 'https://semopenalex.org/authorship/W2117070909A5027830035', 'https://semopenalex.org/authorship/W1028196162A5027830035', 'https://semopenalex.org/authorship/W2107882641A5027830035', 'https://semopenalex.org/authorship/W2892075135A5017511611', 'https://semopenalex.org/authorship/W4315606073A5027830035', 'https://semopenalex.org/authorship/W2106903616A5027830035', 'https://semopenalex.org/authorship/W3163624263A5027830035', 'https://semopenalex.org/authorship/W2764441237A5027830035', 'https://semopenalex.org/authorship/W1532372374A5027830035', 'https://semopenalex.org/authorship/W2162160876A5027830035', 'https://semopenalex.org/authorship/W4312628239A5017511611', 'https://semopenalex.org/authorship/W2142195632A5017511611', 'https://semopenalex.org/authorship/W2136510471A5027830035', 'https://semopenalex.org/authorship/W2108017142A5027830035', 'https://semopenalex.org/authorship/W4386728269A5027830035', 'https://semopenalex.org/authorship/W2033769372A5027830035', 'https://semopenalex.org/authorship/W2155624091A5027830035', 'https://semopenalex.org/authorship/W1999564901A5027830035', 'https://semopenalex.org/authorship/W2035561336A5027830035', 'https://semopenalex.org/authorship/W2025458350A5027830035', 'https://semopenalex.org/authorship/W2213498014A5027830035', 'https://semopenalex.org/authorship/W2150474553A5027830035', 'https://semopenalex.org/authorship/W4308236214A5017511611', 'https://semopenalex.org/authorship/W4297422548A5027830035', 'https://semopenalex.org/authorship/W2140333889A5027830035', 'https://semopenalex.org/authorship/W2160318164A5027830035', 'https://semopenalex.org/authorship/W2117687155A5027830035', 'https://semopenalex.org/authorship/W1967447459A5027830035', 'https://semopenalex.org/authorship/W4313525046A5027830035', 'https://semopenalex.org/authorship/W2979998822A5027830035', 'https://semopenalex.org/authorship/W2891725356A5027830035', 'https://semopenalex.org/authorship/W2055070400A5027830035', 'https://semopenalex.org/authorship/W2963345994A5027830035', 'https://semopenalex.org/authorship/W4362508498A5027830035', 'https://semopenalex.org/authorship/W4256256581A5027830035', 'https://semopenalex.org/authorship/W2158537680A5017511611', 'https://semopenalex.org/authorship/W2158228464A5027830035', 'https://semopenalex.org/authorship/W2165131653A5027830035', 'https://semopenalex.org/authorship/W605016662A5027830035', 'https://semopenalex.org/authorship/W4309830289A5027830035', 'https://semopenalex.org/authorship/W2122768752A5027830035', 'https://semopenalex.org/authorship/W2998913556A5027830035', 'https://semopenalex.org/authorship/W2245018327A5017511611', 'https://semopenalex.org/authorship/W2094507611A5027830035', 'https://semopenalex.org/authorship/W4307934118A5027830035', 'https://semopenalex.org/authorship/W2086931264A5017511611', 'https://semopenalex.org/authorship/W2476492488A5027830035', 'https://semopenalex.org/authorship/W1945620949A5027830035', 'https://semopenalex.org/authorship/W4298174976A5027830035', 'https://semopenalex.org/authorship/W1984896113A5027830035', 'https://semopenalex.org/authorship/W2078098401A5017511611', 'https://semopenalex.org/authorship/W2002799652A5027830035', 'https://semopenalex.org/authorship/W2113885710A5017511611', 'https://semopenalex.org/authorship/W2591258888A5027830035', 'https://semopenalex.org/authorship/W4399062274A5027830035', 'https://semopenalex.org/authorship/W1820714040A5027830035', 'https://semopenalex.org/authorship/W2115645605A5027830035', 'https://semopenalex.org/authorship/W2109153110A5027830035', 'https://semopenalex.org/authorship/W2991868466A5027830035', 'https://semopenalex.org/authorship/W2075650606A5027830035', 'https://semopenalex.org/authorship/W2123717445A5027830035', 'https://semopenalex.org/authorship/W2003260793A5027830035', 'https://semopenalex.org/authorship/W2039574235A5027830035', 'https://semopenalex.org/authorship/W2151679725A5027830035', 'https://semopenalex.org/authorship/W2172222182A5027830035', 'https://semopenalex.org/authorship/W3026501815A5017511611', 'https://semopenalex.org/authorship/W2097076848A5027830035', 'https://semopenalex.org/authorship/W2099998345A5027830035', 'https://semopenalex.org/authorship/W1818779082A5027830035', 'https://semopenalex.org/authorship/W2128821548A5027830035', 'https://semopenalex.org/authorship/W4388118224A5017511611', 'https://semopenalex.org/authorship/W2134429331A5027830035', 'https://semopenalex.org/authorship/W2242734504A5027830035', 'https://semopenalex.org/authorship/W3003820456A5027830035', 'https://semopenalex.org/authorship/W3176828173A5017511611', 'https://semopenalex.org/authorship/W4385652243A5027830035', 'https://semopenalex.org/authorship/W2106900553A5027830035', 'https://semopenalex.org/authorship/W1966326250A5027830035', 'https://semopenalex.org/authorship/W2153058280A5027830035', 'https://semopenalex.org/authorship/W2165066371A5017511611', 'https://semopenalex.org/authorship/W4301499895A5027830035', 'https://semopenalex.org/authorship/W2949618677A5027830035', 'https://semopenalex.org/authorship/W1997581342A5027830035', 'https://semopenalex.org/authorship/W2791120428A5027830035', 'https://semopenalex.org/authorship/W4287666146A5027830035', 'https://semopenalex.org/authorship/W1995899361A5027830035', 'https://semopenalex.org/authorship/W2100556278A5017511611', 'https://semopenalex.org/authorship/W2130561641A5027830035', 'https://semopenalex.org/authorship/W6747142A5027830035', 'https://semopenalex.org/authorship/W1976452778A5027830035', 'https://semopenalex.org/authorship/W1861730306A5027830035', 'https://semopenalex.org/authorship/W1775735896A5027830035', 'https://semopenalex.org/authorship/W2095121969A5027830035', 'https://semopenalex.org/authorship/W4224949960A5027830035', 'https://semopenalex.org/authorship/W2129299867A5027830035', 'https://semopenalex.org/authorship/W2293327468A5027830035', 'https://semopenalex.org/authorship/W2111182668A5027830035', 'https://semopenalex.org/authorship/W2133913871A5027830035', 'https://semopenalex.org/authorship/W2122776646A5027830035', 'https://semopenalex.org/authorship/W2148907823A5027830035', 'https://semopenalex.org/authorship/W252315070A5027830035', 'https://semopenalex.org/authorship/W1947239887A5027830035', 'https://semopenalex.org/authorship/W2111934195A5027830035', 'https://semopenalex.org/authorship/W2076199721A5027830035', 'https://semopenalex.org/authorship/W2128722362A5027830035', 'https://semopenalex.org/authorship/W2040835538A5027830035', 'https://semopenalex.org/authorship/W2014068777A5017511611', 'https://semopenalex.org/authorship/W1501647712A5027830035', 'https://semopenalex.org/authorship/W4388567240A5027830035', 'https://semopenalex.org/authorship/W4288374763A5027830035', 'https://semopenalex.org/authorship/W2805259552A5027830035', 'https://semopenalex.org/authorship/W2172643935A5027830035', 'https://semopenalex.org/authorship/W2167187798A5027830035', 'https://semopenalex.org/authorship/W2133118701A5027830035', 'https://semopenalex.org/authorship/W1868782008A5027830035', 'https://semopenalex.org/authorship/W2587913063A5027830035', 'https://semopenalex.org/authorship/W1624008340A5017511611', 'https://semopenalex.org/authorship/W2108057985A5027830035', 'https://semopenalex.org/authorship/W2124699087A5017511611', 'https://semopenalex.org/authorship/W2139649788A5017511611', 'https://semopenalex.org/authorship/W2187527650A5027830035', 'https://semopenalex.org/authorship/W2441173492A5027830035', 'https://semopenalex.org/authorship/W4313478262A5027830035', 'https://semopenalex.org/authorship/W2125523397A5027830035', 'https://semopenalex.org/authorship/W2045551387A5027830035', 'https://semopenalex.org/authorship/W2135431044A5017511611', 'https://semopenalex.org/authorship/W1883544968A5027830035', 'https://semopenalex.org/authorship/W1989282861A5027830035', 'https://semopenalex.org/authorship/W2080412418A5027830035', 'https://semopenalex.org/authorship/W3200113339A5017511611', 'https://semopenalex.org/authorship/W1963919043A5027830035', 'https://semopenalex.org/authorship/W3130481183A5017511611', 'https://semopenalex.org/authorship/W2118345904A5027830035', 'https://semopenalex.org/authorship/W2118103599A5027830035', 'https://semopenalex.org/authorship/W3015454417A5017511611', 'https://semopenalex.org/authorship/W2784488119A5027830035', 'https://semopenalex.org/authorship/W2121752514A5027830035', 'https://semopenalex.org/authorship/W2023804683A5027830035', 'https://semopenalex.org/authorship/W855221475A5027830035', 'https://semopenalex.org/authorship/W1990472383A5027830035', 'https://semopenalex.org/authorship/W2558578462A5027830035', 'https://semopenalex.org/authorship/W2111557101A5027830035', 'https://semopenalex.org/authorship/W3009810166A5027830035', 'https://semopenalex.org/authorship/W2150258751A5027830035', 'https://semopenalex.org/authorship/W2143780518A5027830035', 'https://semopenalex.org/authorship/W1975277950A5027830035', 'https://semopenalex.org/authorship/W4388483721A5017511611', 'https://semopenalex.org/authorship/W2034340815A5027830035', 'https://semopenalex.org/aut</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/authorship/W2968293343A5056183585', 'https://semopenalex.org/authorship/W1522158218A5056183585', 'https://semopenalex.org/authorship/W2129488573A5019693610', 'https://semopenalex.org/authorship/W1834136374A5056183585', 'https://semopenalex.org/authorship/W2294561329A5019693610', 'https://semopenalex.org/authorship/W4386163788A5019693610', 'https://semopenalex.org/authorship/W4366597679A5056183585', 'https://semopenalex.org/authorship/W2054886944A5056183585', 'https://semopenalex.org/authorship/W4393752214A5019693610', 'https://semopenalex.org/authorship/W3198359754A5019693610', 'https://semopenalex.org/authorship/W4386929049A5019693610', 'https://semopenalex.org/authorship/W4383220643A5056183585', 'https://semopenalex.org/authorship/W2591593006A5056183585', 'https://semopenalex.org/authorship/W2114418543A5056183585', 'https://semopenalex.org/authorship/W4239396382A5019693610', 'https://semopenalex.org/authorship/W1860259465A5056183585', 'https://semopenalex.org/authorship/W2528963299A5056183585', 'https://semopenalex.org/authorship/W2072697691A5056183585', 'https://semopenalex.org/authorship/W2072490274A5019693610', 'https://semopenalex.org/authorship/W2344158693A5056183585', 'https://semopenalex.org/authorship/W2602397751A5056183585', 'https://semopenalex.org/authorship/W2896178739A5056183585', 'https://semopenalex.org/authorship/W4229043996A5019693610', 'https://semopenalex.org/authorship/W1976594634A5056183585', 'https://semopenalex.org/authorship/W2789478762A5019693610', 'https://semopenalex.org/authorship/W3184531492A5056183585', 'https://semopenalex.org/authorship/W2903417746A5056183585', 'https://semopenalex.org/authorship/W4392429145A5019693610', 'https://semopenalex.org/authorship/W2977911811A5056183585', 'https://semopenalex.org/authorship/W2137846113A5056183585', 'https://semopenalex.org/authorship/W2972702127A5056183585', 'https://semopenalex.org/authorship/W4393908582A5019693610', 'https://semopenalex.org/authorship/W2520352456A5056183585', 'https://semopenalex.org/authorship/W2768260654A5056183585', 'https://semopenalex.org/authorship/W2902563098A5056183585', 'https://semopenalex.org/authorship/W2019487042A5056183585', 'https://semopenalex.org/authorship/W2515389026A5019693610', 'https://semopenalex.org/authorship/W3009160614A5019693610', 'https://semopenalex.org/authorship/W2975736083A5056183585', 'https://semopenalex.org/authorship/W3112877194A5019693610', 'https://semopenalex.org/authorship/W2738622408A5056183585', 'https://semopenalex.org/authorship/W3007521088A5019693610', 'https://semopenalex.org/authorship/W3165155612A5019693610', 'https://semopenalex.org/authorship/W2977597077A5056183585', 'https://semopenalex.org/authorship/W3162832522A5056183585', 'https://semopenalex.org/authorship/W2078369692A5056183585', 'https://semopenalex.org/authorship/W4213455276A5056183585', 'https://semopenalex.org/authorship/W2067004171A5056183585', 'https://semopenalex.org/authorship/W2102667737A5056183585', 'https://semopenalex.org/authorship/W2567779880A5056183585', 'https://semopenalex.org/authorship/W4404915142A5056183585', 'https://semopenalex.org/authorship/W3095367321A5019693610', 'https://semopenalex.org/authorship/W2082538501A5056183585', 'https://semopenalex.org/authorship/W4307204790A5019693610', 'https://semopenalex.org/authorship/W4224255688A5056183585', 'https://semopenalex.org/authorship/W2986358413A5056183585', 'https://semopenalex.org/authorship/W4366547357A5056183585', 'https://semopenalex.org/authorship/W2972419497A5056183585', 'https://semopenalex.org/authorship/W2187647369A5056183585', 'https://semopenalex.org/authorship/W2898145840A5056183585', 'https://semopenalex.org/authorship/W3034123328A5056183585', 'https://semopenalex.org/authorship/W3206366132A5019693610', 'https://semopenalex.org/authorship/W2898822823A5056183585', 'https://semopenalex.org/authorship/W4214504130A5056183585', 'https://semopenalex.org/authorship/W2752561456A5056183585', 'https://semopenalex.org/authorship/W2075286904A5019693610', 'https://semopenalex.org/authorship/W3033480106A5056183585', 'https://semopenalex.org/authorship/W3215451397A5019693610', 'https://semopenalex.org/authorship/W1985504739A5056183585', 'https://semopenalex.org/authorship/W3033839905A5056183585', 'https://semopenalex.org/authorship/W2901616108A5019693610', 'https://semopenalex.org/authorship/W3062298123A5056183585', 'https://semopenalex.org/authorship/W3032662532A5019693610', 'https://semopenalex.org/authorship/W4221065578A5056183585', 'https://semopenalex.org/authorship/W3095347735A5056183585', 'https://semopenalex.org/authorship/W3161974712A5019693610', 'https://semopenalex.org/authorship/W4366598255A5056183585', 'https://semopenalex.org/authorship/W3030577208A5056183585', 'https://semopenalex.org/authorship/W4401406766A5019693610', 'https://semopenalex.org/authorship/W4366583171A5019693610', 'https://semopenalex.org/authorship/W4393877125A5019693610', 'https://semopenalex.org/authorship/W1246643588A5019693610', 'https://semopenalex.org/authorship/W2159491375A5056183585', 'https://semopenalex.org/authorship/W3171875220A5019693610', 'https://semopenalex.org/authorship/W3143959337A5056183585', 'https://semopenalex.org/authorship/W2294361658A5056183585', 'https://semopenalex.org/authorship/W2293208404A5019693610', 'https://semopenalex.org/authorship/W2410138785A5019693610', 'https://semopenalex.org/authorship/W2318574332A5019693610', 'https://semopenalex.org/authorship/W2610780371A5056183585', 'https://semopenalex.org/authorship/W2063007215A5056183585', 'https://semopenalex.org/authorship/W2752658305A5056183585', 'https://semopenalex.org/authorship/W4402722131A5019693610', 'https://semopenalex.org/authorship/W3186694431A5019693610', 'https://semopenalex.org/authorship/W4389256452A5019693610', 'https://semopenalex.org/authorship/W2610274107A5056183585', 'https://semopenalex.org/authorship/W2929751249A5019693610', 'https://semopenalex.org/authorship/W2519558346A5056183585', 'https://semopenalex.org/authorship/W3094759305A5056183585', 'https://semopenalex.org/authorship/W4214684069A5056183585', 'https://semopenalex.org/authorship/W3178374478A5056183585', 'https://semopenalex.org/authorship/W2973132733A5056183585', 'https://semopenalex.org/authorship/W3190617503A5056183585', 'https://semopenalex.org/authorship/W2088502162A5056183585', 'https://semopenalex.org/authorship/W3182364466A5056183585', 'https://semopenalex.org/authorship/W2548042282A5056183585', 'https://semopenalex.org/authorship/W3015284588A5056183585', 'https://semopenalex.org/authorship/W2602429360A5056183585', 'https://semopenalex.org/authorship/W2940716241A5019693610', 'https://semopenalex.org/authorship/W4225473762A5056183585', 'https://semopenalex.org/authorship/W4404977899A5056183585', 'https://semopenalex.org/authorship/W2519730427A5019693610', 'https://semopenalex.org/authorship/W2007978709A5056183585', 'https://semopenalex.org/authorship/W2737450254A5056183585', 'https://semopenalex.org/authorship/W4366549587A5019693610', 'https://semopenalex.org/authorship/W2519458229A5056183585', 'https://semopenalex.org/authorship/W2973016298A5056183585', 'https://semopenalex.org/authorship/W4234952088A5056183585', 'https://semopenalex.org/authorship/W2898627444A5019693610', 'https://semopenalex.org/authorship/W3202016550A5056183585', 'https://semopenalex.org/authorship/W2920869031A5019693610', 'https://semopenalex.org/authorship/W3028790862A5056183585', 'https://semopenalex.org/authorship/W3141512745A5056183585', 'https://semopenalex.org/authorship/W4224305168A5056183585', 'https://semopenalex.org/authorship/W1771936601A5056183585', 'https://semopenalex.org/authorship/W4238249729A5056183585', 'https://semopenalex.org/authorship/W4312282153A5056183585', 'https://semopenalex.org/authorship/W4211095911A5056183585', 'https://semopenalex.org/authorship/W3032857618A5056183585', 'https://semopenalex.org/authorship/W2754101670A5019693610', 'https://semopenalex.org/authorship/W2537880674A5056183585', 'https://semopenalex.org/authorship/W4387085789A5019693610', 'https://semopenalex.org/authorship/W2165066165A5056183585', 'https://semopenalex.org/authorship/W2033617925A5056183585', 'https://semopenalex.org/authorship/W2079488626A5056183585', 'https://semopenalex.org/authorship/W2024357873A5019693610', 'https://semopenalex.org/authorship/W3035628382A5019693610', 'https://semopenalex.org/authorship/W3177151358A5056183585', 'https://semopenalex.org/authorship/W2288812598A5056183585', 'https://semopenalex.org/authorship/W2087800309A5019693610', 'https://semopenalex.org/authorship/W4312646439A5056183585', 'https://semopenalex.org/authorship/W2092202628A5056183585', 'https://semopenalex.org/authorship/W3193396842A5056183585', 'https://semopenalex.org/authorship/W4404026276A5019693610', 'https://semopenalex.org/authorship/W3183940262A5019693610', 'https://semopenalex.org/authorship/W2946308339A5056183585', 'https://semopenalex.org/authorship/W2978422619A5056183585', 'https://semopenalex.org/authorship/W2119929248A5056183585', 'https://semopenalex.org/authorship/W4389891943A5019693610', 'https://semopenalex.org/authorship/W2901616108A5056183585', 'https://semopenalex.org/authorship/W2133951180A5056183585', 'https://semopenalex.org/authorship/W2942738233A5019693610', 'https://semopenalex.org/authorship/W3206712787A5019693610', 'https://semopenalex.org/authorship/W4245844025A5019693610', 'https://semopenalex.org/authorship/W2131570437A5056183585', 'https://semopenalex.org/authorship/W2753801751A5056183585', 'https://semopenalex.org/authorship/W4400189062A5019693610', 'https://semopenalex.org/authorship/W2169202944A5019693610', 'https://semopenalex.org/authorship/W2177601947A5019693610', 'https://semopenalex.org/authorship/W1877041815A5056183585', 'https://semopenalex.org/authorship/W2102905932A5056183585', 'https://semopenalex.org/authorship/W2899305210A5056183585', 'https://semopenalex.org/authorship/W4391423303A5019693610', 'https://semopenalex.org/authorship/W2798335699A5019693610', 'https://semopenalex.org/authorship/W2972759039A5056183585', 'https://semopenalex.org/authorship/W3160199101A5019693610', 'https://semopenalex.org/authorship/W2409578015A5019693610', 'https://semopenalex.org/authorship/W4294891921A5056183585', 'https://semopenalex.org/authorship/W2899389394A5019693610', 'https://semopenalex.org/authorship/W2795581336A5019693610', 'https://semopenalex.org/authorship/W4377250056A5056183585', 'https://semopenalex.org/authorship/W2513683703A5056183585', 'https://semopenalex.org/authorship/W4315777028A5056183585', 'https://semopenalex.org/authorship/W2068367136A5056183585', 'https://semopenalex.org/authorship/W2898667062A5056183585', 'https://semopenalex.org/authorship/W4312841490A5019693610', 'https://semopenalex.org/authorship/W3142764819A5056183585', 'https://semopenalex.org/authorship/W2944843734A5019693610', 'https://semopenalex.org/authorship/W2810881717A5056183585', 'https://semopenalex.org/authorship/W4210768549A5056183585', 'https://semopenalex.org/authorship/W2944843734A5056183585', 'https://semopenalex.org/authorship/W2899333601A5056183585', 'https://semopenalex.org/authorship/W4230032809A5056183585', 'https://semopenalex.org/authorship/W791468510A5056183585', 'https://semopenalex.org/authorship/W2052607251A5056183585', 'https://semopenalex.org/authorship/W4256454723A5056183585', 'https://semopenalex.org/authorship/W3096658838A5056183585', 'https://semopenalex.org/authorship/W4242142265A5056183585', 'https://semopenalex.org/authorship/W2751429127A5056183585', 'https://semopenalex.org/authorship/W2518694405A5019693610', 'https://semopenalex.org/authorship/W2942324097A5019693610', 'https://semopenalex.org/authorship/W2520661109A5056183585', 'https://semopenalex.org/authorship/W2557881781A5019693610', 'https://semopenalex.org/authorship/W2519914856A5056183585', 'https://semopenalex.org/authorship/W2978280554A5056183585', 'https://semopenalex.org/authorship/W3161889270A5056183585', 'https://semopenalex.org/authorship/W2519250278A5056183585', 'https://semopenalex.org/authorship/W4366967286A5019693610', 'https://semopenalex.org/authorship/W4312572845A5019693610', 'https://semopenalex.org/authorship/W3084729599A5019693610', 'https://semopenalex.org/authorship/W4287071181A5019693610', 'https://semopenalex.org/authorship/W2755506150A5019693610', 'https://semopenalex.org/authorship/W1510660243A5056183585', 'https://semopenalex.org/authorship/W3112090964A5056183585', 'https://semopenalex.org/authorship/W4393067390A5056183585', 'https://semopenalex.org/authorship/W3035727063A5056183585', 'https://semopenalex.org/authorship/W4393752214A5056183585', 'https://semopenalex.org/authorship/W2520077052A5019693610', 'https://semopenalex.org/authorship/W2346600598A5019693610', 'https://semopenalex.org/authorship/W4239396382A5056183585', 'https://semopenalex.org/authorship/W4200018492A5019693610', 'https://semopenalex.org/authorship/W2972600126A5056183585', 'https://semopenalex.org/authorship/W2012358521A5056183585', 'https://semopenalex.org/authorship/W4210450354A5019693610', 'https://semopenalex.org/authorship/W4230967253A5019693610', 'https://semopenalex.org/authorship/W2139733095A5019693610', 'https://semopenalex.org/authorship/W2156243282A5056183585', 'https://semopenalex.org/authorship/W2024357873A5056183585', 'https://semopenalex.org/authorship/W2942324097A5056183585', 'https://semopenalex.org/authorship/W3204393727A5056183585', 'https://semopenalex.org/authorship/W3030735111A5019693610', 'https://semopenalex.org/authorship/W3091007149A5019693610', 'https://semopenalex.org/authorship/W2256119246A5056183585', 'https://semopenalex.org/authorship/W1484203263A5056183585', 'https://semopenalex.org/authorship/W4393102879A5056183585', 'https://semopenalex.org/authorship/W2752493326A5019693610', 'https://semopenalex.org/authorship/W3161959528A5056183585', 'https://semopenalex.org/authorship/W4310446060A5019693610', 'https://semopenalex.org/authorship/W4214593503A5056183585', 'https://semopenalex.org/authorship/W3096988350A5056183585', 'https://semopenalex.org/authorship/W2977617583A5056183585', 'https://semopenalex.org/authorship/W2899470128A5056183585', 'https://semopenalex.org/authorship/W1993984611A5019693610', 'https://semopenalex.org/authorship/W2972889118A5056183585', 'https://semopenalex.org/authorship/W4319452484A5019693610', 'https://semopenalex.org/authorship/W4283397308A5019693610', 'https://semopenalex.org/authorship/W2774467220A5056183585', 'https://semopenalex.org/authorship/W2752042616A5056183585', 'https://semopenalex.org/authorship/W4308467568A5056183585', 'https://semopenalex.org/authorship/W2791540051A5056183585', 'https://semopenalex.org/authorship/W2725971658A5019693610', 'https://semopenalex.org/authorship/W1993514406A5056183585', 'https://semopenalex.org/authorship/W4393877125A5056183585', 'https://semopenalex.org/authorship/W4406805368A5019693610', 'https://semopenalex.org/authorship/W3188420011A5056183585', 'https://semopenalex.org/authorship/W3126826400A5019693610', 'https://semopenalex.org/authorship/W2465877051A5056183585', 'https://semopenalex.org/authorship/W4324151651A5056183585', 'https://semopenalex.org/authorship/W4361189030A5056183585', 'https://semopenalex.org/authorship/W2909558410A5019693610', 'https://semopenalex.org/authorship/W4200525013A5056183585', 'https://semopenalex.org/authorship/W2752031858A5019693610', 'https://semopenalex.org/authorship/W1553133540A5056183585', 'https://semopenalex.org/authorship/W4366588423A5056183585', 'https://semopenalex.org/authorship/W2576215493A5056183585', 'https://semopenalex.org/authorship/W3000816869A5019693610', 'https://semopenalex.org/authorship/W2795503716A5019693610', 'https://semopenalex.org/authorship/W4307475355A5056183585', 'https://semopenalex.org/authorship/W4287729941A5056183585', 'https://semopenalex.org/authorship/W2273076933A5056183585', 'https://semopenalex.org/authorship/W2061583538A5056183585', 'https://semopenalex.org/authorship/W3196785132A5019693610', 'https://semopenalex.org/authorship/W1985142918A5056183585', 'https://semopenalex.org/authorship/W2752490344A5019693610', 'https://semopenalex.org/authorship/W4241289669A5019693610', 'https://semopenalex.org/authorship/W3090583924A5019693610', 'https://semopenalex.org/authorship/W3022986551A5019693610', 'https://semopenalex.org/authorship/W3095740806A5056183585', 'https://semopenalex.org/authorship/W2611685970A5056183585', 'https://semopenalex.org/authorship/W4396832885A5056183585', 'https://semopenalex.org/authorship/W2149683870A5019693610', 'https://semopenalex.org/authorship/W2798335699A5056183585', 'https://semopenalex.org/authorship/W3024164567A5019693610', 'https://semopenalex.org/authorship/W3033866035A5056183585', 'https://semopenalex.org/authorship/W3011317564A5019693610', 'https://semopenalex.org/authorship/W4232727837A5056183585', 'https://semopenalex.org/authorship/W3201213010A5056183585', 'https://semopenalex.org/authorship/W2091382943A5019693610', 'https://semopenalex.org/authorship/W2561633795A5056183585', 'https://semopenalex.org/authorship/W4292261957A5056183585', 'https://semopenalex.org/authorship/W4391210282A5056183585', 'https://semopenalex.org/authorship/W4394825420A5019693610', 'https://semopenalex.org/authorship/W4324152586A5056183585', 'https://semopenalex.org/authorship/W3028180736A5056183585', 'https://semopenalex.org/authorship/W4224279084A5056183585', 'https://semopenalex.org/authorship/W2921533080A5056183585', 'https://semopenalex.org/authorship/W1998431265A5019693610', 'https://semopenalex.org/authorship/W4312605566A5019693610', 'https://semopenalex.org/authorship/W1568803211A5056183585', 'https://semopenalex.org/authorship/W3036463368A5056183585', 'https://semopenalex.org/authorship/W2598459295A5056183585', 'https://semopenalex.org/authorship/W4309619903A5019693610', 'https://semopenalex.org/authorship/W1975028026A5056183585', 'https://semopenalex.org/authorship/W2753671526A5056183585', 'https://semopenalex.org/authorship/W2033680836A5056183585', 'https://semopenalex.org/authorship/W3043824623A5056183585', 'https://semopenalex.org/authorship/W2108512685A5056183585', 'https://semopenalex.org/authorship/W2610676428A5056183585', 'https://semopenalex.org/authorship/W2903849727A5019693610', 'https://semopenalex.org/authorship/W4366583934A5019693610', 'https://semopenalex.org/authorship/W2008208122A5019693610', 'https://semopenalex.org/authorship/W4389897704A5019693610', 'https://semopenalex.org/authorship/W2346600598A5056183585', 'https://semopenalex.org/authorship/W2973140914A5056183585', 'https://semopenalex.org/authorship/W3130372017A5056183585', 'https://semopenalex.org/authorship/W4220905243A5056183585', 'https://semopenalex.org/authorship/W3047192924A5056183585', 'https://semopenalex.org/authorship/W2263778529A5056183585', 'https://semopenalex.org/authorship/W4385856456A5056183585', 'https://semopenalex.org/authorship/W4399126764A5056183585', 'https://semopenalex.org/authorship/W1704771702A5056183585', 'https://semopenalex.org/authorship/W2811468211A5056183585', 'https://semopenalex.org/authorship/W3181801907A5056183585', 'https://semopenalex.org/authorship/W3197280612A5056183585', 'https://semopenalex.org/authorship/W2551155618A5056183585', 'https://semopenalex.org/authorship/W2753363725A5056183585', 'https://semopenalex.org/authorship/W2976524236A5056183585', 'https://semopenalex.org/authorship/W1982984133A5019693610', 'https://semopenalex.org/authorship/W2611151946A5019693610', 'https://semopenalex.org/authorship/W4400430993A5019693610', 'https://semopenalex.org/authorship/W862033376A5056183585', 'https://semopenalex.org/authorship/W3005470382A5056183585', 'https://semopenalex.org/authorship/W4224242333A5056183585', 'https://semopenalex.org/authorship/W2790187313A5056183585', 'https://semopenalex.org/authorship/W2461856634A5019693610', 'https://semopenalex.org/authorship/W3030149602A5056183585', 'https://semopenalex.org/authorship/W3163327897A5056183585', 'https://semopenalex.org/authorship/W2060118520A5019693610', 'https://semopenalex.org/authorship/W3193717464A5056183585', 'https://semopenalex.org/authorship/W2888386951A5056183585', 'https://semopenalex.org/authorship/W2921058600A5056183585', 'https://semopenalex.org/authorship/W4379879736A5019693610', 'https://semopenalex.org/authorship/W1751138515A5019693610', 'https://semopenalex.org/authorship/W4394883037A5019693610', 'https://semopenalex.org/authorship/W3037695612A5019693610', 'https://semopenalex.org/authorship/W2520077052A5056183585', 'https://semopenalex.org/authorship/W2055070571A5019693610', 'https://semopenalex.org/authorship/W4387606708A5019693610', 'https://semopenalex.org/authorship/W2057014910A5056183585', 'https://semopenalex.org/authorship/W3033704563A5056183585', 'https://semopenalex.org/authorship/W3135072684A5056183585', 'https://semopenalex.org/authorship/W2346027641A5019693610', 'https://semopenalex.org/authorship/W3119309106A5019693610', 'https://semopenalex.org/authorship/W4393908582A5056183585', 'https://semopenalex.org/authorship/W2121082751A5056183585', 'https://semopenalex.org/authorship/W2090841027A5019693610', 'https://semopenalex.org/authorship/W2152557601A5056183585', 'https://semopenalex.org/authorship/W2139733095A5056183585', 'https://semopenalex.org/authorship/W3204110051A5056183585', 'https://semopenalex.org/authorship/W2973046614A5056183585', 'https://semopenalex.org/authorship/W2613908791A5056183585', 'https://semopenalex.org/authorship/W4324150573A5056183585', 'https://semopenalex.org/authorship/W2966384546A5056183585', 'https://semopenalex.org/authorship/W1965526182A5056183585', 'https://semopenalex.org/authorship/W3203088685A5019693610', 'https://semopenalex.org/authorship/W4379033872A5019693610', 'https://semopenalex.org/authorship/W2750727230A5056183585', 'https://semopenalex.org/authorship/W2136876773A5056183585', 'https://semopenalex.org/authorship/W3121062173A5019693610', 'https://semopenalex.org/authorship/W4404873047A5019693610', 'https://semopenalex.org/authorship/W2154752229A5056183585', 'https://semopenalex.org/authorship/W2968884122A5056183585', 'https://semopenalex.org/authorship/W3029899401A5056183585', 'https://semopenalex.org/authorship/W4402722090A5056183585', 'https://semopenalex.org/authorship/W3003369003A5056183585', 'https://semopenalex.org/authorship/W3160545975A5019693610', 'https://semopenalex.org/authorship/W4225133274A5019693610', 'https://semopenalex.org/authorship/W4387421144A5056183585', 'https://semopenalex.org/authorship/W1524596993A5056183585', 'https://semopenalex.org/authorship/W2977979696A5056183585', 'https://semopenalex.org/authorship/W2057014910A5019693610', 'https://semopenalex.org/authorship/W2904910662A5019693610', 'https://semopenalex.org/authorship/W2913594206A5056183585', 'https://semopenalex.org/authorship/W2110284634A5056183585', 'https://semopenalex.org/authorship/W3206712787A5056183585', 'https://semopenalex.org/authorship/W4225088745A5019693610', 'https://semopenalex.org/authorship/W2089266363A5056183585', 'https://semopenalex.org/authorship/W3003204379A5019693610', 'https://semopenalex.org/authorship/W2898820983A5056183585', 'https://semopenalex.org/authorship/W2037697732A5056183585', 'https://semopenalex.org/authorship/W3110591323A5056183585', 'https://semopenalex.org/authorship/W2902941289A5056183585', 'https://semopenalex.org/authorship/W3161202338A5019693610', 'https://semopenalex.org/authorship/W2752493326A5056183585', 'https://semopenalex.org/authorship/W2625122753A5019693610', 'https://semopenalex.org/authorship/W2108911539A5056183585', 'https://semopenalex.org/authorship/W3201451193A5019693610', 'https://semopenalex.org/authorship/W4241528240A5019693610', 'https://semopenalex.org/authorship/W4324150147A5056183585', 'https://semopenalex.org/authorship/W2789478762A5056183585', 'https://semopenalex.org/authorship/W2921194733A5056183585', 'https://semopenalex.org/authorship/W2725971658A5056183585', 'https://semopenalex.org/authorship/W2755164339A5019693610', 'https://semopenalex.org/authorship/W2751622533A5056183585', 'https://semopenalex.org/authorship/W2736312195A5056183585', 'https://semopenalex.org/authorship/W4233748389A5056183585', 'https://semopenalex.org/authorship/W4404373433A5056183585', 'https://semopenalex.org/authorship/W3163921267A5056183585', 'https://semopenalex.org/authorship/W2897414246A5056183585', 'https://semopenalex.org/authorship/W3110075456A5056183585', 'https://semopenalex.org/authorship/W3196772354A5056183585', 'https://semopenalex.org/authorship/W1981715407A5019693610', 'https://semopenalex.org/authorship/W3162177365A5056183585', 'https://semopenalex.org/authorship/W3163085734A5019693610', 'https://semopenalex.org/authorship/W3200245219A5056183585', 'https://semopenalex.org/authorship/W3194688439A5019693610', 'https://semopenalex.org/authorship/W1710215999A5056183585', 'https://semopenalex.org/authorship/W4324154015A5056183585', 'https://semopenalex.org/authorship/W2017727997A5056183585', 'https://semopenalex.org/authorship/W3031395001A5019693610', 'https://semopenalex.org/authorship/W2981708234A5019693610', 'https://semopenalex.org/authorship/W2605978692A5056183585', 'https://semopenalex.org/authorship/W3028614762A5056183585', 'https://semopenalex.org/authorship/W2762577600A5019693610', 'https://semopenalex.org/authorship/W3188766356A5019693610', 'https://semopenalex.org/authorship/W4399763801A5019693610', 'https://semopenalex.org/authorship/W4393067517A5056183585', 'https://semopenalex.org/authorship/W3117330688A5019693610', 'https://semopenalex.org/authorship/W3121775658A5019693610', 'https://semopenalex.org/authorship/W4404569483A5019693610', 'https://semopenalex.org/authorship/W2775793881A5056183585', 'https://semopenalex.org/authorship/W2054886944A5019693610', 'https://semopenalex.org/authorship/W4200616097A5056183585', 'https://semopenalex.org/authorship/W2793897377A5056183585', 'https://semopenalex.org/authorship/W2962975962A5056183585', 'https://semopenalex.org/authorship/W4251839844A5056183585', 'https://semopenalex.org/authorship/W2885122621A5056183585', 'https://semopenalex.org/authorship/W2088270376A5056183585', 'https://semopenalex.org/authorship/W2895512277A5056183585', 'https://semopenalex.org/authorship/W2978827769A5019693610', 'https://semopenalex.org/authorship/W3163078982A5019693610', 'https://semopenalex.org/authorship/W2913475584A5056183585', 'https://semopenalex.org/authorship/W2346980133A5056183585', 'https://semopenalex.org/authorship/W4211259494A5056183585', 'https://semopenalex.org/authorship/W2401872729A5019693610', 'https://semopenalex.org/authorship/W3163521409A5019693610', 'https://semopenalex.org/authorship/W2080327955A5019693610']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/authorship/W4253265224A5051587506', 'https://semopenalex.org/authorship/W2145747218A5051587506', 'https://semopenalex.org/authorship/W4390512166A5051587506', 'https://semopenalex.org/authorship/W1860740456A5051587506', 'https://semopenalex.org/authorship/W2078326945A5051587506', 'https://semopenalex.org/authorship/W2748533023A5051587506', 'https://semopenalex.org/authorship/W1526915766A5056164318', 'https://semopenalex.org/authorship/W4285172618A5056164318', 'https://semopenalex.org/authorship/W3162144158A5051587506', 'https://semopenalex.org/authorship/W1518248903A5051587506', 'https://semopenalex.org/authorship/W2785105341A5051587506', 'https://semopenalex.org/authorship/W2171606781A5051587506', 'https://semopenalex.org/authorship/W2034507787A5051587506', 'https://semopenalex.org/authorship/W2124703480A5051587506', 'https://semopenalex.org/authorship/W2246286794A5051587506', 'https://semopenalex.org/authorship/W2786772278A5051587506', 'https://semopenalex.org/authorship/W2166217821A5051587506', 'https://semopenalex.org/authorship/W2075578427A5056164318', 'https://semopenalex.org/authorship/W2998201073A5051587506', 'https://semopenalex.org/authorship/W2024468903A5051587506', 'https://semopenalex.org/authorship/W146617261A5051587506', 'https://semopenalex.org/authorship/W2125308824A5051587506', 'https://semopenalex.org/authorship/W1922706319A5051587506', 'https://semopenalex.org/authorship/W2120216356A5051587506', 'https://semopenalex.org/authorship/W1870822388A5051587506', 'https://semopenalex.org/authorship/W4400946519A5051587506', 'https://semopenalex.org/authorship/W2068524892A5051587506', 'https://semopenalex.org/authorship/W2136654140A5051587506', 'https://semopenalex.org/authorship/W2161454411A5051587506', 'https://semopenalex.org/authorship/W2475285031A5051587506', 'https://semopenalex.org/authorship/W2982452767A5051587506', 'https://semopenalex.org/authorship/W25440647A5051587506', 'https://semopenalex.org/authorship/W2484374542A5051587506', 'https://semopenalex.org/authorship/W2615205062A5051587506', 'https://semopenalex.org/authorship/W2074068839A5051587506', 'https://semopenalex.org/authorship/W4306173842A5051587506', 'https://semopenalex.org/authorship/W2756387886A5051587506', 'https://semopenalex.org/authorship/W2288294525A5051587506', 'https://semopenalex.org/authorship/W2034179412A5051587506', 'https://semopenalex.org/authorship/W1573590416A5051587506', 'https://semopenalex.org/authorship/W1501172792A5056164318', 'https://semopenalex.org/authorship/W4367360059A5056164318', 'https://semopenalex.org/authorship/W4404030648A5051587506', 'https://semopenalex.org/authorship/W2064672353A5051587506', 'https://semopenalex.org/authorship/W4396665589A5056164318', 'https://semopenalex.org/authorship/W2092005371A5051587506', 'https://semopenalex.org/authorship/W2202036745A5051587506', 'https://semopenalex.org/authorship/W2576879514A5051587506', 'https://semopenalex.org/authorship/W2145701421A5051587506', 'https://semopenalex.org/authorship/W4252981000A5056164318', 'https://semopenalex.org/authorship/W3129067525A5051587506', 'https://semopenalex.org/authorship/W2043269074A5051587506', 'https://semopenalex.org/authorship/W4401578804A5056164318', 'https://semopenalex.org/authorship/W4366964206A5056164318', 'https://semopenalex.org/authorship/W1492737188A5051587506', 'https://semopenalex.org/authorship/W2579158977A5056164318', 'https://semopenalex.org/authorship/W160837981A5051587506', 'https://semopenalex.org/authorship/W2532152395A5051587506', 'https://semopenalex.org/authorship/W2289584941A5051587506', 'https://semopenalex.org/authorship/W1999149743A5051587506', 'https://semopenalex.org/authorship/W1508821613A5056164318', 'https://semopenalex.org/authorship/W2123532445A5051587506', 'https://semopenalex.org/authorship/W1448329507A5051587506', 'https://semopenalex.org/authorship/W1544524730A5051587506', 'https://semopenalex.org/authorship/W1995950498A5051587506', 'https://semopenalex.org/authorship/W4393146711A5051587506', 'https://semopenalex.org/authorship/W2150298155A5051587506', 'https://semopenalex.org/authorship/W2108240852A5051587506', 'https://semopenalex.org/authorship/W2041108261A5056164318', 'https://semopenalex.org/authorship/W2139255754A5051587506', 'https://semopenalex.org/authorship/W1971283588A5051587506', 'https://semopenalex.org/authorship/W2490092534A5051587506', 'https://semopenalex.org/authorship/W2744837872A5051587506', 'https://semopenalex.org/authorship/W2883856658A5051587506', 'https://semopenalex.org/authorship/W4401021691A5051587506', 'https://semopenalex.org/authorship/W2293095660A5051587506', 'https://semopenalex.org/authorship/W2610600517A5051587506', 'https://semopenalex.org/authorship/W1992253076A5051587506', 'https://semopenalex.org/authorship/W4247476769A5051587506', 'https://semopenalex.org/authorship/W2073709132A5051587506', 'https://semopenalex.org/authorship/W49790452A5051587506', 'https://semopenalex.org/authorship/W1979289740A5056164318', 'https://semopenalex.org/authorship/W2042756792A5051587506', 'https://semopenalex.org/authorship/W2149899452A5051587506', 'https://semopenalex.org/authorship/W1520936229A5051587506', 'https://semopenalex.org/authorship/W2929921254A5051587506', 'https://semopenalex.org/authorship/W2165818457A5056164318', 'https://semopenalex.org/authorship/W2794572176A5056164318', 'https://semopenalex.org/authorship/W2052982204A5051587506', 'https://semopenalex.org/authorship/W2789263069A5056164318', 'https://semopenalex.org/authorship/W2475545374A5051587506', 'https://semopenalex.org/authorship/W3085760006A5056164318', 'https://semopenalex.org/authorship/W1969462495A5051587506', 'https://semopenalex.org/authorship/W2903545243A5051587506', 'https://semopenalex.org/authorship/W2992245431A5051587506', 'https://semopenalex.org/authorship/W4389321773A5056164318', 'https://semopenalex.org/authorship/W2166520679A5051587506', 'https://semopenalex.org/authorship/W3211844447A5051587506', 'https://semopenalex.org/authorship/W2413288731A5051587506', 'https://semopenalex.org/authorship/W2055278155A5051587506', 'https://semopenalex.org/authorship/W2903177638A5051587506', 'https://semopenalex.org/authorship/W2786657846A5051587506', 'https://semopenalex.org/authorship/W2600068329A5051587506', 'https://semopenalex.org/authorship/W3130320973A5056164318', 'https://semopenalex.org/authorship/W2064476539A5051587506', 'https://semopenalex.org/authorship/W2288534976A5051587506', 'https://semopenalex.org/authorship/W2341007259A5051587506', 'https://semopenalex.org/authorship/W2953533689A5056164318', 'https://semopenalex.org/authorship/W2004738891A5051587506', 'https://semopenalex.org/authorship/W2016989291A5051587506', 'https://semopenalex.org/authorship/W4238734812A5051587506', 'https://semopenalex.org/authorship/W2155718231A5051587506', 'https://semopenalex.org/authorship/W1584206897A5056164318', 'https://semopenalex.org/authorship/W1967677932A5051587506', 'https://semopenalex.org/authorship/W72692433A5051587506', 'https://semopenalex.org/authorship/W2935942569A5051587506', 'https://semopenalex.org/authorship/W2085435476A5051587506', 'https://semopenalex.org/authorship/W2550667658A5051587506', 'https://semopenalex.org/authorship/W3196495759A5051587506', 'https://semopenalex.org/authorship/W2111964097A5056164318', 'https://semopenalex.org/authorship/W2620890574A5056164318', 'https://semopenalex.org/authorship/W2109186457A5056164318', 'https://semopenalex.org/authorship/W857122145A5051587506', 'https://semopenalex.org/authorship/W1497865469A5051587506', 'https://semopenalex.org/authorship/W2015849174A5051587506', 'https://semopenalex.org/authorship/W2407231546A5051587506', 'https://semopenalex.org/authorship/W2079895649A5056164318', 'https://semopenalex.org/authorship/W2923039095A5051587506', 'https://semopenalex.org/authorship/W4210708907A5051587506', 'https://semopenalex.org/authorship/W2163881253A5051587506', 'https://semopenalex.org/authorship/W2917706508A5051587506', 'https://semopenalex.org/authorship/W2019708772A5056164318', 'https://semopenalex.org/authorship/W2094708864A5056164318', 'https://semopenalex.org/authorship/W2761828172A5051587506', 'https://semopenalex.org/authorship/W2625256202A5051587506', 'https://semopenalex.org/authorship/W2895817859A5051587506', 'https://semopenalex.org/authorship/W2138320177A5051587506', 'https://semopenalex.org/authorship/W2024612964A5051587506', 'https://semopenalex.org/authorship/W1982314073A5056164318', 'https://semopenalex.org/authorship/W3206850855A5051587506', 'https://semopenalex.org/authorship/W2144918660A5051587506', 'https://semopenalex.org/authorship/W2029818237A5056164318', 'https://semopenalex.org/authorship/W67894965A5051587506', 'https://semopenalex.org/authorship/W2129869483A5056164318', 'https://semopenalex.org/authorship/W2002312562A5051587506', 'https://semopenalex.org/authorship/W2137861763A5056164318', 'https://semopenalex.org/authorship/W1577463177A5051587506', 'https://semopenalex.org/authorship/W2111424373A5051587506', 'https://semopenalex.org/authorship/W2028566173A5056164318', 'https://semopenalex.org/authorship/W2789144447A5056164318', 'https://semopenalex.org/authorship/W1494063694A5051587506', 'https://semopenalex.org/authorship/W2077200079A5051587506', 'https://semopenalex.org/authorship/W1969516436A5051587506', 'https://semopenalex.org/authorship/W2146033518A5051587506', 'https://semopenalex.org/authorship/W565256208A5051587506', 'https://semopenalex.org/authorship/W2068973986A5051587506', 'https://semopenalex.org/authorship/W3206640136A5051587506', 'https://semopenalex.org/authorship/W4286571613A5051587506', 'https://semopenalex.org/authorship/W2132364404A5051587506', 'https://semopenalex.org/authorship/W2890543403A5056164318', 'https://semopenalex.org/authorship/W2156138095A5051587506', 'https://semopenalex.org/authorship/W3023797106A5051587506', 'https://semopenalex.org/authorship/W3136727059A5056164318', 'https://semopenalex.org/authorship/W2625986270A5051587506', 'https://semopenalex.org/authorship/W4376526615A5051587506', 'https://semopenalex.org/authorship/W2130803541A5051587506', 'https://semopenalex.org/authorship/W196228518A5051587506', 'https://semopenalex.org/authorship/W2538630038A5056164318', 'https://semopenalex.org/authorship/W2906163189A5051587506', 'https://semopenalex.org/authorship/W1986540981A5056164318', 'https://semopenalex.org/authorship/W2060283246A5051587506', 'https://semopenalex.org/authorship/W2158569759A5051587506', 'https://semopenalex.org/authorship/W2106211998A5051587506', 'https://semopenalex.org/authorship/W2061231005A5051587506', 'https://semopenalex.org/authorship/W4240672112A5051587506', 'https://semopenalex.org/authorship/W2965366155A5051587506', 'https://semopenalex.org/authorship/W4386814402A5056164318', 'https://semopenalex.org/authorship/W4316659889A5051587506', 'https://semopenalex.org/authorship/W2188799909A5051587506', 'https://semopenalex.org/authorship/W4285408205A5051587506', 'https://semopenalex.org/authorship/W2027452379A5051587506', 'https://semopenalex.org/authorship/W2751662694A5056164318', 'https://semopenalex.org/authorship/W1967157693A5056164318', 'https://semopenalex.org/authorship/W2968293641A5056164318', 'https://semopenalex.org/authorship/W2044900380A5051587506', 'https://semopenalex.org/authorship/W4392713273A5051587506', 'https://semopenalex.org/authorship/W2967954143A5051587506', 'https://semopenalex.org/authorship/W2166211129A5051587506', 'https://semopenalex.org/authorship/W2130007135A5051587506', 'https://semopenalex.org/authorship/W3097508557A5051587506', 'https://semopenalex.org/authorship/W2730743430A5051587506', 'https://semopenalex.org/authorship/W2150998397A5051587506', 'https://semopenalex.org/authorship/W4205619442A5051587506', 'https://semopenalex.org/authorship/W2413863213A5051587506', 'https://semopenalex.org/authorship/W2041334917A5051587506', 'https://semopenalex.org/authorship/W2033725854A5056164318', 'https://semopenalex.org/authorship/W2961776981A5051587506', 'https://semopenalex.org/authorship/W1874259713A5051587506', 'https://semopenalex.org/authorship/W2025546942A5056164318', 'https://semopenalex.org/authorship/W1661735121A5051587506', 'https://semopenalex.org/authorship/W2559559327A5056164318', 'https://semopenalex.org/authorship/W2293958210A5056164318', 'https://semopenalex.org/authorship/W2743920271A5051587506', 'https://semopenalex.org/authorship/W12268595A5051587506', 'https://semopenalex.org/authorship/W2106421914A5051587506', 'https://semopenalex.org/authorship/W2092477317A5056164318', 'https://semopenalex.org/authorship/W2039163755A5051587506', 'https://semopenalex.org/authorship/W3157283285A5056164318', 'https://semopenalex.org/authorship/W2144750318A5056164318', 'https://semopenalex.org/authorship/W2485878525A5051587506', 'https://semopenalex.org/authorship/W2754307650A5051587506', 'https://semopenalex.org/authorship/W2024336304A5051587506', 'https://semopenalex.org/authorship/W2124560301A5051587506', 'https://semopenalex.org/authorship/W102421301A5051587506', 'https://semopenalex.org/authorship/W328613600A5051587506', 'https://semopenalex.org/authorship/W2124054384A5051587506', 'https://semopenalex.org/authorship/W214032606A5056164318', 'https://semopenalex.org/authorship/W2212338561A5051587506', 'https://semopenalex.org/authorship/W1538415416A5056164318', 'https://semopenalex.org/authorship/W2063650982A5051587506', 'https://semopenalex.org/authorship/W1990091852A5051587506', 'https://semopenalex.org/authorship/W2081189334A5051587506', 'https://semopenalex.org/authorship/W4289655844A5051587506', 'https://semopenalex.org/authorship/W1177607589A5051587506', 'https://semopenalex.org/authorship/W2062957328A5056164318', 'https://semopenalex.org/authorship/W2903213374A5051587506', 'https://semopenalex.org/authorship/W2496554705A5051587506', 'https://semopenalex.org/authorship/W2104408001A5051587506', 'https://semopenalex.org/authorship/W2800308132A5051587506', 'https://semopenalex.org/authorship/W2062957328A5051587506', 'https://semopenalex.org/authorship/W52623672A5056164318', 'https://semopenalex.org/authorship/W2110574373A5051587506', 'https://semopenalex.org/authorship/W2036165062A5051587506', 'https://semopenalex.org/authorship/W2138922641A5051587506', 'https://semopenalex.org/authorship/W4206807237A5051587506', 'https://semopenalex.org/authorship/W1860740456A5056164318', 'https://semopenalex.org/authorship/W2024786226A5051587506', 'https://semopenalex.org/authorship/W2510781223A5051587506', 'https://semopenalex.org/authorship/W2032099346A5051587506', 'https://semopenalex.org/authorship/W2108304242A5051587506', 'https://semopenalex.org/authorship/W1993325111A5051587506', 'https://semopenalex.org/authorship/W2131405606A5056164318', 'https://semopenalex.org/authorship/W2184299809A5051587506', 'https://semopenalex.org/authorship/W2271801361A5056164318', 'https://semopenalex.org/authorship/W33403252A5051587506', 'https://semopenalex.org/authorship/W2161850606A5051587506', 'https://semopenalex.org/authorship/W3095131015A5051587506', 'https://semopenalex.org/authorship/W4240245530A5051587506', 'https://semopenalex.org/authorship/W2401381263A5056164318', 'https://semopenalex.org/authorship/W2159139699A5051587506', 'https://semopenalex.org/authorship/W2148646851A5051587506', 'https://semopenalex.org/authorship/W2275014257A5051587506', 'https://semopenalex.org/authorship/W2014241426A5051587506', 'https://semopenalex.org/authorship/W1943042767A5056164318', 'https://semopenalex.org/authorship/W2789144447A5051587506', 'https://semopenalex.org/authorship/W1967568969A5051587506', 'https://semopenalex.org/authorship/W2290447772A5051587506', 'https://semopenalex.org/authorship/W2124870235A5051587506', 'https://semopenalex.org/authorship/W2029131637A5051587506', 'https://semopenalex.org/authorship/W325059703A5051587506', 'https://semopenalex.org/authorship/W1494162500A5056164318', 'https://semopenalex.org/authorship/W2161545800A5051587506', 'https://semopenalex.org/authorship/W2166826477A5051587506', 'https://semopenalex.org/authorship/W4392188385A5051587506', 'https://semopenalex.org/authorship/W149383384A5051587506', 'https://semopenalex.org/authorship/W2138320177A5056164318', 'https://semopenalex.org/authorship/W2080817506A5056164318', 'https://semopenalex.org/authorship/W2966031361A5051587506', 'https://semopenalex.org/authorship/W4387450689A5051587506', 'https://semopenalex.org/authorship/W2884636426A5051587506', 'https://semopenalex.org/authorship/W4253855517A5051587506', 'https://semopenalex.org/authorship/W2755359845A5051587506', 'https://semopenalex.org/authorship/W3027319226A5056164318', 'https://semopenalex.org/authorship/W4206307909A5051587506', 'https://semopenalex.org/authorship/W3175708501A5051587506', 'https://semopenalex.org/authorship/W3118215277A5051587506', 'https://semopenalex.org/authorship/W2513883066A5051587506', 'https://semopenalex.org/authorship/W2034050419A5051587506', 'https://semopenalex.org/authorship/W3021203574A5051587506', 'https://semopenalex.org/authorship/W2078326945A5056164318', 'https://semopenalex.org/authorship/W4285503152A5051587506', 'https://semopenalex.org/authorship/W1979988378A5051587506', 'https://semopenalex.org/authorship/W2153457047A5051587506', 'https://semopenalex.org/authorship/W1514325539A5051587506', 'https://semopenalex.org/authorship/W2012912450A5056164318', 'https://semopenalex.org/authorship/W2109705305A5056164318', 'https://semopenalex.org/authorship/W2903194584A5051587506', 'https://semopenalex.org/authorship/W2162066092A5051587506', 'https://semopenalex.org/authorship/W3017031701A5051587506', 'https://semopenalex.org/authorship/W1998201483A5051587506', 'https://semopenalex.org/authorship/W2596027452A5051587506', 'https://semopenalex.org/authorship/W1990019789A5051587506', 'https://semopenalex.org/authorship/W1481133633A5051587506', 'https://semopenalex.org/authorship/W1544524730A5056164318', 'https://semopenalex.org/authorship/W2128563460A5051587506', 'https://semopenalex.org/authorship/W4367360032A5051587506', 'https://semopenalex.org/authorship/W2612784784A5051587506', 'https://semopenalex.org/authorship/W3096330417A5051587506', 'https://semopenalex.org/authorship/W2167521347A5051587506', 'https://semopenalex.org/authorship/W652412083A5051587506', 'https://semopenalex.org/authorship/W4321614042A5056164318', 'https://semopenalex.org/authorship/W1587236616A5051587506', 'https://semopenalex.org/authorship/W2154510046A5056164318', 'https://semopenalex.org/authorship/W2145502705A5051587506', 'https://semopenalex.org/authorship/W2515896452A5056164318', 'https://semopenalex.org/authorship/W4327767801A5051587506', 'https://semopenalex.org/authorship/W2291113318A5056164318', 'https://semopenalex.org/authorship/W4392577068A5051587506', 'https://semopenalex.org/authorship/W2397834607A5051587506', 'https://semopenalex.org/authorship/W3092453362A5051587506', 'https://semopenalex.org/authorship/W139668830A5056164318', 'https://semopenalex.org/authorship/W4285216643A5056164318', 'https://semopenalex.org/authorship/W2028754220A5051587506', 'https://semopenalex.org/authorship/W3004301528A5056164318', 'https://semopenalex.org/authorship/W2160391119A5056164318', 'https://semopenalex.org/authorship/W2480965638A5056164318', 'https://semopenalex.org/authorship/W2478910470A5051587506', 'https://semopenalex.org/authorship/W2171510346A5051587506', 'https://semopenalex.org/authorship/W2608491785A5051587506', 'https://semopenalex.org/authorship/W4296365397A5051587506', 'https://semopenalex.org/authorship/W2606501011A5056164318', 'https://semopenalex.org/authorship/W2941373095A5056164318', 'https://semopenalex.org/authorship/W2405266982A5056164318', 'https://semopenalex.org/authorship/W2072209700A5051587506', 'https://semopenalex.org/authorship/W2768928198A5056164318', 'https://semopenalex.org/authorship/W4205613083A5056164318', 'https://semopenalex.org/authorship/W2065803961A5051587506', 'https://semopenalex.org/authorship/W2055684776A5051587506', 'https://semopenalex.org/authorship/W2142484380A5051587506', 'https://semopenalex.org/authorship/W2079466034A5051587506', 'https://semopenalex.org/authorship/W3095279071A5051587506', 'https://semopenalex.org/authorship/W2627083872A5051587506', 'https://semopenalex.org/authorship/W2290200834A5051587506', 'https://semopenalex.org/authorship/W2571158126A5051587506', 'https://semopenalex.org/authorship/W4237745095A5051587506', 'https://semopenalex.org/authorship/W1488510230A5051587506', 'https://semopenalex.org/authorship/W2947626283A5056164318', 'https://semopenalex.org/authorship/W2968852933A5051587506', 'https://semopenalex.org/authorship/W1517253300A5051587506', 'https://semopenalex.org/authorship/W2084854878A5051587506', 'https://semopenalex.org/authorship/W2805153701A5056164318', 'https://semopenalex.org/authorship/W1978851795A5051587506', 'https://semopenalex.org/authorship/W4404030068A5051587506', 'https://semopenalex.org/authorship/W2146520711A5051587506', 'https://semopenalex.org/authorship/W48804293A5051587506', 'https://semopenalex.org/authorship/W2527344267A5051587506', 'https://semopenalex.org/authorship/W2011410844A5051587506', 'https://semopenalex.org/authorship/W1516689139A5051587506', 'https://semopenalex.org/authorship/W2557110996A5056164318', 'https://semopenalex.org/authorship/W1489534528A5051587506', 'https://semopenalex.org/authorship/W2089241417A5051587506', 'https://semopenalex.org/authorship/W1986827696A5051587506', 'https://semopenalex.org/authorship/W4210325270A5051587506', 'https://semopenalex.org/authorship/W159035867A5051587506', 'https://semopenalex.org/authorship/W2122571865A5051587506', 'https://semopenalex.org/authorship/W2076330335A5051587506', 'https://semopenalex.org/authorship/W2157519619A5051587506', 'https://semopenalex.org/authorship/W2749110496A5051587506', 'https://semopenalex.org/authorship/W1933806665A5056164318', 'https://semopenalex.org/authorship/W1422159917A5051587506', 'https://semopenalex.org/authorship/W3160200186A5051587506', 'https://semopenalex.org/authorship/W2896727063A5056164318', 'https://semopenalex.org/authorship/W49611838A5051587506', 'https://semopenalex.org/authorship/W1840794446A5051587506', 'https://semopenalex.org/authorship/W2948995623A5051587506', 'https://semopenalex.org/authorship/W2161966477A5051587506', 'https://semopenalex.org/authorship/W4401808601A5051587506', 'https://semopenalex.org/authorship/W1999631843A5051587506', 'https://semopenalex.org/authorship/W4285815179A5056164318', 'https://semopenalex.org/authorship/W3016161880A5051587506', 'https://semopenalex.org/authorship/W2902487276A5051587506', 'https://semopenalex.org/authorship/W1549886897A5051587506', 'https://semopenalex.org/authorship/W2132364404A5056164318', 'https://semopenalex.org/authorship/W2398987072A5051587506', 'https://semopenalex.org/authorship/W1584206897A5051587506', 'https://semopenalex.org/authorship/W2165377954A5051587506', 'https://semopenalex.org/authorship/W2023972619A5051587506', 'https://semopenalex.org/authorship/W2147895050A5051587506', 'https://semopenalex.org/authorship/W143942840A5051587506', 'https://semopenalex.org/authorship/W2066111880A5051587506', 'https://semopenalex.org/authorship/W2295164153A5051587506', 'https://semopenalex.org/authorship/W1569686365A5056164318', 'https://semopenalex.org/authorship/W4390188024A5051587506', 'https://semopenalex.org/authorship/W4396894716A5051587506', 'https://semopenalex.org/authorship/W2907364096A5051587506', 'https://semopenalex.org/authorship/W2530140145A5051587506', 'https://semopenalex.org/authorship/W3017143302A5051587506', 'https://semopenalex.org/authorship/W1531223514A5051587506', 'https://semopenalex.org/authorship/W1923826352A5051587506', 'https://semopenalex.org/authorship/W4392942581A5051587506', 'https://semopenalex.org/authorship/W2044431283A5056164318', 'https://semopenalex.org/authorship/W2945412056A5051587506', 'https://semopenalex.org/authorship/W1633573314A5051587506', 'https://semopenalex.org/authorship/W4229053674A5056164318', 'https://semopenalex.org/authorship/W4387005904A5056164318', 'https://semopenalex.org/authorship/W2230115501A5051587506', 'https://semopenalex.org/authorship/W4230332361A5051587506', 'https://semopenalex.org/authorship/W2162338867A5056164318', 'https://semopenalex.org/authorship/W2769445687A5056164318', 'https://semopenalex.org/authorship/W4294672395A5051587506', 'https://semopenalex.org/authorship/W1544888628A5051587506', 'https://semopenalex.org/authorship/W2062243122A5051587506', 'https://semopenalex.org/authorship/W2135598717A5056164318', 'https://semopenalex.org/authorship/W2035518282A5056164318', 'https://semopenalex.org/authorship/W2203509984A5051587506', 'https://semopenalex.org/authorship/W2219017076A5051587506', 'https://semopenalex.org/authorship/W2150650760A5051587506', 'https://semopenalex.org/authorship/W2550712691A5051587506', 'https://semopenalex.org/authorship/W2666172191A5051587506', 'https://semopenalex.org/authorship/W1999508547A5051587506', 'https://semopenalex.org/authorship/W1857000584A5056164318', 'https://semopenalex.org/authorship/W1991853935A5051587506', 'https://semopenalex.org/authorship/W1560982985A5051587506', 'https://semopenalex.org/authorship/W2412127048A5051587506', 'https://semopenalex.org/authorship/W2803258972A5051587506', 'https://semopenalex.org/authorship/W4249594017A5051587506', 'https://semopenalex.org/authorship/W2356144191A5056164318', 'https://semopenalex.org/authorship/W126878419A5051587506', 'https://semopenalex.org/authorship/W2747040169A5051587506', 'https://semopenalex.org/authorship/W2755469263A5051587506', 'https://semopenalex.org/authorship/W2140805995A5051587506', 'https://semopenalex.org/authorship/W4244005678A5051587506', 'https://semopenalex.org/authorship/W2108162045A5051587506', 'https://semopenalex.org/authorship/W1419972110A5051587506', 'https://semopenalex.org/authorship/W2058904901A5056164318', 'https://semopenalex.org/authorship/W4233681091A5051587506', 'https://semopenalex.org/authorship/W2954164432A5051587506', 'https://semopenalex.org/authorship/W4376630019A5051587506', 'https://semopenalex.org/authorship/W2111277352A5051587506', 'https://semopenalex.org/authorship/W2070269076A5051587506', 'https://semopenalex.org/authorship/W2095968352A5051587506', 'https://semopenalex.org/authorship/W2484645626A5056164318', 'https://semopenalex.org/authorship/W2624802634A5051587506', 'https://semopenalex.org/authorship/W2964982644A5051587506', 'https://semopenalex.org/authorship/W2163138922A5051587506', 'https://semopenalex.org/authorship/W4401579183A5056164318', 'https://semopenalex.org/authorship/W2127414738A5051587506', 'https://semopenalex.org/authorship/W2165300716A5051587506', 'https://semopenalex.org/authorship/W4237620799A5056164318', 'https://semopenalex.org/authorship/W2742916377A5051587506', 'https://semopenalex.org/authorship/W2172143183A5051587506', 'https://semopenalex.org/authorship/W2072776346A5051587506', 'https://semopenalex.org/authorship/W2895854254A5051587506', 'https://semopenalex.org/authorship/W4205212276A5051587506', 'https://semopenalex.org/authorship/W4405120549A5051587506', 'https://semopenalex.org/authorship/W2112107898A5056164318', 'https://semopenalex.org/authorship/W4385626270A5051587506', 'https://semopenalex.org/authorship/W2886396839A5051587506', 'https://semopenalex.org/authorship/W3157167113A5051587506', 'https://semopenalex.org/authorship/W2062904953A5051587506', 'https://semopenalex.org/authorship/W2085207404A5056164318', 'https://semopenalex.org/authorship/W196228518A5056164318', 'https://semopenalex.org/authorship/W1506027738A5051587506', 'https://semopenalex.org/authorship/W2108876125A5056164318', 'https://semopenalex.org/authorship/W4394742902A5056164318', 'https://semopenalex.org/authorship/W4249963731A5051587506', 'https://semopenalex.org/authorship/W2542642724A5051587506', 'https://semopenalex.org/authorship/W2080996134A5051587506', 'https://semopenalex.org/authorship/W4231226382A5051587506', 'https://semopenalex.org/authorship/W2147456231A5051587506', 'https://semopenalex.org/authorship/W2786606238A5051587506', 'https://semopenalex.org/authorship/W2883395494A5056164318', 'https://semopenalex.org/authorship/W2289149676A5051587506', 'https://semopenalex.org/authorship/W4400946621A5051587506', 'https://semopenalex.org/authorship/W2401333290A5051587506', 'https://semopenalex.org/authorship/W4402830551A5051587506', 'https://semopenalex.org/authorship/W1985701940A5056164318', 'https://semopenalex.org/authorship/W1992495634A5051587506', 'https://semopenalex.org/authorship/W2130832779A5051587506', 'https://semopenalex.org/authorship/W6907768A5051587506', 'https://semopenalex.org/authorship/W2401687993A5051587506', 'https://semopenalex.org/authorship/W2125143433A5051587506', 'https://semopenalex.org/authorship/W2334327213A5051587506', 'https://semopenalex.org/authorship/W1654176175A5051587506', 'https://semopenalex.org/authorship/W1823956242A5051587506', 'https://semopenalex.org/authorship/W2113043545A5051587506', 'https://semopenalex.org/authorship/W2146520711A5056164318', 'https://semopenalex.org/authorship/W2111759980A5051587506', 'https://semopenalex.org/authorship/W2074193071A5051587506', 'https://semopenalex.org/authorship/W1994278842A5051587506', 'https://semopenalex.org/authorship/W2293459815A5056164318', 'https://semopenalex.org/authorship/W4206683427A5051587506', 'https://semopenalex.org/authorship/W1973125618A5051587506', 'https://semopenalex.org/authorship/W4365802790A5051587506', 'https://semopenalex.org/authorship/W2091944075A5051587506', 'https://semopenalex.org/authorship/W4253850266A5051587506', 'https://semopenalex.org/authorship/W2494421230A5051587506', 'https://semopenalex.org/authorship/W1974886156A5051587506', 'https://semopenalex.org/authorship/W402024038A5051587506', 'https://semopenalex.org/authorship/W4405094102A5056164318', 'https://semopenalex.org/authorship/W2516286998A5051587506', 'https://semopenalex.org/authorship/W2950468099A5051587506', 'https://semopenalex.org/authorship/W2532447822A5051587506', 'https://semopenalex.org/authorship/W4401943800A5056164318', 'https://semopenalex.org/authorship/W2170201418A5056164318', 'https://semopenalex.org/authorship/W2482354811A5051587506', 'https://semopenalex.org/authorship/W2497743975A5051587506', 'https://semopenalex.org/authorship/W2098948701A5051587506', 'https://semopenalex.org/authorship/W1973148750A5051587506', 'https://semopenalex.org/authorship/W2536107053A5051587506', 'https://semopenalex.org/authorship/W1574380960A5051587506', 'https://semopenalex.org/authorship/W1526915766A5051587506', 'https://semopenalex.org/authorship/W2528842892A5056164318', 'https://semopenalex.org/authorship/W1857000584A5051587506', 'https://semopenalex.org/authorship/W2170201418A5051587506', 'https://semopenalex.org/authorship/W2170913025A5051587506', 'https://semopenalex.org/authorship/W2095834672A5051587506', 'https://semopenalex.org/authorship/W1965382252A5056164318', 'https://semopenalex.org/authorship/W48804293A5056164318', 'https://semopenalex.org/authorship/W2031625065A5051587506', 'https://semopenalex.org/authorship/W979651393A5051587506', 'https://semopenalex.org/authorship/W2612282432A5056164318', 'https://semopenalex.org/authorship/W2147139299A5051587506', 'https://semopenalex.org/authorship/W2115899637A5051587506', 'https://semopenalex.org/authorship/W1908879184A5051587506', 'https://semopenalex.org/authorship/W2586727473A5051587506', 'https://semopenalex.org/authorship/W2107191431A5056164318', 'https://semopenalex.org/authorship/W1497099843A5051587506', 'https://semopenalex.org/authorship/W2139454561A5051587506', 'https://semopenalex.org/authorship/W3132353162A5051587506', 'https://semopenalex.org/authorship/W1999134690A5051587506', 'https://semopenalex.org/authorship/W2119033694A5051587506', 'https://semopenalex.org/authorship/W2181791275A5051587506', 'https://semopenalex.org/authorship/W2554047600A5051587506', 'https://semopenalex.org/authorship/W2809782991A5056164318', 'https://semopenalex.org/authorship/W2995911827A5051587506', 'https://semopenalex.org/authorship/W3206895939A5051587506', 'https://semopenalex.org/authorship/W3200674364A5051587506', 'https://semopenalex.org/authorship/W4389921335A5051587506', 'https://semopenalex.org/authorship/W2564132746A5051587506', 'https://semopenalex.org/authorship/W4250489070A5051587506', 'https://semopenalex.org/authorship/W2138291705A5051587506', 'https://semopenalex.org/authorship/W1608886591A5056164318', 'https://semopenalex.org/authorship/W2768649200A5051587506', 'https://semopenalex.org/authorship/W2569889271A5051587506', 'https://semopenalex.org/authorship/W2983014989A5056164318', 'https://semopenalex.org/authorship/W2901316497A5051587506', 'https://semopenalex.org/authorship/W2804891820A50</t>
   </si>
 </sst>
 </file>

</xml_diff>